<commit_message>
Lesson plan file modified
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schedule\Documents\TIME_DK\time_colleges\SRET\Focus_Batch_2023-2027\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92244DDD-D22E-44BD-BD76-4E27C570A659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49EFC07-77B1-4ACC-B119-2818779BEA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -838,13 +849,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -866,14 +871,13 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -910,13 +914,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -941,31 +942,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC2EB891-804F-43E8-A06F-387079CE4D81}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC2EB891-804F-43E8-A06F-387079CE4D81}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:C20" xr:uid="{EC2EB891-804F-43E8-A06F-387079CE4D81}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BA9C8891-1203-46DA-B01A-4B17E8515E96}" name="Order" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{EDE8DF91-E7F4-45E1-911B-F8ABD4867ACA}" name="Topic" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{218431B5-9426-4E2F-BF73-B4A99D3E3320}" name="Hours" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{BA9C8891-1203-46DA-B01A-4B17E8515E96}" name="Order" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{EDE8DF91-E7F4-45E1-911B-F8ABD4867ACA}" name="Topic" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{218431B5-9426-4E2F-BF73-B4A99D3E3320}" name="Hours" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{512AC03F-78F7-4FEC-8505-F6AAC24DF528}" name="Table2" displayName="Table2" ref="A1:G108" totalsRowShown="0" headerRowDxfId="10" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{512AC03F-78F7-4FEC-8505-F6AAC24DF528}" name="Table2" displayName="Table2" ref="A1:G108" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:G108" xr:uid="{512AC03F-78F7-4FEC-8505-F6AAC24DF528}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G108">
     <sortCondition ref="A1:A108"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{911CBD74-C633-4B51-85BF-53095DEB2CC8}" name="S.No" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{5CF9DF08-2218-4086-957B-A763D40BD5FE}" name="Topic" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{BD3DE0D9-F294-4850-ABC3-4AC5AC389F23}" name="Subtopic" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{5CF9DF08-2218-4086-957B-A763D40BD5FE}" name="Topic" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{BD3DE0D9-F294-4850-ABC3-4AC5AC389F23}" name="Subtopic" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{D095E8DD-227D-4C1F-937E-D4545535A42D}" name="Hour" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{4ABDE408-207C-41EB-B0D2-66F110860C2E}" name="LeetCode Problem" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{0CD9435E-F9FD-44E9-A221-89DA8A3A11E6}" name="Level" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{C0930A4E-6BCC-4DFF-B424-04E79129EAAD}" name="Remark" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{4ABDE408-207C-41EB-B0D2-66F110860C2E}" name="LeetCode Problem" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{0CD9435E-F9FD-44E9-A221-89DA8A3A11E6}" name="Level" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{C0930A4E-6BCC-4DFF-B424-04E79129EAAD}" name="Remark" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1483,17 +1484,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47E1B90-F79D-473A-8C0F-D2580CDDC346}">
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3856,11 +3855,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>$G$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>$G$2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>$G$3</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Lesson plan: topic and subtopic column merged
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schedule\Documents\TIME_DK\time_colleges\SRET\Focus_Batch_2023-2027\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49EFC07-77B1-4ACC-B119-2818779BEA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FB88E0-C390-458B-9A64-257486D757ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,17 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -957,7 +946,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{512AC03F-78F7-4FEC-8505-F6AAC24DF528}" name="Table2" displayName="Table2" ref="A1:G108" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:G108" xr:uid="{512AC03F-78F7-4FEC-8505-F6AAC24DF528}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G108">
-    <sortCondition ref="A1:A108"/>
+    <sortCondition ref="D1:D108"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{911CBD74-C633-4B51-85BF-53095DEB2CC8}" name="S.No" dataDxfId="8"/>
@@ -1237,7 +1226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1482,9 +1473,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47E1B90-F79D-473A-8C0F-D2580CDDC346}">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1495,9 +1488,10 @@
     <col min="5" max="5" width="50.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -1520,7 +1514,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1542,64 +1536,80 @@
       <c r="G2" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>String: Hashing + Count</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
       <c r="E3" s="7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I3" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>String: Sliding Window</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="1"/>
       <c r="E4" s="7" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I4" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Array: Two Pointer</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>39</v>
@@ -1607,64 +1617,80 @@
       <c r="G5" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Array: Prefix / Sliding</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1"/>
       <c r="E6" s="7" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I6" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Recursion: Base Case + Tree View</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="1"/>
       <c r="E7" s="7" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I7" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Recursion: Divide and Conquer</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="1">
-        <v>3</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>39</v>
@@ -1672,64 +1698,80 @@
       <c r="G8" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Recursion: Subsets</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
       <c r="E9" s="7" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I9" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Searching: Binary Search Basic</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="D10" s="1">
+        <v>11</v>
+      </c>
       <c r="E10" s="7" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I10" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Searching: BS on Answer</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="D11" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>39</v>
@@ -1737,194 +1779,242 @@
       <c r="G11" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Sorting: Basic Sorting Logic</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="D12" s="1">
+        <v>13</v>
+      </c>
       <c r="E12" s="7" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I12" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Sorting: Custom Comparator</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="D13" s="1">
+        <v>14</v>
+      </c>
       <c r="E13" s="7" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I13" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Sorting: Merge Intervals</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="D14" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Sorting: Scheduling Logic</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>99</v>
+      </c>
+      <c r="D15" s="1">
+        <v>16</v>
+      </c>
       <c r="E15" s="7" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I15" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: Reverse LL</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="D16" s="1">
+        <v>17</v>
+      </c>
       <c r="E16" s="7" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I16" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: Detect Cycle</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="D17" s="1">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: Merge LL</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="1">
+        <v>19</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: Intersection Point</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>50</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="1">
+        <v>20</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: Palindrome Check</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>52</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="D20" s="1">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>39</v>
@@ -1932,64 +2022,80 @@
       <c r="G20" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: LRU Cache Logic</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="D21" s="1">
+        <v>22</v>
+      </c>
       <c r="E21" s="7" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I21" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Stack: Stack Basics</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="D22" s="1">
+        <v>23</v>
+      </c>
       <c r="E22" s="7" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I22" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Stack: Monotonic Stack</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="D23" s="1">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>31</v>
@@ -1997,169 +2103,213 @@
       <c r="G23" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Queue: Queue + BFS Intro</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="D24" s="1">
+        <v>25</v>
+      </c>
       <c r="E24" s="7" t="s">
-        <v>74</v>
+        <v>138</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I24" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Queue: Circular Queue</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="D25" s="1">
+        <v>26</v>
+      </c>
       <c r="E25" s="7" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I25" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Queue: Monotonic Queue</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="D26" s="1">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Trees: Traversals</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
+        <v>68</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D27" s="1">
+        <v>28</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="G27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>BST: Search, Insert, Min</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>70</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="B28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D28" s="1">
+        <v>29</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>BST: Validate BST</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>81</v>
+        <v>158</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="D29" s="1">
-        <v>12</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>83</v>
+        <v>30</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I29" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Balanced Tree: AVL Tree</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>74</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" s="1">
+        <v>31</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>34</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Heap: Min Heap Introduction</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="1"/>
+        <v>170</v>
+      </c>
+      <c r="D31" s="1">
+        <v>32</v>
+      </c>
       <c r="E31" s="7" t="s">
         <v>87</v>
       </c>
@@ -2167,24 +2317,28 @@
         <v>39</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I31" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Heap: Kth Largest Element</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
       <c r="D32" s="1">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>39</v>
@@ -2192,43 +2346,53 @@
       <c r="G32" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Heap: Heap + Sorting Logic</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="1"/>
+        <v>178</v>
+      </c>
+      <c r="D33" s="1">
+        <v>34</v>
+      </c>
       <c r="E33" s="7" t="s">
-        <v>90</v>
+        <v>179</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I33" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>HashMap: Frequency Counting</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>91</v>
+        <v>183</v>
       </c>
       <c r="D34" s="1">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>39</v>
@@ -2236,43 +2400,53 @@
       <c r="G34" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I34" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>HashMap: Prefix Sum Technique</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D35" s="1"/>
+        <v>186</v>
+      </c>
+      <c r="D35" s="1">
+        <v>36</v>
+      </c>
       <c r="E35" s="7" t="s">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I35" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>HashMap: Grouping Data</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>81</v>
+        <v>190</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>94</v>
+        <v>191</v>
       </c>
       <c r="D36" s="1">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>95</v>
+        <v>192</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>39</v>
@@ -2280,240 +2454,290 @@
       <c r="G36" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Graph: BFS Traversal</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>81</v>
+        <v>190</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D37" s="1"/>
+        <v>197</v>
+      </c>
+      <c r="D37" s="1">
+        <v>38</v>
+      </c>
       <c r="E37" s="7" t="s">
-        <v>97</v>
+        <v>198</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I37" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Graph: Dijkstra’s (Shortest Path)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>98</v>
+        <v>190</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>99</v>
+        <v>203</v>
       </c>
       <c r="D38" s="1">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>100</v>
+        <v>204</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I38" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Graph: Topological Sort</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>98</v>
+        <v>209</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D39" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D39" s="1">
+        <v>40</v>
+      </c>
       <c r="E39" s="7" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I39" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>DP: Fibonacci with Memo</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>98</v>
+        <v>209</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>103</v>
+        <v>215</v>
       </c>
       <c r="D40" s="1">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I40" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>DP: Longest Common Subseq</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>98</v>
+        <v>209</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D41" s="1">
+        <v>42</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I41" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>DP: Unique Paths (2D Grid)</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>105</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>46</v>
-      </c>
       <c r="B42" s="3" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>107</v>
+        <v>227</v>
       </c>
       <c r="D42" s="1">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I42" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Greedy: Activity Selection (Intervals)</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D43" s="1"/>
+        <v>231</v>
+      </c>
+      <c r="D43" s="1">
+        <v>44</v>
+      </c>
       <c r="E43" s="7" t="s">
-        <v>110</v>
+        <v>232</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I43" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Greedy: Job Scheduling / Max Profit</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>98</v>
+        <v>237</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>111</v>
+        <v>238</v>
       </c>
       <c r="D44" s="1">
-        <v>19</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>112</v>
+        <v>45</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>31</v>
+        <v>240</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I44" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Review: Strategy + Topic Recap</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="7" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I45" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>String: Frequency Matching</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D46" s="1">
-        <v>20</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D46" s="1"/>
       <c r="E46" s="7" t="s">
-        <v>116</v>
+        <v>36</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I46" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>String: Frequency Matching</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="7" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>39</v>
@@ -2521,131 +2745,149 @@
       <c r="G47" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I47" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>String: Sliding Window</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D48" s="1">
-        <v>21</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D48" s="1"/>
       <c r="E48" s="7" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I48" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>String: Sliding Window</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>121</v>
+        <v>44</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="7" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I49" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Array: Two Pointer</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D50" s="1">
-        <v>22</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D50" s="1"/>
       <c r="E50" s="7" t="s">
-        <v>124</v>
+        <v>47</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I50" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Array: Two Pointer</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>123</v>
+        <v>48</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="7" t="s">
-        <v>125</v>
+        <v>50</v>
       </c>
       <c r="F51" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I51" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Array: Prefix / Sliding</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>12</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G51" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>56</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D52" s="1">
-        <v>23</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="G52" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I52" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Array: Prefix / Sliding</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="7" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>31</v>
@@ -2653,108 +2895,124 @@
       <c r="G53" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I53" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Recursion: Base Case Practice</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="7" t="s">
-        <v>131</v>
+        <v>58</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I54" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Recursion: Fibonacci</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
+        <v>17</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D55" s="1">
-        <v>24</v>
-      </c>
+      <c r="D55" s="1"/>
       <c r="E55" s="7" t="s">
-        <v>134</v>
+        <v>61</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I55" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Recursion: Divide and Conquer</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>135</v>
+        <v>62</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="7" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I56" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Recursion: Binary Recursion Tree</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D57" s="1">
-        <v>25</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D57" s="1"/>
       <c r="E57" s="7" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I57" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Recursion: Rec. with State</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>139</v>
+        <v>68</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="7" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>39</v>
@@ -2762,87 +3020,99 @@
       <c r="G58" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I58" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Recursion: Backtrack Base</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D59" s="1">
-        <v>26</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D59" s="1"/>
       <c r="E59" s="7" t="s">
-        <v>142</v>
+        <v>74</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I59" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Searching: First/Last Occurrence</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="7" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="F60" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I60" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Searching: Peak Element</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>31</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G60" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>65</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D61" s="1">
-        <v>27</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="G61" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I61" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Searching: BS on Answer</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>66</v>
-      </c>
       <c r="B62" s="3" t="s">
-        <v>144</v>
+        <v>70</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>145</v>
+        <v>77</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="7" t="s">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>39</v>
@@ -2850,20 +3120,24 @@
       <c r="G62" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I62" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Searching: BS on Answer</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="7" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>39</v>
@@ -2871,87 +3145,99 @@
       <c r="G63" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I63" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Sorting: Selection Practice</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D64" s="1">
-        <v>28</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D64" s="1"/>
       <c r="E64" s="7" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I64" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Sorting: QuickSort</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="7" t="s">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I65" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Sorting: Custom Comparator</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D66" s="1">
-        <v>29</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D66" s="1"/>
       <c r="E66" s="7" t="s">
-        <v>155</v>
+        <v>93</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I66" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Sorting: Merge Intervals</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="7" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>39</v>
@@ -2959,87 +3245,99 @@
       <c r="G67" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I67" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Sorting: Sorting Based Greedy</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>158</v>
+        <v>98</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D68" s="1">
-        <v>30</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>160</v>
+        <v>101</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I68" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: Reverse LL II</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>158</v>
+        <v>98</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>163</v>
+        <v>105</v>
       </c>
       <c r="D69" s="1"/>
-      <c r="E69" s="3" t="s">
-        <v>160</v>
+      <c r="E69" s="7" t="s">
+        <v>106</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I69" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: Cycle II</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D70" s="1">
-        <v>31</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="D70" s="1"/>
       <c r="E70" s="7" t="s">
-        <v>167</v>
+        <v>110</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I70" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: Merge k Lists</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="7" t="s">
-        <v>169</v>
+        <v>114</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>39</v>
@@ -3047,131 +3345,149 @@
       <c r="G71" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I71" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: Remove Nth Node</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D72" s="1">
-        <v>32</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D72" s="1"/>
       <c r="E72" s="7" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I72" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: Odd Even Index</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="7" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I73" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Linked List: Advanced LRU Logic</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>165</v>
+        <v>9</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D74" s="1">
-        <v>33</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D74" s="1"/>
       <c r="E74" s="7" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I74" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Stack: Stack Basics</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>165</v>
+        <v>9</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>175</v>
+        <v>128</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="7" t="s">
-        <v>176</v>
+        <v>129</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I75" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Stack: Next Greater Element</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D76" s="1">
-        <v>34</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D76" s="1"/>
       <c r="E76" s="7" t="s">
-        <v>179</v>
+        <v>131</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I76" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Stack: Largest Rect in Hist</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>177</v>
+        <v>132</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="7" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>31</v>
@@ -3179,64 +3495,74 @@
       <c r="G77" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I77" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Queue: Implement Queue Using Stacks</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>181</v>
+        <v>139</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="7" t="s">
-        <v>182</v>
+        <v>140</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I78" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Queue: Deque</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>177</v>
+        <v>132</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D79" s="1">
-        <v>35</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="D79" s="1"/>
       <c r="E79" s="7" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I79" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Queue: Monotonic Queue</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>184</v>
+        <v>145</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="7" t="s">
-        <v>185</v>
+        <v>147</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>39</v>
@@ -3244,43 +3570,49 @@
       <c r="G80" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I80" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Trees: Traversals</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D81" s="1">
-        <v>36</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="D81" s="1"/>
       <c r="E81" s="7" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I81" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Trees: Views + Height</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>177</v>
+        <v>12</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>188</v>
+        <v>152</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="7" t="s">
-        <v>189</v>
+        <v>153</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>39</v>
@@ -3288,64 +3620,74 @@
       <c r="G82" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I82" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>BST: Deletion</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D83" s="1">
-        <v>37</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="D83" s="1"/>
       <c r="E83" s="7" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I83" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>BST: Lowest Common Ancestor</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="D84" s="1"/>
-      <c r="E84" s="7" t="s">
-        <v>194</v>
+      <c r="E84" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="I84" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Balanced Tree: Red-Black Tree</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="7" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>39</v>
@@ -3353,43 +3695,49 @@
       <c r="G85" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I85" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Heap: Priority Queue Usage</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D86" s="1">
-        <v>38</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D86" s="1"/>
       <c r="E86" s="7" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I86" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Heap: Kth Smallest Element</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="7" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>39</v>
@@ -3397,64 +3745,74 @@
       <c r="G87" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I87" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Heap: Heap + Custom Comparator</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="7" t="s">
-        <v>202</v>
+        <v>34</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G88" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I88" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>HashMap: Frequency Counting</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D89" s="1">
-        <v>39</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="D89" s="1"/>
       <c r="E89" s="7" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I89" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>HashSet: Uniqueness Check</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="7" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="F90" s="3" t="s">
         <v>39</v>
@@ -3462,20 +3820,24 @@
       <c r="G90" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I90" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>HashMap: Prefix Sum Variation</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="7" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>39</v>
@@ -3483,108 +3845,124 @@
       <c r="G91" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I91" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>HashMap: Longest Streak/Length</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D92" s="1">
-        <v>40</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="D92" s="1"/>
       <c r="E92" s="7" t="s">
-        <v>58</v>
+        <v>194</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I92" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Graph: DFS Traversal</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="7" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I93" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Graph: BFS with Distance</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="7" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G94" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I94" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Graph: Union Find</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D95" s="1">
-        <v>41</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="D95" s="1"/>
       <c r="E95" s="7" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I95" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Graph: Cycle Detection</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="7" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="F96" s="3" t="s">
         <v>39</v>
@@ -3592,20 +3970,24 @@
       <c r="G96" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I96" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Graph: Topo + Ordering</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="7" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="F97" s="3" t="s">
         <v>39</v>
@@ -3613,64 +3995,74 @@
       <c r="G97" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I97" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Graph: Kahn’s Algorithm</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>209</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="D98" s="1">
-        <v>42</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="D98" s="1"/>
       <c r="E98" s="7" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I98" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>DP: Climbing Stairs (1D)</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>209</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="7" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G99" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I99" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>DP: Min Cost Climbing</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>209</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="7" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>39</v>
@@ -3678,43 +4070,49 @@
       <c r="G100" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I100" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>DP: Longest Increasing Subseq</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>20</v>
+        <v>209</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D101" s="1">
-        <v>43</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="D101" s="1"/>
       <c r="E101" s="7" t="s">
-        <v>95</v>
+        <v>220</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I101" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>DP: Palindromic Substrings</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>20</v>
+        <v>209</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="7" t="s">
-        <v>92</v>
+        <v>224</v>
       </c>
       <c r="F102" s="3" t="s">
         <v>39</v>
@@ -3722,20 +4120,24 @@
       <c r="G102" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I102" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>DP: Partition Equal Sum</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>20</v>
+        <v>209</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>39</v>
@@ -3743,96 +4145,112 @@
       <c r="G103" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I103" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>DP: Target Sum (state model)</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="D104" s="1">
-        <v>44</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="D104" s="1"/>
       <c r="E104" s="7" t="s">
-        <v>232</v>
+        <v>92</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I104" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Greedy: Interval Merging</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I105" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Greedy: Gas Station Problem</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I106" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Greedy: Resource Assignment</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>110</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D107" s="1"/>
+      <c r="E107" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="F106" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <v>111</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="D107" s="1">
-        <v>45</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>239</v>
-      </c>
       <c r="F107" s="3" t="s">
-        <v>240</v>
+        <v>39</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I107" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Greedy: Jump Game</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>112</v>
       </c>
@@ -3851,6 +4269,10 @@
       </c>
       <c r="G108" s="3" t="s">
         <v>35</v>
+      </c>
+      <c r="I108" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Review: Mock Contest (3–4 problems)</v>
       </c>
     </row>
   </sheetData>
@@ -3864,112 +4286,113 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="https://leetcode.com/problems/first-unique-character-in-a-string" xr:uid="{CACA8992-DEBC-4969-B2F6-EBA7FDC085C1}"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://leetcode.com/problems/ransom-note" xr:uid="{9ACCC9FD-0DC8-4254-BB8B-808F3BDD3784}"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://leetcode.com/problems/valid-anagram" xr:uid="{EE4FEEAF-652D-4D2D-A2A9-CB87731F42BE}"/>
-    <hyperlink ref="E5" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters" xr:uid="{4DD7CB8D-B440-4AF4-B6AB-D727391B9158}"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string" xr:uid="{7CCC4C5F-1CA6-46F8-9DD3-9647C7682498}"/>
-    <hyperlink ref="E7" r:id="rId6" display="https://leetcode.com/problems/minimum-window-substring" xr:uid="{61B1900B-EAF8-4BE8-ACAB-A956DE5F3ED1}"/>
-    <hyperlink ref="E8" r:id="rId7" display="https://leetcode.com/problems/container-with-most-water" xr:uid="{84B1B8CA-3A3C-4909-8DD8-F88A45D68628}"/>
-    <hyperlink ref="E9" r:id="rId8" display="https://leetcode.com/problems/3sum" xr:uid="{42633795-6F73-49FF-B778-78E0CD056E83}"/>
-    <hyperlink ref="E10" r:id="rId9" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array" xr:uid="{DFA525B5-0825-451E-B3E0-9DC93194D4E1}"/>
-    <hyperlink ref="E11" r:id="rId10" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{3640DDE9-2ADF-42E2-AEDE-DA2AC3BA211A}"/>
-    <hyperlink ref="E12" r:id="rId11" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k" xr:uid="{8062781F-458E-4926-B311-804BA6CD3BBB}"/>
-    <hyperlink ref="E13" r:id="rId12" display="https://leetcode.com/problems/maximum-subarray" xr:uid="{3AD35EF8-0181-42B2-9B38-F0FC3F95CFE6}"/>
-    <hyperlink ref="E14" r:id="rId13" display="https://leetcode.com/problems/maximum-depth-of-binary-tree" xr:uid="{44C26DDF-9EB7-417D-B269-6C23AC6E6445}"/>
-    <hyperlink ref="E15" r:id="rId14" display="https://leetcode.com/problems/invert-binary-tree" xr:uid="{14199D52-1EAC-49F1-8883-00C4203FC3E3}"/>
-    <hyperlink ref="E16" r:id="rId15" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{52E248D0-3A46-4957-B7A0-F75EBA672C5B}"/>
-    <hyperlink ref="E17" r:id="rId16" display="https://leetcode.com/problems/different-ways-to-add-parentheses" xr:uid="{9DA410A2-6C01-4EDA-9F51-6FBA009D88DF}"/>
-    <hyperlink ref="E18" r:id="rId17" display="https://leetcode.com/problems/unique-binary-search-trees-ii" xr:uid="{68A314C1-D173-4545-AF04-B8E2F74F893D}"/>
-    <hyperlink ref="E19" r:id="rId18" display="https://leetcode.com/problems/powx-n" xr:uid="{26A0C127-23BD-4BCE-8BC7-8AB1A8F90ADE}"/>
-    <hyperlink ref="E20" r:id="rId19" display="https://leetcode.com/problems/subsets" xr:uid="{22D9BCEB-5D0D-4BEF-A700-0FC47638B9F3}"/>
-    <hyperlink ref="E21" r:id="rId20" display="https://leetcode.com/problems/permutations" xr:uid="{E47F3CB1-204D-4424-914C-698242057FAC}"/>
-    <hyperlink ref="E22" r:id="rId21" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{5F57D8FD-824D-4DB1-892E-1DDFD0F8F33D}"/>
-    <hyperlink ref="E23" r:id="rId22" display="https://leetcode.com/problems/binary-search" xr:uid="{374FFDAF-FCB9-431A-86D2-31AB60378C3A}"/>
-    <hyperlink ref="E24" r:id="rId23" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array" xr:uid="{3F271E59-4045-4398-82DB-BC2F4B35A995}"/>
-    <hyperlink ref="E25" r:id="rId24" display="https://leetcode.com/problems/find-peak-element" xr:uid="{DEF2D431-80D6-4E0B-868E-499158EC2963}"/>
-    <hyperlink ref="E26" r:id="rId25" display="https://leetcode.com/problems/koko-eating-bananas" xr:uid="{B3E73AEB-2A95-4916-A93C-BC5B60CAA1D7}"/>
-    <hyperlink ref="E27" r:id="rId26" display="https://leetcode.com/problems/split-array-largest-sum" xr:uid="{BCAC5094-3A8A-4714-BD84-F606403D9DA0}"/>
-    <hyperlink ref="E28" r:id="rId27" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days" xr:uid="{1965E795-8B07-42CA-9865-3EEF521E25E1}"/>
-    <hyperlink ref="E29" r:id="rId28" display="https://leetcode.com/problems/sort-an-array" xr:uid="{E0B9E0A6-F8E5-418F-87DD-47E7F6723CFF}"/>
-    <hyperlink ref="E30" r:id="rId29" display="https://leetcode.com/problems/insertion-sort-list" xr:uid="{03811762-664A-488F-9B2D-036EAE5AAD21}"/>
-    <hyperlink ref="E31" r:id="rId30" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{4F771129-F99D-4F68-954B-762315CE30B8}"/>
-    <hyperlink ref="E32" r:id="rId31" display="https://leetcode.com/problems/largest-number" xr:uid="{373767EF-F0B1-409B-B448-2E15DEE2A726}"/>
-    <hyperlink ref="E33" r:id="rId32" display="https://leetcode.com/problems/reorder-data-in-log-files" xr:uid="{A0B197A5-BF64-4823-8C80-786CEECF12F4}"/>
-    <hyperlink ref="E34" r:id="rId33" display="https://leetcode.com/problems/merge-intervals" xr:uid="{04E9289A-1232-436E-8E31-F058BBB75316}"/>
-    <hyperlink ref="E35" r:id="rId34" display="https://leetcode.com/problems/insert-interval" xr:uid="{355C5E3F-38DD-4154-ACB8-71E37347CA2D}"/>
-    <hyperlink ref="E36" r:id="rId35" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{73B2795D-90B0-4FEF-BAE2-297C16F48CD8}"/>
-    <hyperlink ref="E37" r:id="rId36" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{A4102035-5F89-45CA-99F6-62571131E444}"/>
-    <hyperlink ref="E38" r:id="rId37" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{213E0623-CF2A-4978-9133-4CAD9B8DDC70}"/>
-    <hyperlink ref="E39" r:id="rId38" display="https://leetcode.com/problems/reverse-linked-list-ii" xr:uid="{3E496F01-EEA1-4941-97A8-3FA083834977}"/>
-    <hyperlink ref="E40" r:id="rId39" display="https://leetcode.com/problems/linked-list-cycle" xr:uid="{9C26BB6C-78AB-4618-BD00-77BAAF16815D}"/>
-    <hyperlink ref="E41" r:id="rId40" display="https://leetcode.com/problems/linked-list-cycle-ii" xr:uid="{EC5A3D70-F195-4C10-9EA2-058F32835B9E}"/>
-    <hyperlink ref="E42" r:id="rId41" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{5C4F4E4B-2209-41D3-A906-19E1F708F9DB}"/>
-    <hyperlink ref="E43" r:id="rId42" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{1C1B8A5C-EA41-461E-8FA3-BD6A6B5B3181}"/>
-    <hyperlink ref="E44" r:id="rId43" display="https://leetcode.com/problems/intersection-of-two-linked-lists" xr:uid="{606E5182-D172-41A2-9D50-33C726FC8AB7}"/>
-    <hyperlink ref="E45" r:id="rId44" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{CD69A99D-FBAA-46B5-B0DF-9DE5139BE679}"/>
-    <hyperlink ref="E46" r:id="rId45" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{5D746582-1B54-4352-BDA4-86F05542CE88}"/>
-    <hyperlink ref="E47" r:id="rId46" display="https://leetcode.com/problems/odd-even-linked-list" xr:uid="{C89465FE-7C33-4395-99CB-4BA5D7CED11B}"/>
-    <hyperlink ref="E48" r:id="rId47" display="https://leetcode.com/problems/lru-cache" xr:uid="{05D0EB4C-0E5B-4E3E-AAB2-1A648C9129E7}"/>
-    <hyperlink ref="E49" r:id="rId48" display="https://leetcode.com/problems/lfu-cache" xr:uid="{DF951C59-83C3-4B8E-98CC-B79E487C918E}"/>
-    <hyperlink ref="E50" r:id="rId49" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{91E7DBEA-4D8A-41C9-AAC9-D9BA3BCE6D19}"/>
-    <hyperlink ref="E51" r:id="rId50" display="https://leetcode.com/problems/backspace-string-compare" xr:uid="{BD0B5108-E7EF-4D79-983A-AF8C10DCB73C}"/>
-    <hyperlink ref="E52" r:id="rId51" display="https://leetcode.com/problems/daily-temperatures" xr:uid="{B087D9B6-012A-40BD-B913-355D4FBD2EFE}"/>
-    <hyperlink ref="E53" r:id="rId52" display="https://leetcode.com/problems/next-greater-element-i" xr:uid="{FB709363-8602-45D4-B45B-8C9367125A7E}"/>
-    <hyperlink ref="E54" r:id="rId53" display="https://leetcode.com/problems/largest-rectangle-in-histogram" xr:uid="{704BEAA6-4976-4029-886F-A6FDCC20AE13}"/>
-    <hyperlink ref="E60" r:id="rId54" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k" xr:uid="{C9B7F519-FC85-48AA-93F2-FB21BD51100E}"/>
-    <hyperlink ref="E59" r:id="rId55" display="https://leetcode.com/problems/sliding-window-maximum" xr:uid="{700AEA2A-73EB-45E0-A7C4-C9B375DDFDD1}"/>
-    <hyperlink ref="E58" r:id="rId56" display="https://leetcode.com/problems/design-circular-deque" xr:uid="{C374A6F7-208C-4F78-840A-5324F48EA186}"/>
-    <hyperlink ref="E57" r:id="rId57" display="https://leetcode.com/problems/design-circular-queue" xr:uid="{9290B313-663F-43FF-8027-AB89DA22F6BD}"/>
-    <hyperlink ref="E56" r:id="rId58" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{8802B7B3-B0D3-4F45-83F5-C1CF53DB69A6}"/>
-    <hyperlink ref="E55" r:id="rId59" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{2B0D8F07-EC59-4BAD-93CF-98C511AC3E21}"/>
-    <hyperlink ref="E61" r:id="rId60" display="https://leetcode.com/problems/binary-tree-inorder-traversal" xr:uid="{1B856373-DA81-4D15-ACC2-F7C093A506A8}"/>
-    <hyperlink ref="E62" r:id="rId61" display="https://leetcode.com/problems/binary-tree-level-order-traversal" xr:uid="{6AAEF83E-F9D9-409A-927C-DDEE7AEA57FC}"/>
-    <hyperlink ref="E63" r:id="rId62" display="https://leetcode.com/problems/binary-tree-right-side-view" xr:uid="{5577EFF4-DB1A-480F-83F5-F19EDE79C4B5}"/>
-    <hyperlink ref="E64" r:id="rId63" display="https://leetcode.com/problems/search-in-a-binary-search-tree" xr:uid="{A758D8A5-36A2-40FF-A15F-1A6A7A69801A}"/>
-    <hyperlink ref="E65" r:id="rId64" display="https://leetcode.com/problems/delete-node-in-a-bst" xr:uid="{591B7EA7-3888-49B3-99EF-BA629CD9A02D}"/>
-    <hyperlink ref="E66" r:id="rId65" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{78FB8ABE-DFC4-47EA-ACA0-CFB46543B8DC}"/>
-    <hyperlink ref="E67" r:id="rId66" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree" xr:uid="{5AA82C0A-C3F6-4840-B663-78DC8E56D219}"/>
-    <hyperlink ref="E70" r:id="rId67" display="https://leetcode.com/problems/last-stone-weight" xr:uid="{CAD60500-B89D-4C41-8574-D33E4F0BB32A}"/>
-    <hyperlink ref="E71" r:id="rId68" display="https://leetcode.com/problems/k-closest-points-to-origin" xr:uid="{BBD06487-6DC3-4A9B-83CC-F430BAF527D5}"/>
-    <hyperlink ref="E72" r:id="rId69" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{88E6C8C5-7B90-4A92-BECC-A629C8A55FEC}"/>
-    <hyperlink ref="E73" r:id="rId70" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix" xr:uid="{4C161606-D259-4AC4-BDFF-44E161BFF6BD}"/>
-    <hyperlink ref="E74" r:id="rId71" display="https://leetcode.com/problems/top-k-frequent-words" xr:uid="{4FD04348-E4BE-4F5E-83FD-752D5452B19E}"/>
-    <hyperlink ref="E75" r:id="rId72" display="https://leetcode.com/problems/top-k-frequent-elements" xr:uid="{31ABA819-3C4C-4002-8FCF-364AEF9823BD}"/>
-    <hyperlink ref="E76" r:id="rId73" display="https://leetcode.com/problems/two-sum" xr:uid="{5B404BE5-D0E3-4728-8498-75AFA5031304}"/>
-    <hyperlink ref="E77" r:id="rId74" display="https://leetcode.com/problems/ransom-note" xr:uid="{E50D5A6F-DB16-4D48-974E-C7847334D093}"/>
-    <hyperlink ref="E78" r:id="rId75" display="https://leetcode.com/problems/contains-duplicate" xr:uid="{EEA73F8B-13F1-431E-A0F1-3A0C6B23527D}"/>
-    <hyperlink ref="E79" r:id="rId76" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{4D7D4589-2B8A-47DC-9FCF-904D6E82FB71}"/>
-    <hyperlink ref="E80" r:id="rId77" display="https://leetcode.com/problems/subarray-sums-divisible-by-k" xr:uid="{D838CB32-0488-4C04-951B-6AA80F72BEA1}"/>
-    <hyperlink ref="E81" r:id="rId78" display="https://leetcode.com/problems/group-anagrams" xr:uid="{E64749FE-4AC2-4B2B-91C7-7180E2DCC00B}"/>
-    <hyperlink ref="E82" r:id="rId79" display="https://leetcode.com/problems/longest-consecutive-sequence" xr:uid="{DE30C124-13F2-439B-9476-17D8DAC27129}"/>
-    <hyperlink ref="E83" r:id="rId80" display="https://leetcode.com/problems/number-of-islands" xr:uid="{8DBAE9D8-4931-4C16-AEED-F66841DA88D4}"/>
-    <hyperlink ref="E84" r:id="rId81" display="https://leetcode.com/problems/max-area-of-island" xr:uid="{1B4C9834-1FC5-4895-806E-038B1DBDDA4B}"/>
-    <hyperlink ref="E85" r:id="rId82" display="https://leetcode.com/problems/01-matrix" xr:uid="{A0E46D51-24FB-432C-9B64-F9A7D564ADF2}"/>
-    <hyperlink ref="E86" r:id="rId83" display="https://leetcode.com/problems/network-delay-time" xr:uid="{F759E8D2-9590-49C8-B0C1-9FDC2453A281}"/>
-    <hyperlink ref="E87" r:id="rId84" display="https://leetcode.com/problems/redundant-connection" xr:uid="{EB3F5CE4-E5E9-420F-8C29-1A45626B6B12}"/>
-    <hyperlink ref="E88" r:id="rId85" display="https://leetcode.com/problems/number-of-provinces" xr:uid="{7F9CCD13-89BD-4996-B7B2-71D1985A3440}"/>
-    <hyperlink ref="E89" r:id="rId86" display="https://leetcode.com/problems/course-schedule" xr:uid="{1BB86DA6-53E2-4F87-8150-7BF6C57A100C}"/>
-    <hyperlink ref="E90" r:id="rId87" display="https://leetcode.com/problems/course-schedule-ii" xr:uid="{5177CC97-2B77-43CF-B33F-3903154A502D}"/>
-    <hyperlink ref="E91" r:id="rId88" display="https://leetcode.com/problems/clone-graph" xr:uid="{16DC6C12-1E3C-4E22-B3FF-A38677E0B8F3}"/>
-    <hyperlink ref="E92" r:id="rId89" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{8E820236-2EA3-409B-AA9C-D43A03343FCB}"/>
-    <hyperlink ref="E93" r:id="rId90" display="https://leetcode.com/problems/climbing-stairs" xr:uid="{40181C74-4968-41A8-B229-0DF250C3A787}"/>
-    <hyperlink ref="E94" r:id="rId91" display="https://leetcode.com/problems/min-cost-climbing-stairs" xr:uid="{9E7BFCA6-DA59-48A0-975B-9589BDC7C276}"/>
-    <hyperlink ref="E95" r:id="rId92" display="https://leetcode.com/problems/longest-common-subsequence" xr:uid="{30F8CF6D-7369-4957-A7D7-160A741AA38C}"/>
-    <hyperlink ref="E96" r:id="rId93" display="https://leetcode.com/problems/longest-increasing-subsequence" xr:uid="{0B0509FA-0F85-46F0-803E-3112FAE33195}"/>
-    <hyperlink ref="E97" r:id="rId94" display="https://leetcode.com/problems/palindromic-substrings" xr:uid="{DAA8A2AD-4DEC-4740-BE2E-FF2A710FC881}"/>
-    <hyperlink ref="E98" r:id="rId95" display="https://leetcode.com/problems/unique-paths" xr:uid="{3BFACFF5-9CEA-445E-837D-80CE02DD15B6}"/>
-    <hyperlink ref="E99" r:id="rId96" display="https://leetcode.com/problems/partition-equal-subset-sum" xr:uid="{7588C036-6A20-4C85-94EE-72396427AA61}"/>
-    <hyperlink ref="E100" r:id="rId97" display="https://leetcode.com/problems/target-sum" xr:uid="{B8B2404F-6A1D-4008-9903-335EA651A7DC}"/>
-    <hyperlink ref="E101" r:id="rId98" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{6B9267CD-AC96-447A-879D-41081B74ECAC}"/>
-    <hyperlink ref="E102" r:id="rId99" display="https://leetcode.com/problems/merge-intervals" xr:uid="{C1AA793D-64CD-400D-A0A9-D182B005CEDC}"/>
-    <hyperlink ref="E103" r:id="rId100" display="https://leetcode.com/problems/gas-station" xr:uid="{9A4CC2B1-7301-4996-8463-5549D190A892}"/>
-    <hyperlink ref="E104" r:id="rId101" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{9AF79B77-6ADE-45DC-A721-A6C56EA49A98}"/>
-    <hyperlink ref="E105" r:id="rId102" display="https://leetcode.com/problems/can-place-flowers" xr:uid="{9BBCC8E1-2E28-48FF-9415-D9250E2D1CFB}"/>
-    <hyperlink ref="E106" r:id="rId103" display="https://leetcode.com/problems/jump-game" xr:uid="{22D973B8-6E8A-41F7-BF66-D13FE9CE93A0}"/>
+    <hyperlink ref="E45" r:id="rId2" display="https://leetcode.com/problems/ransom-note" xr:uid="{9ACCC9FD-0DC8-4254-BB8B-808F3BDD3784}"/>
+    <hyperlink ref="E46" r:id="rId3" display="https://leetcode.com/problems/valid-anagram" xr:uid="{EE4FEEAF-652D-4D2D-A2A9-CB87731F42BE}"/>
+    <hyperlink ref="E3" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters" xr:uid="{4DD7CB8D-B440-4AF4-B6AB-D727391B9158}"/>
+    <hyperlink ref="E47" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string" xr:uid="{7CCC4C5F-1CA6-46F8-9DD3-9647C7682498}"/>
+    <hyperlink ref="E48" r:id="rId6" display="https://leetcode.com/problems/minimum-window-substring" xr:uid="{61B1900B-EAF8-4BE8-ACAB-A956DE5F3ED1}"/>
+    <hyperlink ref="E4" r:id="rId7" display="https://leetcode.com/problems/container-with-most-water" xr:uid="{84B1B8CA-3A3C-4909-8DD8-F88A45D68628}"/>
+    <hyperlink ref="E49" r:id="rId8" display="https://leetcode.com/problems/3sum" xr:uid="{42633795-6F73-49FF-B778-78E0CD056E83}"/>
+    <hyperlink ref="E50" r:id="rId9" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array" xr:uid="{DFA525B5-0825-451E-B3E0-9DC93194D4E1}"/>
+    <hyperlink ref="E5" r:id="rId10" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{3640DDE9-2ADF-42E2-AEDE-DA2AC3BA211A}"/>
+    <hyperlink ref="E51" r:id="rId11" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k" xr:uid="{8062781F-458E-4926-B311-804BA6CD3BBB}"/>
+    <hyperlink ref="E52" r:id="rId12" display="https://leetcode.com/problems/maximum-subarray" xr:uid="{3AD35EF8-0181-42B2-9B38-F0FC3F95CFE6}"/>
+    <hyperlink ref="E6" r:id="rId13" display="https://leetcode.com/problems/maximum-depth-of-binary-tree" xr:uid="{44C26DDF-9EB7-417D-B269-6C23AC6E6445}"/>
+    <hyperlink ref="E53" r:id="rId14" display="https://leetcode.com/problems/invert-binary-tree" xr:uid="{14199D52-1EAC-49F1-8883-00C4203FC3E3}"/>
+    <hyperlink ref="E54" r:id="rId15" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{52E248D0-3A46-4957-B7A0-F75EBA672C5B}"/>
+    <hyperlink ref="E7" r:id="rId16" display="https://leetcode.com/problems/different-ways-to-add-parentheses" xr:uid="{9DA410A2-6C01-4EDA-9F51-6FBA009D88DF}"/>
+    <hyperlink ref="E55" r:id="rId17" display="https://leetcode.com/problems/unique-binary-search-trees-ii" xr:uid="{68A314C1-D173-4545-AF04-B8E2F74F893D}"/>
+    <hyperlink ref="E56" r:id="rId18" display="https://leetcode.com/problems/powx-n" xr:uid="{26A0C127-23BD-4BCE-8BC7-8AB1A8F90ADE}"/>
+    <hyperlink ref="E8" r:id="rId19" display="https://leetcode.com/problems/subsets" xr:uid="{22D9BCEB-5D0D-4BEF-A700-0FC47638B9F3}"/>
+    <hyperlink ref="E57" r:id="rId20" display="https://leetcode.com/problems/permutations" xr:uid="{E47F3CB1-204D-4424-914C-698242057FAC}"/>
+    <hyperlink ref="E58" r:id="rId21" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{5F57D8FD-824D-4DB1-892E-1DDFD0F8F33D}"/>
+    <hyperlink ref="E9" r:id="rId22" display="https://leetcode.com/problems/binary-search" xr:uid="{374FFDAF-FCB9-431A-86D2-31AB60378C3A}"/>
+    <hyperlink ref="E59" r:id="rId23" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array" xr:uid="{3F271E59-4045-4398-82DB-BC2F4B35A995}"/>
+    <hyperlink ref="E60" r:id="rId24" display="https://leetcode.com/problems/find-peak-element" xr:uid="{DEF2D431-80D6-4E0B-868E-499158EC2963}"/>
+    <hyperlink ref="E10" r:id="rId25" display="https://leetcode.com/problems/koko-eating-bananas" xr:uid="{B3E73AEB-2A95-4916-A93C-BC5B60CAA1D7}"/>
+    <hyperlink ref="E61" r:id="rId26" display="https://leetcode.com/problems/split-array-largest-sum" xr:uid="{BCAC5094-3A8A-4714-BD84-F606403D9DA0}"/>
+    <hyperlink ref="E62" r:id="rId27" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days" xr:uid="{1965E795-8B07-42CA-9865-3EEF521E25E1}"/>
+    <hyperlink ref="E11" r:id="rId28" display="https://leetcode.com/problems/sort-an-array" xr:uid="{E0B9E0A6-F8E5-418F-87DD-47E7F6723CFF}"/>
+    <hyperlink ref="E63" r:id="rId29" display="https://leetcode.com/problems/insertion-sort-list" xr:uid="{03811762-664A-488F-9B2D-036EAE5AAD21}"/>
+    <hyperlink ref="E64" r:id="rId30" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{4F771129-F99D-4F68-954B-762315CE30B8}"/>
+    <hyperlink ref="E12" r:id="rId31" display="https://leetcode.com/problems/largest-number" xr:uid="{373767EF-F0B1-409B-B448-2E15DEE2A726}"/>
+    <hyperlink ref="E65" r:id="rId32" display="https://leetcode.com/problems/reorder-data-in-log-files" xr:uid="{A0B197A5-BF64-4823-8C80-786CEECF12F4}"/>
+    <hyperlink ref="E13" r:id="rId33" display="https://leetcode.com/problems/merge-intervals" xr:uid="{04E9289A-1232-436E-8E31-F058BBB75316}"/>
+    <hyperlink ref="E66" r:id="rId34" display="https://leetcode.com/problems/insert-interval" xr:uid="{355C5E3F-38DD-4154-ACB8-71E37347CA2D}"/>
+    <hyperlink ref="E14" r:id="rId35" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{73B2795D-90B0-4FEF-BAE2-297C16F48CD8}"/>
+    <hyperlink ref="E67" r:id="rId36" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{A4102035-5F89-45CA-99F6-62571131E444}"/>
+    <hyperlink ref="E15" r:id="rId37" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{213E0623-CF2A-4978-9133-4CAD9B8DDC70}"/>
+    <hyperlink ref="E68" r:id="rId38" display="https://leetcode.com/problems/reverse-linked-list-ii" xr:uid="{3E496F01-EEA1-4941-97A8-3FA083834977}"/>
+    <hyperlink ref="E16" r:id="rId39" display="https://leetcode.com/problems/linked-list-cycle" xr:uid="{9C26BB6C-78AB-4618-BD00-77BAAF16815D}"/>
+    <hyperlink ref="E69" r:id="rId40" display="https://leetcode.com/problems/linked-list-cycle-ii" xr:uid="{EC5A3D70-F195-4C10-9EA2-058F32835B9E}"/>
+    <hyperlink ref="E17" r:id="rId41" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{5C4F4E4B-2209-41D3-A906-19E1F708F9DB}"/>
+    <hyperlink ref="E70" r:id="rId42" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{1C1B8A5C-EA41-461E-8FA3-BD6A6B5B3181}"/>
+    <hyperlink ref="E18" r:id="rId43" display="https://leetcode.com/problems/intersection-of-two-linked-lists" xr:uid="{606E5182-D172-41A2-9D50-33C726FC8AB7}"/>
+    <hyperlink ref="E71" r:id="rId44" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{CD69A99D-FBAA-46B5-B0DF-9DE5139BE679}"/>
+    <hyperlink ref="E19" r:id="rId45" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{5D746582-1B54-4352-BDA4-86F05542CE88}"/>
+    <hyperlink ref="E72" r:id="rId46" display="https://leetcode.com/problems/odd-even-linked-list" xr:uid="{C89465FE-7C33-4395-99CB-4BA5D7CED11B}"/>
+    <hyperlink ref="E20" r:id="rId47" display="https://leetcode.com/problems/lru-cache" xr:uid="{05D0EB4C-0E5B-4E3E-AAB2-1A648C9129E7}"/>
+    <hyperlink ref="E73" r:id="rId48" display="https://leetcode.com/problems/lfu-cache" xr:uid="{DF951C59-83C3-4B8E-98CC-B79E487C918E}"/>
+    <hyperlink ref="E21" r:id="rId49" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{91E7DBEA-4D8A-41C9-AAC9-D9BA3BCE6D19}"/>
+    <hyperlink ref="E74" r:id="rId50" display="https://leetcode.com/problems/backspace-string-compare" xr:uid="{BD0B5108-E7EF-4D79-983A-AF8C10DCB73C}"/>
+    <hyperlink ref="E22" r:id="rId51" display="https://leetcode.com/problems/daily-temperatures" xr:uid="{B087D9B6-012A-40BD-B913-355D4FBD2EFE}"/>
+    <hyperlink ref="E75" r:id="rId52" display="https://leetcode.com/problems/next-greater-element-i" xr:uid="{FB709363-8602-45D4-B45B-8C9367125A7E}"/>
+    <hyperlink ref="E76" r:id="rId53" display="https://leetcode.com/problems/largest-rectangle-in-histogram" xr:uid="{704BEAA6-4976-4029-886F-A6FDCC20AE13}"/>
+    <hyperlink ref="E79" r:id="rId54" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k" xr:uid="{C9B7F519-FC85-48AA-93F2-FB21BD51100E}"/>
+    <hyperlink ref="E25" r:id="rId55" display="https://leetcode.com/problems/sliding-window-maximum" xr:uid="{700AEA2A-73EB-45E0-A7C4-C9B375DDFDD1}"/>
+    <hyperlink ref="E78" r:id="rId56" display="https://leetcode.com/problems/design-circular-deque" xr:uid="{C374A6F7-208C-4F78-840A-5324F48EA186}"/>
+    <hyperlink ref="E24" r:id="rId57" display="https://leetcode.com/problems/design-circular-queue" xr:uid="{9290B313-663F-43FF-8027-AB89DA22F6BD}"/>
+    <hyperlink ref="E77" r:id="rId58" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{8802B7B3-B0D3-4F45-83F5-C1CF53DB69A6}"/>
+    <hyperlink ref="E23" r:id="rId59" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{2B0D8F07-EC59-4BAD-93CF-98C511AC3E21}"/>
+    <hyperlink ref="E26" r:id="rId60" display="https://leetcode.com/problems/binary-tree-inorder-traversal" xr:uid="{1B856373-DA81-4D15-ACC2-F7C093A506A8}"/>
+    <hyperlink ref="E80" r:id="rId61" display="https://leetcode.com/problems/binary-tree-level-order-traversal" xr:uid="{6AAEF83E-F9D9-409A-927C-DDEE7AEA57FC}"/>
+    <hyperlink ref="E81" r:id="rId62" display="https://leetcode.com/problems/binary-tree-right-side-view" xr:uid="{5577EFF4-DB1A-480F-83F5-F19EDE79C4B5}"/>
+    <hyperlink ref="E27" r:id="rId63" display="https://leetcode.com/problems/search-in-a-binary-search-tree" xr:uid="{A758D8A5-36A2-40FF-A15F-1A6A7A69801A}"/>
+    <hyperlink ref="E82" r:id="rId64" display="https://leetcode.com/problems/delete-node-in-a-bst" xr:uid="{591B7EA7-3888-49B3-99EF-BA629CD9A02D}"/>
+    <hyperlink ref="E28" r:id="rId65" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{78FB8ABE-DFC4-47EA-ACA0-CFB46543B8DC}"/>
+    <hyperlink ref="E83" r:id="rId66" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree" xr:uid="{5AA82C0A-C3F6-4840-B663-78DC8E56D219}"/>
+    <hyperlink ref="E30" r:id="rId67" display="https://leetcode.com/problems/last-stone-weight" xr:uid="{CAD60500-B89D-4C41-8574-D33E4F0BB32A}"/>
+    <hyperlink ref="E85" r:id="rId68" display="https://leetcode.com/problems/k-closest-points-to-origin" xr:uid="{BBD06487-6DC3-4A9B-83CC-F430BAF527D5}"/>
+    <hyperlink ref="E31" r:id="rId69" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{88E6C8C5-7B90-4A92-BECC-A629C8A55FEC}"/>
+    <hyperlink ref="E86" r:id="rId70" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix" xr:uid="{4C161606-D259-4AC4-BDFF-44E161BFF6BD}"/>
+    <hyperlink ref="E32" r:id="rId71" display="https://leetcode.com/problems/top-k-frequent-words" xr:uid="{4FD04348-E4BE-4F5E-83FD-752D5452B19E}"/>
+    <hyperlink ref="E87" r:id="rId72" display="https://leetcode.com/problems/top-k-frequent-elements" xr:uid="{31ABA819-3C4C-4002-8FCF-364AEF9823BD}"/>
+    <hyperlink ref="E33" r:id="rId73" display="https://leetcode.com/problems/two-sum" xr:uid="{5B404BE5-D0E3-4728-8498-75AFA5031304}"/>
+    <hyperlink ref="E88" r:id="rId74" display="https://leetcode.com/problems/ransom-note" xr:uid="{E50D5A6F-DB16-4D48-974E-C7847334D093}"/>
+    <hyperlink ref="E89" r:id="rId75" display="https://leetcode.com/problems/contains-duplicate" xr:uid="{EEA73F8B-13F1-431E-A0F1-3A0C6B23527D}"/>
+    <hyperlink ref="E34" r:id="rId76" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{4D7D4589-2B8A-47DC-9FCF-904D6E82FB71}"/>
+    <hyperlink ref="E90" r:id="rId77" display="https://leetcode.com/problems/subarray-sums-divisible-by-k" xr:uid="{D838CB32-0488-4C04-951B-6AA80F72BEA1}"/>
+    <hyperlink ref="E35" r:id="rId78" display="https://leetcode.com/problems/group-anagrams" xr:uid="{E64749FE-4AC2-4B2B-91C7-7180E2DCC00B}"/>
+    <hyperlink ref="E91" r:id="rId79" display="https://leetcode.com/problems/longest-consecutive-sequence" xr:uid="{DE30C124-13F2-439B-9476-17D8DAC27129}"/>
+    <hyperlink ref="E36" r:id="rId80" display="https://leetcode.com/problems/number-of-islands" xr:uid="{8DBAE9D8-4931-4C16-AEED-F66841DA88D4}"/>
+    <hyperlink ref="E92" r:id="rId81" display="https://leetcode.com/problems/max-area-of-island" xr:uid="{1B4C9834-1FC5-4895-806E-038B1DBDDA4B}"/>
+    <hyperlink ref="E93" r:id="rId82" display="https://leetcode.com/problems/01-matrix" xr:uid="{A0E46D51-24FB-432C-9B64-F9A7D564ADF2}"/>
+    <hyperlink ref="E37" r:id="rId83" display="https://leetcode.com/problems/network-delay-time" xr:uid="{F759E8D2-9590-49C8-B0C1-9FDC2453A281}"/>
+    <hyperlink ref="E94" r:id="rId84" display="https://leetcode.com/problems/redundant-connection" xr:uid="{EB3F5CE4-E5E9-420F-8C29-1A45626B6B12}"/>
+    <hyperlink ref="E95" r:id="rId85" display="https://leetcode.com/problems/number-of-provinces" xr:uid="{7F9CCD13-89BD-4996-B7B2-71D1985A3440}"/>
+    <hyperlink ref="E38" r:id="rId86" display="https://leetcode.com/problems/course-schedule" xr:uid="{1BB86DA6-53E2-4F87-8150-7BF6C57A100C}"/>
+    <hyperlink ref="E96" r:id="rId87" display="https://leetcode.com/problems/course-schedule-ii" xr:uid="{5177CC97-2B77-43CF-B33F-3903154A502D}"/>
+    <hyperlink ref="E97" r:id="rId88" display="https://leetcode.com/problems/clone-graph" xr:uid="{16DC6C12-1E3C-4E22-B3FF-A38677E0B8F3}"/>
+    <hyperlink ref="E39" r:id="rId89" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{8E820236-2EA3-409B-AA9C-D43A03343FCB}"/>
+    <hyperlink ref="E98" r:id="rId90" display="https://leetcode.com/problems/climbing-stairs" xr:uid="{40181C74-4968-41A8-B229-0DF250C3A787}"/>
+    <hyperlink ref="E99" r:id="rId91" display="https://leetcode.com/problems/min-cost-climbing-stairs" xr:uid="{9E7BFCA6-DA59-48A0-975B-9589BDC7C276}"/>
+    <hyperlink ref="E40" r:id="rId92" display="https://leetcode.com/problems/longest-common-subsequence" xr:uid="{30F8CF6D-7369-4957-A7D7-160A741AA38C}"/>
+    <hyperlink ref="E100" r:id="rId93" display="https://leetcode.com/problems/longest-increasing-subsequence" xr:uid="{0B0509FA-0F85-46F0-803E-3112FAE33195}"/>
+    <hyperlink ref="E101" r:id="rId94" display="https://leetcode.com/problems/palindromic-substrings" xr:uid="{DAA8A2AD-4DEC-4740-BE2E-FF2A710FC881}"/>
+    <hyperlink ref="E41" r:id="rId95" display="https://leetcode.com/problems/unique-paths" xr:uid="{3BFACFF5-9CEA-445E-837D-80CE02DD15B6}"/>
+    <hyperlink ref="E102" r:id="rId96" display="https://leetcode.com/problems/partition-equal-subset-sum" xr:uid="{7588C036-6A20-4C85-94EE-72396427AA61}"/>
+    <hyperlink ref="E103" r:id="rId97" display="https://leetcode.com/problems/target-sum" xr:uid="{B8B2404F-6A1D-4008-9903-335EA651A7DC}"/>
+    <hyperlink ref="E42" r:id="rId98" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{6B9267CD-AC96-447A-879D-41081B74ECAC}"/>
+    <hyperlink ref="E104" r:id="rId99" display="https://leetcode.com/problems/merge-intervals" xr:uid="{C1AA793D-64CD-400D-A0A9-D182B005CEDC}"/>
+    <hyperlink ref="E105" r:id="rId100" display="https://leetcode.com/problems/gas-station" xr:uid="{9A4CC2B1-7301-4996-8463-5549D190A892}"/>
+    <hyperlink ref="E43" r:id="rId101" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{9AF79B77-6ADE-45DC-A721-A6C56EA49A98}"/>
+    <hyperlink ref="E106" r:id="rId102" display="https://leetcode.com/problems/can-place-flowers" xr:uid="{9BBCC8E1-2E28-48FF-9415-D9250E2D1CFB}"/>
+    <hyperlink ref="E107" r:id="rId103" display="https://leetcode.com/problems/jump-game" xr:uid="{22D973B8-6E8A-41F7-BF66-D13FE9CE93A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId104"/>
   <tableParts count="1">
-    <tablePart r:id="rId104"/>
+    <tablePart r:id="rId105"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lesson Plan: Backtracking is added
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schedule\Documents\TIME_DK\time_colleges\SRET\Focus_Batch_2023-2027\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FB88E0-C390-458B-9A64-257486D757ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AA92E9-0490-4F7D-AB9D-1E7E88B9F6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="254">
   <si>
     <t>Order</t>
   </si>
@@ -758,6 +758,36 @@
   </si>
   <si>
     <t>Mixed</t>
+  </si>
+  <si>
+    <t>Backtracking</t>
+  </si>
+  <si>
+    <t>N-Queens</t>
+  </si>
+  <si>
+    <t>51. N-Queens</t>
+  </si>
+  <si>
+    <t>52. N-Queens II</t>
+  </si>
+  <si>
+    <t>Subset Gen</t>
+  </si>
+  <si>
+    <t>90. Subsets II</t>
+  </si>
+  <si>
+    <t>Permutations</t>
+  </si>
+  <si>
+    <t>47. Permutations II</t>
+  </si>
+  <si>
+    <t>Combination Sum</t>
+  </si>
+  <si>
+    <t>39. Combination Sum</t>
   </si>
 </sst>
 </file>
@@ -943,10 +973,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{512AC03F-78F7-4FEC-8505-F6AAC24DF528}" name="Table2" displayName="Table2" ref="A1:G108" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:G108" xr:uid="{512AC03F-78F7-4FEC-8505-F6AAC24DF528}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G108">
-    <sortCondition ref="D1:D108"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{512AC03F-78F7-4FEC-8505-F6AAC24DF528}" name="Table2" displayName="Table2" ref="A1:G113" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:G113" xr:uid="{512AC03F-78F7-4FEC-8505-F6AAC24DF528}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G113">
+    <sortCondition ref="A1:A113"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{911CBD74-C633-4B51-85BF-53095DEB2CC8}" name="S.No" dataDxfId="8"/>
@@ -1227,7 +1257,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,22 +1503,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47E1B90-F79D-473A-8C0F-D2580CDDC346}">
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1543,73 +1573,69 @@
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I3" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>String: Sliding Window</v>
+        <v>String: Frequency Matching</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="1">
-        <v>3</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I4" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Array: Two Pointer</v>
+        <v>String: Frequency Matching</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>39</v>
@@ -1619,78 +1645,74 @@
       </c>
       <c r="I5" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Array: Prefix / Sliding</v>
+        <v>String: Sliding Window</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="1">
-        <v>5</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="7" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I6" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Recursion: Base Case + Tree View</v>
+        <v>String: Sliding Window</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="1">
-        <v>6</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="7" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I7" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Recursion: Divide and Conquer</v>
+        <v>String: Sliding Window</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>39</v>
@@ -1700,78 +1722,74 @@
       </c>
       <c r="I8" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Recursion: Subsets</v>
+        <v>Array: Two Pointer</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="1">
-        <v>10</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Searching: Binary Search Basic</v>
+        <v>Array: Two Pointer</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="1">
-        <v>11</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I10" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Searching: BS on Answer</v>
+        <v>Array: Two Pointer</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>39</v>
@@ -1781,240 +1799,228 @@
       </c>
       <c r="I11" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Sorting: Basic Sorting Logic</v>
+        <v>Array: Prefix / Sliding</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="1">
-        <v>13</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="7" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I12" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Sorting: Custom Comparator</v>
+        <v>Array: Prefix / Sliding</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="1">
-        <v>14</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="7" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I13" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Sorting: Merge Intervals</v>
+        <v>Array: Prefix / Sliding</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I14" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Sorting: Scheduling Logic</v>
+        <v>Recursion: Base Case + Tree View</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D15" s="1">
-        <v>16</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="7" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I15" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: Reverse LL</v>
+        <v>Recursion: Base Case Practice</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="1">
-        <v>17</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="7" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I16" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: Detect Cycle</v>
+        <v>Recursion: Fibonacci</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="D17" s="1">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I17" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: Merge LL</v>
+        <v>Recursion: Divide and Conquer</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D18" s="1">
-        <v>19</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="7" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I18" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: Intersection Point</v>
+        <v>Recursion: Divide and Conquer</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" s="1">
-        <v>20</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="7" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I19" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: Palindrome Check</v>
+        <v>Recursion: Binary Recursion Tree</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>39</v>
@@ -2024,294 +2030,280 @@
       </c>
       <c r="I20" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: LRU Cache Logic</v>
+        <v>Recursion: Subsets</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="1">
-        <v>22</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="7" t="s">
-        <v>124</v>
+        <v>67</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I21" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Stack: Stack Basics</v>
+        <v>Recursion: Rec. with State</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D22" s="1">
-        <v>23</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="7" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I22" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Stack: Monotonic Stack</v>
+        <v>Recursion: Backtrack Base</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>132</v>
+        <v>244</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>133</v>
+        <v>245</v>
       </c>
       <c r="D23" s="1">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>134</v>
+        <v>246</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I23" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Queue: Queue + BFS Intro</v>
+        <v>Backtracking: N-Queens</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>132</v>
+        <v>244</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D24" s="1">
-        <v>25</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="7" t="s">
-        <v>138</v>
+        <v>247</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I24" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Queue: Circular Queue</v>
+        <v>Backtracking: N-Queens</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>132</v>
+        <v>244</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>141</v>
+        <v>248</v>
       </c>
       <c r="D25" s="1">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>142</v>
+        <v>249</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I25" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Queue: Monotonic Queue</v>
+        <v>Backtracking: Subset Gen</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>144</v>
+        <v>244</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D26" s="1">
-        <v>27</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="D26" s="3"/>
       <c r="E26" s="7" t="s">
-        <v>146</v>
+        <v>251</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I26" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Trees: Traversals</v>
+        <v>Backtracking: Permutations</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>12</v>
+        <v>244</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D27" s="1">
-        <v>28</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="7" t="s">
-        <v>151</v>
+        <v>253</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I27" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>BST: Search, Insert, Min</v>
+        <v>Backtracking: Combination Sum</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="C28" s="3" t="s">
-        <v>154</v>
+        <v>71</v>
       </c>
       <c r="D28" s="1">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>155</v>
+        <v>72</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I28" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>BST: Validate BST</v>
+        <v>Searching: Binary Search Basic</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D29" s="1">
-        <v>30</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>160</v>
+        <v>73</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>162</v>
+        <v>35</v>
       </c>
       <c r="I29" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Balanced Tree: AVL Tree</v>
+        <v>Searching: First/Last Occurrence</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>165</v>
+        <v>70</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D30" s="1">
-        <v>31</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="7" t="s">
-        <v>167</v>
+        <v>76</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I30" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Heap: Min Heap Introduction</v>
+        <v>Searching: Peak Element</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>165</v>
+        <v>70</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>170</v>
+        <v>77</v>
       </c>
       <c r="D31" s="1">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>39</v>
@@ -2321,78 +2313,74 @@
       </c>
       <c r="I31" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Heap: Kth Largest Element</v>
+        <v>Searching: BS on Answer</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>165</v>
+        <v>70</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D32" s="1">
-        <v>33</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D32" s="1"/>
       <c r="E32" s="7" t="s">
-        <v>174</v>
+        <v>79</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I32" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Heap: Heap + Sorting Logic</v>
+        <v>Searching: BS on Answer</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D33" s="1">
-        <v>34</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>179</v>
-      </c>
       <c r="F33" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I33" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>HashMap: Frequency Counting</v>
+        <v>Searching: BS on Answer</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="1">
+        <v>12</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D34" s="1">
-        <v>35</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>39</v>
@@ -2402,78 +2390,74 @@
       </c>
       <c r="I34" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>HashMap: Prefix Sum Technique</v>
+        <v>Sorting: Basic Sorting Logic</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D35" s="1">
-        <v>36</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>187</v>
-      </c>
       <c r="F35" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I35" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>HashMap: Grouping Data</v>
+        <v>Sorting: Selection Practice</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D36" s="1">
-        <v>37</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>192</v>
-      </c>
       <c r="F36" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I36" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Graph: BFS Traversal</v>
+        <v>Sorting: QuickSort</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>190</v>
+        <v>81</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>197</v>
+        <v>88</v>
       </c>
       <c r="D37" s="1">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>198</v>
+        <v>89</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>39</v>
@@ -2483,105 +2467,101 @@
       </c>
       <c r="I37" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Graph: Dijkstra’s (Shortest Path)</v>
+        <v>Sorting: Custom Comparator</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>190</v>
+        <v>81</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D38" s="1">
-        <v>39</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="D38" s="1"/>
       <c r="E38" s="7" t="s">
-        <v>204</v>
+        <v>90</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I38" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Graph: Topological Sort</v>
+        <v>Sorting: Custom Comparator</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>209</v>
+        <v>81</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>210</v>
+        <v>91</v>
       </c>
       <c r="D39" s="1">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I39" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>DP: Fibonacci with Memo</v>
+        <v>Sorting: Merge Intervals</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>209</v>
+        <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D40" s="1">
-        <v>41</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="7" t="s">
-        <v>216</v>
+        <v>93</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I40" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>DP: Longest Common Subseq</v>
+        <v>Sorting: Merge Intervals</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>209</v>
+        <v>81</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>221</v>
+        <v>94</v>
       </c>
       <c r="D41" s="1">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>222</v>
+        <v>95</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>39</v>
@@ -2591,178 +2571,178 @@
       </c>
       <c r="I41" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>DP: Unique Paths (2D Grid)</v>
+        <v>Sorting: Scheduling Logic</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D42" s="1">
-        <v>43</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I42" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Greedy: Activity Selection (Intervals)</v>
+        <v>Sorting: Sorting Based Greedy</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>231</v>
+        <v>99</v>
       </c>
       <c r="D43" s="1">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>232</v>
+        <v>100</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I43" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Greedy: Job Scheduling / Max Profit</v>
+        <v>Linked List: Reverse LL</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>111</v>
+        <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>237</v>
+        <v>98</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="D44" s="1">
-        <v>45</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>239</v>
+        <v>101</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>240</v>
+        <v>39</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I44" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Review: Strategy + Topic Recap</v>
+        <v>Linked List: Reverse LL II</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="D45" s="1">
+        <v>17</v>
+      </c>
       <c r="E45" s="7" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I45" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>String: Frequency Matching</v>
+        <v>Linked List: Detect Cycle</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="7" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I46" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>String: Frequency Matching</v>
+        <v>Linked List: Cycle II</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D47" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="D47" s="1">
+        <v>18</v>
+      </c>
       <c r="E47" s="7" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I47" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>String: Sliding Window</v>
+        <v>Linked List: Merge LL</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="7" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>42</v>
@@ -2772,372 +2752,386 @@
       </c>
       <c r="I48" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>String: Sliding Window</v>
+        <v>Linked List: Merge k Lists</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D49" s="1"/>
+        <v>111</v>
+      </c>
+      <c r="D49" s="1">
+        <v>19</v>
+      </c>
       <c r="E49" s="7" t="s">
-        <v>46</v>
+        <v>112</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I49" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Array: Two Pointer</v>
+        <v>Linked List: Intersection Point</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="7" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I50" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Array: Two Pointer</v>
+        <v>Linked List: Remove Nth Node</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D51" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="D51" s="1">
+        <v>20</v>
+      </c>
       <c r="E51" s="7" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I51" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Array: Prefix / Sliding</v>
+        <v>Linked List: Palindrome Check</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="7" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I52" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Array: Prefix / Sliding</v>
+        <v>Linked List: Odd Even Index</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D53" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="D53" s="1">
+        <v>21</v>
+      </c>
       <c r="E53" s="7" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I53" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Recursion: Base Case Practice</v>
+        <v>Linked List: LRU Cache Logic</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="7" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I54" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Recursion: Fibonacci</v>
+        <v>Linked List: Advanced LRU Logic</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D55" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="D55" s="1">
+        <v>22</v>
+      </c>
       <c r="E55" s="7" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I55" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Recursion: Divide and Conquer</v>
+        <v>Stack: Stack Basics</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="7" t="s">
-        <v>63</v>
+        <v>125</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I56" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Recursion: Binary Recursion Tree</v>
+        <v>Stack: Stack Basics</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D57" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="D57" s="1">
+        <v>23</v>
+      </c>
       <c r="E57" s="7" t="s">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I57" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Recursion: Rec. with State</v>
+        <v>Stack: Monotonic Stack</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="7" t="s">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I58" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Recursion: Backtrack Base</v>
+        <v>Stack: Next Greater Element</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="7" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I59" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Searching: First/Last Occurrence</v>
+        <v>Stack: Largest Rect in Hist</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D60" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="D60" s="1">
+        <v>24</v>
+      </c>
       <c r="E60" s="7" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I60" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Searching: Peak Element</v>
+        <v>Queue: Queue + BFS Intro</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="7" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I61" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Searching: BS on Answer</v>
+        <v>Queue: Implement Queue Using Stacks</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D62" s="1">
+        <v>25</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G62" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D62" s="1"/>
-      <c r="E62" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="I62" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Searching: BS on Answer</v>
+        <v>Queue: Circular Queue</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="7" t="s">
-        <v>85</v>
+        <v>140</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>39</v>
@@ -3147,97 +3141,101 @@
       </c>
       <c r="I63" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Sorting: Selection Practice</v>
+        <v>Queue: Deque</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D64" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="D64" s="1">
+        <v>26</v>
+      </c>
       <c r="E64" s="7" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I64" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Sorting: QuickSort</v>
+        <v>Queue: Monotonic Queue</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>88</v>
+        <v>141</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="7" t="s">
-        <v>90</v>
+        <v>143</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I65" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Sorting: Custom Comparator</v>
+        <v>Queue: Monotonic Queue</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D66" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="D66" s="1">
+        <v>27</v>
+      </c>
       <c r="E66" s="7" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I66" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Sorting: Merge Intervals</v>
+        <v>Trees: Traversals</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>96</v>
+        <v>145</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="7" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>39</v>
@@ -3247,22 +3245,22 @@
       </c>
       <c r="I67" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Sorting: Sorting Based Greedy</v>
+        <v>Trees: Traversals</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="7" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>39</v>
@@ -3272,97 +3270,101 @@
       </c>
       <c r="I68" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: Reverse LL II</v>
+        <v>Trees: Views + Height</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D69" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="D69" s="1">
+        <v>28</v>
+      </c>
       <c r="E69" s="7" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I69" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: Cycle II</v>
+        <v>BST: Search, Insert, Min</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="7" t="s">
-        <v>110</v>
+        <v>153</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I70" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: Merge k Lists</v>
+        <v>BST: Deletion</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D71" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="D71" s="1">
+        <v>29</v>
+      </c>
       <c r="E71" s="7" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I71" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: Remove Nth Node</v>
+        <v>BST: Validate BST</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="7" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>39</v>
@@ -3372,147 +3374,153 @@
       </c>
       <c r="I72" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: Odd Even Index</v>
+        <v>BST: Lowest Common Ancestor</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="7" t="s">
-        <v>122</v>
+        <v>159</v>
+      </c>
+      <c r="D73" s="1">
+        <v>30</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>42</v>
+        <v>161</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>35</v>
+        <v>162</v>
       </c>
       <c r="I73" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Linked List: Advanced LRU Logic</v>
+        <v>Balanced Tree: AVL Tree</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>9</v>
+        <v>158</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="D74" s="1"/>
-      <c r="E74" s="7" t="s">
-        <v>125</v>
+      <c r="E74" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>31</v>
+        <v>161</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>35</v>
+        <v>164</v>
       </c>
       <c r="I74" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Stack: Stack Basics</v>
+        <v>Balanced Tree: Red-Black Tree</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>9</v>
+        <v>165</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D75" s="1"/>
+        <v>166</v>
+      </c>
+      <c r="D75" s="1">
+        <v>31</v>
+      </c>
       <c r="E75" s="7" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I75" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Stack: Next Greater Element</v>
+        <v>Heap: Min Heap Introduction</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>9</v>
+        <v>165</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="7" t="s">
-        <v>131</v>
+        <v>169</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I76" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Stack: Largest Rect in Hist</v>
+        <v>Heap: Priority Queue Usage</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D77" s="1"/>
+        <v>170</v>
+      </c>
+      <c r="D77" s="1">
+        <v>32</v>
+      </c>
       <c r="E77" s="7" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I77" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Queue: Implement Queue Using Stacks</v>
+        <v>Heap: Kth Largest Element</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="7" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>39</v>
@@ -3522,47 +3530,49 @@
       </c>
       <c r="I78" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Queue: Deque</v>
+        <v>Heap: Kth Smallest Element</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D79" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="D79" s="1">
+        <v>33</v>
+      </c>
       <c r="E79" s="7" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I79" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Queue: Monotonic Queue</v>
+        <v>Heap: Heap + Sorting Logic</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="7" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>39</v>
@@ -3572,122 +3582,126 @@
       </c>
       <c r="I80" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Trees: Traversals</v>
+        <v>Heap: Heap + Custom Comparator</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>144</v>
+        <v>177</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D81" s="1"/>
+        <v>178</v>
+      </c>
+      <c r="D81" s="1">
+        <v>34</v>
+      </c>
       <c r="E81" s="7" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I81" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Trees: Views + Height</v>
+        <v>HashMap: Frequency Counting</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="7" t="s">
-        <v>153</v>
+        <v>34</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I82" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>BST: Deletion</v>
+        <v>HashMap: Frequency Counting</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>12</v>
+        <v>180</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="7" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G83" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I83" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>BST: Lowest Common Ancestor</v>
+        <v>HashSet: Uniqueness Check</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D84" s="1"/>
-      <c r="E84" s="3" t="s">
-        <v>160</v>
+        <v>183</v>
+      </c>
+      <c r="D84" s="1">
+        <v>35</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>164</v>
+        <v>32</v>
       </c>
       <c r="I84" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Balanced Tree: Red-Black Tree</v>
+        <v>HashMap: Prefix Sum Technique</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="7" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>39</v>
@@ -3697,47 +3711,49 @@
       </c>
       <c r="I85" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Heap: Priority Queue Usage</v>
+        <v>HashMap: Prefix Sum Variation</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D86" s="1"/>
+        <v>186</v>
+      </c>
+      <c r="D86" s="1">
+        <v>36</v>
+      </c>
       <c r="E86" s="7" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I86" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Heap: Kth Smallest Element</v>
+        <v>HashMap: Grouping Data</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="7" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>39</v>
@@ -3747,72 +3763,74 @@
       </c>
       <c r="I87" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Heap: Heap + Custom Comparator</v>
+        <v>HashMap: Longest Streak/Length</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D88" s="1"/>
+        <v>191</v>
+      </c>
+      <c r="D88" s="1">
+        <v>37</v>
+      </c>
       <c r="E88" s="7" t="s">
-        <v>34</v>
+        <v>192</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I88" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>HashMap: Frequency Counting</v>
+        <v>Graph: BFS Traversal</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="7" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G89" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I89" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>HashSet: Uniqueness Check</v>
+        <v>Graph: DFS Traversal</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="7" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="F90" s="3" t="s">
         <v>39</v>
@@ -3822,47 +3840,49 @@
       </c>
       <c r="I90" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>HashMap: Prefix Sum Variation</v>
+        <v>Graph: BFS with Distance</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D91" s="1"/>
+        <v>197</v>
+      </c>
+      <c r="D91" s="1">
+        <v>38</v>
+      </c>
       <c r="E91" s="7" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I91" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>HashMap: Longest Streak/Length</v>
+        <v>Graph: Dijkstra’s (Shortest Path)</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>190</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="7" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="F92" s="3" t="s">
         <v>39</v>
@@ -3872,22 +3892,22 @@
       </c>
       <c r="I92" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Graph: DFS Traversal</v>
+        <v>Graph: Union Find</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>190</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="7" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>39</v>
@@ -3897,47 +3917,49 @@
       </c>
       <c r="I93" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Graph: BFS with Distance</v>
+        <v>Graph: Cycle Detection</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>190</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D94" s="1"/>
+        <v>203</v>
+      </c>
+      <c r="D94" s="1">
+        <v>39</v>
+      </c>
       <c r="E94" s="7" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I94" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Graph: Union Find</v>
+        <v>Graph: Topological Sort</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>190</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="7" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>39</v>
@@ -3947,22 +3969,22 @@
       </c>
       <c r="I95" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Graph: Cycle Detection</v>
+        <v>Graph: Topo + Ordering</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>190</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F96" s="3" t="s">
         <v>39</v>
@@ -3972,32 +3994,34 @@
       </c>
       <c r="I96" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Graph: Topo + Ordering</v>
+        <v>Graph: Kahn’s Algorithm</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D97" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D97" s="1">
+        <v>40</v>
+      </c>
       <c r="E97" s="7" t="s">
-        <v>208</v>
+        <v>58</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I97" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Graph: Kahn’s Algorithm</v>
+        <v>DP: Fibonacci with Memo</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4052,42 +4076,44 @@
     </row>
     <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>209</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D100" s="1"/>
+        <v>215</v>
+      </c>
+      <c r="D100" s="1">
+        <v>41</v>
+      </c>
       <c r="E100" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I100" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>DP: Longest Increasing Subseq</v>
+        <v>DP: Longest Common Subseq</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>209</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>39</v>
@@ -4097,22 +4123,22 @@
       </c>
       <c r="I101" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>DP: Palindromic Substrings</v>
+        <v>DP: Longest Increasing Subseq</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>209</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F102" s="3" t="s">
         <v>39</v>
@@ -4122,47 +4148,49 @@
       </c>
       <c r="I102" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>DP: Partition Equal Sum</v>
+        <v>DP: Palindromic Substrings</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>209</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="D103" s="1"/>
+        <v>221</v>
+      </c>
+      <c r="D103" s="1">
+        <v>42</v>
+      </c>
       <c r="E103" s="7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I103" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>DP: Target Sum (state model)</v>
+        <v>DP: Unique Paths (2D Grid)</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>20</v>
+        <v>209</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="7" t="s">
-        <v>92</v>
+        <v>224</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>39</v>
@@ -4172,22 +4200,22 @@
       </c>
       <c r="I104" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Greedy: Interval Merging</v>
+        <v>DP: Partition Equal Sum</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>20</v>
+        <v>209</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F105" s="3" t="s">
         <v>39</v>
@@ -4197,47 +4225,49 @@
       </c>
       <c r="I105" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Greedy: Gas Station Problem</v>
+        <v>DP: Target Sum (state model)</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D106" s="1"/>
+        <v>227</v>
+      </c>
+      <c r="D106" s="1">
+        <v>43</v>
+      </c>
       <c r="E106" s="7" t="s">
-        <v>234</v>
+        <v>95</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I106" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Greedy: Resource Assignment</v>
+        <v>Greedy: Activity Selection (Intervals)</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="7" t="s">
-        <v>236</v>
+        <v>92</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>39</v>
@@ -4247,36 +4277,161 @@
       </c>
       <c r="I107" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Greedy: Jump Game</v>
+        <v>Greedy: Interval Merging</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D108" s="1"/>
+      <c r="E108" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I108" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Greedy: Gas Station Problem</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D109" s="1">
+        <v>44</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I109" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Greedy: Job Scheduling / Max Profit</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D110" s="1"/>
+      <c r="E110" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I110" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Greedy: Resource Assignment</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D111" s="1"/>
+      <c r="E111" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I111" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Greedy: Jump Game</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>111</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D112" s="1">
+        <v>45</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I112" t="str">
+        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
+        <v>Review: Strategy + Topic Recap</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
         <v>112</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C113" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D108" s="1"/>
-      <c r="E108" s="3" t="s">
+      <c r="D113" s="1"/>
+      <c r="E113" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="F108" s="3" t="s">
+      <c r="F113" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="G108" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I108" t="str">
-        <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Review: Mock Contest (3–4 problems)</v>
+      <c r="G113" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576">
+  <conditionalFormatting sqref="G1:G22 G28:G1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
@@ -4286,113 +4441,118 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="https://leetcode.com/problems/first-unique-character-in-a-string" xr:uid="{CACA8992-DEBC-4969-B2F6-EBA7FDC085C1}"/>
-    <hyperlink ref="E45" r:id="rId2" display="https://leetcode.com/problems/ransom-note" xr:uid="{9ACCC9FD-0DC8-4254-BB8B-808F3BDD3784}"/>
-    <hyperlink ref="E46" r:id="rId3" display="https://leetcode.com/problems/valid-anagram" xr:uid="{EE4FEEAF-652D-4D2D-A2A9-CB87731F42BE}"/>
-    <hyperlink ref="E3" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters" xr:uid="{4DD7CB8D-B440-4AF4-B6AB-D727391B9158}"/>
-    <hyperlink ref="E47" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string" xr:uid="{7CCC4C5F-1CA6-46F8-9DD3-9647C7682498}"/>
-    <hyperlink ref="E48" r:id="rId6" display="https://leetcode.com/problems/minimum-window-substring" xr:uid="{61B1900B-EAF8-4BE8-ACAB-A956DE5F3ED1}"/>
-    <hyperlink ref="E4" r:id="rId7" display="https://leetcode.com/problems/container-with-most-water" xr:uid="{84B1B8CA-3A3C-4909-8DD8-F88A45D68628}"/>
-    <hyperlink ref="E49" r:id="rId8" display="https://leetcode.com/problems/3sum" xr:uid="{42633795-6F73-49FF-B778-78E0CD056E83}"/>
-    <hyperlink ref="E50" r:id="rId9" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array" xr:uid="{DFA525B5-0825-451E-B3E0-9DC93194D4E1}"/>
-    <hyperlink ref="E5" r:id="rId10" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{3640DDE9-2ADF-42E2-AEDE-DA2AC3BA211A}"/>
-    <hyperlink ref="E51" r:id="rId11" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k" xr:uid="{8062781F-458E-4926-B311-804BA6CD3BBB}"/>
-    <hyperlink ref="E52" r:id="rId12" display="https://leetcode.com/problems/maximum-subarray" xr:uid="{3AD35EF8-0181-42B2-9B38-F0FC3F95CFE6}"/>
-    <hyperlink ref="E6" r:id="rId13" display="https://leetcode.com/problems/maximum-depth-of-binary-tree" xr:uid="{44C26DDF-9EB7-417D-B269-6C23AC6E6445}"/>
-    <hyperlink ref="E53" r:id="rId14" display="https://leetcode.com/problems/invert-binary-tree" xr:uid="{14199D52-1EAC-49F1-8883-00C4203FC3E3}"/>
-    <hyperlink ref="E54" r:id="rId15" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{52E248D0-3A46-4957-B7A0-F75EBA672C5B}"/>
-    <hyperlink ref="E7" r:id="rId16" display="https://leetcode.com/problems/different-ways-to-add-parentheses" xr:uid="{9DA410A2-6C01-4EDA-9F51-6FBA009D88DF}"/>
-    <hyperlink ref="E55" r:id="rId17" display="https://leetcode.com/problems/unique-binary-search-trees-ii" xr:uid="{68A314C1-D173-4545-AF04-B8E2F74F893D}"/>
-    <hyperlink ref="E56" r:id="rId18" display="https://leetcode.com/problems/powx-n" xr:uid="{26A0C127-23BD-4BCE-8BC7-8AB1A8F90ADE}"/>
-    <hyperlink ref="E8" r:id="rId19" display="https://leetcode.com/problems/subsets" xr:uid="{22D9BCEB-5D0D-4BEF-A700-0FC47638B9F3}"/>
-    <hyperlink ref="E57" r:id="rId20" display="https://leetcode.com/problems/permutations" xr:uid="{E47F3CB1-204D-4424-914C-698242057FAC}"/>
-    <hyperlink ref="E58" r:id="rId21" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{5F57D8FD-824D-4DB1-892E-1DDFD0F8F33D}"/>
-    <hyperlink ref="E9" r:id="rId22" display="https://leetcode.com/problems/binary-search" xr:uid="{374FFDAF-FCB9-431A-86D2-31AB60378C3A}"/>
-    <hyperlink ref="E59" r:id="rId23" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array" xr:uid="{3F271E59-4045-4398-82DB-BC2F4B35A995}"/>
-    <hyperlink ref="E60" r:id="rId24" display="https://leetcode.com/problems/find-peak-element" xr:uid="{DEF2D431-80D6-4E0B-868E-499158EC2963}"/>
-    <hyperlink ref="E10" r:id="rId25" display="https://leetcode.com/problems/koko-eating-bananas" xr:uid="{B3E73AEB-2A95-4916-A93C-BC5B60CAA1D7}"/>
-    <hyperlink ref="E61" r:id="rId26" display="https://leetcode.com/problems/split-array-largest-sum" xr:uid="{BCAC5094-3A8A-4714-BD84-F606403D9DA0}"/>
-    <hyperlink ref="E62" r:id="rId27" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days" xr:uid="{1965E795-8B07-42CA-9865-3EEF521E25E1}"/>
-    <hyperlink ref="E11" r:id="rId28" display="https://leetcode.com/problems/sort-an-array" xr:uid="{E0B9E0A6-F8E5-418F-87DD-47E7F6723CFF}"/>
-    <hyperlink ref="E63" r:id="rId29" display="https://leetcode.com/problems/insertion-sort-list" xr:uid="{03811762-664A-488F-9B2D-036EAE5AAD21}"/>
-    <hyperlink ref="E64" r:id="rId30" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{4F771129-F99D-4F68-954B-762315CE30B8}"/>
-    <hyperlink ref="E12" r:id="rId31" display="https://leetcode.com/problems/largest-number" xr:uid="{373767EF-F0B1-409B-B448-2E15DEE2A726}"/>
-    <hyperlink ref="E65" r:id="rId32" display="https://leetcode.com/problems/reorder-data-in-log-files" xr:uid="{A0B197A5-BF64-4823-8C80-786CEECF12F4}"/>
-    <hyperlink ref="E13" r:id="rId33" display="https://leetcode.com/problems/merge-intervals" xr:uid="{04E9289A-1232-436E-8E31-F058BBB75316}"/>
-    <hyperlink ref="E66" r:id="rId34" display="https://leetcode.com/problems/insert-interval" xr:uid="{355C5E3F-38DD-4154-ACB8-71E37347CA2D}"/>
-    <hyperlink ref="E14" r:id="rId35" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{73B2795D-90B0-4FEF-BAE2-297C16F48CD8}"/>
-    <hyperlink ref="E67" r:id="rId36" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{A4102035-5F89-45CA-99F6-62571131E444}"/>
-    <hyperlink ref="E15" r:id="rId37" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{213E0623-CF2A-4978-9133-4CAD9B8DDC70}"/>
-    <hyperlink ref="E68" r:id="rId38" display="https://leetcode.com/problems/reverse-linked-list-ii" xr:uid="{3E496F01-EEA1-4941-97A8-3FA083834977}"/>
-    <hyperlink ref="E16" r:id="rId39" display="https://leetcode.com/problems/linked-list-cycle" xr:uid="{9C26BB6C-78AB-4618-BD00-77BAAF16815D}"/>
-    <hyperlink ref="E69" r:id="rId40" display="https://leetcode.com/problems/linked-list-cycle-ii" xr:uid="{EC5A3D70-F195-4C10-9EA2-058F32835B9E}"/>
-    <hyperlink ref="E17" r:id="rId41" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{5C4F4E4B-2209-41D3-A906-19E1F708F9DB}"/>
-    <hyperlink ref="E70" r:id="rId42" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{1C1B8A5C-EA41-461E-8FA3-BD6A6B5B3181}"/>
-    <hyperlink ref="E18" r:id="rId43" display="https://leetcode.com/problems/intersection-of-two-linked-lists" xr:uid="{606E5182-D172-41A2-9D50-33C726FC8AB7}"/>
-    <hyperlink ref="E71" r:id="rId44" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{CD69A99D-FBAA-46B5-B0DF-9DE5139BE679}"/>
-    <hyperlink ref="E19" r:id="rId45" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{5D746582-1B54-4352-BDA4-86F05542CE88}"/>
-    <hyperlink ref="E72" r:id="rId46" display="https://leetcode.com/problems/odd-even-linked-list" xr:uid="{C89465FE-7C33-4395-99CB-4BA5D7CED11B}"/>
-    <hyperlink ref="E20" r:id="rId47" display="https://leetcode.com/problems/lru-cache" xr:uid="{05D0EB4C-0E5B-4E3E-AAB2-1A648C9129E7}"/>
-    <hyperlink ref="E73" r:id="rId48" display="https://leetcode.com/problems/lfu-cache" xr:uid="{DF951C59-83C3-4B8E-98CC-B79E487C918E}"/>
-    <hyperlink ref="E21" r:id="rId49" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{91E7DBEA-4D8A-41C9-AAC9-D9BA3BCE6D19}"/>
-    <hyperlink ref="E74" r:id="rId50" display="https://leetcode.com/problems/backspace-string-compare" xr:uid="{BD0B5108-E7EF-4D79-983A-AF8C10DCB73C}"/>
-    <hyperlink ref="E22" r:id="rId51" display="https://leetcode.com/problems/daily-temperatures" xr:uid="{B087D9B6-012A-40BD-B913-355D4FBD2EFE}"/>
-    <hyperlink ref="E75" r:id="rId52" display="https://leetcode.com/problems/next-greater-element-i" xr:uid="{FB709363-8602-45D4-B45B-8C9367125A7E}"/>
-    <hyperlink ref="E76" r:id="rId53" display="https://leetcode.com/problems/largest-rectangle-in-histogram" xr:uid="{704BEAA6-4976-4029-886F-A6FDCC20AE13}"/>
-    <hyperlink ref="E79" r:id="rId54" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k" xr:uid="{C9B7F519-FC85-48AA-93F2-FB21BD51100E}"/>
-    <hyperlink ref="E25" r:id="rId55" display="https://leetcode.com/problems/sliding-window-maximum" xr:uid="{700AEA2A-73EB-45E0-A7C4-C9B375DDFDD1}"/>
-    <hyperlink ref="E78" r:id="rId56" display="https://leetcode.com/problems/design-circular-deque" xr:uid="{C374A6F7-208C-4F78-840A-5324F48EA186}"/>
-    <hyperlink ref="E24" r:id="rId57" display="https://leetcode.com/problems/design-circular-queue" xr:uid="{9290B313-663F-43FF-8027-AB89DA22F6BD}"/>
-    <hyperlink ref="E77" r:id="rId58" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{8802B7B3-B0D3-4F45-83F5-C1CF53DB69A6}"/>
-    <hyperlink ref="E23" r:id="rId59" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{2B0D8F07-EC59-4BAD-93CF-98C511AC3E21}"/>
-    <hyperlink ref="E26" r:id="rId60" display="https://leetcode.com/problems/binary-tree-inorder-traversal" xr:uid="{1B856373-DA81-4D15-ACC2-F7C093A506A8}"/>
-    <hyperlink ref="E80" r:id="rId61" display="https://leetcode.com/problems/binary-tree-level-order-traversal" xr:uid="{6AAEF83E-F9D9-409A-927C-DDEE7AEA57FC}"/>
-    <hyperlink ref="E81" r:id="rId62" display="https://leetcode.com/problems/binary-tree-right-side-view" xr:uid="{5577EFF4-DB1A-480F-83F5-F19EDE79C4B5}"/>
-    <hyperlink ref="E27" r:id="rId63" display="https://leetcode.com/problems/search-in-a-binary-search-tree" xr:uid="{A758D8A5-36A2-40FF-A15F-1A6A7A69801A}"/>
-    <hyperlink ref="E82" r:id="rId64" display="https://leetcode.com/problems/delete-node-in-a-bst" xr:uid="{591B7EA7-3888-49B3-99EF-BA629CD9A02D}"/>
-    <hyperlink ref="E28" r:id="rId65" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{78FB8ABE-DFC4-47EA-ACA0-CFB46543B8DC}"/>
-    <hyperlink ref="E83" r:id="rId66" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree" xr:uid="{5AA82C0A-C3F6-4840-B663-78DC8E56D219}"/>
-    <hyperlink ref="E30" r:id="rId67" display="https://leetcode.com/problems/last-stone-weight" xr:uid="{CAD60500-B89D-4C41-8574-D33E4F0BB32A}"/>
-    <hyperlink ref="E85" r:id="rId68" display="https://leetcode.com/problems/k-closest-points-to-origin" xr:uid="{BBD06487-6DC3-4A9B-83CC-F430BAF527D5}"/>
-    <hyperlink ref="E31" r:id="rId69" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{88E6C8C5-7B90-4A92-BECC-A629C8A55FEC}"/>
-    <hyperlink ref="E86" r:id="rId70" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix" xr:uid="{4C161606-D259-4AC4-BDFF-44E161BFF6BD}"/>
-    <hyperlink ref="E32" r:id="rId71" display="https://leetcode.com/problems/top-k-frequent-words" xr:uid="{4FD04348-E4BE-4F5E-83FD-752D5452B19E}"/>
-    <hyperlink ref="E87" r:id="rId72" display="https://leetcode.com/problems/top-k-frequent-elements" xr:uid="{31ABA819-3C4C-4002-8FCF-364AEF9823BD}"/>
-    <hyperlink ref="E33" r:id="rId73" display="https://leetcode.com/problems/two-sum" xr:uid="{5B404BE5-D0E3-4728-8498-75AFA5031304}"/>
-    <hyperlink ref="E88" r:id="rId74" display="https://leetcode.com/problems/ransom-note" xr:uid="{E50D5A6F-DB16-4D48-974E-C7847334D093}"/>
-    <hyperlink ref="E89" r:id="rId75" display="https://leetcode.com/problems/contains-duplicate" xr:uid="{EEA73F8B-13F1-431E-A0F1-3A0C6B23527D}"/>
-    <hyperlink ref="E34" r:id="rId76" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{4D7D4589-2B8A-47DC-9FCF-904D6E82FB71}"/>
-    <hyperlink ref="E90" r:id="rId77" display="https://leetcode.com/problems/subarray-sums-divisible-by-k" xr:uid="{D838CB32-0488-4C04-951B-6AA80F72BEA1}"/>
-    <hyperlink ref="E35" r:id="rId78" display="https://leetcode.com/problems/group-anagrams" xr:uid="{E64749FE-4AC2-4B2B-91C7-7180E2DCC00B}"/>
-    <hyperlink ref="E91" r:id="rId79" display="https://leetcode.com/problems/longest-consecutive-sequence" xr:uid="{DE30C124-13F2-439B-9476-17D8DAC27129}"/>
-    <hyperlink ref="E36" r:id="rId80" display="https://leetcode.com/problems/number-of-islands" xr:uid="{8DBAE9D8-4931-4C16-AEED-F66841DA88D4}"/>
-    <hyperlink ref="E92" r:id="rId81" display="https://leetcode.com/problems/max-area-of-island" xr:uid="{1B4C9834-1FC5-4895-806E-038B1DBDDA4B}"/>
-    <hyperlink ref="E93" r:id="rId82" display="https://leetcode.com/problems/01-matrix" xr:uid="{A0E46D51-24FB-432C-9B64-F9A7D564ADF2}"/>
-    <hyperlink ref="E37" r:id="rId83" display="https://leetcode.com/problems/network-delay-time" xr:uid="{F759E8D2-9590-49C8-B0C1-9FDC2453A281}"/>
-    <hyperlink ref="E94" r:id="rId84" display="https://leetcode.com/problems/redundant-connection" xr:uid="{EB3F5CE4-E5E9-420F-8C29-1A45626B6B12}"/>
-    <hyperlink ref="E95" r:id="rId85" display="https://leetcode.com/problems/number-of-provinces" xr:uid="{7F9CCD13-89BD-4996-B7B2-71D1985A3440}"/>
-    <hyperlink ref="E38" r:id="rId86" display="https://leetcode.com/problems/course-schedule" xr:uid="{1BB86DA6-53E2-4F87-8150-7BF6C57A100C}"/>
-    <hyperlink ref="E96" r:id="rId87" display="https://leetcode.com/problems/course-schedule-ii" xr:uid="{5177CC97-2B77-43CF-B33F-3903154A502D}"/>
-    <hyperlink ref="E97" r:id="rId88" display="https://leetcode.com/problems/clone-graph" xr:uid="{16DC6C12-1E3C-4E22-B3FF-A38677E0B8F3}"/>
-    <hyperlink ref="E39" r:id="rId89" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{8E820236-2EA3-409B-AA9C-D43A03343FCB}"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://leetcode.com/problems/ransom-note" xr:uid="{9ACCC9FD-0DC8-4254-BB8B-808F3BDD3784}"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://leetcode.com/problems/valid-anagram" xr:uid="{EE4FEEAF-652D-4D2D-A2A9-CB87731F42BE}"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters" xr:uid="{4DD7CB8D-B440-4AF4-B6AB-D727391B9158}"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string" xr:uid="{7CCC4C5F-1CA6-46F8-9DD3-9647C7682498}"/>
+    <hyperlink ref="E7" r:id="rId6" display="https://leetcode.com/problems/minimum-window-substring" xr:uid="{61B1900B-EAF8-4BE8-ACAB-A956DE5F3ED1}"/>
+    <hyperlink ref="E8" r:id="rId7" display="https://leetcode.com/problems/container-with-most-water" xr:uid="{84B1B8CA-3A3C-4909-8DD8-F88A45D68628}"/>
+    <hyperlink ref="E9" r:id="rId8" display="https://leetcode.com/problems/3sum" xr:uid="{42633795-6F73-49FF-B778-78E0CD056E83}"/>
+    <hyperlink ref="E10" r:id="rId9" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array" xr:uid="{DFA525B5-0825-451E-B3E0-9DC93194D4E1}"/>
+    <hyperlink ref="E11" r:id="rId10" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{3640DDE9-2ADF-42E2-AEDE-DA2AC3BA211A}"/>
+    <hyperlink ref="E12" r:id="rId11" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k" xr:uid="{8062781F-458E-4926-B311-804BA6CD3BBB}"/>
+    <hyperlink ref="E13" r:id="rId12" display="https://leetcode.com/problems/maximum-subarray" xr:uid="{3AD35EF8-0181-42B2-9B38-F0FC3F95CFE6}"/>
+    <hyperlink ref="E14" r:id="rId13" display="https://leetcode.com/problems/maximum-depth-of-binary-tree" xr:uid="{44C26DDF-9EB7-417D-B269-6C23AC6E6445}"/>
+    <hyperlink ref="E15" r:id="rId14" display="https://leetcode.com/problems/invert-binary-tree" xr:uid="{14199D52-1EAC-49F1-8883-00C4203FC3E3}"/>
+    <hyperlink ref="E16" r:id="rId15" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{52E248D0-3A46-4957-B7A0-F75EBA672C5B}"/>
+    <hyperlink ref="E17" r:id="rId16" display="https://leetcode.com/problems/different-ways-to-add-parentheses" xr:uid="{9DA410A2-6C01-4EDA-9F51-6FBA009D88DF}"/>
+    <hyperlink ref="E18" r:id="rId17" display="https://leetcode.com/problems/unique-binary-search-trees-ii" xr:uid="{68A314C1-D173-4545-AF04-B8E2F74F893D}"/>
+    <hyperlink ref="E19" r:id="rId18" display="https://leetcode.com/problems/powx-n" xr:uid="{26A0C127-23BD-4BCE-8BC7-8AB1A8F90ADE}"/>
+    <hyperlink ref="E20" r:id="rId19" display="https://leetcode.com/problems/subsets" xr:uid="{22D9BCEB-5D0D-4BEF-A700-0FC47638B9F3}"/>
+    <hyperlink ref="E21" r:id="rId20" display="https://leetcode.com/problems/permutations" xr:uid="{E47F3CB1-204D-4424-914C-698242057FAC}"/>
+    <hyperlink ref="E22" r:id="rId21" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{5F57D8FD-824D-4DB1-892E-1DDFD0F8F33D}"/>
+    <hyperlink ref="E28" r:id="rId22" display="https://leetcode.com/problems/binary-search" xr:uid="{374FFDAF-FCB9-431A-86D2-31AB60378C3A}"/>
+    <hyperlink ref="E29" r:id="rId23" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array" xr:uid="{3F271E59-4045-4398-82DB-BC2F4B35A995}"/>
+    <hyperlink ref="E30" r:id="rId24" display="https://leetcode.com/problems/find-peak-element" xr:uid="{DEF2D431-80D6-4E0B-868E-499158EC2963}"/>
+    <hyperlink ref="E31" r:id="rId25" display="https://leetcode.com/problems/koko-eating-bananas" xr:uid="{B3E73AEB-2A95-4916-A93C-BC5B60CAA1D7}"/>
+    <hyperlink ref="E32" r:id="rId26" display="https://leetcode.com/problems/split-array-largest-sum" xr:uid="{BCAC5094-3A8A-4714-BD84-F606403D9DA0}"/>
+    <hyperlink ref="E33" r:id="rId27" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days" xr:uid="{1965E795-8B07-42CA-9865-3EEF521E25E1}"/>
+    <hyperlink ref="E34" r:id="rId28" display="https://leetcode.com/problems/sort-an-array" xr:uid="{E0B9E0A6-F8E5-418F-87DD-47E7F6723CFF}"/>
+    <hyperlink ref="E35" r:id="rId29" display="https://leetcode.com/problems/insertion-sort-list" xr:uid="{03811762-664A-488F-9B2D-036EAE5AAD21}"/>
+    <hyperlink ref="E36" r:id="rId30" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{4F771129-F99D-4F68-954B-762315CE30B8}"/>
+    <hyperlink ref="E37" r:id="rId31" display="https://leetcode.com/problems/largest-number" xr:uid="{373767EF-F0B1-409B-B448-2E15DEE2A726}"/>
+    <hyperlink ref="E38" r:id="rId32" display="https://leetcode.com/problems/reorder-data-in-log-files" xr:uid="{A0B197A5-BF64-4823-8C80-786CEECF12F4}"/>
+    <hyperlink ref="E39" r:id="rId33" display="https://leetcode.com/problems/merge-intervals" xr:uid="{04E9289A-1232-436E-8E31-F058BBB75316}"/>
+    <hyperlink ref="E40" r:id="rId34" display="https://leetcode.com/problems/insert-interval" xr:uid="{355C5E3F-38DD-4154-ACB8-71E37347CA2D}"/>
+    <hyperlink ref="E41" r:id="rId35" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{73B2795D-90B0-4FEF-BAE2-297C16F48CD8}"/>
+    <hyperlink ref="E42" r:id="rId36" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{A4102035-5F89-45CA-99F6-62571131E444}"/>
+    <hyperlink ref="E43" r:id="rId37" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{213E0623-CF2A-4978-9133-4CAD9B8DDC70}"/>
+    <hyperlink ref="E44" r:id="rId38" display="https://leetcode.com/problems/reverse-linked-list-ii" xr:uid="{3E496F01-EEA1-4941-97A8-3FA083834977}"/>
+    <hyperlink ref="E45" r:id="rId39" display="https://leetcode.com/problems/linked-list-cycle" xr:uid="{9C26BB6C-78AB-4618-BD00-77BAAF16815D}"/>
+    <hyperlink ref="E46" r:id="rId40" display="https://leetcode.com/problems/linked-list-cycle-ii" xr:uid="{EC5A3D70-F195-4C10-9EA2-058F32835B9E}"/>
+    <hyperlink ref="E47" r:id="rId41" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{5C4F4E4B-2209-41D3-A906-19E1F708F9DB}"/>
+    <hyperlink ref="E48" r:id="rId42" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{1C1B8A5C-EA41-461E-8FA3-BD6A6B5B3181}"/>
+    <hyperlink ref="E49" r:id="rId43" display="https://leetcode.com/problems/intersection-of-two-linked-lists" xr:uid="{606E5182-D172-41A2-9D50-33C726FC8AB7}"/>
+    <hyperlink ref="E50" r:id="rId44" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{CD69A99D-FBAA-46B5-B0DF-9DE5139BE679}"/>
+    <hyperlink ref="E51" r:id="rId45" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{5D746582-1B54-4352-BDA4-86F05542CE88}"/>
+    <hyperlink ref="E52" r:id="rId46" display="https://leetcode.com/problems/odd-even-linked-list" xr:uid="{C89465FE-7C33-4395-99CB-4BA5D7CED11B}"/>
+    <hyperlink ref="E53" r:id="rId47" display="https://leetcode.com/problems/lru-cache" xr:uid="{05D0EB4C-0E5B-4E3E-AAB2-1A648C9129E7}"/>
+    <hyperlink ref="E54" r:id="rId48" display="https://leetcode.com/problems/lfu-cache" xr:uid="{DF951C59-83C3-4B8E-98CC-B79E487C918E}"/>
+    <hyperlink ref="E55" r:id="rId49" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{91E7DBEA-4D8A-41C9-AAC9-D9BA3BCE6D19}"/>
+    <hyperlink ref="E56" r:id="rId50" display="https://leetcode.com/problems/backspace-string-compare" xr:uid="{BD0B5108-E7EF-4D79-983A-AF8C10DCB73C}"/>
+    <hyperlink ref="E57" r:id="rId51" display="https://leetcode.com/problems/daily-temperatures" xr:uid="{B087D9B6-012A-40BD-B913-355D4FBD2EFE}"/>
+    <hyperlink ref="E58" r:id="rId52" display="https://leetcode.com/problems/next-greater-element-i" xr:uid="{FB709363-8602-45D4-B45B-8C9367125A7E}"/>
+    <hyperlink ref="E59" r:id="rId53" display="https://leetcode.com/problems/largest-rectangle-in-histogram" xr:uid="{704BEAA6-4976-4029-886F-A6FDCC20AE13}"/>
+    <hyperlink ref="E65" r:id="rId54" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k" xr:uid="{C9B7F519-FC85-48AA-93F2-FB21BD51100E}"/>
+    <hyperlink ref="E64" r:id="rId55" display="https://leetcode.com/problems/sliding-window-maximum" xr:uid="{700AEA2A-73EB-45E0-A7C4-C9B375DDFDD1}"/>
+    <hyperlink ref="E63" r:id="rId56" display="https://leetcode.com/problems/design-circular-deque" xr:uid="{C374A6F7-208C-4F78-840A-5324F48EA186}"/>
+    <hyperlink ref="E62" r:id="rId57" display="https://leetcode.com/problems/design-circular-queue" xr:uid="{9290B313-663F-43FF-8027-AB89DA22F6BD}"/>
+    <hyperlink ref="E61" r:id="rId58" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{8802B7B3-B0D3-4F45-83F5-C1CF53DB69A6}"/>
+    <hyperlink ref="E60" r:id="rId59" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{2B0D8F07-EC59-4BAD-93CF-98C511AC3E21}"/>
+    <hyperlink ref="E66" r:id="rId60" display="https://leetcode.com/problems/binary-tree-inorder-traversal" xr:uid="{1B856373-DA81-4D15-ACC2-F7C093A506A8}"/>
+    <hyperlink ref="E67" r:id="rId61" display="https://leetcode.com/problems/binary-tree-level-order-traversal" xr:uid="{6AAEF83E-F9D9-409A-927C-DDEE7AEA57FC}"/>
+    <hyperlink ref="E68" r:id="rId62" display="https://leetcode.com/problems/binary-tree-right-side-view" xr:uid="{5577EFF4-DB1A-480F-83F5-F19EDE79C4B5}"/>
+    <hyperlink ref="E69" r:id="rId63" display="https://leetcode.com/problems/search-in-a-binary-search-tree" xr:uid="{A758D8A5-36A2-40FF-A15F-1A6A7A69801A}"/>
+    <hyperlink ref="E70" r:id="rId64" display="https://leetcode.com/problems/delete-node-in-a-bst" xr:uid="{591B7EA7-3888-49B3-99EF-BA629CD9A02D}"/>
+    <hyperlink ref="E71" r:id="rId65" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{78FB8ABE-DFC4-47EA-ACA0-CFB46543B8DC}"/>
+    <hyperlink ref="E72" r:id="rId66" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree" xr:uid="{5AA82C0A-C3F6-4840-B663-78DC8E56D219}"/>
+    <hyperlink ref="E75" r:id="rId67" display="https://leetcode.com/problems/last-stone-weight" xr:uid="{CAD60500-B89D-4C41-8574-D33E4F0BB32A}"/>
+    <hyperlink ref="E76" r:id="rId68" display="https://leetcode.com/problems/k-closest-points-to-origin" xr:uid="{BBD06487-6DC3-4A9B-83CC-F430BAF527D5}"/>
+    <hyperlink ref="E77" r:id="rId69" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{88E6C8C5-7B90-4A92-BECC-A629C8A55FEC}"/>
+    <hyperlink ref="E78" r:id="rId70" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix" xr:uid="{4C161606-D259-4AC4-BDFF-44E161BFF6BD}"/>
+    <hyperlink ref="E79" r:id="rId71" display="https://leetcode.com/problems/top-k-frequent-words" xr:uid="{4FD04348-E4BE-4F5E-83FD-752D5452B19E}"/>
+    <hyperlink ref="E80" r:id="rId72" display="https://leetcode.com/problems/top-k-frequent-elements" xr:uid="{31ABA819-3C4C-4002-8FCF-364AEF9823BD}"/>
+    <hyperlink ref="E81" r:id="rId73" display="https://leetcode.com/problems/two-sum" xr:uid="{5B404BE5-D0E3-4728-8498-75AFA5031304}"/>
+    <hyperlink ref="E82" r:id="rId74" display="https://leetcode.com/problems/ransom-note" xr:uid="{E50D5A6F-DB16-4D48-974E-C7847334D093}"/>
+    <hyperlink ref="E83" r:id="rId75" display="https://leetcode.com/problems/contains-duplicate" xr:uid="{EEA73F8B-13F1-431E-A0F1-3A0C6B23527D}"/>
+    <hyperlink ref="E84" r:id="rId76" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{4D7D4589-2B8A-47DC-9FCF-904D6E82FB71}"/>
+    <hyperlink ref="E85" r:id="rId77" display="https://leetcode.com/problems/subarray-sums-divisible-by-k" xr:uid="{D838CB32-0488-4C04-951B-6AA80F72BEA1}"/>
+    <hyperlink ref="E86" r:id="rId78" display="https://leetcode.com/problems/group-anagrams" xr:uid="{E64749FE-4AC2-4B2B-91C7-7180E2DCC00B}"/>
+    <hyperlink ref="E87" r:id="rId79" display="https://leetcode.com/problems/longest-consecutive-sequence" xr:uid="{DE30C124-13F2-439B-9476-17D8DAC27129}"/>
+    <hyperlink ref="E88" r:id="rId80" display="https://leetcode.com/problems/number-of-islands" xr:uid="{8DBAE9D8-4931-4C16-AEED-F66841DA88D4}"/>
+    <hyperlink ref="E89" r:id="rId81" display="https://leetcode.com/problems/max-area-of-island" xr:uid="{1B4C9834-1FC5-4895-806E-038B1DBDDA4B}"/>
+    <hyperlink ref="E90" r:id="rId82" display="https://leetcode.com/problems/01-matrix" xr:uid="{A0E46D51-24FB-432C-9B64-F9A7D564ADF2}"/>
+    <hyperlink ref="E91" r:id="rId83" display="https://leetcode.com/problems/network-delay-time" xr:uid="{F759E8D2-9590-49C8-B0C1-9FDC2453A281}"/>
+    <hyperlink ref="E92" r:id="rId84" display="https://leetcode.com/problems/redundant-connection" xr:uid="{EB3F5CE4-E5E9-420F-8C29-1A45626B6B12}"/>
+    <hyperlink ref="E93" r:id="rId85" display="https://leetcode.com/problems/number-of-provinces" xr:uid="{7F9CCD13-89BD-4996-B7B2-71D1985A3440}"/>
+    <hyperlink ref="E94" r:id="rId86" display="https://leetcode.com/problems/course-schedule" xr:uid="{1BB86DA6-53E2-4F87-8150-7BF6C57A100C}"/>
+    <hyperlink ref="E95" r:id="rId87" display="https://leetcode.com/problems/course-schedule-ii" xr:uid="{5177CC97-2B77-43CF-B33F-3903154A502D}"/>
+    <hyperlink ref="E96" r:id="rId88" display="https://leetcode.com/problems/clone-graph" xr:uid="{16DC6C12-1E3C-4E22-B3FF-A38677E0B8F3}"/>
+    <hyperlink ref="E97" r:id="rId89" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{8E820236-2EA3-409B-AA9C-D43A03343FCB}"/>
     <hyperlink ref="E98" r:id="rId90" display="https://leetcode.com/problems/climbing-stairs" xr:uid="{40181C74-4968-41A8-B229-0DF250C3A787}"/>
     <hyperlink ref="E99" r:id="rId91" display="https://leetcode.com/problems/min-cost-climbing-stairs" xr:uid="{9E7BFCA6-DA59-48A0-975B-9589BDC7C276}"/>
-    <hyperlink ref="E40" r:id="rId92" display="https://leetcode.com/problems/longest-common-subsequence" xr:uid="{30F8CF6D-7369-4957-A7D7-160A741AA38C}"/>
-    <hyperlink ref="E100" r:id="rId93" display="https://leetcode.com/problems/longest-increasing-subsequence" xr:uid="{0B0509FA-0F85-46F0-803E-3112FAE33195}"/>
-    <hyperlink ref="E101" r:id="rId94" display="https://leetcode.com/problems/palindromic-substrings" xr:uid="{DAA8A2AD-4DEC-4740-BE2E-FF2A710FC881}"/>
-    <hyperlink ref="E41" r:id="rId95" display="https://leetcode.com/problems/unique-paths" xr:uid="{3BFACFF5-9CEA-445E-837D-80CE02DD15B6}"/>
-    <hyperlink ref="E102" r:id="rId96" display="https://leetcode.com/problems/partition-equal-subset-sum" xr:uid="{7588C036-6A20-4C85-94EE-72396427AA61}"/>
-    <hyperlink ref="E103" r:id="rId97" display="https://leetcode.com/problems/target-sum" xr:uid="{B8B2404F-6A1D-4008-9903-335EA651A7DC}"/>
-    <hyperlink ref="E42" r:id="rId98" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{6B9267CD-AC96-447A-879D-41081B74ECAC}"/>
-    <hyperlink ref="E104" r:id="rId99" display="https://leetcode.com/problems/merge-intervals" xr:uid="{C1AA793D-64CD-400D-A0A9-D182B005CEDC}"/>
-    <hyperlink ref="E105" r:id="rId100" display="https://leetcode.com/problems/gas-station" xr:uid="{9A4CC2B1-7301-4996-8463-5549D190A892}"/>
-    <hyperlink ref="E43" r:id="rId101" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{9AF79B77-6ADE-45DC-A721-A6C56EA49A98}"/>
-    <hyperlink ref="E106" r:id="rId102" display="https://leetcode.com/problems/can-place-flowers" xr:uid="{9BBCC8E1-2E28-48FF-9415-D9250E2D1CFB}"/>
-    <hyperlink ref="E107" r:id="rId103" display="https://leetcode.com/problems/jump-game" xr:uid="{22D973B8-6E8A-41F7-BF66-D13FE9CE93A0}"/>
+    <hyperlink ref="E100" r:id="rId92" display="https://leetcode.com/problems/longest-common-subsequence" xr:uid="{30F8CF6D-7369-4957-A7D7-160A741AA38C}"/>
+    <hyperlink ref="E101" r:id="rId93" display="https://leetcode.com/problems/longest-increasing-subsequence" xr:uid="{0B0509FA-0F85-46F0-803E-3112FAE33195}"/>
+    <hyperlink ref="E102" r:id="rId94" display="https://leetcode.com/problems/palindromic-substrings" xr:uid="{DAA8A2AD-4DEC-4740-BE2E-FF2A710FC881}"/>
+    <hyperlink ref="E103" r:id="rId95" display="https://leetcode.com/problems/unique-paths" xr:uid="{3BFACFF5-9CEA-445E-837D-80CE02DD15B6}"/>
+    <hyperlink ref="E104" r:id="rId96" display="https://leetcode.com/problems/partition-equal-subset-sum" xr:uid="{7588C036-6A20-4C85-94EE-72396427AA61}"/>
+    <hyperlink ref="E105" r:id="rId97" display="https://leetcode.com/problems/target-sum" xr:uid="{B8B2404F-6A1D-4008-9903-335EA651A7DC}"/>
+    <hyperlink ref="E106" r:id="rId98" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{6B9267CD-AC96-447A-879D-41081B74ECAC}"/>
+    <hyperlink ref="E107" r:id="rId99" display="https://leetcode.com/problems/merge-intervals" xr:uid="{C1AA793D-64CD-400D-A0A9-D182B005CEDC}"/>
+    <hyperlink ref="E108" r:id="rId100" display="https://leetcode.com/problems/gas-station" xr:uid="{9A4CC2B1-7301-4996-8463-5549D190A892}"/>
+    <hyperlink ref="E109" r:id="rId101" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{9AF79B77-6ADE-45DC-A721-A6C56EA49A98}"/>
+    <hyperlink ref="E110" r:id="rId102" display="https://leetcode.com/problems/can-place-flowers" xr:uid="{9BBCC8E1-2E28-48FF-9415-D9250E2D1CFB}"/>
+    <hyperlink ref="E111" r:id="rId103" display="https://leetcode.com/problems/jump-game" xr:uid="{22D973B8-6E8A-41F7-BF66-D13FE9CE93A0}"/>
+    <hyperlink ref="E23" r:id="rId104" display="https://leetcode.com/problems/n-queens" xr:uid="{69BB437F-E482-4232-B7A6-D86FFB9B9B11}"/>
+    <hyperlink ref="E24" r:id="rId105" display="https://leetcode.com/problems/n-queens-ii" xr:uid="{E91B232D-5ED5-407F-BC79-BA4E584B16DD}"/>
+    <hyperlink ref="E25" r:id="rId106" display="https://leetcode.com/problems/subsets-ii" xr:uid="{E82CECCF-46F9-40BE-919A-4DF7D362F5FD}"/>
+    <hyperlink ref="E26" r:id="rId107" display="https://leetcode.com/problems/permutations-ii" xr:uid="{BB9406D1-F97D-422E-81C5-BED20DBD5DE4}"/>
+    <hyperlink ref="E27" r:id="rId108" display="https://leetcode.com/problems/combination-sum" xr:uid="{523178B6-AF5B-4927-8BC6-3484B292F8FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId104"/>
+  <pageSetup orientation="portrait" r:id="rId109"/>
   <tableParts count="1">
-    <tablePart r:id="rId105"/>
+    <tablePart r:id="rId110"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(leetcode): added solutions for problems 38, 76, 242, and 383 chore(lesson-plan): updated with Leetcode problem numbers discussed on June 20, 2025 feat(material): updated string material with product-based company focus topics
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schedule\Documents\TIME_DK\time_colleges\SRET\Focus_Batch_2023-2027\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2_TIME_College\SRET\sret-focus-batch-23-27\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AA92E9-0490-4F7D-AB9D-1E7E88B9F6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hours Alloted" sheetId="1" r:id="rId1"/>
     <sheet name="Lesson Plan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="256">
   <si>
     <t>Order</t>
   </si>
@@ -788,13 +787,19 @@
   </si>
   <si>
     <t>39. Combination Sum</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>38. Count and Say</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -818,13 +823,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -836,11 +860,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -863,12 +888,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -888,6 +923,9 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -927,7 +965,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -961,31 +998,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC2EB891-804F-43E8-A06F-387079CE4D81}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:C20" xr:uid="{EC2EB891-804F-43E8-A06F-387079CE4D81}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:C20"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BA9C8891-1203-46DA-B01A-4B17E8515E96}" name="Order" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{EDE8DF91-E7F4-45E1-911B-F8ABD4867ACA}" name="Topic" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{218431B5-9426-4E2F-BF73-B4A99D3E3320}" name="Hours" dataDxfId="11"/>
+    <tableColumn id="1" name="Order" dataDxfId="14"/>
+    <tableColumn id="2" name="Topic" dataDxfId="13"/>
+    <tableColumn id="3" name="Hours" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{512AC03F-78F7-4FEC-8505-F6AAC24DF528}" name="Table2" displayName="Table2" ref="A1:G113" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:G113" xr:uid="{512AC03F-78F7-4FEC-8505-F6AAC24DF528}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:H113"/>
+  <sortState ref="A2:G113">
     <sortCondition ref="A1:A113"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{911CBD74-C633-4B51-85BF-53095DEB2CC8}" name="S.No" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{5CF9DF08-2218-4086-957B-A763D40BD5FE}" name="Topic" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{BD3DE0D9-F294-4850-ABC3-4AC5AC389F23}" name="Subtopic" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{D095E8DD-227D-4C1F-937E-D4545535A42D}" name="Hour" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{4ABDE408-207C-41EB-B0D2-66F110860C2E}" name="LeetCode Problem" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{0CD9435E-F9FD-44E9-A221-89DA8A3A11E6}" name="Level" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{C0930A4E-6BCC-4DFF-B424-04E79129EAAD}" name="Remark" dataDxfId="2"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="S.No" dataDxfId="9"/>
+    <tableColumn id="2" name="Topic" dataDxfId="8"/>
+    <tableColumn id="3" name="Subtopic" dataDxfId="7"/>
+    <tableColumn id="4" name="Hour" dataDxfId="6"/>
+    <tableColumn id="5" name="LeetCode Problem" dataDxfId="5"/>
+    <tableColumn id="6" name="Level" dataDxfId="4"/>
+    <tableColumn id="7" name="Remark" dataDxfId="3"/>
+    <tableColumn id="8" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1253,21 +1291,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6"/>
+    <col min="1" max="1" width="9.109375" style="6"/>
+    <col min="2" max="2" width="60.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1278,7 +1316,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1289,7 +1327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1300,7 +1338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1311,7 +1349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1322,7 +1360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1333,7 +1371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1344,7 +1382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1355,7 +1393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1366,7 +1404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1377,7 +1415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1388,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1399,7 +1437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1410,7 +1448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1421,7 +1459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1432,7 +1470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1443,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1454,7 +1492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1465,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1476,7 +1514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1487,7 +1525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" s="6">
         <f>SUM(C2:C21)</f>
         <v>45</v>
@@ -1502,26 +1540,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47E1B90-F79D-473A-8C0F-D2580CDDC346}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.28515625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.77734375" customWidth="1"/>
+    <col min="9" max="9" width="36.33203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -1543,8 +1582,11 @@
       <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1557,7 +1599,7 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1566,12 +1608,15 @@
       <c r="G2" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H2" s="10" t="s">
+        <v>255</v>
+      </c>
       <c r="I2" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>String: Hashing + Count</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1582,7 +1627,7 @@
         <v>33</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1591,12 +1636,13 @@
       <c r="G3" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H3" s="3"/>
       <c r="I3" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>String: Frequency Matching</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1607,7 +1653,7 @@
         <v>33</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -1616,12 +1662,13 @@
       <c r="G4" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H4" s="3"/>
       <c r="I4" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>String: Frequency Matching</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1635,20 +1682,21 @@
         <v>2</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H5" s="3"/>
       <c r="I5" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1668,12 +1716,13 @@
       <c r="G6" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H6" s="3"/>
       <c r="I6" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1685,20 +1734,21 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H7" s="3"/>
       <c r="I7" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1720,12 +1770,13 @@
       <c r="G8" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H8" s="3"/>
       <c r="I8" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1745,12 +1796,13 @@
       <c r="G9" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H9" s="3"/>
       <c r="I9" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1770,12 +1822,13 @@
       <c r="G10" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H10" s="3"/>
       <c r="I10" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1797,12 +1850,13 @@
       <c r="G11" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H11" s="3"/>
       <c r="I11" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1822,12 +1876,13 @@
       <c r="G12" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H12" s="3"/>
       <c r="I12" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1847,12 +1902,13 @@
       <c r="G13" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H13" s="3"/>
       <c r="I13" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1874,12 +1930,13 @@
       <c r="G14" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H14" s="3"/>
       <c r="I14" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Recursion: Base Case + Tree View</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1899,12 +1956,13 @@
       <c r="G15" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H15" s="3"/>
       <c r="I15" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Recursion: Base Case Practice</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1924,12 +1982,13 @@
       <c r="G16" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H16" s="3"/>
       <c r="I16" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Recursion: Fibonacci</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1951,12 +2010,13 @@
       <c r="G17" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H17" s="3"/>
       <c r="I17" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Recursion: Divide and Conquer</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1976,12 +2036,13 @@
       <c r="G18" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H18" s="3"/>
       <c r="I18" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Recursion: Divide and Conquer</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2001,12 +2062,13 @@
       <c r="G19" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H19" s="3"/>
       <c r="I19" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Recursion: Binary Recursion Tree</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2028,12 +2090,13 @@
       <c r="G20" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H20" s="3"/>
       <c r="I20" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Recursion: Subsets</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2053,12 +2116,13 @@
       <c r="G21" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H21" s="3"/>
       <c r="I21" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Recursion: Rec. with State</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2078,12 +2142,13 @@
       <c r="G22" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H22" s="3"/>
       <c r="I22" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Recursion: Backtrack Base</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2105,12 +2170,13 @@
       <c r="G23" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H23" s="3"/>
       <c r="I23" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Backtracking: N-Queens</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2130,12 +2196,13 @@
       <c r="G24" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H24" s="3"/>
       <c r="I24" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Backtracking: N-Queens</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2157,12 +2224,13 @@
       <c r="G25" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H25" s="3"/>
       <c r="I25" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Backtracking: Subset Gen</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2182,12 +2250,13 @@
       <c r="G26" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H26" s="3"/>
       <c r="I26" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Backtracking: Permutations</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2207,12 +2276,13 @@
       <c r="G27" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H27" s="3"/>
       <c r="I27" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Backtracking: Combination Sum</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2234,12 +2304,13 @@
       <c r="G28" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H28" s="3"/>
       <c r="I28" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Searching: Binary Search Basic</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2259,12 +2330,13 @@
       <c r="G29" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H29" s="3"/>
       <c r="I29" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Searching: First/Last Occurrence</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2284,12 +2356,13 @@
       <c r="G30" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H30" s="3"/>
       <c r="I30" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Searching: Peak Element</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2311,12 +2384,13 @@
       <c r="G31" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H31" s="3"/>
       <c r="I31" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2336,12 +2410,13 @@
       <c r="G32" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H32" s="3"/>
       <c r="I32" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2361,12 +2436,13 @@
       <c r="G33" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H33" s="3"/>
       <c r="I33" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2388,12 +2464,13 @@
       <c r="G34" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H34" s="3"/>
       <c r="I34" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Sorting: Basic Sorting Logic</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2413,12 +2490,13 @@
       <c r="G35" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H35" s="3"/>
       <c r="I35" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Sorting: Selection Practice</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2438,12 +2516,13 @@
       <c r="G36" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H36" s="3"/>
       <c r="I36" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Sorting: QuickSort</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2465,12 +2544,13 @@
       <c r="G37" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H37" s="3"/>
       <c r="I37" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Sorting: Custom Comparator</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2490,12 +2570,13 @@
       <c r="G38" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H38" s="3"/>
       <c r="I38" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Sorting: Custom Comparator</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2517,12 +2598,13 @@
       <c r="G39" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H39" s="3"/>
       <c r="I39" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Sorting: Merge Intervals</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2542,12 +2624,13 @@
       <c r="G40" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H40" s="3"/>
       <c r="I40" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Sorting: Merge Intervals</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2569,12 +2652,13 @@
       <c r="G41" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H41" s="3"/>
       <c r="I41" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Sorting: Scheduling Logic</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2594,12 +2678,13 @@
       <c r="G42" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H42" s="3"/>
       <c r="I42" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Sorting: Sorting Based Greedy</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2621,12 +2706,13 @@
       <c r="G43" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H43" s="3"/>
       <c r="I43" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: Reverse LL</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2646,12 +2732,13 @@
       <c r="G44" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H44" s="3"/>
       <c r="I44" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: Reverse LL II</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2673,12 +2760,13 @@
       <c r="G45" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H45" s="3"/>
       <c r="I45" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: Detect Cycle</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2698,12 +2786,13 @@
       <c r="G46" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H46" s="3"/>
       <c r="I46" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: Cycle II</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2725,12 +2814,13 @@
       <c r="G47" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H47" s="3"/>
       <c r="I47" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: Merge LL</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2750,12 +2840,13 @@
       <c r="G48" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H48" s="3"/>
       <c r="I48" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: Merge k Lists</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2777,12 +2868,13 @@
       <c r="G49" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H49" s="3"/>
       <c r="I49" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: Intersection Point</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2802,12 +2894,13 @@
       <c r="G50" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H50" s="3"/>
       <c r="I50" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: Remove Nth Node</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2829,12 +2922,13 @@
       <c r="G51" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H51" s="3"/>
       <c r="I51" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: Palindrome Check</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2854,12 +2948,13 @@
       <c r="G52" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H52" s="3"/>
       <c r="I52" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: Odd Even Index</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2881,12 +2976,13 @@
       <c r="G53" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H53" s="3"/>
       <c r="I53" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: LRU Cache Logic</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2906,12 +3002,13 @@
       <c r="G54" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H54" s="3"/>
       <c r="I54" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Linked List: Advanced LRU Logic</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2933,12 +3030,13 @@
       <c r="G55" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H55" s="3"/>
       <c r="I55" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Stack: Stack Basics</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2958,12 +3056,13 @@
       <c r="G56" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H56" s="3"/>
       <c r="I56" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Stack: Stack Basics</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2985,12 +3084,13 @@
       <c r="G57" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H57" s="3"/>
       <c r="I57" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Stack: Monotonic Stack</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3010,12 +3110,13 @@
       <c r="G58" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H58" s="3"/>
       <c r="I58" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Stack: Next Greater Element</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3035,12 +3136,13 @@
       <c r="G59" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H59" s="3"/>
       <c r="I59" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Stack: Largest Rect in Hist</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3062,12 +3164,13 @@
       <c r="G60" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H60" s="3"/>
       <c r="I60" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Queue: Queue + BFS Intro</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3087,12 +3190,13 @@
       <c r="G61" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H61" s="3"/>
       <c r="I61" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Queue: Implement Queue Using Stacks</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3114,12 +3218,13 @@
       <c r="G62" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H62" s="3"/>
       <c r="I62" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Queue: Circular Queue</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3139,12 +3244,13 @@
       <c r="G63" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H63" s="3"/>
       <c r="I63" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Queue: Deque</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3166,12 +3272,13 @@
       <c r="G64" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H64" s="3"/>
       <c r="I64" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Queue: Monotonic Queue</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3191,12 +3298,13 @@
       <c r="G65" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H65" s="3"/>
       <c r="I65" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Queue: Monotonic Queue</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3218,12 +3326,13 @@
       <c r="G66" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H66" s="3"/>
       <c r="I66" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Trees: Traversals</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3243,12 +3352,13 @@
       <c r="G67" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H67" s="3"/>
       <c r="I67" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Trees: Traversals</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3268,12 +3378,13 @@
       <c r="G68" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H68" s="3"/>
       <c r="I68" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Trees: Views + Height</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3295,12 +3406,13 @@
       <c r="G69" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H69" s="3"/>
       <c r="I69" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>BST: Search, Insert, Min</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3320,12 +3432,13 @@
       <c r="G70" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H70" s="3"/>
       <c r="I70" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>BST: Deletion</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3347,12 +3460,13 @@
       <c r="G71" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H71" s="3"/>
       <c r="I71" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>BST: Validate BST</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3372,12 +3486,13 @@
       <c r="G72" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H72" s="3"/>
       <c r="I72" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>BST: Lowest Common Ancestor</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3399,12 +3514,13 @@
       <c r="G73" s="3" t="s">
         <v>162</v>
       </c>
+      <c r="H73" s="3"/>
       <c r="I73" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Balanced Tree: AVL Tree</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3424,12 +3540,13 @@
       <c r="G74" s="3" t="s">
         <v>164</v>
       </c>
+      <c r="H74" s="3"/>
       <c r="I74" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Balanced Tree: Red-Black Tree</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3451,12 +3568,13 @@
       <c r="G75" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H75" s="3"/>
       <c r="I75" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Heap: Min Heap Introduction</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3476,12 +3594,13 @@
       <c r="G76" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H76" s="3"/>
       <c r="I76" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Heap: Priority Queue Usage</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3503,12 +3622,13 @@
       <c r="G77" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H77" s="3"/>
       <c r="I77" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Heap: Kth Largest Element</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3528,12 +3648,13 @@
       <c r="G78" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H78" s="3"/>
       <c r="I78" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Heap: Kth Smallest Element</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3555,12 +3676,13 @@
       <c r="G79" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H79" s="3"/>
       <c r="I79" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Heap: Heap + Sorting Logic</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3580,12 +3702,13 @@
       <c r="G80" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H80" s="3"/>
       <c r="I80" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Heap: Heap + Custom Comparator</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3607,12 +3730,13 @@
       <c r="G81" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H81" s="3"/>
       <c r="I81" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>HashMap: Frequency Counting</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3632,12 +3756,13 @@
       <c r="G82" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H82" s="3"/>
       <c r="I82" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>HashMap: Frequency Counting</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3657,12 +3782,13 @@
       <c r="G83" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H83" s="3"/>
       <c r="I83" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>HashSet: Uniqueness Check</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3684,12 +3810,13 @@
       <c r="G84" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H84" s="3"/>
       <c r="I84" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>HashMap: Prefix Sum Technique</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3709,12 +3836,13 @@
       <c r="G85" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H85" s="3"/>
       <c r="I85" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>HashMap: Prefix Sum Variation</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -3736,12 +3864,13 @@
       <c r="G86" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H86" s="3"/>
       <c r="I86" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>HashMap: Grouping Data</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -3761,12 +3890,13 @@
       <c r="G87" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H87" s="3"/>
       <c r="I87" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>HashMap: Longest Streak/Length</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -3788,12 +3918,13 @@
       <c r="G88" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H88" s="3"/>
       <c r="I88" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Graph: BFS Traversal</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -3813,12 +3944,13 @@
       <c r="G89" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H89" s="3"/>
       <c r="I89" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Graph: DFS Traversal</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -3838,12 +3970,13 @@
       <c r="G90" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H90" s="3"/>
       <c r="I90" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Graph: BFS with Distance</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -3865,12 +3998,13 @@
       <c r="G91" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H91" s="3"/>
       <c r="I91" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Graph: Dijkstra’s (Shortest Path)</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -3890,12 +4024,13 @@
       <c r="G92" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H92" s="3"/>
       <c r="I92" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Graph: Union Find</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -3915,12 +4050,13 @@
       <c r="G93" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H93" s="3"/>
       <c r="I93" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Graph: Cycle Detection</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -3942,12 +4078,13 @@
       <c r="G94" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H94" s="3"/>
       <c r="I94" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Graph: Topological Sort</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -3967,12 +4104,13 @@
       <c r="G95" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H95" s="3"/>
       <c r="I95" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Graph: Topo + Ordering</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -3992,12 +4130,13 @@
       <c r="G96" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H96" s="3"/>
       <c r="I96" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Graph: Kahn’s Algorithm</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4019,12 +4158,13 @@
       <c r="G97" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H97" s="3"/>
       <c r="I97" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>DP: Fibonacci with Memo</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4044,12 +4184,13 @@
       <c r="G98" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H98" s="3"/>
       <c r="I98" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>DP: Climbing Stairs (1D)</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4069,12 +4210,13 @@
       <c r="G99" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H99" s="3"/>
       <c r="I99" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>DP: Min Cost Climbing</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4096,12 +4238,13 @@
       <c r="G100" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H100" s="3"/>
       <c r="I100" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>DP: Longest Common Subseq</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4121,12 +4264,13 @@
       <c r="G101" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H101" s="3"/>
       <c r="I101" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>DP: Longest Increasing Subseq</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4146,12 +4290,13 @@
       <c r="G102" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H102" s="3"/>
       <c r="I102" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>DP: Palindromic Substrings</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -4173,12 +4318,13 @@
       <c r="G103" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H103" s="3"/>
       <c r="I103" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>DP: Unique Paths (2D Grid)</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -4198,12 +4344,13 @@
       <c r="G104" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H104" s="3"/>
       <c r="I104" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>DP: Partition Equal Sum</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -4223,12 +4370,13 @@
       <c r="G105" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H105" s="3"/>
       <c r="I105" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>DP: Target Sum (state model)</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -4250,12 +4398,13 @@
       <c r="G106" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H106" s="3"/>
       <c r="I106" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Greedy: Activity Selection (Intervals)</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -4275,12 +4424,13 @@
       <c r="G107" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H107" s="3"/>
       <c r="I107" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Greedy: Interval Merging</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -4300,12 +4450,13 @@
       <c r="G108" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H108" s="3"/>
       <c r="I108" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Greedy: Gas Station Problem</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -4327,12 +4478,13 @@
       <c r="G109" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H109" s="3"/>
       <c r="I109" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Greedy: Job Scheduling / Max Profit</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -4352,12 +4504,13 @@
       <c r="G110" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H110" s="3"/>
       <c r="I110" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Greedy: Resource Assignment</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -4377,12 +4530,13 @@
       <c r="G111" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H111" s="3"/>
       <c r="I111" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Greedy: Jump Game</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -4404,12 +4558,13 @@
       <c r="G112" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="H112" s="3"/>
       <c r="I112" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Review: Strategy + Topic Recap</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -4429,6 +4584,7 @@
       <c r="G113" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="H113" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G22 G28:G1048576">
@@ -4440,119 +4596,120 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://leetcode.com/problems/first-unique-character-in-a-string" xr:uid="{CACA8992-DEBC-4969-B2F6-EBA7FDC085C1}"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://leetcode.com/problems/ransom-note" xr:uid="{9ACCC9FD-0DC8-4254-BB8B-808F3BDD3784}"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://leetcode.com/problems/valid-anagram" xr:uid="{EE4FEEAF-652D-4D2D-A2A9-CB87731F42BE}"/>
-    <hyperlink ref="E5" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters" xr:uid="{4DD7CB8D-B440-4AF4-B6AB-D727391B9158}"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string" xr:uid="{7CCC4C5F-1CA6-46F8-9DD3-9647C7682498}"/>
-    <hyperlink ref="E7" r:id="rId6" display="https://leetcode.com/problems/minimum-window-substring" xr:uid="{61B1900B-EAF8-4BE8-ACAB-A956DE5F3ED1}"/>
-    <hyperlink ref="E8" r:id="rId7" display="https://leetcode.com/problems/container-with-most-water" xr:uid="{84B1B8CA-3A3C-4909-8DD8-F88A45D68628}"/>
-    <hyperlink ref="E9" r:id="rId8" display="https://leetcode.com/problems/3sum" xr:uid="{42633795-6F73-49FF-B778-78E0CD056E83}"/>
-    <hyperlink ref="E10" r:id="rId9" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array" xr:uid="{DFA525B5-0825-451E-B3E0-9DC93194D4E1}"/>
-    <hyperlink ref="E11" r:id="rId10" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{3640DDE9-2ADF-42E2-AEDE-DA2AC3BA211A}"/>
-    <hyperlink ref="E12" r:id="rId11" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k" xr:uid="{8062781F-458E-4926-B311-804BA6CD3BBB}"/>
-    <hyperlink ref="E13" r:id="rId12" display="https://leetcode.com/problems/maximum-subarray" xr:uid="{3AD35EF8-0181-42B2-9B38-F0FC3F95CFE6}"/>
-    <hyperlink ref="E14" r:id="rId13" display="https://leetcode.com/problems/maximum-depth-of-binary-tree" xr:uid="{44C26DDF-9EB7-417D-B269-6C23AC6E6445}"/>
-    <hyperlink ref="E15" r:id="rId14" display="https://leetcode.com/problems/invert-binary-tree" xr:uid="{14199D52-1EAC-49F1-8883-00C4203FC3E3}"/>
-    <hyperlink ref="E16" r:id="rId15" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{52E248D0-3A46-4957-B7A0-F75EBA672C5B}"/>
-    <hyperlink ref="E17" r:id="rId16" display="https://leetcode.com/problems/different-ways-to-add-parentheses" xr:uid="{9DA410A2-6C01-4EDA-9F51-6FBA009D88DF}"/>
-    <hyperlink ref="E18" r:id="rId17" display="https://leetcode.com/problems/unique-binary-search-trees-ii" xr:uid="{68A314C1-D173-4545-AF04-B8E2F74F893D}"/>
-    <hyperlink ref="E19" r:id="rId18" display="https://leetcode.com/problems/powx-n" xr:uid="{26A0C127-23BD-4BCE-8BC7-8AB1A8F90ADE}"/>
-    <hyperlink ref="E20" r:id="rId19" display="https://leetcode.com/problems/subsets" xr:uid="{22D9BCEB-5D0D-4BEF-A700-0FC47638B9F3}"/>
-    <hyperlink ref="E21" r:id="rId20" display="https://leetcode.com/problems/permutations" xr:uid="{E47F3CB1-204D-4424-914C-698242057FAC}"/>
-    <hyperlink ref="E22" r:id="rId21" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{5F57D8FD-824D-4DB1-892E-1DDFD0F8F33D}"/>
-    <hyperlink ref="E28" r:id="rId22" display="https://leetcode.com/problems/binary-search" xr:uid="{374FFDAF-FCB9-431A-86D2-31AB60378C3A}"/>
-    <hyperlink ref="E29" r:id="rId23" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array" xr:uid="{3F271E59-4045-4398-82DB-BC2F4B35A995}"/>
-    <hyperlink ref="E30" r:id="rId24" display="https://leetcode.com/problems/find-peak-element" xr:uid="{DEF2D431-80D6-4E0B-868E-499158EC2963}"/>
-    <hyperlink ref="E31" r:id="rId25" display="https://leetcode.com/problems/koko-eating-bananas" xr:uid="{B3E73AEB-2A95-4916-A93C-BC5B60CAA1D7}"/>
-    <hyperlink ref="E32" r:id="rId26" display="https://leetcode.com/problems/split-array-largest-sum" xr:uid="{BCAC5094-3A8A-4714-BD84-F606403D9DA0}"/>
-    <hyperlink ref="E33" r:id="rId27" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days" xr:uid="{1965E795-8B07-42CA-9865-3EEF521E25E1}"/>
-    <hyperlink ref="E34" r:id="rId28" display="https://leetcode.com/problems/sort-an-array" xr:uid="{E0B9E0A6-F8E5-418F-87DD-47E7F6723CFF}"/>
-    <hyperlink ref="E35" r:id="rId29" display="https://leetcode.com/problems/insertion-sort-list" xr:uid="{03811762-664A-488F-9B2D-036EAE5AAD21}"/>
-    <hyperlink ref="E36" r:id="rId30" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{4F771129-F99D-4F68-954B-762315CE30B8}"/>
-    <hyperlink ref="E37" r:id="rId31" display="https://leetcode.com/problems/largest-number" xr:uid="{373767EF-F0B1-409B-B448-2E15DEE2A726}"/>
-    <hyperlink ref="E38" r:id="rId32" display="https://leetcode.com/problems/reorder-data-in-log-files" xr:uid="{A0B197A5-BF64-4823-8C80-786CEECF12F4}"/>
-    <hyperlink ref="E39" r:id="rId33" display="https://leetcode.com/problems/merge-intervals" xr:uid="{04E9289A-1232-436E-8E31-F058BBB75316}"/>
-    <hyperlink ref="E40" r:id="rId34" display="https://leetcode.com/problems/insert-interval" xr:uid="{355C5E3F-38DD-4154-ACB8-71E37347CA2D}"/>
-    <hyperlink ref="E41" r:id="rId35" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{73B2795D-90B0-4FEF-BAE2-297C16F48CD8}"/>
-    <hyperlink ref="E42" r:id="rId36" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{A4102035-5F89-45CA-99F6-62571131E444}"/>
-    <hyperlink ref="E43" r:id="rId37" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{213E0623-CF2A-4978-9133-4CAD9B8DDC70}"/>
-    <hyperlink ref="E44" r:id="rId38" display="https://leetcode.com/problems/reverse-linked-list-ii" xr:uid="{3E496F01-EEA1-4941-97A8-3FA083834977}"/>
-    <hyperlink ref="E45" r:id="rId39" display="https://leetcode.com/problems/linked-list-cycle" xr:uid="{9C26BB6C-78AB-4618-BD00-77BAAF16815D}"/>
-    <hyperlink ref="E46" r:id="rId40" display="https://leetcode.com/problems/linked-list-cycle-ii" xr:uid="{EC5A3D70-F195-4C10-9EA2-058F32835B9E}"/>
-    <hyperlink ref="E47" r:id="rId41" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{5C4F4E4B-2209-41D3-A906-19E1F708F9DB}"/>
-    <hyperlink ref="E48" r:id="rId42" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{1C1B8A5C-EA41-461E-8FA3-BD6A6B5B3181}"/>
-    <hyperlink ref="E49" r:id="rId43" display="https://leetcode.com/problems/intersection-of-two-linked-lists" xr:uid="{606E5182-D172-41A2-9D50-33C726FC8AB7}"/>
-    <hyperlink ref="E50" r:id="rId44" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{CD69A99D-FBAA-46B5-B0DF-9DE5139BE679}"/>
-    <hyperlink ref="E51" r:id="rId45" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{5D746582-1B54-4352-BDA4-86F05542CE88}"/>
-    <hyperlink ref="E52" r:id="rId46" display="https://leetcode.com/problems/odd-even-linked-list" xr:uid="{C89465FE-7C33-4395-99CB-4BA5D7CED11B}"/>
-    <hyperlink ref="E53" r:id="rId47" display="https://leetcode.com/problems/lru-cache" xr:uid="{05D0EB4C-0E5B-4E3E-AAB2-1A648C9129E7}"/>
-    <hyperlink ref="E54" r:id="rId48" display="https://leetcode.com/problems/lfu-cache" xr:uid="{DF951C59-83C3-4B8E-98CC-B79E487C918E}"/>
-    <hyperlink ref="E55" r:id="rId49" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{91E7DBEA-4D8A-41C9-AAC9-D9BA3BCE6D19}"/>
-    <hyperlink ref="E56" r:id="rId50" display="https://leetcode.com/problems/backspace-string-compare" xr:uid="{BD0B5108-E7EF-4D79-983A-AF8C10DCB73C}"/>
-    <hyperlink ref="E57" r:id="rId51" display="https://leetcode.com/problems/daily-temperatures" xr:uid="{B087D9B6-012A-40BD-B913-355D4FBD2EFE}"/>
-    <hyperlink ref="E58" r:id="rId52" display="https://leetcode.com/problems/next-greater-element-i" xr:uid="{FB709363-8602-45D4-B45B-8C9367125A7E}"/>
-    <hyperlink ref="E59" r:id="rId53" display="https://leetcode.com/problems/largest-rectangle-in-histogram" xr:uid="{704BEAA6-4976-4029-886F-A6FDCC20AE13}"/>
-    <hyperlink ref="E65" r:id="rId54" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k" xr:uid="{C9B7F519-FC85-48AA-93F2-FB21BD51100E}"/>
-    <hyperlink ref="E64" r:id="rId55" display="https://leetcode.com/problems/sliding-window-maximum" xr:uid="{700AEA2A-73EB-45E0-A7C4-C9B375DDFDD1}"/>
-    <hyperlink ref="E63" r:id="rId56" display="https://leetcode.com/problems/design-circular-deque" xr:uid="{C374A6F7-208C-4F78-840A-5324F48EA186}"/>
-    <hyperlink ref="E62" r:id="rId57" display="https://leetcode.com/problems/design-circular-queue" xr:uid="{9290B313-663F-43FF-8027-AB89DA22F6BD}"/>
-    <hyperlink ref="E61" r:id="rId58" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{8802B7B3-B0D3-4F45-83F5-C1CF53DB69A6}"/>
-    <hyperlink ref="E60" r:id="rId59" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{2B0D8F07-EC59-4BAD-93CF-98C511AC3E21}"/>
-    <hyperlink ref="E66" r:id="rId60" display="https://leetcode.com/problems/binary-tree-inorder-traversal" xr:uid="{1B856373-DA81-4D15-ACC2-F7C093A506A8}"/>
-    <hyperlink ref="E67" r:id="rId61" display="https://leetcode.com/problems/binary-tree-level-order-traversal" xr:uid="{6AAEF83E-F9D9-409A-927C-DDEE7AEA57FC}"/>
-    <hyperlink ref="E68" r:id="rId62" display="https://leetcode.com/problems/binary-tree-right-side-view" xr:uid="{5577EFF4-DB1A-480F-83F5-F19EDE79C4B5}"/>
-    <hyperlink ref="E69" r:id="rId63" display="https://leetcode.com/problems/search-in-a-binary-search-tree" xr:uid="{A758D8A5-36A2-40FF-A15F-1A6A7A69801A}"/>
-    <hyperlink ref="E70" r:id="rId64" display="https://leetcode.com/problems/delete-node-in-a-bst" xr:uid="{591B7EA7-3888-49B3-99EF-BA629CD9A02D}"/>
-    <hyperlink ref="E71" r:id="rId65" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{78FB8ABE-DFC4-47EA-ACA0-CFB46543B8DC}"/>
-    <hyperlink ref="E72" r:id="rId66" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree" xr:uid="{5AA82C0A-C3F6-4840-B663-78DC8E56D219}"/>
-    <hyperlink ref="E75" r:id="rId67" display="https://leetcode.com/problems/last-stone-weight" xr:uid="{CAD60500-B89D-4C41-8574-D33E4F0BB32A}"/>
-    <hyperlink ref="E76" r:id="rId68" display="https://leetcode.com/problems/k-closest-points-to-origin" xr:uid="{BBD06487-6DC3-4A9B-83CC-F430BAF527D5}"/>
-    <hyperlink ref="E77" r:id="rId69" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{88E6C8C5-7B90-4A92-BECC-A629C8A55FEC}"/>
-    <hyperlink ref="E78" r:id="rId70" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix" xr:uid="{4C161606-D259-4AC4-BDFF-44E161BFF6BD}"/>
-    <hyperlink ref="E79" r:id="rId71" display="https://leetcode.com/problems/top-k-frequent-words" xr:uid="{4FD04348-E4BE-4F5E-83FD-752D5452B19E}"/>
-    <hyperlink ref="E80" r:id="rId72" display="https://leetcode.com/problems/top-k-frequent-elements" xr:uid="{31ABA819-3C4C-4002-8FCF-364AEF9823BD}"/>
-    <hyperlink ref="E81" r:id="rId73" display="https://leetcode.com/problems/two-sum" xr:uid="{5B404BE5-D0E3-4728-8498-75AFA5031304}"/>
-    <hyperlink ref="E82" r:id="rId74" display="https://leetcode.com/problems/ransom-note" xr:uid="{E50D5A6F-DB16-4D48-974E-C7847334D093}"/>
-    <hyperlink ref="E83" r:id="rId75" display="https://leetcode.com/problems/contains-duplicate" xr:uid="{EEA73F8B-13F1-431E-A0F1-3A0C6B23527D}"/>
-    <hyperlink ref="E84" r:id="rId76" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{4D7D4589-2B8A-47DC-9FCF-904D6E82FB71}"/>
-    <hyperlink ref="E85" r:id="rId77" display="https://leetcode.com/problems/subarray-sums-divisible-by-k" xr:uid="{D838CB32-0488-4C04-951B-6AA80F72BEA1}"/>
-    <hyperlink ref="E86" r:id="rId78" display="https://leetcode.com/problems/group-anagrams" xr:uid="{E64749FE-4AC2-4B2B-91C7-7180E2DCC00B}"/>
-    <hyperlink ref="E87" r:id="rId79" display="https://leetcode.com/problems/longest-consecutive-sequence" xr:uid="{DE30C124-13F2-439B-9476-17D8DAC27129}"/>
-    <hyperlink ref="E88" r:id="rId80" display="https://leetcode.com/problems/number-of-islands" xr:uid="{8DBAE9D8-4931-4C16-AEED-F66841DA88D4}"/>
-    <hyperlink ref="E89" r:id="rId81" display="https://leetcode.com/problems/max-area-of-island" xr:uid="{1B4C9834-1FC5-4895-806E-038B1DBDDA4B}"/>
-    <hyperlink ref="E90" r:id="rId82" display="https://leetcode.com/problems/01-matrix" xr:uid="{A0E46D51-24FB-432C-9B64-F9A7D564ADF2}"/>
-    <hyperlink ref="E91" r:id="rId83" display="https://leetcode.com/problems/network-delay-time" xr:uid="{F759E8D2-9590-49C8-B0C1-9FDC2453A281}"/>
-    <hyperlink ref="E92" r:id="rId84" display="https://leetcode.com/problems/redundant-connection" xr:uid="{EB3F5CE4-E5E9-420F-8C29-1A45626B6B12}"/>
-    <hyperlink ref="E93" r:id="rId85" display="https://leetcode.com/problems/number-of-provinces" xr:uid="{7F9CCD13-89BD-4996-B7B2-71D1985A3440}"/>
-    <hyperlink ref="E94" r:id="rId86" display="https://leetcode.com/problems/course-schedule" xr:uid="{1BB86DA6-53E2-4F87-8150-7BF6C57A100C}"/>
-    <hyperlink ref="E95" r:id="rId87" display="https://leetcode.com/problems/course-schedule-ii" xr:uid="{5177CC97-2B77-43CF-B33F-3903154A502D}"/>
-    <hyperlink ref="E96" r:id="rId88" display="https://leetcode.com/problems/clone-graph" xr:uid="{16DC6C12-1E3C-4E22-B3FF-A38677E0B8F3}"/>
-    <hyperlink ref="E97" r:id="rId89" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{8E820236-2EA3-409B-AA9C-D43A03343FCB}"/>
-    <hyperlink ref="E98" r:id="rId90" display="https://leetcode.com/problems/climbing-stairs" xr:uid="{40181C74-4968-41A8-B229-0DF250C3A787}"/>
-    <hyperlink ref="E99" r:id="rId91" display="https://leetcode.com/problems/min-cost-climbing-stairs" xr:uid="{9E7BFCA6-DA59-48A0-975B-9589BDC7C276}"/>
-    <hyperlink ref="E100" r:id="rId92" display="https://leetcode.com/problems/longest-common-subsequence" xr:uid="{30F8CF6D-7369-4957-A7D7-160A741AA38C}"/>
-    <hyperlink ref="E101" r:id="rId93" display="https://leetcode.com/problems/longest-increasing-subsequence" xr:uid="{0B0509FA-0F85-46F0-803E-3112FAE33195}"/>
-    <hyperlink ref="E102" r:id="rId94" display="https://leetcode.com/problems/palindromic-substrings" xr:uid="{DAA8A2AD-4DEC-4740-BE2E-FF2A710FC881}"/>
-    <hyperlink ref="E103" r:id="rId95" display="https://leetcode.com/problems/unique-paths" xr:uid="{3BFACFF5-9CEA-445E-837D-80CE02DD15B6}"/>
-    <hyperlink ref="E104" r:id="rId96" display="https://leetcode.com/problems/partition-equal-subset-sum" xr:uid="{7588C036-6A20-4C85-94EE-72396427AA61}"/>
-    <hyperlink ref="E105" r:id="rId97" display="https://leetcode.com/problems/target-sum" xr:uid="{B8B2404F-6A1D-4008-9903-335EA651A7DC}"/>
-    <hyperlink ref="E106" r:id="rId98" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{6B9267CD-AC96-447A-879D-41081B74ECAC}"/>
-    <hyperlink ref="E107" r:id="rId99" display="https://leetcode.com/problems/merge-intervals" xr:uid="{C1AA793D-64CD-400D-A0A9-D182B005CEDC}"/>
-    <hyperlink ref="E108" r:id="rId100" display="https://leetcode.com/problems/gas-station" xr:uid="{9A4CC2B1-7301-4996-8463-5549D190A892}"/>
-    <hyperlink ref="E109" r:id="rId101" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{9AF79B77-6ADE-45DC-A721-A6C56EA49A98}"/>
-    <hyperlink ref="E110" r:id="rId102" display="https://leetcode.com/problems/can-place-flowers" xr:uid="{9BBCC8E1-2E28-48FF-9415-D9250E2D1CFB}"/>
-    <hyperlink ref="E111" r:id="rId103" display="https://leetcode.com/problems/jump-game" xr:uid="{22D973B8-6E8A-41F7-BF66-D13FE9CE93A0}"/>
-    <hyperlink ref="E23" r:id="rId104" display="https://leetcode.com/problems/n-queens" xr:uid="{69BB437F-E482-4232-B7A6-D86FFB9B9B11}"/>
-    <hyperlink ref="E24" r:id="rId105" display="https://leetcode.com/problems/n-queens-ii" xr:uid="{E91B232D-5ED5-407F-BC79-BA4E584B16DD}"/>
-    <hyperlink ref="E25" r:id="rId106" display="https://leetcode.com/problems/subsets-ii" xr:uid="{E82CECCF-46F9-40BE-919A-4DF7D362F5FD}"/>
-    <hyperlink ref="E26" r:id="rId107" display="https://leetcode.com/problems/permutations-ii" xr:uid="{BB9406D1-F97D-422E-81C5-BED20DBD5DE4}"/>
-    <hyperlink ref="E27" r:id="rId108" display="https://leetcode.com/problems/combination-sum" xr:uid="{523178B6-AF5B-4927-8BC6-3484B292F8FF}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://leetcode.com/problems/first-unique-character-in-a-string"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://leetcode.com/problems/ransom-note"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://leetcode.com/problems/valid-anagram"/>
+    <hyperlink ref="E7" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string"/>
+    <hyperlink ref="E8" r:id="rId6" display="https://leetcode.com/problems/container-with-most-water"/>
+    <hyperlink ref="E9" r:id="rId7" display="https://leetcode.com/problems/3sum"/>
+    <hyperlink ref="E10" r:id="rId8" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array"/>
+    <hyperlink ref="E11" r:id="rId9" display="https://leetcode.com/problems/subarray-sum-equals-k"/>
+    <hyperlink ref="E12" r:id="rId10" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k"/>
+    <hyperlink ref="E13" r:id="rId11" display="https://leetcode.com/problems/maximum-subarray"/>
+    <hyperlink ref="E14" r:id="rId12" display="https://leetcode.com/problems/maximum-depth-of-binary-tree"/>
+    <hyperlink ref="E15" r:id="rId13" display="https://leetcode.com/problems/invert-binary-tree"/>
+    <hyperlink ref="E16" r:id="rId14" display="https://leetcode.com/problems/fibonacci-number"/>
+    <hyperlink ref="E17" r:id="rId15" display="https://leetcode.com/problems/different-ways-to-add-parentheses"/>
+    <hyperlink ref="E18" r:id="rId16" display="https://leetcode.com/problems/unique-binary-search-trees-ii"/>
+    <hyperlink ref="E19" r:id="rId17" display="https://leetcode.com/problems/powx-n"/>
+    <hyperlink ref="E20" r:id="rId18" display="https://leetcode.com/problems/subsets"/>
+    <hyperlink ref="E21" r:id="rId19" display="https://leetcode.com/problems/permutations"/>
+    <hyperlink ref="E22" r:id="rId20" display="https://leetcode.com/problems/generate-parentheses"/>
+    <hyperlink ref="E28" r:id="rId21" display="https://leetcode.com/problems/binary-search"/>
+    <hyperlink ref="E29" r:id="rId22" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array"/>
+    <hyperlink ref="E30" r:id="rId23" display="https://leetcode.com/problems/find-peak-element"/>
+    <hyperlink ref="E31" r:id="rId24" display="https://leetcode.com/problems/koko-eating-bananas"/>
+    <hyperlink ref="E32" r:id="rId25" display="https://leetcode.com/problems/split-array-largest-sum"/>
+    <hyperlink ref="E33" r:id="rId26" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days"/>
+    <hyperlink ref="E34" r:id="rId27" display="https://leetcode.com/problems/sort-an-array"/>
+    <hyperlink ref="E35" r:id="rId28" display="https://leetcode.com/problems/insertion-sort-list"/>
+    <hyperlink ref="E36" r:id="rId29" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
+    <hyperlink ref="E37" r:id="rId30" display="https://leetcode.com/problems/largest-number"/>
+    <hyperlink ref="E38" r:id="rId31" display="https://leetcode.com/problems/reorder-data-in-log-files"/>
+    <hyperlink ref="E39" r:id="rId32" display="https://leetcode.com/problems/merge-intervals"/>
+    <hyperlink ref="E40" r:id="rId33" display="https://leetcode.com/problems/insert-interval"/>
+    <hyperlink ref="E41" r:id="rId34" display="https://leetcode.com/problems/non-overlapping-intervals"/>
+    <hyperlink ref="E42" r:id="rId35" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
+    <hyperlink ref="E43" r:id="rId36" display="https://leetcode.com/problems/reverse-linked-list"/>
+    <hyperlink ref="E44" r:id="rId37" display="https://leetcode.com/problems/reverse-linked-list-ii"/>
+    <hyperlink ref="E45" r:id="rId38" display="https://leetcode.com/problems/linked-list-cycle"/>
+    <hyperlink ref="E46" r:id="rId39" display="https://leetcode.com/problems/linked-list-cycle-ii"/>
+    <hyperlink ref="E47" r:id="rId40" display="https://leetcode.com/problems/merge-two-sorted-lists"/>
+    <hyperlink ref="E48" r:id="rId41" display="https://leetcode.com/problems/merge-k-sorted-lists"/>
+    <hyperlink ref="E49" r:id="rId42" display="https://leetcode.com/problems/intersection-of-two-linked-lists"/>
+    <hyperlink ref="E50" r:id="rId43" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list"/>
+    <hyperlink ref="E51" r:id="rId44" display="https://leetcode.com/problems/palindrome-linked-list"/>
+    <hyperlink ref="E52" r:id="rId45" display="https://leetcode.com/problems/odd-even-linked-list"/>
+    <hyperlink ref="E53" r:id="rId46" display="https://leetcode.com/problems/lru-cache"/>
+    <hyperlink ref="E54" r:id="rId47" display="https://leetcode.com/problems/lfu-cache"/>
+    <hyperlink ref="E55" r:id="rId48" display="https://leetcode.com/problems/valid-parentheses"/>
+    <hyperlink ref="E56" r:id="rId49" display="https://leetcode.com/problems/backspace-string-compare"/>
+    <hyperlink ref="E57" r:id="rId50" display="https://leetcode.com/problems/daily-temperatures"/>
+    <hyperlink ref="E58" r:id="rId51" display="https://leetcode.com/problems/next-greater-element-i"/>
+    <hyperlink ref="E59" r:id="rId52" display="https://leetcode.com/problems/largest-rectangle-in-histogram"/>
+    <hyperlink ref="E65" r:id="rId53" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k"/>
+    <hyperlink ref="E64" r:id="rId54" display="https://leetcode.com/problems/sliding-window-maximum"/>
+    <hyperlink ref="E63" r:id="rId55" display="https://leetcode.com/problems/design-circular-deque"/>
+    <hyperlink ref="E62" r:id="rId56" display="https://leetcode.com/problems/design-circular-queue"/>
+    <hyperlink ref="E61" r:id="rId57" display="https://leetcode.com/problems/implement-queue-using-stacks"/>
+    <hyperlink ref="E60" r:id="rId58" display="https://leetcode.com/problems/number-of-recent-calls"/>
+    <hyperlink ref="E66" r:id="rId59" display="https://leetcode.com/problems/binary-tree-inorder-traversal"/>
+    <hyperlink ref="E67" r:id="rId60" display="https://leetcode.com/problems/binary-tree-level-order-traversal"/>
+    <hyperlink ref="E68" r:id="rId61" display="https://leetcode.com/problems/binary-tree-right-side-view"/>
+    <hyperlink ref="E69" r:id="rId62" display="https://leetcode.com/problems/search-in-a-binary-search-tree"/>
+    <hyperlink ref="E70" r:id="rId63" display="https://leetcode.com/problems/delete-node-in-a-bst"/>
+    <hyperlink ref="E71" r:id="rId64" display="https://leetcode.com/problems/validate-binary-search-tree"/>
+    <hyperlink ref="E72" r:id="rId65" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree"/>
+    <hyperlink ref="E75" r:id="rId66" display="https://leetcode.com/problems/last-stone-weight"/>
+    <hyperlink ref="E76" r:id="rId67" display="https://leetcode.com/problems/k-closest-points-to-origin"/>
+    <hyperlink ref="E77" r:id="rId68" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
+    <hyperlink ref="E78" r:id="rId69" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix"/>
+    <hyperlink ref="E79" r:id="rId70" display="https://leetcode.com/problems/top-k-frequent-words"/>
+    <hyperlink ref="E80" r:id="rId71" display="https://leetcode.com/problems/top-k-frequent-elements"/>
+    <hyperlink ref="E81" r:id="rId72" display="https://leetcode.com/problems/two-sum"/>
+    <hyperlink ref="E82" r:id="rId73" display="https://leetcode.com/problems/ransom-note"/>
+    <hyperlink ref="E83" r:id="rId74" display="https://leetcode.com/problems/contains-duplicate"/>
+    <hyperlink ref="E84" r:id="rId75" display="https://leetcode.com/problems/subarray-sum-equals-k"/>
+    <hyperlink ref="E85" r:id="rId76" display="https://leetcode.com/problems/subarray-sums-divisible-by-k"/>
+    <hyperlink ref="E86" r:id="rId77" display="https://leetcode.com/problems/group-anagrams"/>
+    <hyperlink ref="E87" r:id="rId78" display="https://leetcode.com/problems/longest-consecutive-sequence"/>
+    <hyperlink ref="E88" r:id="rId79" display="https://leetcode.com/problems/number-of-islands"/>
+    <hyperlink ref="E89" r:id="rId80" display="https://leetcode.com/problems/max-area-of-island"/>
+    <hyperlink ref="E90" r:id="rId81" display="https://leetcode.com/problems/01-matrix"/>
+    <hyperlink ref="E91" r:id="rId82" display="https://leetcode.com/problems/network-delay-time"/>
+    <hyperlink ref="E92" r:id="rId83" display="https://leetcode.com/problems/redundant-connection"/>
+    <hyperlink ref="E93" r:id="rId84" display="https://leetcode.com/problems/number-of-provinces"/>
+    <hyperlink ref="E94" r:id="rId85" display="https://leetcode.com/problems/course-schedule"/>
+    <hyperlink ref="E95" r:id="rId86" display="https://leetcode.com/problems/course-schedule-ii"/>
+    <hyperlink ref="E96" r:id="rId87" display="https://leetcode.com/problems/clone-graph"/>
+    <hyperlink ref="E97" r:id="rId88" display="https://leetcode.com/problems/fibonacci-number"/>
+    <hyperlink ref="E98" r:id="rId89" display="https://leetcode.com/problems/climbing-stairs"/>
+    <hyperlink ref="E99" r:id="rId90" display="https://leetcode.com/problems/min-cost-climbing-stairs"/>
+    <hyperlink ref="E100" r:id="rId91" display="https://leetcode.com/problems/longest-common-subsequence"/>
+    <hyperlink ref="E101" r:id="rId92" display="https://leetcode.com/problems/longest-increasing-subsequence"/>
+    <hyperlink ref="E102" r:id="rId93" display="https://leetcode.com/problems/palindromic-substrings"/>
+    <hyperlink ref="E103" r:id="rId94" display="https://leetcode.com/problems/unique-paths"/>
+    <hyperlink ref="E104" r:id="rId95" display="https://leetcode.com/problems/partition-equal-subset-sum"/>
+    <hyperlink ref="E105" r:id="rId96" display="https://leetcode.com/problems/target-sum"/>
+    <hyperlink ref="E106" r:id="rId97" display="https://leetcode.com/problems/non-overlapping-intervals"/>
+    <hyperlink ref="E107" r:id="rId98" display="https://leetcode.com/problems/merge-intervals"/>
+    <hyperlink ref="E108" r:id="rId99" display="https://leetcode.com/problems/gas-station"/>
+    <hyperlink ref="E109" r:id="rId100" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
+    <hyperlink ref="E110" r:id="rId101" display="https://leetcode.com/problems/can-place-flowers"/>
+    <hyperlink ref="E111" r:id="rId102" display="https://leetcode.com/problems/jump-game"/>
+    <hyperlink ref="E23" r:id="rId103" display="https://leetcode.com/problems/n-queens"/>
+    <hyperlink ref="E24" r:id="rId104" display="https://leetcode.com/problems/n-queens-ii"/>
+    <hyperlink ref="E25" r:id="rId105" display="https://leetcode.com/problems/subsets-ii"/>
+    <hyperlink ref="E26" r:id="rId106" display="https://leetcode.com/problems/permutations-ii"/>
+    <hyperlink ref="E27" r:id="rId107" display="https://leetcode.com/problems/combination-sum"/>
+    <hyperlink ref="H2" r:id="rId108" display="https://leetcode.com/problems/count-and-say/"/>
+    <hyperlink ref="E5" r:id="rId109" display="https://leetcode.com/problems/minimum-window-substring"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId109"/>
+  <pageSetup orientation="portrait" r:id="rId110"/>
   <tableParts count="1">
-    <tablePart r:id="rId110"/>
+    <tablePart r:id="rId111"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore(lesson plan): no modification
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -905,26 +905,6 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -970,6 +950,26 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1010,20 +1010,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H113"/>
   <sortState ref="A2:G113">
     <sortCondition ref="A1:A113"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="S.No" dataDxfId="9"/>
-    <tableColumn id="2" name="Topic" dataDxfId="8"/>
-    <tableColumn id="3" name="Subtopic" dataDxfId="7"/>
-    <tableColumn id="4" name="Hour" dataDxfId="6"/>
-    <tableColumn id="5" name="LeetCode Problem" dataDxfId="5"/>
-    <tableColumn id="6" name="Level" dataDxfId="4"/>
-    <tableColumn id="7" name="Remark" dataDxfId="3"/>
-    <tableColumn id="8" name="Notes" dataDxfId="2"/>
+    <tableColumn id="1" name="S.No" dataDxfId="7"/>
+    <tableColumn id="2" name="Topic" dataDxfId="6"/>
+    <tableColumn id="3" name="Subtopic" dataDxfId="5"/>
+    <tableColumn id="4" name="Hour" dataDxfId="4"/>
+    <tableColumn id="5" name="LeetCode Problem" dataDxfId="3"/>
+    <tableColumn id="6" name="Level" dataDxfId="2"/>
+    <tableColumn id="7" name="Remark" dataDxfId="1"/>
+    <tableColumn id="8" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1544,7 +1544,7 @@
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4588,10 +4588,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G22 G28:G1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
chore(lesson-plan): updated 25.06.2025 session from array two-pointer to string doubt clarification
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="257">
   <si>
     <t>Order</t>
   </si>
@@ -793,6 +793,9 @@
   </si>
   <si>
     <t>38. Count and Say</t>
+  </si>
+  <si>
+    <t>String Doubt Clarification Session</t>
   </si>
 </sst>
 </file>
@@ -894,7 +897,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1544,7 +1547,7 @@
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1681,7 +1684,7 @@
       <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -1707,7 +1710,7 @@
         <v>37</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="8" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1733,7 +1736,7 @@
         <v>37</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>38</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1770,7 +1773,9 @@
       <c r="G8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="8" t="s">
+        <v>256</v>
+      </c>
       <c r="I8" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Array: Two Pointer</v>

</xml_diff>

<commit_message>
chore(lesson-plan): updated structure chore(leetcode): standardized solution document format
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -795,7 +795,14 @@
     <t>38. Count and Say</t>
   </si>
   <si>
-    <t>String Doubt Clarification Session</t>
+    <t xml:space="preserve">String Doubt Clarification Session.
+DataStructure Study Plan
+1. Creation
+2. Access
+3. Insert
+4. Delete
+5. Update
+</t>
   </si>
 </sst>
 </file>
@@ -1547,7 +1554,7 @@
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1751,7 +1758,7 @@
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1764,7 +1771,7 @@
       <c r="D8" s="1">
         <v>3</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="3" t="s">

</xml_diff>

<commit_message>
chore(lesson-plan): highlighted problem completion status up to 27 June 2025 feat(leetcode): added solutions for problems 15, 26, and 560
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2_TIME_College\SRET\sret-focus-batch-23-27\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schedule\Documents\TIME_DK\time_colleges\SRET\Focus_Batch_2023-2027\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFE2A8E-924A-49C3-9C45-C67355B12596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11040" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hours Alloted" sheetId="1" r:id="rId1"/>
     <sheet name="Lesson Plan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -808,7 +809,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -915,6 +916,26 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -960,26 +981,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1008,32 +1009,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:C20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:C20" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Order" dataDxfId="14"/>
-    <tableColumn id="2" name="Topic" dataDxfId="13"/>
-    <tableColumn id="3" name="Hours" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Topic" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hours" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H113"/>
-  <sortState ref="A2:G113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:H113" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G113">
     <sortCondition ref="A1:A113"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="S.No" dataDxfId="7"/>
-    <tableColumn id="2" name="Topic" dataDxfId="6"/>
-    <tableColumn id="3" name="Subtopic" dataDxfId="5"/>
-    <tableColumn id="4" name="Hour" dataDxfId="4"/>
-    <tableColumn id="5" name="LeetCode Problem" dataDxfId="3"/>
-    <tableColumn id="6" name="Level" dataDxfId="2"/>
-    <tableColumn id="7" name="Remark" dataDxfId="1"/>
-    <tableColumn id="8" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="S.No" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Topic" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Subtopic" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Hour" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="LeetCode Problem" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Level" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Remark" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1301,21 +1302,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="6"/>
-    <col min="2" max="2" width="60.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="6"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1326,7 +1327,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1337,7 +1338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1348,7 +1349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1359,7 +1360,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1370,7 +1371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1392,7 +1393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1403,7 +1404,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1414,7 +1415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1425,7 +1426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1436,7 +1437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1447,7 +1448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1458,7 +1459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1469,7 +1470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1480,7 +1481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1491,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1513,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1524,7 +1525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="6">
         <f>SUM(C2:C21)</f>
         <v>45</v>
@@ -1550,27 +1551,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.77734375" customWidth="1"/>
-    <col min="9" max="9" width="36.33203125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.7109375" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1626,7 +1627,7 @@
         <v>String: Hashing + Count</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1652,7 +1653,7 @@
         <v>String: Frequency Matching</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1678,7 +1679,7 @@
         <v>String: Frequency Matching</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1706,7 +1707,7 @@
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1732,7 +1733,7 @@
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1758,7 +1759,7 @@
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1788,7 +1789,7 @@
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>44</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>46</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1814,7 +1815,7 @@
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1825,7 +1826,7 @@
         <v>44</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>47</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -1840,7 +1841,7 @@
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1853,7 +1854,7 @@
       <c r="D11" s="1">
         <v>4</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="8" t="s">
         <v>49</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -1868,7 +1869,7 @@
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1894,7 +1895,7 @@
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1920,7 +1921,7 @@
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1948,7 +1949,7 @@
         <v>Recursion: Base Case + Tree View</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1974,7 +1975,7 @@
         <v>Recursion: Base Case Practice</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2000,7 +2001,7 @@
         <v>Recursion: Fibonacci</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2028,7 +2029,7 @@
         <v>Recursion: Divide and Conquer</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2054,7 +2055,7 @@
         <v>Recursion: Divide and Conquer</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2080,7 +2081,7 @@
         <v>Recursion: Binary Recursion Tree</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2108,7 +2109,7 @@
         <v>Recursion: Subsets</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2134,7 +2135,7 @@
         <v>Recursion: Rec. with State</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>Recursion: Backtrack Base</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2188,7 +2189,7 @@
         <v>Backtracking: N-Queens</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2214,7 +2215,7 @@
         <v>Backtracking: N-Queens</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2242,7 +2243,7 @@
         <v>Backtracking: Subset Gen</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2268,7 +2269,7 @@
         <v>Backtracking: Permutations</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2294,7 +2295,7 @@
         <v>Backtracking: Combination Sum</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2322,7 +2323,7 @@
         <v>Searching: Binary Search Basic</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2348,7 +2349,7 @@
         <v>Searching: First/Last Occurrence</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2374,7 +2375,7 @@
         <v>Searching: Peak Element</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2402,7 +2403,7 @@
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2428,7 +2429,7 @@
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2482,7 +2483,7 @@
         <v>Sorting: Basic Sorting Logic</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2508,7 +2509,7 @@
         <v>Sorting: Selection Practice</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2534,7 +2535,7 @@
         <v>Sorting: QuickSort</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2562,7 +2563,7 @@
         <v>Sorting: Custom Comparator</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2588,7 +2589,7 @@
         <v>Sorting: Custom Comparator</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>Sorting: Merge Intervals</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2642,7 +2643,7 @@
         <v>Sorting: Merge Intervals</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2670,7 +2671,7 @@
         <v>Sorting: Scheduling Logic</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2696,7 +2697,7 @@
         <v>Sorting: Sorting Based Greedy</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2724,7 +2725,7 @@
         <v>Linked List: Reverse LL</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2750,7 +2751,7 @@
         <v>Linked List: Reverse LL II</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2778,7 +2779,7 @@
         <v>Linked List: Detect Cycle</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2804,7 +2805,7 @@
         <v>Linked List: Cycle II</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2832,7 +2833,7 @@
         <v>Linked List: Merge LL</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2858,7 +2859,7 @@
         <v>Linked List: Merge k Lists</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2886,7 +2887,7 @@
         <v>Linked List: Intersection Point</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2912,7 +2913,7 @@
         <v>Linked List: Remove Nth Node</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2940,7 +2941,7 @@
         <v>Linked List: Palindrome Check</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2966,7 +2967,7 @@
         <v>Linked List: Odd Even Index</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2994,7 +2995,7 @@
         <v>Linked List: LRU Cache Logic</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3020,7 +3021,7 @@
         <v>Linked List: Advanced LRU Logic</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3048,7 +3049,7 @@
         <v>Stack: Stack Basics</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3074,7 +3075,7 @@
         <v>Stack: Stack Basics</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3102,7 +3103,7 @@
         <v>Stack: Monotonic Stack</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3128,7 +3129,7 @@
         <v>Stack: Next Greater Element</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3154,7 +3155,7 @@
         <v>Stack: Largest Rect in Hist</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3182,7 +3183,7 @@
         <v>Queue: Queue + BFS Intro</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3208,7 +3209,7 @@
         <v>Queue: Implement Queue Using Stacks</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3236,7 +3237,7 @@
         <v>Queue: Circular Queue</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3262,7 +3263,7 @@
         <v>Queue: Deque</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3290,7 +3291,7 @@
         <v>Queue: Monotonic Queue</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3316,7 +3317,7 @@
         <v>Queue: Monotonic Queue</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3344,7 +3345,7 @@
         <v>Trees: Traversals</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3370,7 +3371,7 @@
         <v>Trees: Traversals</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3396,7 +3397,7 @@
         <v>Trees: Views + Height</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3424,7 +3425,7 @@
         <v>BST: Search, Insert, Min</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3450,7 +3451,7 @@
         <v>BST: Deletion</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3478,7 +3479,7 @@
         <v>BST: Validate BST</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3504,7 +3505,7 @@
         <v>BST: Lowest Common Ancestor</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3532,7 +3533,7 @@
         <v>Balanced Tree: AVL Tree</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3558,7 +3559,7 @@
         <v>Balanced Tree: Red-Black Tree</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3586,7 +3587,7 @@
         <v>Heap: Min Heap Introduction</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3612,7 +3613,7 @@
         <v>Heap: Priority Queue Usage</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3640,7 +3641,7 @@
         <v>Heap: Kth Largest Element</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3666,7 +3667,7 @@
         <v>Heap: Kth Smallest Element</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3694,7 +3695,7 @@
         <v>Heap: Heap + Sorting Logic</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3720,7 +3721,7 @@
         <v>Heap: Heap + Custom Comparator</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3748,7 +3749,7 @@
         <v>HashMap: Frequency Counting</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3774,7 +3775,7 @@
         <v>HashMap: Frequency Counting</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3800,7 +3801,7 @@
         <v>HashSet: Uniqueness Check</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3828,7 +3829,7 @@
         <v>HashMap: Prefix Sum Technique</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3854,7 +3855,7 @@
         <v>HashMap: Prefix Sum Variation</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -3882,7 +3883,7 @@
         <v>HashMap: Grouping Data</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -3908,7 +3909,7 @@
         <v>HashMap: Longest Streak/Length</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -3936,7 +3937,7 @@
         <v>Graph: BFS Traversal</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -3962,7 +3963,7 @@
         <v>Graph: DFS Traversal</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -3988,7 +3989,7 @@
         <v>Graph: BFS with Distance</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -4016,7 +4017,7 @@
         <v>Graph: Dijkstra’s (Shortest Path)</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -4042,7 +4043,7 @@
         <v>Graph: Union Find</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -4068,7 +4069,7 @@
         <v>Graph: Cycle Detection</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -4096,7 +4097,7 @@
         <v>Graph: Topological Sort</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -4122,7 +4123,7 @@
         <v>Graph: Topo + Ordering</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -4148,7 +4149,7 @@
         <v>Graph: Kahn’s Algorithm</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4176,7 +4177,7 @@
         <v>DP: Fibonacci with Memo</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4202,7 +4203,7 @@
         <v>DP: Climbing Stairs (1D)</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4228,7 +4229,7 @@
         <v>DP: Min Cost Climbing</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4256,7 +4257,7 @@
         <v>DP: Longest Common Subseq</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4282,7 +4283,7 @@
         <v>DP: Longest Increasing Subseq</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4308,7 +4309,7 @@
         <v>DP: Palindromic Substrings</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -4336,7 +4337,7 @@
         <v>DP: Unique Paths (2D Grid)</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -4362,7 +4363,7 @@
         <v>DP: Partition Equal Sum</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -4388,7 +4389,7 @@
         <v>DP: Target Sum (state model)</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -4416,7 +4417,7 @@
         <v>Greedy: Activity Selection (Intervals)</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -4442,7 +4443,7 @@
         <v>Greedy: Interval Merging</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -4468,7 +4469,7 @@
         <v>Greedy: Gas Station Problem</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -4496,7 +4497,7 @@
         <v>Greedy: Job Scheduling / Max Profit</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -4522,7 +4523,7 @@
         <v>Greedy: Resource Assignment</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -4548,7 +4549,7 @@
         <v>Greedy: Jump Game</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -4576,7 +4577,7 @@
         <v>Review: Strategy + Topic Recap</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -4600,123 +4601,123 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G22 G28:G1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://leetcode.com/problems/first-unique-character-in-a-string"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://leetcode.com/problems/ransom-note"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://leetcode.com/problems/valid-anagram"/>
-    <hyperlink ref="E7" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string"/>
-    <hyperlink ref="E8" r:id="rId6" display="https://leetcode.com/problems/container-with-most-water"/>
-    <hyperlink ref="E9" r:id="rId7" display="https://leetcode.com/problems/3sum"/>
-    <hyperlink ref="E10" r:id="rId8" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array"/>
-    <hyperlink ref="E11" r:id="rId9" display="https://leetcode.com/problems/subarray-sum-equals-k"/>
-    <hyperlink ref="E12" r:id="rId10" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k"/>
-    <hyperlink ref="E13" r:id="rId11" display="https://leetcode.com/problems/maximum-subarray"/>
-    <hyperlink ref="E14" r:id="rId12" display="https://leetcode.com/problems/maximum-depth-of-binary-tree"/>
-    <hyperlink ref="E15" r:id="rId13" display="https://leetcode.com/problems/invert-binary-tree"/>
-    <hyperlink ref="E16" r:id="rId14" display="https://leetcode.com/problems/fibonacci-number"/>
-    <hyperlink ref="E17" r:id="rId15" display="https://leetcode.com/problems/different-ways-to-add-parentheses"/>
-    <hyperlink ref="E18" r:id="rId16" display="https://leetcode.com/problems/unique-binary-search-trees-ii"/>
-    <hyperlink ref="E19" r:id="rId17" display="https://leetcode.com/problems/powx-n"/>
-    <hyperlink ref="E20" r:id="rId18" display="https://leetcode.com/problems/subsets"/>
-    <hyperlink ref="E21" r:id="rId19" display="https://leetcode.com/problems/permutations"/>
-    <hyperlink ref="E22" r:id="rId20" display="https://leetcode.com/problems/generate-parentheses"/>
-    <hyperlink ref="E28" r:id="rId21" display="https://leetcode.com/problems/binary-search"/>
-    <hyperlink ref="E29" r:id="rId22" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array"/>
-    <hyperlink ref="E30" r:id="rId23" display="https://leetcode.com/problems/find-peak-element"/>
-    <hyperlink ref="E31" r:id="rId24" display="https://leetcode.com/problems/koko-eating-bananas"/>
-    <hyperlink ref="E32" r:id="rId25" display="https://leetcode.com/problems/split-array-largest-sum"/>
-    <hyperlink ref="E33" r:id="rId26" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days"/>
-    <hyperlink ref="E34" r:id="rId27" display="https://leetcode.com/problems/sort-an-array"/>
-    <hyperlink ref="E35" r:id="rId28" display="https://leetcode.com/problems/insertion-sort-list"/>
-    <hyperlink ref="E36" r:id="rId29" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
-    <hyperlink ref="E37" r:id="rId30" display="https://leetcode.com/problems/largest-number"/>
-    <hyperlink ref="E38" r:id="rId31" display="https://leetcode.com/problems/reorder-data-in-log-files"/>
-    <hyperlink ref="E39" r:id="rId32" display="https://leetcode.com/problems/merge-intervals"/>
-    <hyperlink ref="E40" r:id="rId33" display="https://leetcode.com/problems/insert-interval"/>
-    <hyperlink ref="E41" r:id="rId34" display="https://leetcode.com/problems/non-overlapping-intervals"/>
-    <hyperlink ref="E42" r:id="rId35" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
-    <hyperlink ref="E43" r:id="rId36" display="https://leetcode.com/problems/reverse-linked-list"/>
-    <hyperlink ref="E44" r:id="rId37" display="https://leetcode.com/problems/reverse-linked-list-ii"/>
-    <hyperlink ref="E45" r:id="rId38" display="https://leetcode.com/problems/linked-list-cycle"/>
-    <hyperlink ref="E46" r:id="rId39" display="https://leetcode.com/problems/linked-list-cycle-ii"/>
-    <hyperlink ref="E47" r:id="rId40" display="https://leetcode.com/problems/merge-two-sorted-lists"/>
-    <hyperlink ref="E48" r:id="rId41" display="https://leetcode.com/problems/merge-k-sorted-lists"/>
-    <hyperlink ref="E49" r:id="rId42" display="https://leetcode.com/problems/intersection-of-two-linked-lists"/>
-    <hyperlink ref="E50" r:id="rId43" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list"/>
-    <hyperlink ref="E51" r:id="rId44" display="https://leetcode.com/problems/palindrome-linked-list"/>
-    <hyperlink ref="E52" r:id="rId45" display="https://leetcode.com/problems/odd-even-linked-list"/>
-    <hyperlink ref="E53" r:id="rId46" display="https://leetcode.com/problems/lru-cache"/>
-    <hyperlink ref="E54" r:id="rId47" display="https://leetcode.com/problems/lfu-cache"/>
-    <hyperlink ref="E55" r:id="rId48" display="https://leetcode.com/problems/valid-parentheses"/>
-    <hyperlink ref="E56" r:id="rId49" display="https://leetcode.com/problems/backspace-string-compare"/>
-    <hyperlink ref="E57" r:id="rId50" display="https://leetcode.com/problems/daily-temperatures"/>
-    <hyperlink ref="E58" r:id="rId51" display="https://leetcode.com/problems/next-greater-element-i"/>
-    <hyperlink ref="E59" r:id="rId52" display="https://leetcode.com/problems/largest-rectangle-in-histogram"/>
-    <hyperlink ref="E65" r:id="rId53" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k"/>
-    <hyperlink ref="E64" r:id="rId54" display="https://leetcode.com/problems/sliding-window-maximum"/>
-    <hyperlink ref="E63" r:id="rId55" display="https://leetcode.com/problems/design-circular-deque"/>
-    <hyperlink ref="E62" r:id="rId56" display="https://leetcode.com/problems/design-circular-queue"/>
-    <hyperlink ref="E61" r:id="rId57" display="https://leetcode.com/problems/implement-queue-using-stacks"/>
-    <hyperlink ref="E60" r:id="rId58" display="https://leetcode.com/problems/number-of-recent-calls"/>
-    <hyperlink ref="E66" r:id="rId59" display="https://leetcode.com/problems/binary-tree-inorder-traversal"/>
-    <hyperlink ref="E67" r:id="rId60" display="https://leetcode.com/problems/binary-tree-level-order-traversal"/>
-    <hyperlink ref="E68" r:id="rId61" display="https://leetcode.com/problems/binary-tree-right-side-view"/>
-    <hyperlink ref="E69" r:id="rId62" display="https://leetcode.com/problems/search-in-a-binary-search-tree"/>
-    <hyperlink ref="E70" r:id="rId63" display="https://leetcode.com/problems/delete-node-in-a-bst"/>
-    <hyperlink ref="E71" r:id="rId64" display="https://leetcode.com/problems/validate-binary-search-tree"/>
-    <hyperlink ref="E72" r:id="rId65" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree"/>
-    <hyperlink ref="E75" r:id="rId66" display="https://leetcode.com/problems/last-stone-weight"/>
-    <hyperlink ref="E76" r:id="rId67" display="https://leetcode.com/problems/k-closest-points-to-origin"/>
-    <hyperlink ref="E77" r:id="rId68" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
-    <hyperlink ref="E78" r:id="rId69" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix"/>
-    <hyperlink ref="E79" r:id="rId70" display="https://leetcode.com/problems/top-k-frequent-words"/>
-    <hyperlink ref="E80" r:id="rId71" display="https://leetcode.com/problems/top-k-frequent-elements"/>
-    <hyperlink ref="E81" r:id="rId72" display="https://leetcode.com/problems/two-sum"/>
-    <hyperlink ref="E82" r:id="rId73" display="https://leetcode.com/problems/ransom-note"/>
-    <hyperlink ref="E83" r:id="rId74" display="https://leetcode.com/problems/contains-duplicate"/>
-    <hyperlink ref="E84" r:id="rId75" display="https://leetcode.com/problems/subarray-sum-equals-k"/>
-    <hyperlink ref="E85" r:id="rId76" display="https://leetcode.com/problems/subarray-sums-divisible-by-k"/>
-    <hyperlink ref="E86" r:id="rId77" display="https://leetcode.com/problems/group-anagrams"/>
-    <hyperlink ref="E87" r:id="rId78" display="https://leetcode.com/problems/longest-consecutive-sequence"/>
-    <hyperlink ref="E88" r:id="rId79" display="https://leetcode.com/problems/number-of-islands"/>
-    <hyperlink ref="E89" r:id="rId80" display="https://leetcode.com/problems/max-area-of-island"/>
-    <hyperlink ref="E90" r:id="rId81" display="https://leetcode.com/problems/01-matrix"/>
-    <hyperlink ref="E91" r:id="rId82" display="https://leetcode.com/problems/network-delay-time"/>
-    <hyperlink ref="E92" r:id="rId83" display="https://leetcode.com/problems/redundant-connection"/>
-    <hyperlink ref="E93" r:id="rId84" display="https://leetcode.com/problems/number-of-provinces"/>
-    <hyperlink ref="E94" r:id="rId85" display="https://leetcode.com/problems/course-schedule"/>
-    <hyperlink ref="E95" r:id="rId86" display="https://leetcode.com/problems/course-schedule-ii"/>
-    <hyperlink ref="E96" r:id="rId87" display="https://leetcode.com/problems/clone-graph"/>
-    <hyperlink ref="E97" r:id="rId88" display="https://leetcode.com/problems/fibonacci-number"/>
-    <hyperlink ref="E98" r:id="rId89" display="https://leetcode.com/problems/climbing-stairs"/>
-    <hyperlink ref="E99" r:id="rId90" display="https://leetcode.com/problems/min-cost-climbing-stairs"/>
-    <hyperlink ref="E100" r:id="rId91" display="https://leetcode.com/problems/longest-common-subsequence"/>
-    <hyperlink ref="E101" r:id="rId92" display="https://leetcode.com/problems/longest-increasing-subsequence"/>
-    <hyperlink ref="E102" r:id="rId93" display="https://leetcode.com/problems/palindromic-substrings"/>
-    <hyperlink ref="E103" r:id="rId94" display="https://leetcode.com/problems/unique-paths"/>
-    <hyperlink ref="E104" r:id="rId95" display="https://leetcode.com/problems/partition-equal-subset-sum"/>
-    <hyperlink ref="E105" r:id="rId96" display="https://leetcode.com/problems/target-sum"/>
-    <hyperlink ref="E106" r:id="rId97" display="https://leetcode.com/problems/non-overlapping-intervals"/>
-    <hyperlink ref="E107" r:id="rId98" display="https://leetcode.com/problems/merge-intervals"/>
-    <hyperlink ref="E108" r:id="rId99" display="https://leetcode.com/problems/gas-station"/>
-    <hyperlink ref="E109" r:id="rId100" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
-    <hyperlink ref="E110" r:id="rId101" display="https://leetcode.com/problems/can-place-flowers"/>
-    <hyperlink ref="E111" r:id="rId102" display="https://leetcode.com/problems/jump-game"/>
-    <hyperlink ref="E23" r:id="rId103" display="https://leetcode.com/problems/n-queens"/>
-    <hyperlink ref="E24" r:id="rId104" display="https://leetcode.com/problems/n-queens-ii"/>
-    <hyperlink ref="E25" r:id="rId105" display="https://leetcode.com/problems/subsets-ii"/>
-    <hyperlink ref="E26" r:id="rId106" display="https://leetcode.com/problems/permutations-ii"/>
-    <hyperlink ref="E27" r:id="rId107" display="https://leetcode.com/problems/combination-sum"/>
-    <hyperlink ref="H2" r:id="rId108" display="https://leetcode.com/problems/count-and-say/"/>
-    <hyperlink ref="E5" r:id="rId109" display="https://leetcode.com/problems/minimum-window-substring"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://leetcode.com/problems/first-unique-character-in-a-string" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://leetcode.com/problems/ransom-note" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://leetcode.com/problems/valid-anagram" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E7" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E8" r:id="rId6" display="https://leetcode.com/problems/container-with-most-water" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E9" r:id="rId7" display="https://leetcode.com/problems/3sum" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E10" r:id="rId8" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E11" r:id="rId9" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E12" r:id="rId10" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E13" r:id="rId11" display="https://leetcode.com/problems/maximum-subarray" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E14" r:id="rId12" display="https://leetcode.com/problems/maximum-depth-of-binary-tree" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="E15" r:id="rId13" display="https://leetcode.com/problems/invert-binary-tree" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="E16" r:id="rId14" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="E17" r:id="rId15" display="https://leetcode.com/problems/different-ways-to-add-parentheses" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="E18" r:id="rId16" display="https://leetcode.com/problems/unique-binary-search-trees-ii" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="E19" r:id="rId17" display="https://leetcode.com/problems/powx-n" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="E20" r:id="rId18" display="https://leetcode.com/problems/subsets" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="E21" r:id="rId19" display="https://leetcode.com/problems/permutations" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="E22" r:id="rId20" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="E28" r:id="rId21" display="https://leetcode.com/problems/binary-search" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="E29" r:id="rId22" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="E30" r:id="rId23" display="https://leetcode.com/problems/find-peak-element" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="E31" r:id="rId24" display="https://leetcode.com/problems/koko-eating-bananas" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="E32" r:id="rId25" display="https://leetcode.com/problems/split-array-largest-sum" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="E33" r:id="rId26" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="E34" r:id="rId27" display="https://leetcode.com/problems/sort-an-array" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="E35" r:id="rId28" display="https://leetcode.com/problems/insertion-sort-list" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="E36" r:id="rId29" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="E37" r:id="rId30" display="https://leetcode.com/problems/largest-number" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="E38" r:id="rId31" display="https://leetcode.com/problems/reorder-data-in-log-files" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="E39" r:id="rId32" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="E40" r:id="rId33" display="https://leetcode.com/problems/insert-interval" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="E41" r:id="rId34" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="E42" r:id="rId35" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="E43" r:id="rId36" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="E44" r:id="rId37" display="https://leetcode.com/problems/reverse-linked-list-ii" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="E45" r:id="rId38" display="https://leetcode.com/problems/linked-list-cycle" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="E46" r:id="rId39" display="https://leetcode.com/problems/linked-list-cycle-ii" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="E47" r:id="rId40" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="E48" r:id="rId41" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="E49" r:id="rId42" display="https://leetcode.com/problems/intersection-of-two-linked-lists" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="E50" r:id="rId43" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="E51" r:id="rId44" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="E52" r:id="rId45" display="https://leetcode.com/problems/odd-even-linked-list" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="E53" r:id="rId46" display="https://leetcode.com/problems/lru-cache" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="E54" r:id="rId47" display="https://leetcode.com/problems/lfu-cache" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="E55" r:id="rId48" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="E56" r:id="rId49" display="https://leetcode.com/problems/backspace-string-compare" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="E57" r:id="rId50" display="https://leetcode.com/problems/daily-temperatures" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="E58" r:id="rId51" display="https://leetcode.com/problems/next-greater-element-i" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="E59" r:id="rId52" display="https://leetcode.com/problems/largest-rectangle-in-histogram" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="E65" r:id="rId53" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="E64" r:id="rId54" display="https://leetcode.com/problems/sliding-window-maximum" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="E63" r:id="rId55" display="https://leetcode.com/problems/design-circular-deque" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="E62" r:id="rId56" display="https://leetcode.com/problems/design-circular-queue" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="E61" r:id="rId57" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="E60" r:id="rId58" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="E66" r:id="rId59" display="https://leetcode.com/problems/binary-tree-inorder-traversal" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="E67" r:id="rId60" display="https://leetcode.com/problems/binary-tree-level-order-traversal" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="E68" r:id="rId61" display="https://leetcode.com/problems/binary-tree-right-side-view" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="E69" r:id="rId62" display="https://leetcode.com/problems/search-in-a-binary-search-tree" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="E70" r:id="rId63" display="https://leetcode.com/problems/delete-node-in-a-bst" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="E71" r:id="rId64" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="E72" r:id="rId65" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="E75" r:id="rId66" display="https://leetcode.com/problems/last-stone-weight" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="E76" r:id="rId67" display="https://leetcode.com/problems/k-closest-points-to-origin" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="E77" r:id="rId68" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="E78" r:id="rId69" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="E79" r:id="rId70" display="https://leetcode.com/problems/top-k-frequent-words" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="E80" r:id="rId71" display="https://leetcode.com/problems/top-k-frequent-elements" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="E81" r:id="rId72" display="https://leetcode.com/problems/two-sum" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="E82" r:id="rId73" display="https://leetcode.com/problems/ransom-note" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="E83" r:id="rId74" display="https://leetcode.com/problems/contains-duplicate" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="E84" r:id="rId75" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="E85" r:id="rId76" display="https://leetcode.com/problems/subarray-sums-divisible-by-k" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="E86" r:id="rId77" display="https://leetcode.com/problems/group-anagrams" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="E87" r:id="rId78" display="https://leetcode.com/problems/longest-consecutive-sequence" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="E88" r:id="rId79" display="https://leetcode.com/problems/number-of-islands" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="E89" r:id="rId80" display="https://leetcode.com/problems/max-area-of-island" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="E90" r:id="rId81" display="https://leetcode.com/problems/01-matrix" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="E91" r:id="rId82" display="https://leetcode.com/problems/network-delay-time" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="E92" r:id="rId83" display="https://leetcode.com/problems/redundant-connection" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="E93" r:id="rId84" display="https://leetcode.com/problems/number-of-provinces" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="E94" r:id="rId85" display="https://leetcode.com/problems/course-schedule" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="E95" r:id="rId86" display="https://leetcode.com/problems/course-schedule-ii" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="E96" r:id="rId87" display="https://leetcode.com/problems/clone-graph" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="E97" r:id="rId88" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="E98" r:id="rId89" display="https://leetcode.com/problems/climbing-stairs" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="E99" r:id="rId90" display="https://leetcode.com/problems/min-cost-climbing-stairs" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="E100" r:id="rId91" display="https://leetcode.com/problems/longest-common-subsequence" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="E101" r:id="rId92" display="https://leetcode.com/problems/longest-increasing-subsequence" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="E102" r:id="rId93" display="https://leetcode.com/problems/palindromic-substrings" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="E103" r:id="rId94" display="https://leetcode.com/problems/unique-paths" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="E104" r:id="rId95" display="https://leetcode.com/problems/partition-equal-subset-sum" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="E105" r:id="rId96" display="https://leetcode.com/problems/target-sum" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="E106" r:id="rId97" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="E107" r:id="rId98" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="E108" r:id="rId99" display="https://leetcode.com/problems/gas-station" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="E109" r:id="rId100" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="E110" r:id="rId101" display="https://leetcode.com/problems/can-place-flowers" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="E111" r:id="rId102" display="https://leetcode.com/problems/jump-game" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="E23" r:id="rId103" display="https://leetcode.com/problems/n-queens" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="E24" r:id="rId104" display="https://leetcode.com/problems/n-queens-ii" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="E25" r:id="rId105" display="https://leetcode.com/problems/subsets-ii" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="E26" r:id="rId106" display="https://leetcode.com/problems/permutations-ii" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="E27" r:id="rId107" display="https://leetcode.com/problems/combination-sum" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="H2" r:id="rId108" display="https://leetcode.com/problems/count-and-say/" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="E5" r:id="rId109" display="https://leetcode.com/problems/minimum-window-substring" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId110"/>

</xml_diff>

<commit_message>
chore(lesson-plan): updated problem statement for recursion topic feat(leetcode): added solutions for problems 53, 172, and 325
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schedule\Documents\TIME_DK\time_colleges\SRET\Focus_Batch_2023-2027\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFE2A8E-924A-49C3-9C45-C67355B12596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F9CA52-1E3F-4EA1-B00E-07F8DBCBD58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="256">
   <si>
     <t>Order</t>
   </si>
@@ -187,16 +187,7 @@
     <t>Recursion</t>
   </si>
   <si>
-    <t>Base Case + Tree View</t>
-  </si>
-  <si>
-    <t>104. Maximum Depth of Binary Tree</t>
-  </si>
-  <si>
     <t>Base Case Practice</t>
-  </si>
-  <si>
-    <t>226. Invert Binary Tree</t>
   </si>
   <si>
     <t>Fibonacci</t>
@@ -804,6 +795,12 @@
 4. Delete
 5. Update
 </t>
+  </si>
+  <si>
+    <t>172. Factorial Trailing Zeroes</t>
+  </si>
+  <si>
+    <t>Base Case</t>
   </si>
 </sst>
 </file>
@@ -876,7 +873,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -907,6 +904,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1554,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1597,7 @@
         <v>27</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1620,7 +1623,7 @@
         <v>32</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I2" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
@@ -1782,7 +1785,7 @@
         <v>32</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="I8" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
@@ -1880,7 +1883,7 @@
         <v>48</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="8" t="s">
         <v>50</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -1906,7 +1909,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="8" t="s">
         <v>51</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -1929,13 +1932,13 @@
         <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>53</v>
+        <v>255</v>
       </c>
       <c r="D14" s="1">
         <v>5</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>54</v>
+      <c r="E14" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>31</v>
@@ -1946,7 +1949,7 @@
       <c r="H14" s="3"/>
       <c r="I14" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
-        <v>Recursion: Base Case + Tree View</v>
+        <v>Recursion: Base Case</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1957,11 +1960,11 @@
         <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="7" t="s">
-        <v>56</v>
+      <c r="E15" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>31</v>
@@ -1983,11 +1986,11 @@
         <v>52</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>31</v>
@@ -2009,13 +2012,13 @@
         <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1">
         <v>6</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>39</v>
@@ -2037,11 +2040,11 @@
         <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>39</v>
@@ -2063,11 +2066,11 @@
         <v>52</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>39</v>
@@ -2089,13 +2092,13 @@
         <v>52</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D20" s="1">
         <v>7</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>39</v>
@@ -2117,11 +2120,11 @@
         <v>52</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>39</v>
@@ -2143,11 +2146,11 @@
         <v>52</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>39</v>
@@ -2166,16 +2169,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D23" s="1">
         <v>8</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>42</v>
@@ -2194,14 +2197,14 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>42</v>
@@ -2220,16 +2223,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D25" s="1">
         <v>9</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>39</v>
@@ -2248,14 +2251,14 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>39</v>
@@ -2274,14 +2277,14 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>39</v>
@@ -2300,16 +2303,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D28" s="1">
         <v>10</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>31</v>
@@ -2328,14 +2331,14 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>39</v>
@@ -2354,14 +2357,14 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>39</v>
@@ -2380,16 +2383,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D31" s="1">
         <v>11</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>39</v>
@@ -2408,14 +2411,14 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>42</v>
@@ -2434,14 +2437,14 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>39</v>
@@ -2460,16 +2463,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D34" s="1">
         <v>12</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>39</v>
@@ -2488,14 +2491,14 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>39</v>
@@ -2514,14 +2517,14 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>39</v>
@@ -2540,16 +2543,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D37" s="1">
         <v>13</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>39</v>
@@ -2568,14 +2571,14 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>31</v>
@@ -2594,16 +2597,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D39" s="1">
         <v>14</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>39</v>
@@ -2622,14 +2625,14 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>39</v>
@@ -2648,16 +2651,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D41" s="1">
         <v>15</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>39</v>
@@ -2676,14 +2679,14 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>39</v>
@@ -2702,16 +2705,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D43" s="1">
         <v>16</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>31</v>
@@ -2730,14 +2733,14 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>39</v>
@@ -2756,16 +2759,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D45" s="1">
         <v>17</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>31</v>
@@ -2784,14 +2787,14 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>39</v>
@@ -2810,16 +2813,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D47" s="1">
         <v>18</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>31</v>
@@ -2838,14 +2841,14 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>42</v>
@@ -2864,16 +2867,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D49" s="1">
         <v>19</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>31</v>
@@ -2892,14 +2895,14 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>39</v>
@@ -2918,16 +2921,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D51" s="1">
         <v>20</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>31</v>
@@ -2946,14 +2949,14 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>39</v>
@@ -2972,16 +2975,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D53" s="1">
         <v>21</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>39</v>
@@ -3000,14 +3003,14 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>42</v>
@@ -3029,13 +3032,13 @@
         <v>9</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D55" s="1">
         <v>22</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>31</v>
@@ -3057,11 +3060,11 @@
         <v>9</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>31</v>
@@ -3083,13 +3086,13 @@
         <v>9</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D57" s="1">
         <v>23</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>39</v>
@@ -3111,11 +3114,11 @@
         <v>9</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>31</v>
@@ -3137,11 +3140,11 @@
         <v>9</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>42</v>
@@ -3160,16 +3163,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D60" s="1">
         <v>24</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>31</v>
@@ -3188,14 +3191,14 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>31</v>
@@ -3214,16 +3217,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D62" s="1">
         <v>25</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>39</v>
@@ -3242,14 +3245,14 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>39</v>
@@ -3268,16 +3271,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D64" s="1">
         <v>26</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>42</v>
@@ -3296,14 +3299,14 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>42</v>
@@ -3322,16 +3325,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D66" s="1">
         <v>27</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>31</v>
@@ -3350,14 +3353,14 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>39</v>
@@ -3376,14 +3379,14 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>39</v>
@@ -3405,13 +3408,13 @@
         <v>12</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D69" s="1">
         <v>28</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>31</v>
@@ -3433,11 +3436,11 @@
         <v>12</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>39</v>
@@ -3459,13 +3462,13 @@
         <v>12</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D71" s="1">
         <v>29</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>39</v>
@@ -3487,11 +3490,11 @@
         <v>12</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>39</v>
@@ -3510,22 +3513,22 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D73" s="1">
         <v>30</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H73" s="3"/>
       <c r="I73" t="str">
@@ -3538,20 +3541,20 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F74" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G74" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="H74" s="3"/>
       <c r="I74" t="str">
@@ -3564,16 +3567,16 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D75" s="1">
         <v>31</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>31</v>
@@ -3592,14 +3595,14 @@
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>39</v>
@@ -3618,16 +3621,16 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D77" s="1">
         <v>32</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>39</v>
@@ -3646,14 +3649,14 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>39</v>
@@ -3672,16 +3675,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D79" s="1">
         <v>33</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>39</v>
@@ -3700,14 +3703,14 @@
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>39</v>
@@ -3726,16 +3729,16 @@
         <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D81" s="1">
         <v>34</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>31</v>
@@ -3754,10 +3757,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="7" t="s">
@@ -3780,14 +3783,14 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>31</v>
@@ -3806,10 +3809,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D84" s="1">
         <v>35</v>
@@ -3834,14 +3837,14 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>39</v>
@@ -3860,16 +3863,16 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D86" s="1">
         <v>36</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>39</v>
@@ -3888,14 +3891,14 @@
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>39</v>
@@ -3914,16 +3917,16 @@
         <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D88" s="1">
         <v>37</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>39</v>
@@ -3942,14 +3945,14 @@
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>39</v>
@@ -3968,14 +3971,14 @@
         <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F90" s="3" t="s">
         <v>39</v>
@@ -3994,16 +3997,16 @@
         <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D91" s="1">
         <v>38</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>39</v>
@@ -4022,14 +4025,14 @@
         <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F92" s="3" t="s">
         <v>39</v>
@@ -4048,14 +4051,14 @@
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>39</v>
@@ -4074,16 +4077,16 @@
         <v>93</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D94" s="1">
         <v>39</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>39</v>
@@ -4102,14 +4105,14 @@
         <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>39</v>
@@ -4128,14 +4131,14 @@
         <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F96" s="3" t="s">
         <v>39</v>
@@ -4154,16 +4157,16 @@
         <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D97" s="1">
         <v>40</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F97" s="3" t="s">
         <v>31</v>
@@ -4182,14 +4185,14 @@
         <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F98" s="3" t="s">
         <v>31</v>
@@ -4208,14 +4211,14 @@
         <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F99" s="3" t="s">
         <v>31</v>
@@ -4234,16 +4237,16 @@
         <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D100" s="1">
         <v>41</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>39</v>
@@ -4262,14 +4265,14 @@
         <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>39</v>
@@ -4288,14 +4291,14 @@
         <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F102" s="3" t="s">
         <v>39</v>
@@ -4314,16 +4317,16 @@
         <v>102</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D103" s="1">
         <v>42</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>39</v>
@@ -4342,14 +4345,14 @@
         <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>39</v>
@@ -4368,14 +4371,14 @@
         <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F105" s="3" t="s">
         <v>39</v>
@@ -4397,13 +4400,13 @@
         <v>20</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D106" s="1">
         <v>43</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F106" s="3" t="s">
         <v>39</v>
@@ -4425,11 +4428,11 @@
         <v>20</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>39</v>
@@ -4451,11 +4454,11 @@
         <v>20</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F108" s="3" t="s">
         <v>39</v>
@@ -4477,13 +4480,13 @@
         <v>20</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D109" s="1">
         <v>44</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F109" s="3" t="s">
         <v>39</v>
@@ -4505,11 +4508,11 @@
         <v>20</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F110" s="3" t="s">
         <v>31</v>
@@ -4531,11 +4534,11 @@
         <v>20</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F111" s="3" t="s">
         <v>39</v>
@@ -4554,19 +4557,19 @@
         <v>111</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D112" s="1">
         <v>45</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>32</v>
@@ -4582,17 +4585,17 @@
         <v>112</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G113" s="3" t="s">
         <v>35</v>
@@ -4620,104 +4623,104 @@
     <hyperlink ref="E11" r:id="rId9" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
     <hyperlink ref="E12" r:id="rId10" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
     <hyperlink ref="E13" r:id="rId11" display="https://leetcode.com/problems/maximum-subarray" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="E14" r:id="rId12" display="https://leetcode.com/problems/maximum-depth-of-binary-tree" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="E15" r:id="rId13" display="https://leetcode.com/problems/invert-binary-tree" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="E16" r:id="rId14" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="E17" r:id="rId15" display="https://leetcode.com/problems/different-ways-to-add-parentheses" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="E18" r:id="rId16" display="https://leetcode.com/problems/unique-binary-search-trees-ii" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="E19" r:id="rId17" display="https://leetcode.com/problems/powx-n" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="E20" r:id="rId18" display="https://leetcode.com/problems/subsets" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="E21" r:id="rId19" display="https://leetcode.com/problems/permutations" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="E22" r:id="rId20" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="E28" r:id="rId21" display="https://leetcode.com/problems/binary-search" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="E29" r:id="rId22" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="E30" r:id="rId23" display="https://leetcode.com/problems/find-peak-element" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="E31" r:id="rId24" display="https://leetcode.com/problems/koko-eating-bananas" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="E32" r:id="rId25" display="https://leetcode.com/problems/split-array-largest-sum" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="E33" r:id="rId26" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="E34" r:id="rId27" display="https://leetcode.com/problems/sort-an-array" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="E35" r:id="rId28" display="https://leetcode.com/problems/insertion-sort-list" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="E36" r:id="rId29" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="E37" r:id="rId30" display="https://leetcode.com/problems/largest-number" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="E38" r:id="rId31" display="https://leetcode.com/problems/reorder-data-in-log-files" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="E39" r:id="rId32" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="E40" r:id="rId33" display="https://leetcode.com/problems/insert-interval" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="E41" r:id="rId34" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="E42" r:id="rId35" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="E43" r:id="rId36" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="E44" r:id="rId37" display="https://leetcode.com/problems/reverse-linked-list-ii" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="E45" r:id="rId38" display="https://leetcode.com/problems/linked-list-cycle" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="E46" r:id="rId39" display="https://leetcode.com/problems/linked-list-cycle-ii" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="E47" r:id="rId40" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="E48" r:id="rId41" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="E49" r:id="rId42" display="https://leetcode.com/problems/intersection-of-two-linked-lists" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="E50" r:id="rId43" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="E51" r:id="rId44" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="E52" r:id="rId45" display="https://leetcode.com/problems/odd-even-linked-list" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="E53" r:id="rId46" display="https://leetcode.com/problems/lru-cache" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="E54" r:id="rId47" display="https://leetcode.com/problems/lfu-cache" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="E55" r:id="rId48" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="E56" r:id="rId49" display="https://leetcode.com/problems/backspace-string-compare" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="E57" r:id="rId50" display="https://leetcode.com/problems/daily-temperatures" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="E58" r:id="rId51" display="https://leetcode.com/problems/next-greater-element-i" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="E59" r:id="rId52" display="https://leetcode.com/problems/largest-rectangle-in-histogram" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="E65" r:id="rId53" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="E64" r:id="rId54" display="https://leetcode.com/problems/sliding-window-maximum" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="E63" r:id="rId55" display="https://leetcode.com/problems/design-circular-deque" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="E62" r:id="rId56" display="https://leetcode.com/problems/design-circular-queue" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="E61" r:id="rId57" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="E60" r:id="rId58" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
-    <hyperlink ref="E66" r:id="rId59" display="https://leetcode.com/problems/binary-tree-inorder-traversal" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
-    <hyperlink ref="E67" r:id="rId60" display="https://leetcode.com/problems/binary-tree-level-order-traversal" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
-    <hyperlink ref="E68" r:id="rId61" display="https://leetcode.com/problems/binary-tree-right-side-view" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="E69" r:id="rId62" display="https://leetcode.com/problems/search-in-a-binary-search-tree" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
-    <hyperlink ref="E70" r:id="rId63" display="https://leetcode.com/problems/delete-node-in-a-bst" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
-    <hyperlink ref="E71" r:id="rId64" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
-    <hyperlink ref="E72" r:id="rId65" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
-    <hyperlink ref="E75" r:id="rId66" display="https://leetcode.com/problems/last-stone-weight" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
-    <hyperlink ref="E76" r:id="rId67" display="https://leetcode.com/problems/k-closest-points-to-origin" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
-    <hyperlink ref="E77" r:id="rId68" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
-    <hyperlink ref="E78" r:id="rId69" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
-    <hyperlink ref="E79" r:id="rId70" display="https://leetcode.com/problems/top-k-frequent-words" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
-    <hyperlink ref="E80" r:id="rId71" display="https://leetcode.com/problems/top-k-frequent-elements" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
-    <hyperlink ref="E81" r:id="rId72" display="https://leetcode.com/problems/two-sum" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
-    <hyperlink ref="E82" r:id="rId73" display="https://leetcode.com/problems/ransom-note" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
-    <hyperlink ref="E83" r:id="rId74" display="https://leetcode.com/problems/contains-duplicate" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
-    <hyperlink ref="E84" r:id="rId75" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
-    <hyperlink ref="E85" r:id="rId76" display="https://leetcode.com/problems/subarray-sums-divisible-by-k" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
-    <hyperlink ref="E86" r:id="rId77" display="https://leetcode.com/problems/group-anagrams" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
-    <hyperlink ref="E87" r:id="rId78" display="https://leetcode.com/problems/longest-consecutive-sequence" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
-    <hyperlink ref="E88" r:id="rId79" display="https://leetcode.com/problems/number-of-islands" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
-    <hyperlink ref="E89" r:id="rId80" display="https://leetcode.com/problems/max-area-of-island" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
-    <hyperlink ref="E90" r:id="rId81" display="https://leetcode.com/problems/01-matrix" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
-    <hyperlink ref="E91" r:id="rId82" display="https://leetcode.com/problems/network-delay-time" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
-    <hyperlink ref="E92" r:id="rId83" display="https://leetcode.com/problems/redundant-connection" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
-    <hyperlink ref="E93" r:id="rId84" display="https://leetcode.com/problems/number-of-provinces" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
-    <hyperlink ref="E94" r:id="rId85" display="https://leetcode.com/problems/course-schedule" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
-    <hyperlink ref="E95" r:id="rId86" display="https://leetcode.com/problems/course-schedule-ii" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
-    <hyperlink ref="E96" r:id="rId87" display="https://leetcode.com/problems/clone-graph" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
-    <hyperlink ref="E97" r:id="rId88" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
-    <hyperlink ref="E98" r:id="rId89" display="https://leetcode.com/problems/climbing-stairs" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
-    <hyperlink ref="E99" r:id="rId90" display="https://leetcode.com/problems/min-cost-climbing-stairs" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
-    <hyperlink ref="E100" r:id="rId91" display="https://leetcode.com/problems/longest-common-subsequence" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
-    <hyperlink ref="E101" r:id="rId92" display="https://leetcode.com/problems/longest-increasing-subsequence" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
-    <hyperlink ref="E102" r:id="rId93" display="https://leetcode.com/problems/palindromic-substrings" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
-    <hyperlink ref="E103" r:id="rId94" display="https://leetcode.com/problems/unique-paths" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
-    <hyperlink ref="E104" r:id="rId95" display="https://leetcode.com/problems/partition-equal-subset-sum" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
-    <hyperlink ref="E105" r:id="rId96" display="https://leetcode.com/problems/target-sum" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
-    <hyperlink ref="E106" r:id="rId97" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
-    <hyperlink ref="E107" r:id="rId98" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
-    <hyperlink ref="E108" r:id="rId99" display="https://leetcode.com/problems/gas-station" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
-    <hyperlink ref="E109" r:id="rId100" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
-    <hyperlink ref="E110" r:id="rId101" display="https://leetcode.com/problems/can-place-flowers" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
-    <hyperlink ref="E111" r:id="rId102" display="https://leetcode.com/problems/jump-game" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
-    <hyperlink ref="E23" r:id="rId103" display="https://leetcode.com/problems/n-queens" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
-    <hyperlink ref="E24" r:id="rId104" display="https://leetcode.com/problems/n-queens-ii" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
-    <hyperlink ref="E25" r:id="rId105" display="https://leetcode.com/problems/subsets-ii" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
-    <hyperlink ref="E26" r:id="rId106" display="https://leetcode.com/problems/permutations-ii" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
-    <hyperlink ref="E27" r:id="rId107" display="https://leetcode.com/problems/combination-sum" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
-    <hyperlink ref="H2" r:id="rId108" display="https://leetcode.com/problems/count-and-say/" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
-    <hyperlink ref="E5" r:id="rId109" display="https://leetcode.com/problems/minimum-window-substring" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
+    <hyperlink ref="E16" r:id="rId12" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="E17" r:id="rId13" display="https://leetcode.com/problems/different-ways-to-add-parentheses" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="E18" r:id="rId14" display="https://leetcode.com/problems/unique-binary-search-trees-ii" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="E19" r:id="rId15" display="https://leetcode.com/problems/powx-n" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="E20" r:id="rId16" display="https://leetcode.com/problems/subsets" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="E21" r:id="rId17" display="https://leetcode.com/problems/permutations" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="E22" r:id="rId18" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="E28" r:id="rId19" display="https://leetcode.com/problems/binary-search" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="E29" r:id="rId20" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="E30" r:id="rId21" display="https://leetcode.com/problems/find-peak-element" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="E31" r:id="rId22" display="https://leetcode.com/problems/koko-eating-bananas" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="E32" r:id="rId23" display="https://leetcode.com/problems/split-array-largest-sum" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="E33" r:id="rId24" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="E34" r:id="rId25" display="https://leetcode.com/problems/sort-an-array" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="E35" r:id="rId26" display="https://leetcode.com/problems/insertion-sort-list" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="E36" r:id="rId27" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="E37" r:id="rId28" display="https://leetcode.com/problems/largest-number" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="E38" r:id="rId29" display="https://leetcode.com/problems/reorder-data-in-log-files" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="E39" r:id="rId30" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="E40" r:id="rId31" display="https://leetcode.com/problems/insert-interval" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="E41" r:id="rId32" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="E42" r:id="rId33" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="E43" r:id="rId34" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="E44" r:id="rId35" display="https://leetcode.com/problems/reverse-linked-list-ii" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="E45" r:id="rId36" display="https://leetcode.com/problems/linked-list-cycle" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="E46" r:id="rId37" display="https://leetcode.com/problems/linked-list-cycle-ii" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="E47" r:id="rId38" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="E48" r:id="rId39" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="E49" r:id="rId40" display="https://leetcode.com/problems/intersection-of-two-linked-lists" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="E50" r:id="rId41" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="E51" r:id="rId42" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="E52" r:id="rId43" display="https://leetcode.com/problems/odd-even-linked-list" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="E53" r:id="rId44" display="https://leetcode.com/problems/lru-cache" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="E54" r:id="rId45" display="https://leetcode.com/problems/lfu-cache" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="E55" r:id="rId46" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="E56" r:id="rId47" display="https://leetcode.com/problems/backspace-string-compare" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="E57" r:id="rId48" display="https://leetcode.com/problems/daily-temperatures" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="E58" r:id="rId49" display="https://leetcode.com/problems/next-greater-element-i" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="E59" r:id="rId50" display="https://leetcode.com/problems/largest-rectangle-in-histogram" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="E65" r:id="rId51" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="E64" r:id="rId52" display="https://leetcode.com/problems/sliding-window-maximum" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="E63" r:id="rId53" display="https://leetcode.com/problems/design-circular-deque" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="E62" r:id="rId54" display="https://leetcode.com/problems/design-circular-queue" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="E61" r:id="rId55" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="E60" r:id="rId56" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="E66" r:id="rId57" display="https://leetcode.com/problems/binary-tree-inorder-traversal" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="E67" r:id="rId58" display="https://leetcode.com/problems/binary-tree-level-order-traversal" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="E68" r:id="rId59" display="https://leetcode.com/problems/binary-tree-right-side-view" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="E69" r:id="rId60" display="https://leetcode.com/problems/search-in-a-binary-search-tree" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="E70" r:id="rId61" display="https://leetcode.com/problems/delete-node-in-a-bst" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="E71" r:id="rId62" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="E72" r:id="rId63" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="E75" r:id="rId64" display="https://leetcode.com/problems/last-stone-weight" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="E76" r:id="rId65" display="https://leetcode.com/problems/k-closest-points-to-origin" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="E77" r:id="rId66" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="E78" r:id="rId67" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="E79" r:id="rId68" display="https://leetcode.com/problems/top-k-frequent-words" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="E80" r:id="rId69" display="https://leetcode.com/problems/top-k-frequent-elements" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="E81" r:id="rId70" display="https://leetcode.com/problems/two-sum" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="E82" r:id="rId71" display="https://leetcode.com/problems/ransom-note" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="E83" r:id="rId72" display="https://leetcode.com/problems/contains-duplicate" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="E84" r:id="rId73" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="E85" r:id="rId74" display="https://leetcode.com/problems/subarray-sums-divisible-by-k" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="E86" r:id="rId75" display="https://leetcode.com/problems/group-anagrams" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="E87" r:id="rId76" display="https://leetcode.com/problems/longest-consecutive-sequence" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="E88" r:id="rId77" display="https://leetcode.com/problems/number-of-islands" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="E89" r:id="rId78" display="https://leetcode.com/problems/max-area-of-island" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="E90" r:id="rId79" display="https://leetcode.com/problems/01-matrix" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="E91" r:id="rId80" display="https://leetcode.com/problems/network-delay-time" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="E92" r:id="rId81" display="https://leetcode.com/problems/redundant-connection" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="E93" r:id="rId82" display="https://leetcode.com/problems/number-of-provinces" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="E94" r:id="rId83" display="https://leetcode.com/problems/course-schedule" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="E95" r:id="rId84" display="https://leetcode.com/problems/course-schedule-ii" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="E96" r:id="rId85" display="https://leetcode.com/problems/clone-graph" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="E97" r:id="rId86" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="E98" r:id="rId87" display="https://leetcode.com/problems/climbing-stairs" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="E99" r:id="rId88" display="https://leetcode.com/problems/min-cost-climbing-stairs" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="E100" r:id="rId89" display="https://leetcode.com/problems/longest-common-subsequence" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="E101" r:id="rId90" display="https://leetcode.com/problems/longest-increasing-subsequence" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="E102" r:id="rId91" display="https://leetcode.com/problems/palindromic-substrings" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="E103" r:id="rId92" display="https://leetcode.com/problems/unique-paths" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="E104" r:id="rId93" display="https://leetcode.com/problems/partition-equal-subset-sum" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="E105" r:id="rId94" display="https://leetcode.com/problems/target-sum" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="E106" r:id="rId95" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="E107" r:id="rId96" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="E108" r:id="rId97" display="https://leetcode.com/problems/gas-station" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="E109" r:id="rId98" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="E110" r:id="rId99" display="https://leetcode.com/problems/can-place-flowers" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="E111" r:id="rId100" display="https://leetcode.com/problems/jump-game" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="E23" r:id="rId101" display="https://leetcode.com/problems/n-queens" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="E24" r:id="rId102" display="https://leetcode.com/problems/n-queens-ii" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="E25" r:id="rId103" display="https://leetcode.com/problems/subsets-ii" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="E26" r:id="rId104" display="https://leetcode.com/problems/permutations-ii" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="E27" r:id="rId105" display="https://leetcode.com/problems/combination-sum" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="H2" r:id="rId106" display="https://leetcode.com/problems/count-and-say/" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="E5" r:id="rId107" display="https://leetcode.com/problems/minimum-window-substring" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
+    <hyperlink ref="E15" r:id="rId108" display="https://leetcode.com/problems/subsets/" xr:uid="{0D3C85A9-3A8D-4ABC-A1C9-8458E66D17AA}"/>
+    <hyperlink ref="E14" r:id="rId109" display="https://leetcode.com/problems/factorial-trailing-zeroes/" xr:uid="{B4BAC095-9651-4A4F-AD5C-C25CE7ADDECA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId110"/>

</xml_diff>

<commit_message>
feet(leetcode): added solution for problems 46, 47, 50, 95
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schedule\Documents\TIME_DK\time_colleges\SRET\Focus_Batch_2023-2027\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2_TIME_College\SRET\sret-focus-batch-23-27\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F9CA52-1E3F-4EA1-B00E-07F8DBCBD58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hours Alloted" sheetId="1" r:id="rId1"/>
     <sheet name="Lesson Plan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -806,7 +805,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -905,11 +904,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -918,26 +917,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -984,6 +963,26 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1012,32 +1011,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:C20" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:C20"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Topic" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hours" dataDxfId="12"/>
+    <tableColumn id="1" name="Order" dataDxfId="14"/>
+    <tableColumn id="2" name="Topic" dataDxfId="13"/>
+    <tableColumn id="3" name="Hours" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:H113" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H113"/>
+  <sortState ref="A2:G113">
     <sortCondition ref="A1:A113"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="S.No" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Topic" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Subtopic" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Hour" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="LeetCode Problem" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Level" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Remark" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="1" name="S.No" dataDxfId="7"/>
+    <tableColumn id="2" name="Topic" dataDxfId="6"/>
+    <tableColumn id="3" name="Subtopic" dataDxfId="5"/>
+    <tableColumn id="4" name="Hour" dataDxfId="4"/>
+    <tableColumn id="5" name="LeetCode Problem" dataDxfId="3"/>
+    <tableColumn id="6" name="Level" dataDxfId="2"/>
+    <tableColumn id="7" name="Remark" dataDxfId="1"/>
+    <tableColumn id="8" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1305,21 +1304,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6"/>
+    <col min="1" max="1" width="9.109375" style="6"/>
+    <col min="2" max="2" width="60.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1329,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1341,7 +1340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1352,7 +1351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1363,7 +1362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1374,7 +1373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1385,7 +1384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1396,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1407,7 +1406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1418,7 +1417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1429,7 +1428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1440,7 +1439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1451,7 +1450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1462,7 +1461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1495,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1506,7 +1505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1528,7 +1527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" s="6">
         <f>SUM(C2:C21)</f>
         <v>45</v>
@@ -1554,27 +1553,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.7109375" customWidth="1"/>
-    <col min="9" max="9" width="36.28515625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.6640625" customWidth="1"/>
+    <col min="9" max="9" width="36.33203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -1600,7 +1599,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1630,7 +1629,7 @@
         <v>String: Hashing + Count</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1656,7 +1655,7 @@
         <v>String: Frequency Matching</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1682,7 +1681,7 @@
         <v>String: Frequency Matching</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1710,7 +1709,7 @@
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1736,7 +1735,7 @@
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1762,7 +1761,7 @@
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1792,7 +1791,7 @@
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1818,7 +1817,7 @@
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1844,7 +1843,7 @@
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1872,7 +1871,7 @@
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1898,7 +1897,7 @@
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1924,7 +1923,7 @@
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1937,7 +1936,7 @@
       <c r="D14" s="1">
         <v>5</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>254</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -1952,7 +1951,7 @@
         <v>Recursion: Base Case</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1978,7 +1977,7 @@
         <v>Recursion: Base Case Practice</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1989,7 +1988,7 @@
         <v>54</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="8" t="s">
         <v>55</v>
       </c>
       <c r="F16" s="3" t="s">
@@ -2004,7 +2003,7 @@
         <v>Recursion: Fibonacci</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2017,7 +2016,7 @@
       <c r="D17" s="1">
         <v>6</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="8" t="s">
         <v>57</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -2032,7 +2031,7 @@
         <v>Recursion: Divide and Conquer</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2043,7 +2042,7 @@
         <v>56</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="8" t="s">
         <v>58</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -2058,7 +2057,7 @@
         <v>Recursion: Divide and Conquer</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2069,7 +2068,7 @@
         <v>59</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="8" t="s">
         <v>60</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -2084,7 +2083,7 @@
         <v>Recursion: Binary Recursion Tree</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2097,8 +2096,8 @@
       <c r="D20" s="1">
         <v>7</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>62</v>
+      <c r="E20" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>39</v>
@@ -2106,13 +2105,13 @@
       <c r="G20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="3"/>
+      <c r="H20" s="7"/>
       <c r="I20" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Recursion: Subsets</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2123,8 +2122,8 @@
         <v>63</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="7" t="s">
-        <v>64</v>
+      <c r="E21" s="12" t="s">
+        <v>248</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>39</v>
@@ -2138,7 +2137,7 @@
         <v>Recursion: Rec. with State</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2164,7 +2163,7 @@
         <v>Recursion: Backtrack Base</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2192,7 +2191,7 @@
         <v>Backtracking: N-Queens</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2218,7 +2217,7 @@
         <v>Backtracking: N-Queens</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2246,7 +2245,7 @@
         <v>Backtracking: Subset Gen</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2272,7 +2271,7 @@
         <v>Backtracking: Permutations</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2298,7 +2297,7 @@
         <v>Backtracking: Combination Sum</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2326,7 +2325,7 @@
         <v>Searching: Binary Search Basic</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2352,7 +2351,7 @@
         <v>Searching: First/Last Occurrence</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2378,7 +2377,7 @@
         <v>Searching: Peak Element</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2406,7 +2405,7 @@
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2458,7 +2457,7 @@
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2486,7 +2485,7 @@
         <v>Sorting: Basic Sorting Logic</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2512,7 +2511,7 @@
         <v>Sorting: Selection Practice</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2538,7 +2537,7 @@
         <v>Sorting: QuickSort</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2566,7 +2565,7 @@
         <v>Sorting: Custom Comparator</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2592,7 +2591,7 @@
         <v>Sorting: Custom Comparator</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2620,7 +2619,7 @@
         <v>Sorting: Merge Intervals</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>Sorting: Merge Intervals</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2674,7 +2673,7 @@
         <v>Sorting: Scheduling Logic</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2700,7 +2699,7 @@
         <v>Sorting: Sorting Based Greedy</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2728,7 +2727,7 @@
         <v>Linked List: Reverse LL</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2754,7 +2753,7 @@
         <v>Linked List: Reverse LL II</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2782,7 +2781,7 @@
         <v>Linked List: Detect Cycle</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2808,7 +2807,7 @@
         <v>Linked List: Cycle II</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2836,7 +2835,7 @@
         <v>Linked List: Merge LL</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>Linked List: Merge k Lists</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2890,7 +2889,7 @@
         <v>Linked List: Intersection Point</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2916,7 +2915,7 @@
         <v>Linked List: Remove Nth Node</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2944,7 +2943,7 @@
         <v>Linked List: Palindrome Check</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2970,7 +2969,7 @@
         <v>Linked List: Odd Even Index</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2998,7 +2997,7 @@
         <v>Linked List: LRU Cache Logic</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3024,7 +3023,7 @@
         <v>Linked List: Advanced LRU Logic</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3052,7 +3051,7 @@
         <v>Stack: Stack Basics</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3078,7 +3077,7 @@
         <v>Stack: Stack Basics</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3106,7 +3105,7 @@
         <v>Stack: Monotonic Stack</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3132,7 +3131,7 @@
         <v>Stack: Next Greater Element</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3158,7 +3157,7 @@
         <v>Stack: Largest Rect in Hist</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3186,7 +3185,7 @@
         <v>Queue: Queue + BFS Intro</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3212,7 +3211,7 @@
         <v>Queue: Implement Queue Using Stacks</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3240,7 +3239,7 @@
         <v>Queue: Circular Queue</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3266,7 +3265,7 @@
         <v>Queue: Deque</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3294,7 +3293,7 @@
         <v>Queue: Monotonic Queue</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3320,7 +3319,7 @@
         <v>Queue: Monotonic Queue</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3348,7 +3347,7 @@
         <v>Trees: Traversals</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3374,7 +3373,7 @@
         <v>Trees: Traversals</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3400,7 +3399,7 @@
         <v>Trees: Views + Height</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3428,7 +3427,7 @@
         <v>BST: Search, Insert, Min</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3454,7 +3453,7 @@
         <v>BST: Deletion</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3482,7 +3481,7 @@
         <v>BST: Validate BST</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>BST: Lowest Common Ancestor</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3536,7 +3535,7 @@
         <v>Balanced Tree: AVL Tree</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3562,7 +3561,7 @@
         <v>Balanced Tree: Red-Black Tree</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3590,7 +3589,7 @@
         <v>Heap: Min Heap Introduction</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3616,7 +3615,7 @@
         <v>Heap: Priority Queue Usage</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3644,7 +3643,7 @@
         <v>Heap: Kth Largest Element</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3670,7 +3669,7 @@
         <v>Heap: Kth Smallest Element</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3698,7 +3697,7 @@
         <v>Heap: Heap + Sorting Logic</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3724,7 +3723,7 @@
         <v>Heap: Heap + Custom Comparator</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3752,7 +3751,7 @@
         <v>HashMap: Frequency Counting</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3778,7 +3777,7 @@
         <v>HashMap: Frequency Counting</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3804,7 +3803,7 @@
         <v>HashSet: Uniqueness Check</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3832,7 +3831,7 @@
         <v>HashMap: Prefix Sum Technique</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3858,7 +3857,7 @@
         <v>HashMap: Prefix Sum Variation</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -3886,7 +3885,7 @@
         <v>HashMap: Grouping Data</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -3912,7 +3911,7 @@
         <v>HashMap: Longest Streak/Length</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -3940,7 +3939,7 @@
         <v>Graph: BFS Traversal</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -3966,7 +3965,7 @@
         <v>Graph: DFS Traversal</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -3992,7 +3991,7 @@
         <v>Graph: BFS with Distance</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -4020,7 +4019,7 @@
         <v>Graph: Dijkstra’s (Shortest Path)</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -4046,7 +4045,7 @@
         <v>Graph: Union Find</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -4072,7 +4071,7 @@
         <v>Graph: Cycle Detection</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -4100,7 +4099,7 @@
         <v>Graph: Topological Sort</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -4126,7 +4125,7 @@
         <v>Graph: Topo + Ordering</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -4152,7 +4151,7 @@
         <v>Graph: Kahn’s Algorithm</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4180,7 +4179,7 @@
         <v>DP: Fibonacci with Memo</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4206,7 +4205,7 @@
         <v>DP: Climbing Stairs (1D)</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4232,7 +4231,7 @@
         <v>DP: Min Cost Climbing</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4260,7 +4259,7 @@
         <v>DP: Longest Common Subseq</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4286,7 +4285,7 @@
         <v>DP: Longest Increasing Subseq</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4312,7 +4311,7 @@
         <v>DP: Palindromic Substrings</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -4340,7 +4339,7 @@
         <v>DP: Unique Paths (2D Grid)</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -4366,7 +4365,7 @@
         <v>DP: Partition Equal Sum</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -4392,7 +4391,7 @@
         <v>DP: Target Sum (state model)</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -4420,7 +4419,7 @@
         <v>Greedy: Activity Selection (Intervals)</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -4446,7 +4445,7 @@
         <v>Greedy: Interval Merging</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -4472,7 +4471,7 @@
         <v>Greedy: Gas Station Problem</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -4500,7 +4499,7 @@
         <v>Greedy: Job Scheduling / Max Profit</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -4526,7 +4525,7 @@
         <v>Greedy: Resource Assignment</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -4552,7 +4551,7 @@
         <v>Greedy: Jump Game</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -4580,7 +4579,7 @@
         <v>Review: Strategy + Topic Recap</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -4604,123 +4603,123 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G22 G28:G1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://leetcode.com/problems/first-unique-character-in-a-string" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://leetcode.com/problems/ransom-note" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://leetcode.com/problems/valid-anagram" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="E7" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="E8" r:id="rId6" display="https://leetcode.com/problems/container-with-most-water" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="E9" r:id="rId7" display="https://leetcode.com/problems/3sum" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="E10" r:id="rId8" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="E11" r:id="rId9" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="E12" r:id="rId10" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="E13" r:id="rId11" display="https://leetcode.com/problems/maximum-subarray" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="E16" r:id="rId12" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="E17" r:id="rId13" display="https://leetcode.com/problems/different-ways-to-add-parentheses" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="E18" r:id="rId14" display="https://leetcode.com/problems/unique-binary-search-trees-ii" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="E19" r:id="rId15" display="https://leetcode.com/problems/powx-n" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="E20" r:id="rId16" display="https://leetcode.com/problems/subsets" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="E21" r:id="rId17" display="https://leetcode.com/problems/permutations" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="E22" r:id="rId18" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="E28" r:id="rId19" display="https://leetcode.com/problems/binary-search" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="E29" r:id="rId20" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="E30" r:id="rId21" display="https://leetcode.com/problems/find-peak-element" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="E31" r:id="rId22" display="https://leetcode.com/problems/koko-eating-bananas" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="E32" r:id="rId23" display="https://leetcode.com/problems/split-array-largest-sum" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="E33" r:id="rId24" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="E34" r:id="rId25" display="https://leetcode.com/problems/sort-an-array" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="E35" r:id="rId26" display="https://leetcode.com/problems/insertion-sort-list" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="E36" r:id="rId27" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="E37" r:id="rId28" display="https://leetcode.com/problems/largest-number" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="E38" r:id="rId29" display="https://leetcode.com/problems/reorder-data-in-log-files" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="E39" r:id="rId30" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="E40" r:id="rId31" display="https://leetcode.com/problems/insert-interval" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="E41" r:id="rId32" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="E42" r:id="rId33" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="E43" r:id="rId34" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="E44" r:id="rId35" display="https://leetcode.com/problems/reverse-linked-list-ii" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="E45" r:id="rId36" display="https://leetcode.com/problems/linked-list-cycle" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="E46" r:id="rId37" display="https://leetcode.com/problems/linked-list-cycle-ii" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="E47" r:id="rId38" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="E48" r:id="rId39" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="E49" r:id="rId40" display="https://leetcode.com/problems/intersection-of-two-linked-lists" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="E50" r:id="rId41" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="E51" r:id="rId42" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="E52" r:id="rId43" display="https://leetcode.com/problems/odd-even-linked-list" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="E53" r:id="rId44" display="https://leetcode.com/problems/lru-cache" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="E54" r:id="rId45" display="https://leetcode.com/problems/lfu-cache" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="E55" r:id="rId46" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="E56" r:id="rId47" display="https://leetcode.com/problems/backspace-string-compare" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="E57" r:id="rId48" display="https://leetcode.com/problems/daily-temperatures" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="E58" r:id="rId49" display="https://leetcode.com/problems/next-greater-element-i" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="E59" r:id="rId50" display="https://leetcode.com/problems/largest-rectangle-in-histogram" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="E65" r:id="rId51" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="E64" r:id="rId52" display="https://leetcode.com/problems/sliding-window-maximum" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="E63" r:id="rId53" display="https://leetcode.com/problems/design-circular-deque" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="E62" r:id="rId54" display="https://leetcode.com/problems/design-circular-queue" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="E61" r:id="rId55" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="E60" r:id="rId56" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
-    <hyperlink ref="E66" r:id="rId57" display="https://leetcode.com/problems/binary-tree-inorder-traversal" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
-    <hyperlink ref="E67" r:id="rId58" display="https://leetcode.com/problems/binary-tree-level-order-traversal" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
-    <hyperlink ref="E68" r:id="rId59" display="https://leetcode.com/problems/binary-tree-right-side-view" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="E69" r:id="rId60" display="https://leetcode.com/problems/search-in-a-binary-search-tree" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
-    <hyperlink ref="E70" r:id="rId61" display="https://leetcode.com/problems/delete-node-in-a-bst" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
-    <hyperlink ref="E71" r:id="rId62" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
-    <hyperlink ref="E72" r:id="rId63" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
-    <hyperlink ref="E75" r:id="rId64" display="https://leetcode.com/problems/last-stone-weight" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
-    <hyperlink ref="E76" r:id="rId65" display="https://leetcode.com/problems/k-closest-points-to-origin" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
-    <hyperlink ref="E77" r:id="rId66" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
-    <hyperlink ref="E78" r:id="rId67" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
-    <hyperlink ref="E79" r:id="rId68" display="https://leetcode.com/problems/top-k-frequent-words" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
-    <hyperlink ref="E80" r:id="rId69" display="https://leetcode.com/problems/top-k-frequent-elements" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
-    <hyperlink ref="E81" r:id="rId70" display="https://leetcode.com/problems/two-sum" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
-    <hyperlink ref="E82" r:id="rId71" display="https://leetcode.com/problems/ransom-note" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
-    <hyperlink ref="E83" r:id="rId72" display="https://leetcode.com/problems/contains-duplicate" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
-    <hyperlink ref="E84" r:id="rId73" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
-    <hyperlink ref="E85" r:id="rId74" display="https://leetcode.com/problems/subarray-sums-divisible-by-k" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
-    <hyperlink ref="E86" r:id="rId75" display="https://leetcode.com/problems/group-anagrams" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
-    <hyperlink ref="E87" r:id="rId76" display="https://leetcode.com/problems/longest-consecutive-sequence" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
-    <hyperlink ref="E88" r:id="rId77" display="https://leetcode.com/problems/number-of-islands" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
-    <hyperlink ref="E89" r:id="rId78" display="https://leetcode.com/problems/max-area-of-island" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
-    <hyperlink ref="E90" r:id="rId79" display="https://leetcode.com/problems/01-matrix" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
-    <hyperlink ref="E91" r:id="rId80" display="https://leetcode.com/problems/network-delay-time" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
-    <hyperlink ref="E92" r:id="rId81" display="https://leetcode.com/problems/redundant-connection" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
-    <hyperlink ref="E93" r:id="rId82" display="https://leetcode.com/problems/number-of-provinces" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
-    <hyperlink ref="E94" r:id="rId83" display="https://leetcode.com/problems/course-schedule" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
-    <hyperlink ref="E95" r:id="rId84" display="https://leetcode.com/problems/course-schedule-ii" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
-    <hyperlink ref="E96" r:id="rId85" display="https://leetcode.com/problems/clone-graph" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
-    <hyperlink ref="E97" r:id="rId86" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
-    <hyperlink ref="E98" r:id="rId87" display="https://leetcode.com/problems/climbing-stairs" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
-    <hyperlink ref="E99" r:id="rId88" display="https://leetcode.com/problems/min-cost-climbing-stairs" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
-    <hyperlink ref="E100" r:id="rId89" display="https://leetcode.com/problems/longest-common-subsequence" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
-    <hyperlink ref="E101" r:id="rId90" display="https://leetcode.com/problems/longest-increasing-subsequence" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
-    <hyperlink ref="E102" r:id="rId91" display="https://leetcode.com/problems/palindromic-substrings" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
-    <hyperlink ref="E103" r:id="rId92" display="https://leetcode.com/problems/unique-paths" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
-    <hyperlink ref="E104" r:id="rId93" display="https://leetcode.com/problems/partition-equal-subset-sum" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
-    <hyperlink ref="E105" r:id="rId94" display="https://leetcode.com/problems/target-sum" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
-    <hyperlink ref="E106" r:id="rId95" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
-    <hyperlink ref="E107" r:id="rId96" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
-    <hyperlink ref="E108" r:id="rId97" display="https://leetcode.com/problems/gas-station" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
-    <hyperlink ref="E109" r:id="rId98" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
-    <hyperlink ref="E110" r:id="rId99" display="https://leetcode.com/problems/can-place-flowers" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
-    <hyperlink ref="E111" r:id="rId100" display="https://leetcode.com/problems/jump-game" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
-    <hyperlink ref="E23" r:id="rId101" display="https://leetcode.com/problems/n-queens" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
-    <hyperlink ref="E24" r:id="rId102" display="https://leetcode.com/problems/n-queens-ii" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
-    <hyperlink ref="E25" r:id="rId103" display="https://leetcode.com/problems/subsets-ii" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
-    <hyperlink ref="E26" r:id="rId104" display="https://leetcode.com/problems/permutations-ii" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
-    <hyperlink ref="E27" r:id="rId105" display="https://leetcode.com/problems/combination-sum" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
-    <hyperlink ref="H2" r:id="rId106" display="https://leetcode.com/problems/count-and-say/" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
-    <hyperlink ref="E5" r:id="rId107" display="https://leetcode.com/problems/minimum-window-substring" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
-    <hyperlink ref="E15" r:id="rId108" display="https://leetcode.com/problems/subsets/" xr:uid="{0D3C85A9-3A8D-4ABC-A1C9-8458E66D17AA}"/>
-    <hyperlink ref="E14" r:id="rId109" display="https://leetcode.com/problems/factorial-trailing-zeroes/" xr:uid="{B4BAC095-9651-4A4F-AD5C-C25CE7ADDECA}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://leetcode.com/problems/first-unique-character-in-a-string"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://leetcode.com/problems/ransom-note"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://leetcode.com/problems/valid-anagram"/>
+    <hyperlink ref="E7" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string"/>
+    <hyperlink ref="E8" r:id="rId6" display="https://leetcode.com/problems/container-with-most-water"/>
+    <hyperlink ref="E9" r:id="rId7" display="https://leetcode.com/problems/3sum"/>
+    <hyperlink ref="E10" r:id="rId8" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array"/>
+    <hyperlink ref="E11" r:id="rId9" display="https://leetcode.com/problems/subarray-sum-equals-k"/>
+    <hyperlink ref="E12" r:id="rId10" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k"/>
+    <hyperlink ref="E13" r:id="rId11" display="https://leetcode.com/problems/maximum-subarray"/>
+    <hyperlink ref="E16" r:id="rId12" display="https://leetcode.com/problems/fibonacci-number"/>
+    <hyperlink ref="E17" r:id="rId13" display="https://leetcode.com/problems/different-ways-to-add-parentheses"/>
+    <hyperlink ref="E18" r:id="rId14" display="https://leetcode.com/problems/unique-binary-search-trees-ii"/>
+    <hyperlink ref="E19" r:id="rId15" display="https://leetcode.com/problems/powx-n"/>
+    <hyperlink ref="E22" r:id="rId16" display="https://leetcode.com/problems/generate-parentheses"/>
+    <hyperlink ref="E28" r:id="rId17" display="https://leetcode.com/problems/binary-search"/>
+    <hyperlink ref="E29" r:id="rId18" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array"/>
+    <hyperlink ref="E30" r:id="rId19" display="https://leetcode.com/problems/find-peak-element"/>
+    <hyperlink ref="E31" r:id="rId20" display="https://leetcode.com/problems/koko-eating-bananas"/>
+    <hyperlink ref="E32" r:id="rId21" display="https://leetcode.com/problems/split-array-largest-sum"/>
+    <hyperlink ref="E33" r:id="rId22" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days"/>
+    <hyperlink ref="E34" r:id="rId23" display="https://leetcode.com/problems/sort-an-array"/>
+    <hyperlink ref="E35" r:id="rId24" display="https://leetcode.com/problems/insertion-sort-list"/>
+    <hyperlink ref="E36" r:id="rId25" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
+    <hyperlink ref="E37" r:id="rId26" display="https://leetcode.com/problems/largest-number"/>
+    <hyperlink ref="E38" r:id="rId27" display="https://leetcode.com/problems/reorder-data-in-log-files"/>
+    <hyperlink ref="E39" r:id="rId28" display="https://leetcode.com/problems/merge-intervals"/>
+    <hyperlink ref="E40" r:id="rId29" display="https://leetcode.com/problems/insert-interval"/>
+    <hyperlink ref="E41" r:id="rId30" display="https://leetcode.com/problems/non-overlapping-intervals"/>
+    <hyperlink ref="E42" r:id="rId31" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
+    <hyperlink ref="E43" r:id="rId32" display="https://leetcode.com/problems/reverse-linked-list"/>
+    <hyperlink ref="E44" r:id="rId33" display="https://leetcode.com/problems/reverse-linked-list-ii"/>
+    <hyperlink ref="E45" r:id="rId34" display="https://leetcode.com/problems/linked-list-cycle"/>
+    <hyperlink ref="E46" r:id="rId35" display="https://leetcode.com/problems/linked-list-cycle-ii"/>
+    <hyperlink ref="E47" r:id="rId36" display="https://leetcode.com/problems/merge-two-sorted-lists"/>
+    <hyperlink ref="E48" r:id="rId37" display="https://leetcode.com/problems/merge-k-sorted-lists"/>
+    <hyperlink ref="E49" r:id="rId38" display="https://leetcode.com/problems/intersection-of-two-linked-lists"/>
+    <hyperlink ref="E50" r:id="rId39" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list"/>
+    <hyperlink ref="E51" r:id="rId40" display="https://leetcode.com/problems/palindrome-linked-list"/>
+    <hyperlink ref="E52" r:id="rId41" display="https://leetcode.com/problems/odd-even-linked-list"/>
+    <hyperlink ref="E53" r:id="rId42" display="https://leetcode.com/problems/lru-cache"/>
+    <hyperlink ref="E54" r:id="rId43" display="https://leetcode.com/problems/lfu-cache"/>
+    <hyperlink ref="E55" r:id="rId44" display="https://leetcode.com/problems/valid-parentheses"/>
+    <hyperlink ref="E56" r:id="rId45" display="https://leetcode.com/problems/backspace-string-compare"/>
+    <hyperlink ref="E57" r:id="rId46" display="https://leetcode.com/problems/daily-temperatures"/>
+    <hyperlink ref="E58" r:id="rId47" display="https://leetcode.com/problems/next-greater-element-i"/>
+    <hyperlink ref="E59" r:id="rId48" display="https://leetcode.com/problems/largest-rectangle-in-histogram"/>
+    <hyperlink ref="E65" r:id="rId49" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k"/>
+    <hyperlink ref="E64" r:id="rId50" display="https://leetcode.com/problems/sliding-window-maximum"/>
+    <hyperlink ref="E63" r:id="rId51" display="https://leetcode.com/problems/design-circular-deque"/>
+    <hyperlink ref="E62" r:id="rId52" display="https://leetcode.com/problems/design-circular-queue"/>
+    <hyperlink ref="E61" r:id="rId53" display="https://leetcode.com/problems/implement-queue-using-stacks"/>
+    <hyperlink ref="E60" r:id="rId54" display="https://leetcode.com/problems/number-of-recent-calls"/>
+    <hyperlink ref="E66" r:id="rId55" display="https://leetcode.com/problems/binary-tree-inorder-traversal"/>
+    <hyperlink ref="E67" r:id="rId56" display="https://leetcode.com/problems/binary-tree-level-order-traversal"/>
+    <hyperlink ref="E68" r:id="rId57" display="https://leetcode.com/problems/binary-tree-right-side-view"/>
+    <hyperlink ref="E69" r:id="rId58" display="https://leetcode.com/problems/search-in-a-binary-search-tree"/>
+    <hyperlink ref="E70" r:id="rId59" display="https://leetcode.com/problems/delete-node-in-a-bst"/>
+    <hyperlink ref="E71" r:id="rId60" display="https://leetcode.com/problems/validate-binary-search-tree"/>
+    <hyperlink ref="E72" r:id="rId61" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree"/>
+    <hyperlink ref="E75" r:id="rId62" display="https://leetcode.com/problems/last-stone-weight"/>
+    <hyperlink ref="E76" r:id="rId63" display="https://leetcode.com/problems/k-closest-points-to-origin"/>
+    <hyperlink ref="E77" r:id="rId64" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
+    <hyperlink ref="E78" r:id="rId65" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix"/>
+    <hyperlink ref="E79" r:id="rId66" display="https://leetcode.com/problems/top-k-frequent-words"/>
+    <hyperlink ref="E80" r:id="rId67" display="https://leetcode.com/problems/top-k-frequent-elements"/>
+    <hyperlink ref="E81" r:id="rId68" display="https://leetcode.com/problems/two-sum"/>
+    <hyperlink ref="E82" r:id="rId69" display="https://leetcode.com/problems/ransom-note"/>
+    <hyperlink ref="E83" r:id="rId70" display="https://leetcode.com/problems/contains-duplicate"/>
+    <hyperlink ref="E84" r:id="rId71" display="https://leetcode.com/problems/subarray-sum-equals-k"/>
+    <hyperlink ref="E85" r:id="rId72" display="https://leetcode.com/problems/subarray-sums-divisible-by-k"/>
+    <hyperlink ref="E86" r:id="rId73" display="https://leetcode.com/problems/group-anagrams"/>
+    <hyperlink ref="E87" r:id="rId74" display="https://leetcode.com/problems/longest-consecutive-sequence"/>
+    <hyperlink ref="E88" r:id="rId75" display="https://leetcode.com/problems/number-of-islands"/>
+    <hyperlink ref="E89" r:id="rId76" display="https://leetcode.com/problems/max-area-of-island"/>
+    <hyperlink ref="E90" r:id="rId77" display="https://leetcode.com/problems/01-matrix"/>
+    <hyperlink ref="E91" r:id="rId78" display="https://leetcode.com/problems/network-delay-time"/>
+    <hyperlink ref="E92" r:id="rId79" display="https://leetcode.com/problems/redundant-connection"/>
+    <hyperlink ref="E93" r:id="rId80" display="https://leetcode.com/problems/number-of-provinces"/>
+    <hyperlink ref="E94" r:id="rId81" display="https://leetcode.com/problems/course-schedule"/>
+    <hyperlink ref="E95" r:id="rId82" display="https://leetcode.com/problems/course-schedule-ii"/>
+    <hyperlink ref="E96" r:id="rId83" display="https://leetcode.com/problems/clone-graph"/>
+    <hyperlink ref="E97" r:id="rId84" display="https://leetcode.com/problems/fibonacci-number"/>
+    <hyperlink ref="E98" r:id="rId85" display="https://leetcode.com/problems/climbing-stairs"/>
+    <hyperlink ref="E99" r:id="rId86" display="https://leetcode.com/problems/min-cost-climbing-stairs"/>
+    <hyperlink ref="E100" r:id="rId87" display="https://leetcode.com/problems/longest-common-subsequence"/>
+    <hyperlink ref="E101" r:id="rId88" display="https://leetcode.com/problems/longest-increasing-subsequence"/>
+    <hyperlink ref="E102" r:id="rId89" display="https://leetcode.com/problems/palindromic-substrings"/>
+    <hyperlink ref="E103" r:id="rId90" display="https://leetcode.com/problems/unique-paths"/>
+    <hyperlink ref="E104" r:id="rId91" display="https://leetcode.com/problems/partition-equal-subset-sum"/>
+    <hyperlink ref="E105" r:id="rId92" display="https://leetcode.com/problems/target-sum"/>
+    <hyperlink ref="E106" r:id="rId93" display="https://leetcode.com/problems/non-overlapping-intervals"/>
+    <hyperlink ref="E107" r:id="rId94" display="https://leetcode.com/problems/merge-intervals"/>
+    <hyperlink ref="E108" r:id="rId95" display="https://leetcode.com/problems/gas-station"/>
+    <hyperlink ref="E109" r:id="rId96" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
+    <hyperlink ref="E110" r:id="rId97" display="https://leetcode.com/problems/can-place-flowers"/>
+    <hyperlink ref="E111" r:id="rId98" display="https://leetcode.com/problems/jump-game"/>
+    <hyperlink ref="E23" r:id="rId99" display="https://leetcode.com/problems/n-queens"/>
+    <hyperlink ref="E24" r:id="rId100" display="https://leetcode.com/problems/n-queens-ii"/>
+    <hyperlink ref="E25" r:id="rId101" display="https://leetcode.com/problems/subsets-ii"/>
+    <hyperlink ref="E26" r:id="rId102" display="https://leetcode.com/problems/permutations-ii"/>
+    <hyperlink ref="E27" r:id="rId103" display="https://leetcode.com/problems/combination-sum"/>
+    <hyperlink ref="H2" r:id="rId104" display="https://leetcode.com/problems/count-and-say/"/>
+    <hyperlink ref="E5" r:id="rId105" display="https://leetcode.com/problems/minimum-window-substring"/>
+    <hyperlink ref="E15" r:id="rId106" display="https://leetcode.com/problems/subsets/"/>
+    <hyperlink ref="E14" r:id="rId107" display="https://leetcode.com/problems/factorial-trailing-zeroes/"/>
+    <hyperlink ref="E20" r:id="rId108" display="https://leetcode.com/problems/permutations"/>
+    <hyperlink ref="E21" r:id="rId109" display="https://leetcode.com/problems/permutations-ii/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId110"/>

</xml_diff>

<commit_message>
feat(leetcode): added solutions for problems 22 and 51
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2_TIME_College\SRET\sret-focus-batch-23-27\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schedule\Documents\TIME_DK\time_colleges\SRET\Focus_Batch_2023-2027\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EEA638-977E-4CD1-8891-BE9DB63C045B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hours Alloted" sheetId="1" r:id="rId1"/>
     <sheet name="Lesson Plan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -805,8 +806,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -844,8 +845,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -855,6 +870,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -867,12 +892,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -907,16 +934,41 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -963,26 +1015,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1011,32 +1043,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:C20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:C20" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Order" dataDxfId="14"/>
-    <tableColumn id="2" name="Topic" dataDxfId="13"/>
-    <tableColumn id="3" name="Hours" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Topic" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hours" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H113"/>
-  <sortState ref="A2:G113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:H113" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G113">
     <sortCondition ref="A1:A113"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="S.No" dataDxfId="7"/>
-    <tableColumn id="2" name="Topic" dataDxfId="6"/>
-    <tableColumn id="3" name="Subtopic" dataDxfId="5"/>
-    <tableColumn id="4" name="Hour" dataDxfId="4"/>
-    <tableColumn id="5" name="LeetCode Problem" dataDxfId="3"/>
-    <tableColumn id="6" name="Level" dataDxfId="2"/>
-    <tableColumn id="7" name="Remark" dataDxfId="1"/>
-    <tableColumn id="8" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="S.No" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Topic" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Subtopic" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Hour" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="LeetCode Problem" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Level" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Remark" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1304,21 +1336,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="6"/>
-    <col min="2" max="2" width="60.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="6"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1329,7 +1361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1340,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1351,7 +1383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1362,7 +1394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1373,7 +1405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1384,7 +1416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1395,7 +1427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1406,7 +1438,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1417,7 +1449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1428,7 +1460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1439,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1450,7 +1482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1461,7 +1493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1472,7 +1504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1483,7 +1515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1494,7 +1526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1505,7 +1537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1516,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1527,7 +1559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1538,7 +1570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="6">
         <f>SUM(C2:C21)</f>
         <v>45</v>
@@ -1553,27 +1585,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.6640625" customWidth="1"/>
-    <col min="9" max="9" width="36.33203125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.7109375" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -1599,7 +1631,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1629,7 +1661,7 @@
         <v>String: Hashing + Count</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1655,7 +1687,7 @@
         <v>String: Frequency Matching</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1681,7 +1713,7 @@
         <v>String: Frequency Matching</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1709,7 +1741,7 @@
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1735,7 +1767,7 @@
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1761,7 +1793,7 @@
         <v>String: Sliding Window</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1791,7 +1823,7 @@
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1817,7 +1849,7 @@
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1843,7 +1875,7 @@
         <v>Array: Two Pointer</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1871,7 +1903,7 @@
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1897,7 +1929,7 @@
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1923,7 +1955,7 @@
         <v>Array: Prefix / Sliding</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1951,7 +1983,7 @@
         <v>Recursion: Base Case</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1977,7 +2009,7 @@
         <v>Recursion: Base Case Practice</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2003,7 +2035,7 @@
         <v>Recursion: Fibonacci</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2031,7 +2063,7 @@
         <v>Recursion: Divide and Conquer</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2057,7 +2089,7 @@
         <v>Recursion: Divide and Conquer</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2083,7 +2115,7 @@
         <v>Recursion: Binary Recursion Tree</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2111,7 +2143,7 @@
         <v>Recursion: Subsets</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2122,7 +2154,7 @@
         <v>63</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="10" t="s">
         <v>248</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -2137,7 +2169,7 @@
         <v>Recursion: Rec. with State</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2148,7 +2180,7 @@
         <v>65</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="8" t="s">
         <v>66</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -2163,7 +2195,7 @@
         <v>Recursion: Backtrack Base</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2176,13 +2208,13 @@
       <c r="D23" s="1">
         <v>8</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="8" t="s">
         <v>243</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H23" s="3"/>
@@ -2191,7 +2223,7 @@
         <v>Backtracking: N-Queens</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2208,7 +2240,7 @@
       <c r="F24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="13" t="s">
         <v>35</v>
       </c>
       <c r="H24" s="3"/>
@@ -2217,7 +2249,7 @@
         <v>Backtracking: N-Queens</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2236,7 +2268,7 @@
       <c r="F25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H25" s="3"/>
@@ -2245,7 +2277,7 @@
         <v>Backtracking: Subset Gen</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2262,7 +2294,7 @@
       <c r="F26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="13" t="s">
         <v>35</v>
       </c>
       <c r="H26" s="3"/>
@@ -2271,7 +2303,7 @@
         <v>Backtracking: Permutations</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2288,7 +2320,7 @@
       <c r="F27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="13" t="s">
         <v>35</v>
       </c>
       <c r="H27" s="3"/>
@@ -2297,7 +2329,7 @@
         <v>Backtracking: Combination Sum</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2325,7 +2357,7 @@
         <v>Searching: Binary Search Basic</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2351,7 +2383,7 @@
         <v>Searching: First/Last Occurrence</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2377,7 +2409,7 @@
         <v>Searching: Peak Element</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2405,7 +2437,7 @@
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2431,7 +2463,7 @@
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2457,7 +2489,7 @@
         <v>Searching: BS on Answer</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2485,7 +2517,7 @@
         <v>Sorting: Basic Sorting Logic</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2511,7 +2543,7 @@
         <v>Sorting: Selection Practice</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2537,7 +2569,7 @@
         <v>Sorting: QuickSort</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2565,7 +2597,7 @@
         <v>Sorting: Custom Comparator</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2591,7 +2623,7 @@
         <v>Sorting: Custom Comparator</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2619,7 +2651,7 @@
         <v>Sorting: Merge Intervals</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2645,7 +2677,7 @@
         <v>Sorting: Merge Intervals</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2673,7 +2705,7 @@
         <v>Sorting: Scheduling Logic</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2699,7 +2731,7 @@
         <v>Sorting: Sorting Based Greedy</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2727,7 +2759,7 @@
         <v>Linked List: Reverse LL</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2753,7 +2785,7 @@
         <v>Linked List: Reverse LL II</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2781,7 +2813,7 @@
         <v>Linked List: Detect Cycle</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2807,7 +2839,7 @@
         <v>Linked List: Cycle II</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2835,7 +2867,7 @@
         <v>Linked List: Merge LL</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2861,7 +2893,7 @@
         <v>Linked List: Merge k Lists</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2889,7 +2921,7 @@
         <v>Linked List: Intersection Point</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2915,7 +2947,7 @@
         <v>Linked List: Remove Nth Node</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2943,7 +2975,7 @@
         <v>Linked List: Palindrome Check</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2969,7 +3001,7 @@
         <v>Linked List: Odd Even Index</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2997,7 +3029,7 @@
         <v>Linked List: LRU Cache Logic</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3023,7 +3055,7 @@
         <v>Linked List: Advanced LRU Logic</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3051,7 +3083,7 @@
         <v>Stack: Stack Basics</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3077,7 +3109,7 @@
         <v>Stack: Stack Basics</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3105,7 +3137,7 @@
         <v>Stack: Monotonic Stack</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3131,7 +3163,7 @@
         <v>Stack: Next Greater Element</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3157,7 +3189,7 @@
         <v>Stack: Largest Rect in Hist</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3185,7 +3217,7 @@
         <v>Queue: Queue + BFS Intro</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3211,7 +3243,7 @@
         <v>Queue: Implement Queue Using Stacks</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3239,7 +3271,7 @@
         <v>Queue: Circular Queue</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3265,7 +3297,7 @@
         <v>Queue: Deque</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3293,7 +3325,7 @@
         <v>Queue: Monotonic Queue</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3319,7 +3351,7 @@
         <v>Queue: Monotonic Queue</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3347,7 +3379,7 @@
         <v>Trees: Traversals</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3373,7 +3405,7 @@
         <v>Trees: Traversals</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3399,7 +3431,7 @@
         <v>Trees: Views + Height</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3427,7 +3459,7 @@
         <v>BST: Search, Insert, Min</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3453,7 +3485,7 @@
         <v>BST: Deletion</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3481,7 +3513,7 @@
         <v>BST: Validate BST</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3507,7 +3539,7 @@
         <v>BST: Lowest Common Ancestor</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3535,7 +3567,7 @@
         <v>Balanced Tree: AVL Tree</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3561,7 +3593,7 @@
         <v>Balanced Tree: Red-Black Tree</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3589,7 +3621,7 @@
         <v>Heap: Min Heap Introduction</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3615,7 +3647,7 @@
         <v>Heap: Priority Queue Usage</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3643,7 +3675,7 @@
         <v>Heap: Kth Largest Element</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3669,7 +3701,7 @@
         <v>Heap: Kth Smallest Element</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3697,7 +3729,7 @@
         <v>Heap: Heap + Sorting Logic</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3723,7 +3755,7 @@
         <v>Heap: Heap + Custom Comparator</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3751,7 +3783,7 @@
         <v>HashMap: Frequency Counting</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3777,7 +3809,7 @@
         <v>HashMap: Frequency Counting</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3803,7 +3835,7 @@
         <v>HashSet: Uniqueness Check</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3831,7 +3863,7 @@
         <v>HashMap: Prefix Sum Technique</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3857,7 +3889,7 @@
         <v>HashMap: Prefix Sum Variation</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -3885,7 +3917,7 @@
         <v>HashMap: Grouping Data</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -3911,7 +3943,7 @@
         <v>HashMap: Longest Streak/Length</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -3939,7 +3971,7 @@
         <v>Graph: BFS Traversal</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -3965,7 +3997,7 @@
         <v>Graph: DFS Traversal</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -3991,7 +4023,7 @@
         <v>Graph: BFS with Distance</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -4019,7 +4051,7 @@
         <v>Graph: Dijkstra’s (Shortest Path)</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -4045,7 +4077,7 @@
         <v>Graph: Union Find</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -4071,7 +4103,7 @@
         <v>Graph: Cycle Detection</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -4099,7 +4131,7 @@
         <v>Graph: Topological Sort</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -4125,7 +4157,7 @@
         <v>Graph: Topo + Ordering</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -4151,7 +4183,7 @@
         <v>Graph: Kahn’s Algorithm</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4179,7 +4211,7 @@
         <v>DP: Fibonacci with Memo</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4205,7 +4237,7 @@
         <v>DP: Climbing Stairs (1D)</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4231,7 +4263,7 @@
         <v>DP: Min Cost Climbing</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4259,7 +4291,7 @@
         <v>DP: Longest Common Subseq</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4285,7 +4317,7 @@
         <v>DP: Longest Increasing Subseq</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4311,7 +4343,7 @@
         <v>DP: Palindromic Substrings</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -4339,7 +4371,7 @@
         <v>DP: Unique Paths (2D Grid)</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -4365,7 +4397,7 @@
         <v>DP: Partition Equal Sum</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -4391,7 +4423,7 @@
         <v>DP: Target Sum (state model)</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -4419,7 +4451,7 @@
         <v>Greedy: Activity Selection (Intervals)</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -4445,7 +4477,7 @@
         <v>Greedy: Interval Merging</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -4471,7 +4503,7 @@
         <v>Greedy: Gas Station Problem</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -4499,7 +4531,7 @@
         <v>Greedy: Job Scheduling / Max Profit</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -4525,7 +4557,7 @@
         <v>Greedy: Resource Assignment</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -4551,7 +4583,7 @@
         <v>Greedy: Jump Game</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -4579,7 +4611,7 @@
         <v>Review: Strategy + Topic Recap</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -4603,123 +4635,123 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G22 G28:G1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://leetcode.com/problems/first-unique-character-in-a-string"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://leetcode.com/problems/ransom-note"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://leetcode.com/problems/valid-anagram"/>
-    <hyperlink ref="E7" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string"/>
-    <hyperlink ref="E8" r:id="rId6" display="https://leetcode.com/problems/container-with-most-water"/>
-    <hyperlink ref="E9" r:id="rId7" display="https://leetcode.com/problems/3sum"/>
-    <hyperlink ref="E10" r:id="rId8" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array"/>
-    <hyperlink ref="E11" r:id="rId9" display="https://leetcode.com/problems/subarray-sum-equals-k"/>
-    <hyperlink ref="E12" r:id="rId10" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k"/>
-    <hyperlink ref="E13" r:id="rId11" display="https://leetcode.com/problems/maximum-subarray"/>
-    <hyperlink ref="E16" r:id="rId12" display="https://leetcode.com/problems/fibonacci-number"/>
-    <hyperlink ref="E17" r:id="rId13" display="https://leetcode.com/problems/different-ways-to-add-parentheses"/>
-    <hyperlink ref="E18" r:id="rId14" display="https://leetcode.com/problems/unique-binary-search-trees-ii"/>
-    <hyperlink ref="E19" r:id="rId15" display="https://leetcode.com/problems/powx-n"/>
-    <hyperlink ref="E22" r:id="rId16" display="https://leetcode.com/problems/generate-parentheses"/>
-    <hyperlink ref="E28" r:id="rId17" display="https://leetcode.com/problems/binary-search"/>
-    <hyperlink ref="E29" r:id="rId18" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array"/>
-    <hyperlink ref="E30" r:id="rId19" display="https://leetcode.com/problems/find-peak-element"/>
-    <hyperlink ref="E31" r:id="rId20" display="https://leetcode.com/problems/koko-eating-bananas"/>
-    <hyperlink ref="E32" r:id="rId21" display="https://leetcode.com/problems/split-array-largest-sum"/>
-    <hyperlink ref="E33" r:id="rId22" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days"/>
-    <hyperlink ref="E34" r:id="rId23" display="https://leetcode.com/problems/sort-an-array"/>
-    <hyperlink ref="E35" r:id="rId24" display="https://leetcode.com/problems/insertion-sort-list"/>
-    <hyperlink ref="E36" r:id="rId25" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
-    <hyperlink ref="E37" r:id="rId26" display="https://leetcode.com/problems/largest-number"/>
-    <hyperlink ref="E38" r:id="rId27" display="https://leetcode.com/problems/reorder-data-in-log-files"/>
-    <hyperlink ref="E39" r:id="rId28" display="https://leetcode.com/problems/merge-intervals"/>
-    <hyperlink ref="E40" r:id="rId29" display="https://leetcode.com/problems/insert-interval"/>
-    <hyperlink ref="E41" r:id="rId30" display="https://leetcode.com/problems/non-overlapping-intervals"/>
-    <hyperlink ref="E42" r:id="rId31" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
-    <hyperlink ref="E43" r:id="rId32" display="https://leetcode.com/problems/reverse-linked-list"/>
-    <hyperlink ref="E44" r:id="rId33" display="https://leetcode.com/problems/reverse-linked-list-ii"/>
-    <hyperlink ref="E45" r:id="rId34" display="https://leetcode.com/problems/linked-list-cycle"/>
-    <hyperlink ref="E46" r:id="rId35" display="https://leetcode.com/problems/linked-list-cycle-ii"/>
-    <hyperlink ref="E47" r:id="rId36" display="https://leetcode.com/problems/merge-two-sorted-lists"/>
-    <hyperlink ref="E48" r:id="rId37" display="https://leetcode.com/problems/merge-k-sorted-lists"/>
-    <hyperlink ref="E49" r:id="rId38" display="https://leetcode.com/problems/intersection-of-two-linked-lists"/>
-    <hyperlink ref="E50" r:id="rId39" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list"/>
-    <hyperlink ref="E51" r:id="rId40" display="https://leetcode.com/problems/palindrome-linked-list"/>
-    <hyperlink ref="E52" r:id="rId41" display="https://leetcode.com/problems/odd-even-linked-list"/>
-    <hyperlink ref="E53" r:id="rId42" display="https://leetcode.com/problems/lru-cache"/>
-    <hyperlink ref="E54" r:id="rId43" display="https://leetcode.com/problems/lfu-cache"/>
-    <hyperlink ref="E55" r:id="rId44" display="https://leetcode.com/problems/valid-parentheses"/>
-    <hyperlink ref="E56" r:id="rId45" display="https://leetcode.com/problems/backspace-string-compare"/>
-    <hyperlink ref="E57" r:id="rId46" display="https://leetcode.com/problems/daily-temperatures"/>
-    <hyperlink ref="E58" r:id="rId47" display="https://leetcode.com/problems/next-greater-element-i"/>
-    <hyperlink ref="E59" r:id="rId48" display="https://leetcode.com/problems/largest-rectangle-in-histogram"/>
-    <hyperlink ref="E65" r:id="rId49" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k"/>
-    <hyperlink ref="E64" r:id="rId50" display="https://leetcode.com/problems/sliding-window-maximum"/>
-    <hyperlink ref="E63" r:id="rId51" display="https://leetcode.com/problems/design-circular-deque"/>
-    <hyperlink ref="E62" r:id="rId52" display="https://leetcode.com/problems/design-circular-queue"/>
-    <hyperlink ref="E61" r:id="rId53" display="https://leetcode.com/problems/implement-queue-using-stacks"/>
-    <hyperlink ref="E60" r:id="rId54" display="https://leetcode.com/problems/number-of-recent-calls"/>
-    <hyperlink ref="E66" r:id="rId55" display="https://leetcode.com/problems/binary-tree-inorder-traversal"/>
-    <hyperlink ref="E67" r:id="rId56" display="https://leetcode.com/problems/binary-tree-level-order-traversal"/>
-    <hyperlink ref="E68" r:id="rId57" display="https://leetcode.com/problems/binary-tree-right-side-view"/>
-    <hyperlink ref="E69" r:id="rId58" display="https://leetcode.com/problems/search-in-a-binary-search-tree"/>
-    <hyperlink ref="E70" r:id="rId59" display="https://leetcode.com/problems/delete-node-in-a-bst"/>
-    <hyperlink ref="E71" r:id="rId60" display="https://leetcode.com/problems/validate-binary-search-tree"/>
-    <hyperlink ref="E72" r:id="rId61" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree"/>
-    <hyperlink ref="E75" r:id="rId62" display="https://leetcode.com/problems/last-stone-weight"/>
-    <hyperlink ref="E76" r:id="rId63" display="https://leetcode.com/problems/k-closest-points-to-origin"/>
-    <hyperlink ref="E77" r:id="rId64" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
-    <hyperlink ref="E78" r:id="rId65" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix"/>
-    <hyperlink ref="E79" r:id="rId66" display="https://leetcode.com/problems/top-k-frequent-words"/>
-    <hyperlink ref="E80" r:id="rId67" display="https://leetcode.com/problems/top-k-frequent-elements"/>
-    <hyperlink ref="E81" r:id="rId68" display="https://leetcode.com/problems/two-sum"/>
-    <hyperlink ref="E82" r:id="rId69" display="https://leetcode.com/problems/ransom-note"/>
-    <hyperlink ref="E83" r:id="rId70" display="https://leetcode.com/problems/contains-duplicate"/>
-    <hyperlink ref="E84" r:id="rId71" display="https://leetcode.com/problems/subarray-sum-equals-k"/>
-    <hyperlink ref="E85" r:id="rId72" display="https://leetcode.com/problems/subarray-sums-divisible-by-k"/>
-    <hyperlink ref="E86" r:id="rId73" display="https://leetcode.com/problems/group-anagrams"/>
-    <hyperlink ref="E87" r:id="rId74" display="https://leetcode.com/problems/longest-consecutive-sequence"/>
-    <hyperlink ref="E88" r:id="rId75" display="https://leetcode.com/problems/number-of-islands"/>
-    <hyperlink ref="E89" r:id="rId76" display="https://leetcode.com/problems/max-area-of-island"/>
-    <hyperlink ref="E90" r:id="rId77" display="https://leetcode.com/problems/01-matrix"/>
-    <hyperlink ref="E91" r:id="rId78" display="https://leetcode.com/problems/network-delay-time"/>
-    <hyperlink ref="E92" r:id="rId79" display="https://leetcode.com/problems/redundant-connection"/>
-    <hyperlink ref="E93" r:id="rId80" display="https://leetcode.com/problems/number-of-provinces"/>
-    <hyperlink ref="E94" r:id="rId81" display="https://leetcode.com/problems/course-schedule"/>
-    <hyperlink ref="E95" r:id="rId82" display="https://leetcode.com/problems/course-schedule-ii"/>
-    <hyperlink ref="E96" r:id="rId83" display="https://leetcode.com/problems/clone-graph"/>
-    <hyperlink ref="E97" r:id="rId84" display="https://leetcode.com/problems/fibonacci-number"/>
-    <hyperlink ref="E98" r:id="rId85" display="https://leetcode.com/problems/climbing-stairs"/>
-    <hyperlink ref="E99" r:id="rId86" display="https://leetcode.com/problems/min-cost-climbing-stairs"/>
-    <hyperlink ref="E100" r:id="rId87" display="https://leetcode.com/problems/longest-common-subsequence"/>
-    <hyperlink ref="E101" r:id="rId88" display="https://leetcode.com/problems/longest-increasing-subsequence"/>
-    <hyperlink ref="E102" r:id="rId89" display="https://leetcode.com/problems/palindromic-substrings"/>
-    <hyperlink ref="E103" r:id="rId90" display="https://leetcode.com/problems/unique-paths"/>
-    <hyperlink ref="E104" r:id="rId91" display="https://leetcode.com/problems/partition-equal-subset-sum"/>
-    <hyperlink ref="E105" r:id="rId92" display="https://leetcode.com/problems/target-sum"/>
-    <hyperlink ref="E106" r:id="rId93" display="https://leetcode.com/problems/non-overlapping-intervals"/>
-    <hyperlink ref="E107" r:id="rId94" display="https://leetcode.com/problems/merge-intervals"/>
-    <hyperlink ref="E108" r:id="rId95" display="https://leetcode.com/problems/gas-station"/>
-    <hyperlink ref="E109" r:id="rId96" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
-    <hyperlink ref="E110" r:id="rId97" display="https://leetcode.com/problems/can-place-flowers"/>
-    <hyperlink ref="E111" r:id="rId98" display="https://leetcode.com/problems/jump-game"/>
-    <hyperlink ref="E23" r:id="rId99" display="https://leetcode.com/problems/n-queens"/>
-    <hyperlink ref="E24" r:id="rId100" display="https://leetcode.com/problems/n-queens-ii"/>
-    <hyperlink ref="E25" r:id="rId101" display="https://leetcode.com/problems/subsets-ii"/>
-    <hyperlink ref="E26" r:id="rId102" display="https://leetcode.com/problems/permutations-ii"/>
-    <hyperlink ref="E27" r:id="rId103" display="https://leetcode.com/problems/combination-sum"/>
-    <hyperlink ref="H2" r:id="rId104" display="https://leetcode.com/problems/count-and-say/"/>
-    <hyperlink ref="E5" r:id="rId105" display="https://leetcode.com/problems/minimum-window-substring"/>
-    <hyperlink ref="E15" r:id="rId106" display="https://leetcode.com/problems/subsets/"/>
-    <hyperlink ref="E14" r:id="rId107" display="https://leetcode.com/problems/factorial-trailing-zeroes/"/>
-    <hyperlink ref="E20" r:id="rId108" display="https://leetcode.com/problems/permutations"/>
-    <hyperlink ref="E21" r:id="rId109" display="https://leetcode.com/problems/permutations-ii/"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://leetcode.com/problems/first-unique-character-in-a-string" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://leetcode.com/problems/ransom-note" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://leetcode.com/problems/valid-anagram" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E7" r:id="rId4" display="https://leetcode.com/problems/longest-substring-without-repeating-characters" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://leetcode.com/problems/permutation-in-string" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E8" r:id="rId6" display="https://leetcode.com/problems/container-with-most-water" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E9" r:id="rId7" display="https://leetcode.com/problems/3sum" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E10" r:id="rId8" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E11" r:id="rId9" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E12" r:id="rId10" display="https://leetcode.com/problems/maximum-size-subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E13" r:id="rId11" display="https://leetcode.com/problems/maximum-subarray" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E16" r:id="rId12" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="E17" r:id="rId13" display="https://leetcode.com/problems/different-ways-to-add-parentheses" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="E18" r:id="rId14" display="https://leetcode.com/problems/unique-binary-search-trees-ii" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="E19" r:id="rId15" display="https://leetcode.com/problems/powx-n" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="E22" r:id="rId16" display="https://leetcode.com/problems/generate-parentheses" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="E28" r:id="rId17" display="https://leetcode.com/problems/binary-search" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="E29" r:id="rId18" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="E30" r:id="rId19" display="https://leetcode.com/problems/find-peak-element" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="E31" r:id="rId20" display="https://leetcode.com/problems/koko-eating-bananas" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="E32" r:id="rId21" display="https://leetcode.com/problems/split-array-largest-sum" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="E33" r:id="rId22" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="E34" r:id="rId23" display="https://leetcode.com/problems/sort-an-array" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="E35" r:id="rId24" display="https://leetcode.com/problems/insertion-sort-list" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="E36" r:id="rId25" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="E37" r:id="rId26" display="https://leetcode.com/problems/largest-number" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="E38" r:id="rId27" display="https://leetcode.com/problems/reorder-data-in-log-files" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="E39" r:id="rId28" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="E40" r:id="rId29" display="https://leetcode.com/problems/insert-interval" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="E41" r:id="rId30" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="E42" r:id="rId31" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="E43" r:id="rId32" display="https://leetcode.com/problems/reverse-linked-list" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="E44" r:id="rId33" display="https://leetcode.com/problems/reverse-linked-list-ii" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="E45" r:id="rId34" display="https://leetcode.com/problems/linked-list-cycle" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="E46" r:id="rId35" display="https://leetcode.com/problems/linked-list-cycle-ii" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="E47" r:id="rId36" display="https://leetcode.com/problems/merge-two-sorted-lists" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="E48" r:id="rId37" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="E49" r:id="rId38" display="https://leetcode.com/problems/intersection-of-two-linked-lists" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="E50" r:id="rId39" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="E51" r:id="rId40" display="https://leetcode.com/problems/palindrome-linked-list" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="E52" r:id="rId41" display="https://leetcode.com/problems/odd-even-linked-list" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="E53" r:id="rId42" display="https://leetcode.com/problems/lru-cache" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="E54" r:id="rId43" display="https://leetcode.com/problems/lfu-cache" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="E55" r:id="rId44" display="https://leetcode.com/problems/valid-parentheses" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="E56" r:id="rId45" display="https://leetcode.com/problems/backspace-string-compare" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="E57" r:id="rId46" display="https://leetcode.com/problems/daily-temperatures" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="E58" r:id="rId47" display="https://leetcode.com/problems/next-greater-element-i" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="E59" r:id="rId48" display="https://leetcode.com/problems/largest-rectangle-in-histogram" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="E65" r:id="rId49" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="E64" r:id="rId50" display="https://leetcode.com/problems/sliding-window-maximum" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="E63" r:id="rId51" display="https://leetcode.com/problems/design-circular-deque" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="E62" r:id="rId52" display="https://leetcode.com/problems/design-circular-queue" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="E61" r:id="rId53" display="https://leetcode.com/problems/implement-queue-using-stacks" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="E60" r:id="rId54" display="https://leetcode.com/problems/number-of-recent-calls" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="E66" r:id="rId55" display="https://leetcode.com/problems/binary-tree-inorder-traversal" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="E67" r:id="rId56" display="https://leetcode.com/problems/binary-tree-level-order-traversal" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="E68" r:id="rId57" display="https://leetcode.com/problems/binary-tree-right-side-view" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="E69" r:id="rId58" display="https://leetcode.com/problems/search-in-a-binary-search-tree" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="E70" r:id="rId59" display="https://leetcode.com/problems/delete-node-in-a-bst" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="E71" r:id="rId60" display="https://leetcode.com/problems/validate-binary-search-tree" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="E72" r:id="rId61" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="E75" r:id="rId62" display="https://leetcode.com/problems/last-stone-weight" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="E76" r:id="rId63" display="https://leetcode.com/problems/k-closest-points-to-origin" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="E77" r:id="rId64" display="https://leetcode.com/problems/kth-largest-element-in-an-array" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="E78" r:id="rId65" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="E79" r:id="rId66" display="https://leetcode.com/problems/top-k-frequent-words" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="E80" r:id="rId67" display="https://leetcode.com/problems/top-k-frequent-elements" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="E81" r:id="rId68" display="https://leetcode.com/problems/two-sum" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="E82" r:id="rId69" display="https://leetcode.com/problems/ransom-note" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="E83" r:id="rId70" display="https://leetcode.com/problems/contains-duplicate" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="E84" r:id="rId71" display="https://leetcode.com/problems/subarray-sum-equals-k" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="E85" r:id="rId72" display="https://leetcode.com/problems/subarray-sums-divisible-by-k" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="E86" r:id="rId73" display="https://leetcode.com/problems/group-anagrams" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="E87" r:id="rId74" display="https://leetcode.com/problems/longest-consecutive-sequence" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="E88" r:id="rId75" display="https://leetcode.com/problems/number-of-islands" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="E89" r:id="rId76" display="https://leetcode.com/problems/max-area-of-island" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="E90" r:id="rId77" display="https://leetcode.com/problems/01-matrix" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="E91" r:id="rId78" display="https://leetcode.com/problems/network-delay-time" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="E92" r:id="rId79" display="https://leetcode.com/problems/redundant-connection" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="E93" r:id="rId80" display="https://leetcode.com/problems/number-of-provinces" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="E94" r:id="rId81" display="https://leetcode.com/problems/course-schedule" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="E95" r:id="rId82" display="https://leetcode.com/problems/course-schedule-ii" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="E96" r:id="rId83" display="https://leetcode.com/problems/clone-graph" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="E97" r:id="rId84" display="https://leetcode.com/problems/fibonacci-number" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="E98" r:id="rId85" display="https://leetcode.com/problems/climbing-stairs" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="E99" r:id="rId86" display="https://leetcode.com/problems/min-cost-climbing-stairs" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="E100" r:id="rId87" display="https://leetcode.com/problems/longest-common-subsequence" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="E101" r:id="rId88" display="https://leetcode.com/problems/longest-increasing-subsequence" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="E102" r:id="rId89" display="https://leetcode.com/problems/palindromic-substrings" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="E103" r:id="rId90" display="https://leetcode.com/problems/unique-paths" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="E104" r:id="rId91" display="https://leetcode.com/problems/partition-equal-subset-sum" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="E105" r:id="rId92" display="https://leetcode.com/problems/target-sum" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="E106" r:id="rId93" display="https://leetcode.com/problems/non-overlapping-intervals" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="E107" r:id="rId94" display="https://leetcode.com/problems/merge-intervals" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="E108" r:id="rId95" display="https://leetcode.com/problems/gas-station" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="E109" r:id="rId96" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="E110" r:id="rId97" display="https://leetcode.com/problems/can-place-flowers" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="E111" r:id="rId98" display="https://leetcode.com/problems/jump-game" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="E23" r:id="rId99" display="https://leetcode.com/problems/n-queens" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="E24" r:id="rId100" display="https://leetcode.com/problems/n-queens-ii" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="E25" r:id="rId101" display="https://leetcode.com/problems/subsets-ii" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="E26" r:id="rId102" display="https://leetcode.com/problems/permutations-ii" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="E27" r:id="rId103" display="https://leetcode.com/problems/combination-sum" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="H2" r:id="rId104" display="https://leetcode.com/problems/count-and-say/" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="E5" r:id="rId105" display="https://leetcode.com/problems/minimum-window-substring" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="E15" r:id="rId106" display="https://leetcode.com/problems/subsets/" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="E14" r:id="rId107" display="https://leetcode.com/problems/factorial-trailing-zeroes/" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="E20" r:id="rId108" display="https://leetcode.com/problems/permutations" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="E21" r:id="rId109" display="https://leetcode.com/problems/permutations-ii/" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId110"/>

</xml_diff>

<commit_message>
feat(leetcode):added solution for problems 4, 39 and 704
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="257">
   <si>
     <t>Order</t>
   </si>
@@ -800,6 +800,9 @@
   </si>
   <si>
     <t>Backtrack</t>
+  </si>
+  <si>
+    <t>4. Median of Two Sorted Arrays</t>
   </si>
 </sst>
 </file>
@@ -949,6 +952,26 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -994,26 +1017,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1054,20 +1057,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:H113"/>
   <sortState ref="A2:G113">
     <sortCondition ref="A1:A113"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="S.No" dataDxfId="7"/>
-    <tableColumn id="2" name="Topic" dataDxfId="6"/>
-    <tableColumn id="3" name="Subtopic" dataDxfId="5"/>
-    <tableColumn id="4" name="Hour" dataDxfId="4"/>
-    <tableColumn id="5" name="LeetCode Problem" dataDxfId="3"/>
-    <tableColumn id="6" name="Level" dataDxfId="2"/>
-    <tableColumn id="7" name="Remark" dataDxfId="1"/>
-    <tableColumn id="8" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" name="S.No" dataDxfId="9"/>
+    <tableColumn id="2" name="Topic" dataDxfId="8"/>
+    <tableColumn id="3" name="Subtopic" dataDxfId="7"/>
+    <tableColumn id="4" name="Hour" dataDxfId="6"/>
+    <tableColumn id="5" name="LeetCode Problem" dataDxfId="5"/>
+    <tableColumn id="6" name="Level" dataDxfId="4"/>
+    <tableColumn id="7" name="Remark" dataDxfId="3"/>
+    <tableColumn id="8" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1587,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2233,7 +2236,7 @@
         <v>241</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="8" t="s">
         <v>243</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -2261,7 +2264,7 @@
       <c r="D25" s="1">
         <v>9</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="8" t="s">
         <v>245</v>
       </c>
       <c r="F25" s="3" t="s">
@@ -2287,7 +2290,7 @@
         <v>246</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="8" t="s">
         <v>247</v>
       </c>
       <c r="F26" s="3" t="s">
@@ -2313,7 +2316,7 @@
         <v>248</v>
       </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="8" t="s">
         <v>249</v>
       </c>
       <c r="F27" s="3" t="s">
@@ -2341,8 +2344,8 @@
       <c r="D28" s="1">
         <v>10</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>68</v>
+      <c r="E28" s="11" t="s">
+        <v>256</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>31</v>
@@ -2350,7 +2353,9 @@
       <c r="G28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H28" s="3"/>
+      <c r="H28" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="I28" t="str">
         <f>Table2[[#This Row],[Topic]] &amp; ": " &amp; Table2[[#This Row],[Subtopic]]</f>
         <v>Searching: Binary Search Basic</v>
@@ -4634,10 +4639,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G22 G28:G1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4658,104 +4663,105 @@
     <hyperlink ref="E18" r:id="rId14" display="https://leetcode.com/problems/unique-binary-search-trees-ii"/>
     <hyperlink ref="E19" r:id="rId15" display="https://leetcode.com/problems/powx-n"/>
     <hyperlink ref="E22" r:id="rId16" display="https://leetcode.com/problems/generate-parentheses"/>
-    <hyperlink ref="E28" r:id="rId17" display="https://leetcode.com/problems/binary-search"/>
-    <hyperlink ref="E29" r:id="rId18" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array"/>
-    <hyperlink ref="E30" r:id="rId19" display="https://leetcode.com/problems/find-peak-element"/>
-    <hyperlink ref="E31" r:id="rId20" display="https://leetcode.com/problems/koko-eating-bananas"/>
-    <hyperlink ref="E32" r:id="rId21" display="https://leetcode.com/problems/split-array-largest-sum"/>
-    <hyperlink ref="E33" r:id="rId22" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days"/>
-    <hyperlink ref="E34" r:id="rId23" display="https://leetcode.com/problems/sort-an-array"/>
-    <hyperlink ref="E35" r:id="rId24" display="https://leetcode.com/problems/insertion-sort-list"/>
-    <hyperlink ref="E36" r:id="rId25" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
-    <hyperlink ref="E37" r:id="rId26" display="https://leetcode.com/problems/largest-number"/>
-    <hyperlink ref="E38" r:id="rId27" display="https://leetcode.com/problems/reorder-data-in-log-files"/>
-    <hyperlink ref="E39" r:id="rId28" display="https://leetcode.com/problems/merge-intervals"/>
-    <hyperlink ref="E40" r:id="rId29" display="https://leetcode.com/problems/insert-interval"/>
-    <hyperlink ref="E41" r:id="rId30" display="https://leetcode.com/problems/non-overlapping-intervals"/>
-    <hyperlink ref="E42" r:id="rId31" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
-    <hyperlink ref="E43" r:id="rId32" display="https://leetcode.com/problems/reverse-linked-list"/>
-    <hyperlink ref="E44" r:id="rId33" display="https://leetcode.com/problems/reverse-linked-list-ii"/>
-    <hyperlink ref="E45" r:id="rId34" display="https://leetcode.com/problems/linked-list-cycle"/>
-    <hyperlink ref="E46" r:id="rId35" display="https://leetcode.com/problems/linked-list-cycle-ii"/>
-    <hyperlink ref="E47" r:id="rId36" display="https://leetcode.com/problems/merge-two-sorted-lists"/>
-    <hyperlink ref="E48" r:id="rId37" display="https://leetcode.com/problems/merge-k-sorted-lists"/>
-    <hyperlink ref="E49" r:id="rId38" display="https://leetcode.com/problems/intersection-of-two-linked-lists"/>
-    <hyperlink ref="E50" r:id="rId39" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list"/>
-    <hyperlink ref="E51" r:id="rId40" display="https://leetcode.com/problems/palindrome-linked-list"/>
-    <hyperlink ref="E52" r:id="rId41" display="https://leetcode.com/problems/odd-even-linked-list"/>
-    <hyperlink ref="E53" r:id="rId42" display="https://leetcode.com/problems/lru-cache"/>
-    <hyperlink ref="E54" r:id="rId43" display="https://leetcode.com/problems/lfu-cache"/>
-    <hyperlink ref="E55" r:id="rId44" display="https://leetcode.com/problems/valid-parentheses"/>
-    <hyperlink ref="E56" r:id="rId45" display="https://leetcode.com/problems/backspace-string-compare"/>
-    <hyperlink ref="E57" r:id="rId46" display="https://leetcode.com/problems/daily-temperatures"/>
-    <hyperlink ref="E58" r:id="rId47" display="https://leetcode.com/problems/next-greater-element-i"/>
-    <hyperlink ref="E59" r:id="rId48" display="https://leetcode.com/problems/largest-rectangle-in-histogram"/>
-    <hyperlink ref="E65" r:id="rId49" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k"/>
-    <hyperlink ref="E64" r:id="rId50" display="https://leetcode.com/problems/sliding-window-maximum"/>
-    <hyperlink ref="E63" r:id="rId51" display="https://leetcode.com/problems/design-circular-deque"/>
-    <hyperlink ref="E62" r:id="rId52" display="https://leetcode.com/problems/design-circular-queue"/>
-    <hyperlink ref="E61" r:id="rId53" display="https://leetcode.com/problems/implement-queue-using-stacks"/>
-    <hyperlink ref="E60" r:id="rId54" display="https://leetcode.com/problems/number-of-recent-calls"/>
-    <hyperlink ref="E66" r:id="rId55" display="https://leetcode.com/problems/binary-tree-inorder-traversal"/>
-    <hyperlink ref="E67" r:id="rId56" display="https://leetcode.com/problems/binary-tree-level-order-traversal"/>
-    <hyperlink ref="E68" r:id="rId57" display="https://leetcode.com/problems/binary-tree-right-side-view"/>
-    <hyperlink ref="E69" r:id="rId58" display="https://leetcode.com/problems/search-in-a-binary-search-tree"/>
-    <hyperlink ref="E70" r:id="rId59" display="https://leetcode.com/problems/delete-node-in-a-bst"/>
-    <hyperlink ref="E71" r:id="rId60" display="https://leetcode.com/problems/validate-binary-search-tree"/>
-    <hyperlink ref="E72" r:id="rId61" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree"/>
-    <hyperlink ref="E75" r:id="rId62" display="https://leetcode.com/problems/last-stone-weight"/>
-    <hyperlink ref="E76" r:id="rId63" display="https://leetcode.com/problems/k-closest-points-to-origin"/>
-    <hyperlink ref="E77" r:id="rId64" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
-    <hyperlink ref="E78" r:id="rId65" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix"/>
-    <hyperlink ref="E79" r:id="rId66" display="https://leetcode.com/problems/top-k-frequent-words"/>
-    <hyperlink ref="E80" r:id="rId67" display="https://leetcode.com/problems/top-k-frequent-elements"/>
-    <hyperlink ref="E81" r:id="rId68" display="https://leetcode.com/problems/two-sum"/>
-    <hyperlink ref="E82" r:id="rId69" display="https://leetcode.com/problems/ransom-note"/>
-    <hyperlink ref="E83" r:id="rId70" display="https://leetcode.com/problems/contains-duplicate"/>
-    <hyperlink ref="E84" r:id="rId71" display="https://leetcode.com/problems/subarray-sum-equals-k"/>
-    <hyperlink ref="E85" r:id="rId72" display="https://leetcode.com/problems/subarray-sums-divisible-by-k"/>
-    <hyperlink ref="E86" r:id="rId73" display="https://leetcode.com/problems/group-anagrams"/>
-    <hyperlink ref="E87" r:id="rId74" display="https://leetcode.com/problems/longest-consecutive-sequence"/>
-    <hyperlink ref="E88" r:id="rId75" display="https://leetcode.com/problems/number-of-islands"/>
-    <hyperlink ref="E89" r:id="rId76" display="https://leetcode.com/problems/max-area-of-island"/>
-    <hyperlink ref="E90" r:id="rId77" display="https://leetcode.com/problems/01-matrix"/>
-    <hyperlink ref="E91" r:id="rId78" display="https://leetcode.com/problems/network-delay-time"/>
-    <hyperlink ref="E92" r:id="rId79" display="https://leetcode.com/problems/redundant-connection"/>
-    <hyperlink ref="E93" r:id="rId80" display="https://leetcode.com/problems/number-of-provinces"/>
-    <hyperlink ref="E94" r:id="rId81" display="https://leetcode.com/problems/course-schedule"/>
-    <hyperlink ref="E95" r:id="rId82" display="https://leetcode.com/problems/course-schedule-ii"/>
-    <hyperlink ref="E96" r:id="rId83" display="https://leetcode.com/problems/clone-graph"/>
-    <hyperlink ref="E97" r:id="rId84" display="https://leetcode.com/problems/fibonacci-number"/>
-    <hyperlink ref="E98" r:id="rId85" display="https://leetcode.com/problems/climbing-stairs"/>
-    <hyperlink ref="E99" r:id="rId86" display="https://leetcode.com/problems/min-cost-climbing-stairs"/>
-    <hyperlink ref="E100" r:id="rId87" display="https://leetcode.com/problems/longest-common-subsequence"/>
-    <hyperlink ref="E101" r:id="rId88" display="https://leetcode.com/problems/longest-increasing-subsequence"/>
-    <hyperlink ref="E102" r:id="rId89" display="https://leetcode.com/problems/palindromic-substrings"/>
-    <hyperlink ref="E103" r:id="rId90" display="https://leetcode.com/problems/unique-paths"/>
-    <hyperlink ref="E104" r:id="rId91" display="https://leetcode.com/problems/partition-equal-subset-sum"/>
-    <hyperlink ref="E105" r:id="rId92" display="https://leetcode.com/problems/target-sum"/>
-    <hyperlink ref="E106" r:id="rId93" display="https://leetcode.com/problems/non-overlapping-intervals"/>
-    <hyperlink ref="E107" r:id="rId94" display="https://leetcode.com/problems/merge-intervals"/>
-    <hyperlink ref="E108" r:id="rId95" display="https://leetcode.com/problems/gas-station"/>
-    <hyperlink ref="E109" r:id="rId96" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
-    <hyperlink ref="E110" r:id="rId97" display="https://leetcode.com/problems/can-place-flowers"/>
-    <hyperlink ref="E111" r:id="rId98" display="https://leetcode.com/problems/jump-game"/>
-    <hyperlink ref="E23" r:id="rId99" display="https://leetcode.com/problems/n-queens"/>
-    <hyperlink ref="E24" r:id="rId100" display="https://leetcode.com/problems/n-queens-ii"/>
-    <hyperlink ref="E25" r:id="rId101" display="https://leetcode.com/problems/subsets-ii"/>
-    <hyperlink ref="E26" r:id="rId102" display="https://leetcode.com/problems/permutations-ii"/>
-    <hyperlink ref="E27" r:id="rId103" display="https://leetcode.com/problems/combination-sum"/>
-    <hyperlink ref="H2" r:id="rId104" display="https://leetcode.com/problems/count-and-say/"/>
-    <hyperlink ref="E5" r:id="rId105" display="https://leetcode.com/problems/minimum-window-substring"/>
-    <hyperlink ref="E15" r:id="rId106" display="https://leetcode.com/problems/subsets/"/>
-    <hyperlink ref="E14" r:id="rId107" display="https://leetcode.com/problems/factorial-trailing-zeroes/"/>
-    <hyperlink ref="E20" r:id="rId108" display="https://leetcode.com/problems/permutations"/>
-    <hyperlink ref="E21" r:id="rId109" display="https://leetcode.com/problems/permutations-ii/"/>
+    <hyperlink ref="E29" r:id="rId17" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array"/>
+    <hyperlink ref="E30" r:id="rId18" display="https://leetcode.com/problems/find-peak-element"/>
+    <hyperlink ref="E31" r:id="rId19" display="https://leetcode.com/problems/koko-eating-bananas"/>
+    <hyperlink ref="E32" r:id="rId20" display="https://leetcode.com/problems/split-array-largest-sum"/>
+    <hyperlink ref="E33" r:id="rId21" display="https://leetcode.com/problems/capacity-to-ship-packages-within-d-days"/>
+    <hyperlink ref="E34" r:id="rId22" display="https://leetcode.com/problems/sort-an-array"/>
+    <hyperlink ref="E35" r:id="rId23" display="https://leetcode.com/problems/insertion-sort-list"/>
+    <hyperlink ref="E36" r:id="rId24" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
+    <hyperlink ref="E37" r:id="rId25" display="https://leetcode.com/problems/largest-number"/>
+    <hyperlink ref="E38" r:id="rId26" display="https://leetcode.com/problems/reorder-data-in-log-files"/>
+    <hyperlink ref="E39" r:id="rId27" display="https://leetcode.com/problems/merge-intervals"/>
+    <hyperlink ref="E40" r:id="rId28" display="https://leetcode.com/problems/insert-interval"/>
+    <hyperlink ref="E41" r:id="rId29" display="https://leetcode.com/problems/non-overlapping-intervals"/>
+    <hyperlink ref="E42" r:id="rId30" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
+    <hyperlink ref="E43" r:id="rId31" display="https://leetcode.com/problems/reverse-linked-list"/>
+    <hyperlink ref="E44" r:id="rId32" display="https://leetcode.com/problems/reverse-linked-list-ii"/>
+    <hyperlink ref="E45" r:id="rId33" display="https://leetcode.com/problems/linked-list-cycle"/>
+    <hyperlink ref="E46" r:id="rId34" display="https://leetcode.com/problems/linked-list-cycle-ii"/>
+    <hyperlink ref="E47" r:id="rId35" display="https://leetcode.com/problems/merge-two-sorted-lists"/>
+    <hyperlink ref="E48" r:id="rId36" display="https://leetcode.com/problems/merge-k-sorted-lists"/>
+    <hyperlink ref="E49" r:id="rId37" display="https://leetcode.com/problems/intersection-of-two-linked-lists"/>
+    <hyperlink ref="E50" r:id="rId38" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list"/>
+    <hyperlink ref="E51" r:id="rId39" display="https://leetcode.com/problems/palindrome-linked-list"/>
+    <hyperlink ref="E52" r:id="rId40" display="https://leetcode.com/problems/odd-even-linked-list"/>
+    <hyperlink ref="E53" r:id="rId41" display="https://leetcode.com/problems/lru-cache"/>
+    <hyperlink ref="E54" r:id="rId42" display="https://leetcode.com/problems/lfu-cache"/>
+    <hyperlink ref="E55" r:id="rId43" display="https://leetcode.com/problems/valid-parentheses"/>
+    <hyperlink ref="E56" r:id="rId44" display="https://leetcode.com/problems/backspace-string-compare"/>
+    <hyperlink ref="E57" r:id="rId45" display="https://leetcode.com/problems/daily-temperatures"/>
+    <hyperlink ref="E58" r:id="rId46" display="https://leetcode.com/problems/next-greater-element-i"/>
+    <hyperlink ref="E59" r:id="rId47" display="https://leetcode.com/problems/largest-rectangle-in-histogram"/>
+    <hyperlink ref="E65" r:id="rId48" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k"/>
+    <hyperlink ref="E64" r:id="rId49" display="https://leetcode.com/problems/sliding-window-maximum"/>
+    <hyperlink ref="E63" r:id="rId50" display="https://leetcode.com/problems/design-circular-deque"/>
+    <hyperlink ref="E62" r:id="rId51" display="https://leetcode.com/problems/design-circular-queue"/>
+    <hyperlink ref="E61" r:id="rId52" display="https://leetcode.com/problems/implement-queue-using-stacks"/>
+    <hyperlink ref="E60" r:id="rId53" display="https://leetcode.com/problems/number-of-recent-calls"/>
+    <hyperlink ref="E66" r:id="rId54" display="https://leetcode.com/problems/binary-tree-inorder-traversal"/>
+    <hyperlink ref="E67" r:id="rId55" display="https://leetcode.com/problems/binary-tree-level-order-traversal"/>
+    <hyperlink ref="E68" r:id="rId56" display="https://leetcode.com/problems/binary-tree-right-side-view"/>
+    <hyperlink ref="E69" r:id="rId57" display="https://leetcode.com/problems/search-in-a-binary-search-tree"/>
+    <hyperlink ref="E70" r:id="rId58" display="https://leetcode.com/problems/delete-node-in-a-bst"/>
+    <hyperlink ref="E71" r:id="rId59" display="https://leetcode.com/problems/validate-binary-search-tree"/>
+    <hyperlink ref="E72" r:id="rId60" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree"/>
+    <hyperlink ref="E75" r:id="rId61" display="https://leetcode.com/problems/last-stone-weight"/>
+    <hyperlink ref="E76" r:id="rId62" display="https://leetcode.com/problems/k-closest-points-to-origin"/>
+    <hyperlink ref="E77" r:id="rId63" display="https://leetcode.com/problems/kth-largest-element-in-an-array"/>
+    <hyperlink ref="E78" r:id="rId64" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix"/>
+    <hyperlink ref="E79" r:id="rId65" display="https://leetcode.com/problems/top-k-frequent-words"/>
+    <hyperlink ref="E80" r:id="rId66" display="https://leetcode.com/problems/top-k-frequent-elements"/>
+    <hyperlink ref="E81" r:id="rId67" display="https://leetcode.com/problems/two-sum"/>
+    <hyperlink ref="E82" r:id="rId68" display="https://leetcode.com/problems/ransom-note"/>
+    <hyperlink ref="E83" r:id="rId69" display="https://leetcode.com/problems/contains-duplicate"/>
+    <hyperlink ref="E84" r:id="rId70" display="https://leetcode.com/problems/subarray-sum-equals-k"/>
+    <hyperlink ref="E85" r:id="rId71" display="https://leetcode.com/problems/subarray-sums-divisible-by-k"/>
+    <hyperlink ref="E86" r:id="rId72" display="https://leetcode.com/problems/group-anagrams"/>
+    <hyperlink ref="E87" r:id="rId73" display="https://leetcode.com/problems/longest-consecutive-sequence"/>
+    <hyperlink ref="E88" r:id="rId74" display="https://leetcode.com/problems/number-of-islands"/>
+    <hyperlink ref="E89" r:id="rId75" display="https://leetcode.com/problems/max-area-of-island"/>
+    <hyperlink ref="E90" r:id="rId76" display="https://leetcode.com/problems/01-matrix"/>
+    <hyperlink ref="E91" r:id="rId77" display="https://leetcode.com/problems/network-delay-time"/>
+    <hyperlink ref="E92" r:id="rId78" display="https://leetcode.com/problems/redundant-connection"/>
+    <hyperlink ref="E93" r:id="rId79" display="https://leetcode.com/problems/number-of-provinces"/>
+    <hyperlink ref="E94" r:id="rId80" display="https://leetcode.com/problems/course-schedule"/>
+    <hyperlink ref="E95" r:id="rId81" display="https://leetcode.com/problems/course-schedule-ii"/>
+    <hyperlink ref="E96" r:id="rId82" display="https://leetcode.com/problems/clone-graph"/>
+    <hyperlink ref="E97" r:id="rId83" display="https://leetcode.com/problems/fibonacci-number"/>
+    <hyperlink ref="E98" r:id="rId84" display="https://leetcode.com/problems/climbing-stairs"/>
+    <hyperlink ref="E99" r:id="rId85" display="https://leetcode.com/problems/min-cost-climbing-stairs"/>
+    <hyperlink ref="E100" r:id="rId86" display="https://leetcode.com/problems/longest-common-subsequence"/>
+    <hyperlink ref="E101" r:id="rId87" display="https://leetcode.com/problems/longest-increasing-subsequence"/>
+    <hyperlink ref="E102" r:id="rId88" display="https://leetcode.com/problems/palindromic-substrings"/>
+    <hyperlink ref="E103" r:id="rId89" display="https://leetcode.com/problems/unique-paths"/>
+    <hyperlink ref="E104" r:id="rId90" display="https://leetcode.com/problems/partition-equal-subset-sum"/>
+    <hyperlink ref="E105" r:id="rId91" display="https://leetcode.com/problems/target-sum"/>
+    <hyperlink ref="E106" r:id="rId92" display="https://leetcode.com/problems/non-overlapping-intervals"/>
+    <hyperlink ref="E107" r:id="rId93" display="https://leetcode.com/problems/merge-intervals"/>
+    <hyperlink ref="E108" r:id="rId94" display="https://leetcode.com/problems/gas-station"/>
+    <hyperlink ref="E109" r:id="rId95" display="https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons"/>
+    <hyperlink ref="E110" r:id="rId96" display="https://leetcode.com/problems/can-place-flowers"/>
+    <hyperlink ref="E111" r:id="rId97" display="https://leetcode.com/problems/jump-game"/>
+    <hyperlink ref="E23" r:id="rId98" display="https://leetcode.com/problems/n-queens"/>
+    <hyperlink ref="E24" r:id="rId99" display="https://leetcode.com/problems/n-queens-ii"/>
+    <hyperlink ref="E25" r:id="rId100" display="https://leetcode.com/problems/subsets-ii"/>
+    <hyperlink ref="E26" r:id="rId101" display="https://leetcode.com/problems/permutations-ii"/>
+    <hyperlink ref="E27" r:id="rId102" display="https://leetcode.com/problems/combination-sum"/>
+    <hyperlink ref="H2" r:id="rId103" display="https://leetcode.com/problems/count-and-say/"/>
+    <hyperlink ref="E5" r:id="rId104" display="https://leetcode.com/problems/minimum-window-substring"/>
+    <hyperlink ref="E15" r:id="rId105" display="https://leetcode.com/problems/subsets/"/>
+    <hyperlink ref="E14" r:id="rId106" display="https://leetcode.com/problems/factorial-trailing-zeroes/"/>
+    <hyperlink ref="E20" r:id="rId107" display="https://leetcode.com/problems/permutations"/>
+    <hyperlink ref="E21" r:id="rId108" display="https://leetcode.com/problems/permutations-ii/"/>
+    <hyperlink ref="E28" r:id="rId109" display="https://leetcode.com/problems/median-of-two-sorted-arrays/"/>
+    <hyperlink ref="H28" r:id="rId110" display="https://leetcode.com/problems/binary-search"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId110"/>
+  <pageSetup orientation="portrait" r:id="rId111"/>
   <tableParts count="1">
-    <tablePart r:id="rId111"/>
+    <tablePart r:id="rId112"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(leetcode): added solutions for problems 34, 875, and 162
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -952,26 +952,6 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1017,6 +997,26 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1057,20 +1057,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H113" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H113"/>
   <sortState ref="A2:G113">
     <sortCondition ref="A1:A113"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="S.No" dataDxfId="9"/>
-    <tableColumn id="2" name="Topic" dataDxfId="8"/>
-    <tableColumn id="3" name="Subtopic" dataDxfId="7"/>
-    <tableColumn id="4" name="Hour" dataDxfId="6"/>
-    <tableColumn id="5" name="LeetCode Problem" dataDxfId="5"/>
-    <tableColumn id="6" name="Level" dataDxfId="4"/>
-    <tableColumn id="7" name="Remark" dataDxfId="3"/>
-    <tableColumn id="8" name="Notes" dataDxfId="2"/>
+    <tableColumn id="1" name="S.No" dataDxfId="7"/>
+    <tableColumn id="2" name="Topic" dataDxfId="6"/>
+    <tableColumn id="3" name="Subtopic" dataDxfId="5"/>
+    <tableColumn id="4" name="Hour" dataDxfId="4"/>
+    <tableColumn id="5" name="LeetCode Problem" dataDxfId="3"/>
+    <tableColumn id="6" name="Level" dataDxfId="2"/>
+    <tableColumn id="7" name="Remark" dataDxfId="1"/>
+    <tableColumn id="8" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1591,7 +1591,7 @@
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2348,7 +2348,7 @@
         <v>256</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>32</v>
@@ -2372,7 +2372,7 @@
         <v>69</v>
       </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F29" s="3" t="s">
@@ -2398,7 +2398,7 @@
         <v>71</v>
       </c>
       <c r="D30" s="1"/>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F30" s="3" t="s">
@@ -2426,7 +2426,7 @@
       <c r="D31" s="1">
         <v>11</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="8" t="s">
         <v>74</v>
       </c>
       <c r="F31" s="3" t="s">
@@ -4639,10 +4639,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G22 G28:G1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
docs(leetcode): 206, 452 added
</commit_message>
<xml_diff>
--- a/Lesson Plan.xlsx
+++ b/Lesson Plan.xlsx
@@ -132,7 +132,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>387. First Unique Character in a String</t>
@@ -148,7 +148,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>38. Count and Say</t>
@@ -164,7 +164,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>383. Ransom Note</t>
@@ -180,7 +180,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>242. Valid Anagram</t>
@@ -193,7 +193,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>76. Minimum Window Substring</t>
@@ -209,7 +209,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>567. Permutation in String</t>
@@ -222,7 +222,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>3. Longest Substring Without Repeating Characters</t>
@@ -238,7 +238,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>11. Container With Most Water</t>
@@ -261,7 +261,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>15. 3Sum</t>
@@ -271,7 +271,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>26. Remove Duplicates from Sorted Array</t>
@@ -284,7 +284,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>560. Subarray Sum Equals K</t>
@@ -297,7 +297,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>325. Maximum Size Subarray Sum Equals k</t>
@@ -307,7 +307,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>53. Maximum Subarray</t>
@@ -323,7 +323,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>172. Factorial Trailing Zeroes</t>
@@ -339,7 +339,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>78. Subsets</t>
@@ -355,7 +355,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>509. Fibonacci Number</t>
@@ -371,7 +371,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>241. Different Ways to Add Parentheses</t>
@@ -384,7 +384,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>95. Unique Binary Search Trees II</t>
@@ -397,7 +397,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>50. Pow(x, n)</t>
@@ -413,7 +413,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>46. Permutations</t>
@@ -429,7 +429,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>47. Permutations II</t>
@@ -445,7 +445,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>22. Generate Parentheses</t>
@@ -464,7 +464,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>51. N-Queens</t>
@@ -477,7 +477,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>52. N-Queens II</t>
@@ -490,7 +490,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>90. Subsets II</t>
@@ -512,7 +512,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>39. Combination Sum</t>
@@ -531,7 +531,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>4. Median of Two Sorted Arrays</t>
@@ -557,7 +557,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>34. Find First and Last Position</t>
@@ -573,7 +573,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>162. Find Peak Element</t>
@@ -589,7 +589,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="18"/>
+        <color indexed="16"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>875. Koko Eating Bananas</t>
@@ -1953,12 +1953,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="18"/>
+      <color indexed="16"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="17"/>
+      <color indexed="18"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1973,7 +1973,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1988,25 +1988,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="19"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="16"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -2019,6 +2019,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="21"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -2217,55 +2223,49 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2277,16 +2277,16 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2295,40 +2295,40 @@
     <xf numFmtId="49" fontId="4" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2337,25 +2337,25 @@
     <xf numFmtId="49" fontId="4" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2364,26 +2364,32 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="ff006100"/>
@@ -2392,17 +2398,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="13"/>
           <bgColor indexed="14"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="ff9c0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="13"/>
-          <bgColor indexed="16"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2426,12 +2421,13 @@
       <rgbColor rgb="00000000"/>
       <rgbColor rgb="ffc6efce"/>
       <rgbColor rgb="ff006100"/>
-      <rgbColor rgb="ffffc7ce"/>
-      <rgbColor rgb="ff9c0006"/>
       <rgbColor rgb="ff9c6500"/>
       <rgbColor rgb="ffffeb9c"/>
+      <rgbColor rgb="ff9c0006"/>
+      <rgbColor rgb="ffffc7ce"/>
       <rgbColor rgb="ff0563c1"/>
       <rgbColor rgb="fffbeba5"/>
+      <rgbColor rgb="fff8ebad"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2630,17 +2626,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2667,10 +2663,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2909,12 +2905,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -3191,7 +3187,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -3218,10 +3214,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3738,15 +3734,15 @@
     </row>
     <row r="21" ht="14.05" customHeight="1">
       <c r="A21" s="17"/>
-      <c r="B21" s="18"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" s="19"/>
+      <c r="A22" s="5"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="20" cm="1">
+      <c r="C22" s="18" cm="1">
         <f t="array" ref="C22">SUM(C2:C21)</f>
         <v>45</v>
       </c>
@@ -3770,99 +3766,99 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.67188" style="21" customWidth="1"/>
-    <col min="2" max="2" width="15.3516" style="21" customWidth="1"/>
-    <col min="3" max="3" width="30.6719" style="21" customWidth="1"/>
-    <col min="4" max="4" width="9.85156" style="21" customWidth="1"/>
-    <col min="5" max="5" width="50.6719" style="21" customWidth="1"/>
-    <col min="6" max="6" width="10.3516" style="21" customWidth="1"/>
-    <col min="7" max="7" width="12.3516" style="21" customWidth="1"/>
-    <col min="8" max="8" width="50.6719" style="21" customWidth="1"/>
-    <col min="9" max="9" hidden="1" width="9" style="21" customWidth="1"/>
-    <col min="10" max="10" width="9" style="21" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="21" customWidth="1"/>
+    <col min="1" max="1" width="9.67188" style="19" customWidth="1"/>
+    <col min="2" max="2" width="15.3516" style="19" customWidth="1"/>
+    <col min="3" max="3" width="30.6719" style="19" customWidth="1"/>
+    <col min="4" max="4" width="9.85156" style="19" customWidth="1"/>
+    <col min="5" max="5" width="50.6719" style="19" customWidth="1"/>
+    <col min="6" max="6" width="10.3516" style="19" customWidth="1"/>
+    <col min="7" max="7" width="12.3516" style="19" customWidth="1"/>
+    <col min="8" max="8" width="50.6719" style="19" customWidth="1"/>
+    <col min="9" max="9" hidden="1" width="9" style="19" customWidth="1"/>
+    <col min="10" max="10" width="9" style="19" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
-      <c r="A1" t="s" s="22">
+      <c r="A1" t="s" s="20">
         <v>22</v>
       </c>
-      <c r="B1" t="s" s="23">
+      <c r="B1" t="s" s="21">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="23">
+      <c r="C1" t="s" s="21">
         <v>23</v>
       </c>
-      <c r="D1" t="s" s="23">
+      <c r="D1" t="s" s="21">
         <v>24</v>
       </c>
-      <c r="E1" t="s" s="23">
+      <c r="E1" t="s" s="21">
         <v>25</v>
       </c>
-      <c r="F1" t="s" s="23">
+      <c r="F1" t="s" s="21">
         <v>26</v>
       </c>
-      <c r="G1" t="s" s="23">
+      <c r="G1" t="s" s="21">
         <v>27</v>
       </c>
-      <c r="H1" t="s" s="23">
+      <c r="H1" t="s" s="21">
         <v>28</v>
       </c>
-      <c r="I1" s="24"/>
+      <c r="I1" s="22"/>
       <c r="J1" s="4"/>
     </row>
     <row r="2" ht="30" customHeight="1">
-      <c r="A2" s="25">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="26">
+      <c r="B2" t="s" s="24">
         <v>29</v>
       </c>
-      <c r="C2" t="s" s="26">
+      <c r="C2" t="s" s="24">
         <v>30</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="25">
         <v>1</v>
       </c>
-      <c r="E2" t="s" s="28">
+      <c r="E2" t="s" s="26">
         <v>31</v>
       </c>
-      <c r="F2" t="s" s="26">
+      <c r="F2" t="s" s="24">
         <v>32</v>
       </c>
-      <c r="G2" t="s" s="26">
+      <c r="G2" t="s" s="24">
         <v>33</v>
       </c>
-      <c r="H2" t="s" s="29">
+      <c r="H2" t="s" s="27">
         <v>34</v>
       </c>
-      <c r="I2" t="str" s="24" cm="1">
+      <c r="I2" t="str" s="22" cm="1">
         <f t="array" ref="I2">B2:B2&amp;": "&amp;C2:C2</f>
         <v>String: Hashing + Count</v>
       </c>
       <c r="J2" s="4"/>
     </row>
     <row r="3" ht="30" customHeight="1">
-      <c r="A3" s="30">
+      <c r="A3" s="28">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="31">
+      <c r="B3" t="s" s="29">
         <v>29</v>
       </c>
-      <c r="C3" t="s" s="31">
+      <c r="C3" t="s" s="29">
         <v>36</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" t="s" s="33">
+      <c r="D3" s="30"/>
+      <c r="E3" t="s" s="31">
         <v>37</v>
       </c>
-      <c r="F3" t="s" s="34">
+      <c r="F3" t="s" s="32">
         <v>32</v>
       </c>
-      <c r="G3" t="s" s="31">
+      <c r="G3" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H3" s="35"/>
+      <c r="H3" s="33"/>
       <c r="I3" t="str" s="5" cm="1">
         <f t="array" ref="I3">B3:B3&amp;": "&amp;C3:C3</f>
         <v>String: Frequency Matching</v>
@@ -3870,55 +3866,55 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" ht="30" customHeight="1">
-      <c r="A4" s="36">
+      <c r="A4" s="34">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="37">
+      <c r="B4" t="s" s="35">
         <v>29</v>
       </c>
-      <c r="C4" t="s" s="37">
+      <c r="C4" t="s" s="35">
         <v>36</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" t="s" s="33">
+      <c r="D4" s="36"/>
+      <c r="E4" t="s" s="31">
         <v>40</v>
       </c>
-      <c r="F4" t="s" s="37">
+      <c r="F4" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G4" t="s" s="37">
+      <c r="G4" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H4" s="39"/>
-      <c r="I4" t="str" s="24" cm="1">
+      <c r="H4" s="37"/>
+      <c r="I4" t="str" s="22" cm="1">
         <f t="array" ref="I4">B4:B4&amp;": "&amp;C4:C4</f>
         <v>String: Frequency Matching</v>
       </c>
       <c r="J4" s="4"/>
     </row>
     <row r="5" ht="30" customHeight="1">
-      <c r="A5" s="30">
+      <c r="A5" s="28">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="31">
+      <c r="B5" t="s" s="29">
         <v>29</v>
       </c>
-      <c r="C5" t="s" s="31">
+      <c r="C5" t="s" s="29">
         <v>41</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="38">
         <v>2</v>
       </c>
-      <c r="E5" t="s" s="33">
+      <c r="E5" t="s" s="31">
         <v>42</v>
       </c>
-      <c r="F5" t="s" s="34">
+      <c r="F5" t="s" s="32">
         <v>43</v>
       </c>
-      <c r="G5" t="s" s="31">
+      <c r="G5" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H5" s="35"/>
+      <c r="H5" s="33"/>
       <c r="I5" t="str" s="5" cm="1">
         <f t="array" ref="I5">B5:B5&amp;": "&amp;C5:C5</f>
         <v>String: Sliding Window</v>
@@ -3926,53 +3922,53 @@
       <c r="J5" s="5"/>
     </row>
     <row r="6" ht="30" customHeight="1">
-      <c r="A6" s="36">
+      <c r="A6" s="34">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="37">
+      <c r="B6" t="s" s="35">
         <v>29</v>
       </c>
-      <c r="C6" t="s" s="37">
+      <c r="C6" t="s" s="35">
         <v>41</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" t="s" s="33">
+      <c r="D6" s="36"/>
+      <c r="E6" t="s" s="31">
         <v>45</v>
       </c>
-      <c r="F6" t="s" s="37">
+      <c r="F6" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G6" t="s" s="37">
+      <c r="G6" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" t="str" s="24" cm="1">
+      <c r="H6" s="37"/>
+      <c r="I6" t="str" s="22" cm="1">
         <f t="array" ref="I6">B6:B6&amp;": "&amp;C6:C6</f>
         <v>String: Sliding Window</v>
       </c>
       <c r="J6" s="4"/>
     </row>
     <row r="7" ht="30" customHeight="1">
-      <c r="A7" s="30">
+      <c r="A7" s="28">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="31">
+      <c r="B7" t="s" s="29">
         <v>29</v>
       </c>
-      <c r="C7" t="s" s="31">
+      <c r="C7" t="s" s="29">
         <v>41</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" t="s" s="33">
+      <c r="D7" s="30"/>
+      <c r="E7" t="s" s="31">
         <v>47</v>
       </c>
-      <c r="F7" t="s" s="34">
+      <c r="F7" t="s" s="32">
         <v>46</v>
       </c>
-      <c r="G7" t="s" s="31">
+      <c r="G7" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H7" s="35"/>
+      <c r="H7" s="33"/>
       <c r="I7" t="str" s="5" cm="1">
         <f t="array" ref="I7">B7:B7&amp;": "&amp;C7:C7</f>
         <v>String: Sliding Window</v>
@@ -3980,57 +3976,57 @@
       <c r="J7" s="5"/>
     </row>
     <row r="8" ht="135" customHeight="1">
-      <c r="A8" s="36">
+      <c r="A8" s="34">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="37">
+      <c r="B8" t="s" s="35">
         <v>48</v>
       </c>
-      <c r="C8" t="s" s="37">
+      <c r="C8" t="s" s="35">
         <v>49</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="39">
         <v>3</v>
       </c>
-      <c r="E8" t="s" s="33">
+      <c r="E8" t="s" s="31">
         <v>50</v>
       </c>
-      <c r="F8" t="s" s="37">
+      <c r="F8" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G8" t="s" s="37">
+      <c r="G8" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H8" t="s" s="33">
+      <c r="H8" t="s" s="31">
         <v>51</v>
       </c>
-      <c r="I8" t="str" s="24" cm="1">
+      <c r="I8" t="str" s="22" cm="1">
         <f t="array" ref="I8">B8:B8&amp;": "&amp;C8:C8</f>
         <v>Array: Two Pointer</v>
       </c>
       <c r="J8" s="4"/>
     </row>
     <row r="9" ht="30" customHeight="1">
-      <c r="A9" s="30">
+      <c r="A9" s="28">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="31">
+      <c r="B9" t="s" s="29">
         <v>48</v>
       </c>
-      <c r="C9" t="s" s="31">
+      <c r="C9" t="s" s="29">
         <v>49</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" t="s" s="33">
+      <c r="D9" s="30"/>
+      <c r="E9" t="s" s="31">
         <v>53</v>
       </c>
-      <c r="F9" t="s" s="34">
+      <c r="F9" t="s" s="32">
         <v>46</v>
       </c>
-      <c r="G9" t="s" s="31">
+      <c r="G9" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H9" s="35"/>
+      <c r="H9" s="33"/>
       <c r="I9" t="str" s="5" cm="1">
         <f t="array" ref="I9">B9:B9&amp;": "&amp;C9:C9</f>
         <v>Array: Two Pointer</v>
@@ -4038,55 +4034,55 @@
       <c r="J9" s="5"/>
     </row>
     <row r="10" ht="30" customHeight="1">
-      <c r="A10" s="36">
+      <c r="A10" s="34">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="37">
+      <c r="B10" t="s" s="35">
         <v>48</v>
       </c>
-      <c r="C10" t="s" s="37">
+      <c r="C10" t="s" s="35">
         <v>49</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" t="s" s="33">
+      <c r="D10" s="36"/>
+      <c r="E10" t="s" s="31">
         <v>54</v>
       </c>
-      <c r="F10" t="s" s="37">
+      <c r="F10" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G10" t="s" s="37">
+      <c r="G10" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H10" s="39"/>
-      <c r="I10" t="str" s="24" cm="1">
+      <c r="H10" s="37"/>
+      <c r="I10" t="str" s="22" cm="1">
         <f t="array" ref="I10">B10:B10&amp;": "&amp;C10:C10</f>
         <v>Array: Two Pointer</v>
       </c>
       <c r="J10" s="4"/>
     </row>
     <row r="11" ht="30" customHeight="1">
-      <c r="A11" s="30">
+      <c r="A11" s="28">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="31">
+      <c r="B11" t="s" s="29">
         <v>48</v>
       </c>
-      <c r="C11" t="s" s="31">
+      <c r="C11" t="s" s="29">
         <v>55</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="38">
         <v>4</v>
       </c>
-      <c r="E11" t="s" s="33">
+      <c r="E11" t="s" s="31">
         <v>56</v>
       </c>
-      <c r="F11" t="s" s="34">
+      <c r="F11" t="s" s="32">
         <v>46</v>
       </c>
-      <c r="G11" t="s" s="31">
+      <c r="G11" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H11" s="35"/>
+      <c r="H11" s="33"/>
       <c r="I11" t="str" s="5" cm="1">
         <f t="array" ref="I11">B11:B11&amp;": "&amp;C11:C11</f>
         <v>Array: Prefix / Sliding</v>
@@ -4094,53 +4090,53 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" ht="30" customHeight="1">
-      <c r="A12" s="36">
+      <c r="A12" s="34">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="37">
+      <c r="B12" t="s" s="35">
         <v>48</v>
       </c>
-      <c r="C12" t="s" s="37">
+      <c r="C12" t="s" s="35">
         <v>55</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" t="s" s="33">
+      <c r="D12" s="36"/>
+      <c r="E12" t="s" s="31">
         <v>58</v>
       </c>
-      <c r="F12" t="s" s="37">
+      <c r="F12" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G12" t="s" s="37">
+      <c r="G12" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" t="str" s="24" cm="1">
+      <c r="H12" s="37"/>
+      <c r="I12" t="str" s="22" cm="1">
         <f t="array" ref="I12">B12:B12&amp;": "&amp;C12:C12</f>
         <v>Array: Prefix / Sliding</v>
       </c>
       <c r="J12" s="4"/>
     </row>
     <row r="13" ht="30" customHeight="1">
-      <c r="A13" s="30">
+      <c r="A13" s="28">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="31">
+      <c r="B13" t="s" s="29">
         <v>48</v>
       </c>
-      <c r="C13" t="s" s="31">
+      <c r="C13" t="s" s="29">
         <v>55</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" t="s" s="33">
+      <c r="D13" s="30"/>
+      <c r="E13" t="s" s="31">
         <v>59</v>
       </c>
-      <c r="F13" t="s" s="34">
+      <c r="F13" t="s" s="32">
         <v>32</v>
       </c>
-      <c r="G13" t="s" s="31">
+      <c r="G13" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H13" s="35"/>
+      <c r="H13" s="33"/>
       <c r="I13" t="str" s="5" cm="1">
         <f t="array" ref="I13">B13:B13&amp;": "&amp;C13:C13</f>
         <v>Array: Prefix / Sliding</v>
@@ -4148,55 +4144,55 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" ht="30" customHeight="1">
-      <c r="A14" s="36">
+      <c r="A14" s="34">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="37">
+      <c r="B14" t="s" s="35">
         <v>60</v>
       </c>
-      <c r="C14" t="s" s="37">
+      <c r="C14" t="s" s="35">
         <v>61</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="39">
         <v>5</v>
       </c>
-      <c r="E14" t="s" s="42">
+      <c r="E14" t="s" s="40">
         <v>62</v>
       </c>
-      <c r="F14" t="s" s="37">
+      <c r="F14" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G14" t="s" s="37">
+      <c r="G14" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H14" s="39"/>
-      <c r="I14" t="str" s="24" cm="1">
+      <c r="H14" s="37"/>
+      <c r="I14" t="str" s="22" cm="1">
         <f t="array" ref="I14">B14:B14&amp;": "&amp;C14:C14</f>
         <v>Recursion: Base Case</v>
       </c>
       <c r="J14" s="4"/>
     </row>
     <row r="15" ht="30" customHeight="1">
-      <c r="A15" s="30">
+      <c r="A15" s="28">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="31">
+      <c r="B15" t="s" s="29">
         <v>60</v>
       </c>
-      <c r="C15" t="s" s="31">
+      <c r="C15" t="s" s="29">
         <v>64</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" t="s" s="42">
+      <c r="D15" s="30"/>
+      <c r="E15" t="s" s="40">
         <v>65</v>
       </c>
-      <c r="F15" t="s" s="34">
+      <c r="F15" t="s" s="32">
         <v>46</v>
       </c>
-      <c r="G15" t="s" s="31">
+      <c r="G15" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H15" s="35"/>
+      <c r="H15" s="33"/>
       <c r="I15" t="str" s="5" cm="1">
         <f t="array" ref="I15">B15:B15&amp;": "&amp;C15:C15</f>
         <v>Recursion: Base Case Practice</v>
@@ -4204,55 +4200,55 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" ht="30" customHeight="1">
-      <c r="A16" s="36">
+      <c r="A16" s="34">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="37">
+      <c r="B16" t="s" s="35">
         <v>60</v>
       </c>
-      <c r="C16" t="s" s="37">
+      <c r="C16" t="s" s="35">
         <v>67</v>
       </c>
-      <c r="D16" s="38"/>
-      <c r="E16" t="s" s="33">
+      <c r="D16" s="36"/>
+      <c r="E16" t="s" s="31">
         <v>68</v>
       </c>
-      <c r="F16" t="s" s="37">
+      <c r="F16" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G16" t="s" s="37">
+      <c r="G16" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H16" s="39"/>
-      <c r="I16" t="str" s="24" cm="1">
+      <c r="H16" s="37"/>
+      <c r="I16" t="str" s="22" cm="1">
         <f t="array" ref="I16">B16:B16&amp;": "&amp;C16:C16</f>
         <v>Recursion: Fibonacci</v>
       </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" ht="30" customHeight="1">
-      <c r="A17" s="30">
+      <c r="A17" s="28">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="31">
+      <c r="B17" t="s" s="29">
         <v>60</v>
       </c>
-      <c r="C17" t="s" s="31">
+      <c r="C17" t="s" s="29">
         <v>70</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="38">
         <v>6</v>
       </c>
-      <c r="E17" t="s" s="33">
+      <c r="E17" t="s" s="31">
         <v>71</v>
       </c>
-      <c r="F17" t="s" s="34">
+      <c r="F17" t="s" s="32">
         <v>46</v>
       </c>
-      <c r="G17" t="s" s="31">
+      <c r="G17" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H17" s="35"/>
+      <c r="H17" s="33"/>
       <c r="I17" t="str" s="5" cm="1">
         <f t="array" ref="I17">B17:B17&amp;": "&amp;C17:C17</f>
         <v>Recursion: Divide and Conquer</v>
@@ -4260,53 +4256,53 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" ht="30" customHeight="1">
-      <c r="A18" s="36">
+      <c r="A18" s="34">
         <v>17</v>
       </c>
-      <c r="B18" t="s" s="37">
+      <c r="B18" t="s" s="35">
         <v>60</v>
       </c>
-      <c r="C18" t="s" s="37">
+      <c r="C18" t="s" s="35">
         <v>70</v>
       </c>
-      <c r="D18" s="38"/>
-      <c r="E18" t="s" s="33">
+      <c r="D18" s="36"/>
+      <c r="E18" t="s" s="31">
         <v>73</v>
       </c>
-      <c r="F18" t="s" s="37">
+      <c r="F18" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G18" t="s" s="37">
+      <c r="G18" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H18" s="39"/>
-      <c r="I18" t="str" s="24" cm="1">
+      <c r="H18" s="37"/>
+      <c r="I18" t="str" s="22" cm="1">
         <f t="array" ref="I18">B18:B18&amp;": "&amp;C18:C18</f>
         <v>Recursion: Divide and Conquer</v>
       </c>
       <c r="J18" s="4"/>
     </row>
     <row r="19" ht="30" customHeight="1">
-      <c r="A19" s="30">
+      <c r="A19" s="28">
         <v>18</v>
       </c>
-      <c r="B19" t="s" s="31">
+      <c r="B19" t="s" s="29">
         <v>60</v>
       </c>
-      <c r="C19" t="s" s="31">
+      <c r="C19" t="s" s="29">
         <v>74</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" t="s" s="33">
+      <c r="D19" s="30"/>
+      <c r="E19" t="s" s="31">
         <v>75</v>
       </c>
-      <c r="F19" t="s" s="34">
+      <c r="F19" t="s" s="32">
         <v>46</v>
       </c>
-      <c r="G19" t="s" s="31">
+      <c r="G19" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H19" s="35"/>
+      <c r="H19" s="33"/>
       <c r="I19" t="str" s="5" cm="1">
         <f t="array" ref="I19">B19:B19&amp;": "&amp;C19:C19</f>
         <v>Recursion: Binary Recursion Tree</v>
@@ -4314,55 +4310,55 @@
       <c r="J19" s="5"/>
     </row>
     <row r="20" ht="30" customHeight="1">
-      <c r="A20" s="36">
+      <c r="A20" s="34">
         <v>19</v>
       </c>
-      <c r="B20" t="s" s="37">
+      <c r="B20" t="s" s="35">
         <v>60</v>
       </c>
-      <c r="C20" t="s" s="37">
+      <c r="C20" t="s" s="35">
         <v>77</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="39">
         <v>7</v>
       </c>
-      <c r="E20" t="s" s="33">
+      <c r="E20" t="s" s="31">
         <v>78</v>
       </c>
-      <c r="F20" t="s" s="37">
+      <c r="F20" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G20" t="s" s="37">
+      <c r="G20" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H20" s="39"/>
-      <c r="I20" t="str" s="24" cm="1">
+      <c r="H20" s="37"/>
+      <c r="I20" t="str" s="22" cm="1">
         <f t="array" ref="I20">B20:B20&amp;": "&amp;C20:C20</f>
         <v>Recursion: Backtrack</v>
       </c>
       <c r="J20" s="4"/>
     </row>
     <row r="21" ht="30" customHeight="1">
-      <c r="A21" s="30">
+      <c r="A21" s="28">
         <v>20</v>
       </c>
-      <c r="B21" t="s" s="31">
+      <c r="B21" t="s" s="29">
         <v>60</v>
       </c>
-      <c r="C21" t="s" s="31">
+      <c r="C21" t="s" s="29">
         <v>80</v>
       </c>
-      <c r="D21" s="32"/>
-      <c r="E21" t="s" s="43">
+      <c r="D21" s="30"/>
+      <c r="E21" t="s" s="41">
         <v>81</v>
       </c>
-      <c r="F21" t="s" s="34">
+      <c r="F21" t="s" s="32">
         <v>46</v>
       </c>
-      <c r="G21" t="s" s="31">
+      <c r="G21" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H21" s="35"/>
+      <c r="H21" s="33"/>
       <c r="I21" t="str" s="5" cm="1">
         <f t="array" ref="I21">B21:B21&amp;": "&amp;C21:C21</f>
         <v>Recursion: Rec. with State</v>
@@ -4370,55 +4366,55 @@
       <c r="J21" s="5"/>
     </row>
     <row r="22" ht="30" customHeight="1">
-      <c r="A22" s="36">
+      <c r="A22" s="34">
         <v>21</v>
       </c>
-      <c r="B22" t="s" s="37">
+      <c r="B22" t="s" s="35">
         <v>60</v>
       </c>
-      <c r="C22" t="s" s="37">
+      <c r="C22" t="s" s="35">
         <v>83</v>
       </c>
-      <c r="D22" s="38"/>
-      <c r="E22" t="s" s="33">
+      <c r="D22" s="36"/>
+      <c r="E22" t="s" s="31">
         <v>84</v>
       </c>
-      <c r="F22" t="s" s="37">
+      <c r="F22" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G22" t="s" s="37">
+      <c r="G22" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H22" s="39"/>
-      <c r="I22" t="str" s="24" cm="1">
+      <c r="H22" s="37"/>
+      <c r="I22" t="str" s="22" cm="1">
         <f t="array" ref="I22">B22:B22&amp;": "&amp;C22:C22</f>
         <v>Recursion: Backtrack Base</v>
       </c>
       <c r="J22" s="4"/>
     </row>
     <row r="23" ht="30" customHeight="1">
-      <c r="A23" s="30">
+      <c r="A23" s="28">
         <v>22</v>
       </c>
-      <c r="B23" t="s" s="31">
+      <c r="B23" t="s" s="29">
         <v>86</v>
       </c>
-      <c r="C23" t="s" s="31">
+      <c r="C23" t="s" s="29">
         <v>87</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="38">
         <v>8</v>
       </c>
-      <c r="E23" t="s" s="33">
+      <c r="E23" t="s" s="31">
         <v>88</v>
       </c>
-      <c r="F23" t="s" s="44">
+      <c r="F23" t="s" s="42">
         <v>43</v>
       </c>
-      <c r="G23" t="s" s="45">
+      <c r="G23" t="s" s="43">
         <v>33</v>
       </c>
-      <c r="H23" s="46"/>
+      <c r="H23" s="44"/>
       <c r="I23" t="str" s="5" cm="1">
         <f t="array" ref="I23">B23:B23&amp;": "&amp;C23:C23</f>
         <v>Backtracking: N-Queens</v>
@@ -4426,55 +4422,55 @@
       <c r="J23" s="5"/>
     </row>
     <row r="24" ht="30" customHeight="1">
-      <c r="A24" s="36">
+      <c r="A24" s="34">
         <v>23</v>
       </c>
-      <c r="B24" t="s" s="37">
+      <c r="B24" t="s" s="35">
         <v>86</v>
       </c>
-      <c r="C24" t="s" s="37">
+      <c r="C24" t="s" s="35">
         <v>87</v>
       </c>
-      <c r="D24" s="38"/>
-      <c r="E24" t="s" s="33">
+      <c r="D24" s="36"/>
+      <c r="E24" t="s" s="31">
         <v>90</v>
       </c>
-      <c r="F24" t="s" s="37">
+      <c r="F24" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="G24" t="s" s="47">
+      <c r="G24" t="s" s="45">
         <v>38</v>
       </c>
-      <c r="H24" s="39"/>
-      <c r="I24" t="str" s="24" cm="1">
+      <c r="H24" s="37"/>
+      <c r="I24" t="str" s="22" cm="1">
         <f t="array" ref="I24">B24:B24&amp;": "&amp;C24:C24</f>
         <v>Backtracking: N-Queens</v>
       </c>
       <c r="J24" s="4"/>
     </row>
     <row r="25" ht="30" customHeight="1">
-      <c r="A25" s="30">
+      <c r="A25" s="28">
         <v>24</v>
       </c>
-      <c r="B25" t="s" s="31">
+      <c r="B25" t="s" s="29">
         <v>86</v>
       </c>
-      <c r="C25" t="s" s="31">
+      <c r="C25" t="s" s="29">
         <v>91</v>
       </c>
-      <c r="D25" s="40">
+      <c r="D25" s="38">
         <v>9</v>
       </c>
-      <c r="E25" t="s" s="33">
+      <c r="E25" t="s" s="31">
         <v>92</v>
       </c>
-      <c r="F25" t="s" s="44">
+      <c r="F25" t="s" s="42">
         <v>46</v>
       </c>
-      <c r="G25" t="s" s="45">
+      <c r="G25" t="s" s="43">
         <v>33</v>
       </c>
-      <c r="H25" s="46"/>
+      <c r="H25" s="44"/>
       <c r="I25" t="str" s="5" cm="1">
         <f t="array" ref="I25">B25:B25&amp;": "&amp;C25:C25</f>
         <v>Backtracking: Subset Gen</v>
@@ -4482,53 +4478,53 @@
       <c r="J25" s="5"/>
     </row>
     <row r="26" ht="30" customHeight="1">
-      <c r="A26" s="36">
+      <c r="A26" s="34">
         <v>25</v>
       </c>
-      <c r="B26" t="s" s="37">
+      <c r="B26" t="s" s="35">
         <v>86</v>
       </c>
-      <c r="C26" t="s" s="37">
+      <c r="C26" t="s" s="35">
         <v>94</v>
       </c>
-      <c r="D26" s="39"/>
-      <c r="E26" t="s" s="33">
+      <c r="D26" s="37"/>
+      <c r="E26" t="s" s="31">
         <v>81</v>
       </c>
-      <c r="F26" t="s" s="37">
+      <c r="F26" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G26" t="s" s="47">
+      <c r="G26" t="s" s="45">
         <v>38</v>
       </c>
-      <c r="H26" s="39"/>
-      <c r="I26" t="str" s="24" cm="1">
+      <c r="H26" s="37"/>
+      <c r="I26" t="str" s="22" cm="1">
         <f t="array" ref="I26">B26:B26&amp;": "&amp;C26:C26</f>
         <v>Backtracking: Permutations</v>
       </c>
       <c r="J26" s="4"/>
     </row>
     <row r="27" ht="30" customHeight="1">
-      <c r="A27" s="30">
+      <c r="A27" s="28">
         <v>26</v>
       </c>
-      <c r="B27" t="s" s="31">
+      <c r="B27" t="s" s="29">
         <v>86</v>
       </c>
-      <c r="C27" t="s" s="31">
+      <c r="C27" t="s" s="29">
         <v>96</v>
       </c>
-      <c r="D27" s="48"/>
-      <c r="E27" t="s" s="33">
+      <c r="D27" s="46"/>
+      <c r="E27" t="s" s="31">
         <v>97</v>
       </c>
-      <c r="F27" t="s" s="44">
+      <c r="F27" t="s" s="42">
         <v>46</v>
       </c>
-      <c r="G27" t="s" s="47">
+      <c r="G27" t="s" s="45">
         <v>38</v>
       </c>
-      <c r="H27" s="46"/>
+      <c r="H27" s="44"/>
       <c r="I27" t="str" s="5" cm="1">
         <f t="array" ref="I27">B27:B27&amp;": "&amp;C27:C27</f>
         <v>Backtracking: Combination Sum</v>
@@ -4536,57 +4532,57 @@
       <c r="J27" s="5"/>
     </row>
     <row r="28" ht="30" customHeight="1">
-      <c r="A28" s="36">
+      <c r="A28" s="34">
         <v>27</v>
       </c>
-      <c r="B28" t="s" s="37">
+      <c r="B28" t="s" s="35">
         <v>99</v>
       </c>
-      <c r="C28" t="s" s="37">
+      <c r="C28" t="s" s="35">
         <v>100</v>
       </c>
-      <c r="D28" s="41">
+      <c r="D28" s="39">
         <v>10</v>
       </c>
-      <c r="E28" t="s" s="42">
+      <c r="E28" t="s" s="40">
         <v>101</v>
       </c>
-      <c r="F28" t="s" s="37">
+      <c r="F28" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="G28" t="s" s="37">
+      <c r="G28" t="s" s="35">
         <v>33</v>
       </c>
       <c r="H28" t="s" s="12">
         <v>102</v>
       </c>
-      <c r="I28" t="str" s="24" cm="1">
+      <c r="I28" t="str" s="22" cm="1">
         <f t="array" ref="I28">B28:B28&amp;": "&amp;C28:C28</f>
         <v>Searching: Binary Search Basic</v>
       </c>
       <c r="J28" s="4"/>
     </row>
     <row r="29" ht="30" customHeight="1">
-      <c r="A29" s="30">
+      <c r="A29" s="28">
         <v>28</v>
       </c>
-      <c r="B29" t="s" s="31">
+      <c r="B29" t="s" s="29">
         <v>99</v>
       </c>
-      <c r="C29" t="s" s="31">
+      <c r="C29" t="s" s="29">
         <v>104</v>
       </c>
-      <c r="D29" s="32"/>
-      <c r="E29" t="s" s="33">
+      <c r="D29" s="30"/>
+      <c r="E29" t="s" s="31">
         <v>105</v>
       </c>
-      <c r="F29" t="s" s="34">
+      <c r="F29" t="s" s="32">
         <v>46</v>
       </c>
-      <c r="G29" t="s" s="31">
+      <c r="G29" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H29" s="35"/>
+      <c r="H29" s="33"/>
       <c r="I29" t="str" s="5" cm="1">
         <f t="array" ref="I29">B29:B29&amp;": "&amp;C29:C29</f>
         <v>Searching: First/Last Occurrence</v>
@@ -4594,55 +4590,55 @@
       <c r="J29" s="5"/>
     </row>
     <row r="30" ht="30" customHeight="1">
-      <c r="A30" s="36">
+      <c r="A30" s="34">
         <v>29</v>
       </c>
-      <c r="B30" t="s" s="37">
+      <c r="B30" t="s" s="35">
         <v>99</v>
       </c>
-      <c r="C30" t="s" s="37">
+      <c r="C30" t="s" s="35">
         <v>107</v>
       </c>
-      <c r="D30" s="38"/>
-      <c r="E30" t="s" s="33">
+      <c r="D30" s="36"/>
+      <c r="E30" t="s" s="31">
         <v>108</v>
       </c>
-      <c r="F30" t="s" s="37">
+      <c r="F30" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G30" t="s" s="37">
+      <c r="G30" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H30" s="39"/>
-      <c r="I30" t="str" s="24" cm="1">
+      <c r="H30" s="37"/>
+      <c r="I30" t="str" s="22" cm="1">
         <f t="array" ref="I30">B30:B30&amp;": "&amp;C30:C30</f>
         <v>Searching: Peak Element</v>
       </c>
       <c r="J30" s="4"/>
     </row>
     <row r="31" ht="30" customHeight="1">
-      <c r="A31" s="30">
+      <c r="A31" s="28">
         <v>30</v>
       </c>
-      <c r="B31" t="s" s="31">
+      <c r="B31" t="s" s="29">
         <v>99</v>
       </c>
-      <c r="C31" t="s" s="31">
+      <c r="C31" t="s" s="29">
         <v>110</v>
       </c>
-      <c r="D31" s="40">
+      <c r="D31" s="38">
         <v>11</v>
       </c>
-      <c r="E31" t="s" s="33">
+      <c r="E31" t="s" s="31">
         <v>111</v>
       </c>
-      <c r="F31" t="s" s="34">
+      <c r="F31" t="s" s="32">
         <v>46</v>
       </c>
-      <c r="G31" t="s" s="31">
+      <c r="G31" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H31" s="35"/>
+      <c r="H31" s="33"/>
       <c r="I31" t="str" s="5" cm="1">
         <f t="array" ref="I31">B31:B31&amp;": "&amp;C31:C31</f>
         <v>Searching: BS on Answer</v>
@@ -4650,53 +4646,53 @@
       <c r="J31" s="5"/>
     </row>
     <row r="32" ht="30" customHeight="1">
-      <c r="A32" s="36">
+      <c r="A32" s="34">
         <v>31</v>
       </c>
-      <c r="B32" t="s" s="37">
+      <c r="B32" t="s" s="35">
         <v>99</v>
       </c>
-      <c r="C32" t="s" s="37">
+      <c r="C32" t="s" s="35">
         <v>110</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" t="s" s="49">
+      <c r="D32" s="36"/>
+      <c r="E32" t="s" s="47">
         <v>113</v>
       </c>
-      <c r="F32" t="s" s="37">
+      <c r="F32" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="G32" t="s" s="37">
+      <c r="G32" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H32" s="39"/>
-      <c r="I32" t="str" s="24" cm="1">
+      <c r="H32" s="37"/>
+      <c r="I32" t="str" s="22" cm="1">
         <f t="array" ref="I32">B32:B32&amp;": "&amp;C32:C32</f>
         <v>Searching: BS on Answer</v>
       </c>
       <c r="J32" s="4"/>
     </row>
     <row r="33" ht="30" customHeight="1">
-      <c r="A33" s="30">
+      <c r="A33" s="28">
         <v>32</v>
       </c>
-      <c r="B33" t="s" s="31">
+      <c r="B33" t="s" s="29">
         <v>99</v>
       </c>
-      <c r="C33" t="s" s="31">
+      <c r="C33" t="s" s="29">
         <v>110</v>
       </c>
-      <c r="D33" s="32"/>
-      <c r="E33" t="s" s="49">
+      <c r="D33" s="30"/>
+      <c r="E33" t="s" s="47">
         <v>114</v>
       </c>
-      <c r="F33" t="s" s="34">
+      <c r="F33" t="s" s="32">
         <v>46</v>
       </c>
-      <c r="G33" t="s" s="31">
+      <c r="G33" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H33" s="35"/>
+      <c r="H33" s="33"/>
       <c r="I33" t="str" s="5" cm="1">
         <f t="array" ref="I33">B33:B33&amp;": "&amp;C33:C33</f>
         <v>Searching: BS on Answer</v>
@@ -4704,55 +4700,55 @@
       <c r="J33" s="5"/>
     </row>
     <row r="34" ht="30" customHeight="1">
-      <c r="A34" s="36">
+      <c r="A34" s="34">
         <v>33</v>
       </c>
-      <c r="B34" t="s" s="37">
+      <c r="B34" t="s" s="35">
         <v>115</v>
       </c>
-      <c r="C34" t="s" s="37">
+      <c r="C34" t="s" s="35">
         <v>116</v>
       </c>
-      <c r="D34" s="41">
+      <c r="D34" s="39">
         <v>12</v>
       </c>
-      <c r="E34" t="s" s="49">
+      <c r="E34" t="s" s="47">
         <v>117</v>
       </c>
-      <c r="F34" t="s" s="37">
+      <c r="F34" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G34" t="s" s="37">
+      <c r="G34" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H34" s="39"/>
-      <c r="I34" t="str" s="24" cm="1">
+      <c r="H34" s="37"/>
+      <c r="I34" t="str" s="22" cm="1">
         <f t="array" ref="I34">B34:B34&amp;": "&amp;C34:C34</f>
         <v>Sorting: Basic Sorting Logic</v>
       </c>
       <c r="J34" s="4"/>
     </row>
     <row r="35" ht="30" customHeight="1">
-      <c r="A35" s="30">
+      <c r="A35" s="28">
         <v>34</v>
       </c>
-      <c r="B35" t="s" s="31">
+      <c r="B35" t="s" s="29">
         <v>115</v>
       </c>
-      <c r="C35" t="s" s="31">
+      <c r="C35" t="s" s="29">
         <v>119</v>
       </c>
-      <c r="D35" s="50"/>
-      <c r="E35" t="s" s="51">
+      <c r="D35" s="48"/>
+      <c r="E35" t="s" s="49">
         <v>120</v>
       </c>
-      <c r="F35" t="s" s="31">
+      <c r="F35" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G35" t="s" s="31">
+      <c r="G35" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H35" s="35"/>
+      <c r="H35" s="33"/>
       <c r="I35" t="str" s="5" cm="1">
         <f t="array" ref="I35">B35:B35&amp;": "&amp;C35:C35</f>
         <v>Sorting: Selection Practice</v>
@@ -4760,55 +4756,55 @@
       <c r="J35" s="5"/>
     </row>
     <row r="36" ht="30" customHeight="1">
-      <c r="A36" s="36">
+      <c r="A36" s="34">
         <v>35</v>
       </c>
-      <c r="B36" t="s" s="37">
+      <c r="B36" t="s" s="35">
         <v>115</v>
       </c>
-      <c r="C36" t="s" s="37">
+      <c r="C36" t="s" s="35">
         <v>122</v>
       </c>
-      <c r="D36" s="38"/>
-      <c r="E36" t="s" s="52">
+      <c r="D36" s="36"/>
+      <c r="E36" t="s" s="50">
         <v>123</v>
       </c>
-      <c r="F36" t="s" s="37">
+      <c r="F36" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G36" t="s" s="37">
+      <c r="G36" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H36" s="39"/>
-      <c r="I36" t="str" s="24" cm="1">
+      <c r="H36" s="37"/>
+      <c r="I36" t="str" s="22" cm="1">
         <f t="array" ref="I36">B36:B36&amp;": "&amp;C36:C36</f>
         <v>Sorting: QuickSort</v>
       </c>
       <c r="J36" s="4"/>
     </row>
     <row r="37" ht="30" customHeight="1">
-      <c r="A37" s="30">
+      <c r="A37" s="28">
         <v>36</v>
       </c>
-      <c r="B37" t="s" s="31">
+      <c r="B37" t="s" s="29">
         <v>115</v>
       </c>
-      <c r="C37" t="s" s="31">
+      <c r="C37" t="s" s="29">
         <v>125</v>
       </c>
-      <c r="D37" s="30">
+      <c r="D37" s="28">
         <v>13</v>
       </c>
-      <c r="E37" t="s" s="51">
+      <c r="E37" t="s" s="49">
         <v>126</v>
       </c>
-      <c r="F37" t="s" s="31">
+      <c r="F37" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G37" t="s" s="31">
+      <c r="G37" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H37" s="35"/>
+      <c r="H37" s="33"/>
       <c r="I37" t="str" s="5" cm="1">
         <f t="array" ref="I37">B37:B37&amp;": "&amp;C37:C37</f>
         <v>Sorting: Custom Comparator</v>
@@ -4816,55 +4812,55 @@
       <c r="J37" s="5"/>
     </row>
     <row r="38" ht="30" customHeight="1">
-      <c r="A38" s="36">
+      <c r="A38" s="34">
         <v>37</v>
       </c>
-      <c r="B38" t="s" s="37">
+      <c r="B38" t="s" s="35">
         <v>115</v>
       </c>
-      <c r="C38" t="s" s="37">
+      <c r="C38" t="s" s="35">
         <v>125</v>
       </c>
-      <c r="D38" s="38"/>
-      <c r="E38" t="s" s="52">
+      <c r="D38" s="36"/>
+      <c r="E38" t="s" s="50">
         <v>128</v>
       </c>
-      <c r="F38" t="s" s="37">
+      <c r="F38" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G38" t="s" s="37">
+      <c r="G38" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H38" s="39"/>
-      <c r="I38" t="str" s="24" cm="1">
+      <c r="H38" s="37"/>
+      <c r="I38" t="str" s="22" cm="1">
         <f t="array" ref="I38">B38:B38&amp;": "&amp;C38:C38</f>
         <v>Sorting: Custom Comparator</v>
       </c>
       <c r="J38" s="4"/>
     </row>
     <row r="39" ht="30" customHeight="1">
-      <c r="A39" s="30">
+      <c r="A39" s="28">
         <v>38</v>
       </c>
-      <c r="B39" t="s" s="31">
+      <c r="B39" t="s" s="29">
         <v>115</v>
       </c>
-      <c r="C39" t="s" s="31">
+      <c r="C39" t="s" s="29">
         <v>129</v>
       </c>
-      <c r="D39" s="30">
+      <c r="D39" s="28">
         <v>14</v>
       </c>
-      <c r="E39" t="s" s="51">
+      <c r="E39" t="s" s="49">
         <v>130</v>
       </c>
-      <c r="F39" t="s" s="31">
+      <c r="F39" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G39" t="s" s="31">
+      <c r="G39" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H39" s="35"/>
+      <c r="H39" s="33"/>
       <c r="I39" t="str" s="5" cm="1">
         <f t="array" ref="I39">B39:B39&amp;": "&amp;C39:C39</f>
         <v>Sorting: Merge Intervals</v>
@@ -4872,55 +4868,55 @@
       <c r="J39" s="5"/>
     </row>
     <row r="40" ht="30" customHeight="1">
-      <c r="A40" s="36">
+      <c r="A40" s="34">
         <v>39</v>
       </c>
-      <c r="B40" t="s" s="37">
+      <c r="B40" t="s" s="35">
         <v>115</v>
       </c>
-      <c r="C40" t="s" s="37">
+      <c r="C40" t="s" s="35">
         <v>129</v>
       </c>
-      <c r="D40" s="38"/>
-      <c r="E40" t="s" s="52">
+      <c r="D40" s="36"/>
+      <c r="E40" t="s" s="50">
         <v>132</v>
       </c>
-      <c r="F40" t="s" s="37">
+      <c r="F40" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G40" t="s" s="37">
+      <c r="G40" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H40" s="39"/>
-      <c r="I40" t="str" s="24" cm="1">
+      <c r="H40" s="37"/>
+      <c r="I40" t="str" s="22" cm="1">
         <f t="array" ref="I40">B40:B40&amp;": "&amp;C40:C40</f>
         <v>Sorting: Merge Intervals</v>
       </c>
       <c r="J40" s="4"/>
     </row>
     <row r="41" ht="30" customHeight="1">
-      <c r="A41" s="30">
+      <c r="A41" s="28">
         <v>40</v>
       </c>
-      <c r="B41" t="s" s="31">
+      <c r="B41" t="s" s="29">
         <v>115</v>
       </c>
-      <c r="C41" t="s" s="31">
+      <c r="C41" t="s" s="29">
         <v>133</v>
       </c>
-      <c r="D41" s="30">
+      <c r="D41" s="28">
         <v>15</v>
       </c>
-      <c r="E41" t="s" s="51">
+      <c r="E41" t="s" s="49">
         <v>134</v>
       </c>
-      <c r="F41" t="s" s="31">
+      <c r="F41" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G41" t="s" s="31">
+      <c r="G41" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H41" s="35"/>
+      <c r="H41" s="33"/>
       <c r="I41" t="str" s="5" cm="1">
         <f t="array" ref="I41">B41:B41&amp;": "&amp;C41:C41</f>
         <v>Sorting: Scheduling Logic</v>
@@ -4928,55 +4924,55 @@
       <c r="J41" s="5"/>
     </row>
     <row r="42" ht="30" customHeight="1">
-      <c r="A42" s="36">
+      <c r="A42" s="34">
         <v>41</v>
       </c>
-      <c r="B42" t="s" s="37">
+      <c r="B42" t="s" s="35">
         <v>115</v>
       </c>
-      <c r="C42" t="s" s="37">
+      <c r="C42" t="s" s="35">
         <v>136</v>
       </c>
-      <c r="D42" s="38"/>
-      <c r="E42" t="s" s="37">
+      <c r="D42" s="36"/>
+      <c r="E42" t="s" s="51">
         <v>137</v>
       </c>
-      <c r="F42" t="s" s="37">
+      <c r="F42" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G42" t="s" s="37">
+      <c r="G42" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H42" s="39"/>
-      <c r="I42" t="str" s="24" cm="1">
+      <c r="H42" s="37"/>
+      <c r="I42" t="str" s="22" cm="1">
         <f t="array" ref="I42">B42:B42&amp;": "&amp;C42:C42</f>
         <v>Sorting: Sorting Based Greedy</v>
       </c>
       <c r="J42" s="4"/>
     </row>
     <row r="43" ht="30" customHeight="1">
-      <c r="A43" s="30">
+      <c r="A43" s="28">
         <v>42</v>
       </c>
-      <c r="B43" t="s" s="31">
+      <c r="B43" t="s" s="29">
         <v>139</v>
       </c>
-      <c r="C43" t="s" s="31">
+      <c r="C43" t="s" s="29">
         <v>140</v>
       </c>
-      <c r="D43" s="30">
+      <c r="D43" s="28">
         <v>16</v>
       </c>
-      <c r="E43" t="s" s="31">
+      <c r="E43" t="s" s="52">
         <v>141</v>
       </c>
-      <c r="F43" t="s" s="31">
+      <c r="F43" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G43" t="s" s="31">
+      <c r="G43" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H43" s="35"/>
+      <c r="H43" s="33"/>
       <c r="I43" t="str" s="5" cm="1">
         <f t="array" ref="I43">B43:B43&amp;": "&amp;C43:C43</f>
         <v>Linked List: Reverse LL</v>
@@ -4984,55 +4980,55 @@
       <c r="J43" s="5"/>
     </row>
     <row r="44" ht="30" customHeight="1">
-      <c r="A44" s="36">
+      <c r="A44" s="34">
         <v>43</v>
       </c>
-      <c r="B44" t="s" s="37">
+      <c r="B44" t="s" s="35">
         <v>139</v>
       </c>
-      <c r="C44" t="s" s="37">
+      <c r="C44" t="s" s="35">
         <v>143</v>
       </c>
-      <c r="D44" s="38"/>
-      <c r="E44" t="s" s="37">
+      <c r="D44" s="36"/>
+      <c r="E44" t="s" s="35">
         <v>144</v>
       </c>
-      <c r="F44" t="s" s="37">
+      <c r="F44" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G44" t="s" s="37">
+      <c r="G44" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H44" s="39"/>
-      <c r="I44" t="str" s="24" cm="1">
+      <c r="H44" s="37"/>
+      <c r="I44" t="str" s="22" cm="1">
         <f t="array" ref="I44">B44:B44&amp;": "&amp;C44:C44</f>
         <v>Linked List: Reverse LL II</v>
       </c>
       <c r="J44" s="4"/>
     </row>
     <row r="45" ht="30" customHeight="1">
-      <c r="A45" s="30">
+      <c r="A45" s="28">
         <v>44</v>
       </c>
-      <c r="B45" t="s" s="31">
+      <c r="B45" t="s" s="29">
         <v>139</v>
       </c>
-      <c r="C45" t="s" s="31">
+      <c r="C45" t="s" s="29">
         <v>146</v>
       </c>
-      <c r="D45" s="30">
+      <c r="D45" s="28">
         <v>17</v>
       </c>
-      <c r="E45" t="s" s="31">
+      <c r="E45" t="s" s="29">
         <v>147</v>
       </c>
-      <c r="F45" t="s" s="31">
+      <c r="F45" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G45" t="s" s="31">
+      <c r="G45" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H45" s="35"/>
+      <c r="H45" s="33"/>
       <c r="I45" t="str" s="5" cm="1">
         <f t="array" ref="I45">B45:B45&amp;": "&amp;C45:C45</f>
         <v>Linked List: Detect Cycle</v>
@@ -5040,55 +5036,55 @@
       <c r="J45" s="5"/>
     </row>
     <row r="46" ht="30" customHeight="1">
-      <c r="A46" s="36">
+      <c r="A46" s="34">
         <v>45</v>
       </c>
-      <c r="B46" t="s" s="37">
+      <c r="B46" t="s" s="35">
         <v>139</v>
       </c>
-      <c r="C46" t="s" s="37">
+      <c r="C46" t="s" s="35">
         <v>149</v>
       </c>
-      <c r="D46" s="38"/>
-      <c r="E46" t="s" s="37">
+      <c r="D46" s="36"/>
+      <c r="E46" t="s" s="35">
         <v>150</v>
       </c>
-      <c r="F46" t="s" s="37">
+      <c r="F46" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G46" t="s" s="37">
+      <c r="G46" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H46" s="39"/>
-      <c r="I46" t="str" s="24" cm="1">
+      <c r="H46" s="37"/>
+      <c r="I46" t="str" s="22" cm="1">
         <f t="array" ref="I46">B46:B46&amp;": "&amp;C46:C46</f>
         <v>Linked List: Cycle II</v>
       </c>
       <c r="J46" s="4"/>
     </row>
     <row r="47" ht="30" customHeight="1">
-      <c r="A47" s="30">
+      <c r="A47" s="28">
         <v>46</v>
       </c>
-      <c r="B47" t="s" s="31">
+      <c r="B47" t="s" s="29">
         <v>139</v>
       </c>
-      <c r="C47" t="s" s="31">
+      <c r="C47" t="s" s="29">
         <v>152</v>
       </c>
-      <c r="D47" s="30">
+      <c r="D47" s="28">
         <v>18</v>
       </c>
-      <c r="E47" t="s" s="31">
+      <c r="E47" t="s" s="29">
         <v>153</v>
       </c>
-      <c r="F47" t="s" s="31">
+      <c r="F47" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G47" t="s" s="31">
+      <c r="G47" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H47" s="35"/>
+      <c r="H47" s="33"/>
       <c r="I47" t="str" s="5" cm="1">
         <f t="array" ref="I47">B47:B47&amp;": "&amp;C47:C47</f>
         <v>Linked List: Merge LL</v>
@@ -5096,55 +5092,55 @@
       <c r="J47" s="5"/>
     </row>
     <row r="48" ht="30" customHeight="1">
-      <c r="A48" s="36">
+      <c r="A48" s="34">
         <v>47</v>
       </c>
-      <c r="B48" t="s" s="37">
+      <c r="B48" t="s" s="35">
         <v>139</v>
       </c>
-      <c r="C48" t="s" s="37">
+      <c r="C48" t="s" s="35">
         <v>155</v>
       </c>
-      <c r="D48" s="38"/>
-      <c r="E48" t="s" s="37">
+      <c r="D48" s="36"/>
+      <c r="E48" t="s" s="35">
         <v>156</v>
       </c>
-      <c r="F48" t="s" s="37">
+      <c r="F48" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="G48" t="s" s="37">
+      <c r="G48" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H48" s="39"/>
-      <c r="I48" t="str" s="24" cm="1">
+      <c r="H48" s="37"/>
+      <c r="I48" t="str" s="22" cm="1">
         <f t="array" ref="I48">B48:B48&amp;": "&amp;C48:C48</f>
         <v>Linked List: Merge k Lists</v>
       </c>
       <c r="J48" s="4"/>
     </row>
     <row r="49" ht="30" customHeight="1">
-      <c r="A49" s="30">
+      <c r="A49" s="28">
         <v>48</v>
       </c>
-      <c r="B49" t="s" s="31">
+      <c r="B49" t="s" s="29">
         <v>139</v>
       </c>
-      <c r="C49" t="s" s="31">
+      <c r="C49" t="s" s="29">
         <v>158</v>
       </c>
-      <c r="D49" s="30">
+      <c r="D49" s="28">
         <v>19</v>
       </c>
-      <c r="E49" t="s" s="31">
+      <c r="E49" t="s" s="29">
         <v>159</v>
       </c>
-      <c r="F49" t="s" s="31">
+      <c r="F49" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G49" t="s" s="31">
+      <c r="G49" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H49" s="35"/>
+      <c r="H49" s="33"/>
       <c r="I49" t="str" s="5" cm="1">
         <f t="array" ref="I49">B49:B49&amp;": "&amp;C49:C49</f>
         <v>Linked List: Intersection Point</v>
@@ -5152,55 +5148,55 @@
       <c r="J49" s="5"/>
     </row>
     <row r="50" ht="30" customHeight="1">
-      <c r="A50" s="36">
+      <c r="A50" s="34">
         <v>49</v>
       </c>
-      <c r="B50" t="s" s="37">
+      <c r="B50" t="s" s="35">
         <v>139</v>
       </c>
-      <c r="C50" t="s" s="37">
+      <c r="C50" t="s" s="35">
         <v>161</v>
       </c>
-      <c r="D50" s="38"/>
-      <c r="E50" t="s" s="37">
+      <c r="D50" s="36"/>
+      <c r="E50" t="s" s="35">
         <v>162</v>
       </c>
-      <c r="F50" t="s" s="37">
+      <c r="F50" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G50" t="s" s="37">
+      <c r="G50" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H50" s="39"/>
-      <c r="I50" t="str" s="24" cm="1">
+      <c r="H50" s="37"/>
+      <c r="I50" t="str" s="22" cm="1">
         <f t="array" ref="I50">B50:B50&amp;": "&amp;C50:C50</f>
         <v>Linked List: Remove Nth Node</v>
       </c>
       <c r="J50" s="4"/>
     </row>
     <row r="51" ht="30" customHeight="1">
-      <c r="A51" s="30">
+      <c r="A51" s="28">
         <v>50</v>
       </c>
-      <c r="B51" t="s" s="31">
+      <c r="B51" t="s" s="29">
         <v>139</v>
       </c>
-      <c r="C51" t="s" s="31">
+      <c r="C51" t="s" s="29">
         <v>164</v>
       </c>
-      <c r="D51" s="30">
+      <c r="D51" s="28">
         <v>20</v>
       </c>
-      <c r="E51" t="s" s="31">
+      <c r="E51" t="s" s="29">
         <v>165</v>
       </c>
-      <c r="F51" t="s" s="31">
+      <c r="F51" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G51" t="s" s="31">
+      <c r="G51" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H51" s="35"/>
+      <c r="H51" s="33"/>
       <c r="I51" t="str" s="5" cm="1">
         <f t="array" ref="I51">B51:B51&amp;": "&amp;C51:C51</f>
         <v>Linked List: Palindrome Check</v>
@@ -5208,55 +5204,55 @@
       <c r="J51" s="5"/>
     </row>
     <row r="52" ht="30" customHeight="1">
-      <c r="A52" s="36">
+      <c r="A52" s="34">
         <v>51</v>
       </c>
-      <c r="B52" t="s" s="37">
+      <c r="B52" t="s" s="35">
         <v>139</v>
       </c>
-      <c r="C52" t="s" s="37">
+      <c r="C52" t="s" s="35">
         <v>167</v>
       </c>
-      <c r="D52" s="38"/>
-      <c r="E52" t="s" s="37">
+      <c r="D52" s="36"/>
+      <c r="E52" t="s" s="35">
         <v>168</v>
       </c>
-      <c r="F52" t="s" s="37">
+      <c r="F52" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G52" t="s" s="37">
+      <c r="G52" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H52" s="39"/>
-      <c r="I52" t="str" s="24" cm="1">
+      <c r="H52" s="37"/>
+      <c r="I52" t="str" s="22" cm="1">
         <f t="array" ref="I52">B52:B52&amp;": "&amp;C52:C52</f>
         <v>Linked List: Odd Even Index</v>
       </c>
       <c r="J52" s="4"/>
     </row>
     <row r="53" ht="30" customHeight="1">
-      <c r="A53" s="30">
+      <c r="A53" s="28">
         <v>52</v>
       </c>
-      <c r="B53" t="s" s="31">
+      <c r="B53" t="s" s="29">
         <v>139</v>
       </c>
-      <c r="C53" t="s" s="31">
+      <c r="C53" t="s" s="29">
         <v>170</v>
       </c>
-      <c r="D53" s="30">
+      <c r="D53" s="28">
         <v>21</v>
       </c>
-      <c r="E53" t="s" s="31">
+      <c r="E53" t="s" s="29">
         <v>171</v>
       </c>
-      <c r="F53" t="s" s="31">
+      <c r="F53" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G53" t="s" s="31">
+      <c r="G53" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H53" s="35"/>
+      <c r="H53" s="33"/>
       <c r="I53" t="str" s="5" cm="1">
         <f t="array" ref="I53">B53:B53&amp;": "&amp;C53:C53</f>
         <v>Linked List: LRU Cache Logic</v>
@@ -5264,55 +5260,55 @@
       <c r="J53" s="5"/>
     </row>
     <row r="54" ht="30" customHeight="1">
-      <c r="A54" s="36">
+      <c r="A54" s="34">
         <v>53</v>
       </c>
-      <c r="B54" t="s" s="37">
+      <c r="B54" t="s" s="35">
         <v>139</v>
       </c>
-      <c r="C54" t="s" s="37">
+      <c r="C54" t="s" s="35">
         <v>173</v>
       </c>
-      <c r="D54" s="38"/>
-      <c r="E54" t="s" s="37">
+      <c r="D54" s="36"/>
+      <c r="E54" t="s" s="35">
         <v>174</v>
       </c>
-      <c r="F54" t="s" s="37">
+      <c r="F54" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="G54" t="s" s="37">
+      <c r="G54" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H54" s="39"/>
-      <c r="I54" t="str" s="24" cm="1">
+      <c r="H54" s="37"/>
+      <c r="I54" t="str" s="22" cm="1">
         <f t="array" ref="I54">B54:B54&amp;": "&amp;C54:C54</f>
         <v>Linked List: Advanced LRU Logic</v>
       </c>
       <c r="J54" s="4"/>
     </row>
     <row r="55" ht="30" customHeight="1">
-      <c r="A55" s="30">
+      <c r="A55" s="28">
         <v>54</v>
       </c>
-      <c r="B55" t="s" s="31">
+      <c r="B55" t="s" s="29">
         <v>10</v>
       </c>
-      <c r="C55" t="s" s="31">
+      <c r="C55" t="s" s="29">
         <v>176</v>
       </c>
-      <c r="D55" s="30">
+      <c r="D55" s="28">
         <v>22</v>
       </c>
-      <c r="E55" t="s" s="31">
+      <c r="E55" t="s" s="29">
         <v>177</v>
       </c>
-      <c r="F55" t="s" s="31">
+      <c r="F55" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G55" t="s" s="31">
+      <c r="G55" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H55" s="35"/>
+      <c r="H55" s="33"/>
       <c r="I55" t="str" s="5" cm="1">
         <f t="array" ref="I55">B55:B55&amp;": "&amp;C55:C55</f>
         <v>Stack: Stack Basics</v>
@@ -5320,55 +5316,55 @@
       <c r="J55" s="5"/>
     </row>
     <row r="56" ht="30" customHeight="1">
-      <c r="A56" s="36">
+      <c r="A56" s="34">
         <v>55</v>
       </c>
-      <c r="B56" t="s" s="37">
+      <c r="B56" t="s" s="35">
         <v>10</v>
       </c>
-      <c r="C56" t="s" s="37">
+      <c r="C56" t="s" s="35">
         <v>176</v>
       </c>
-      <c r="D56" s="38"/>
-      <c r="E56" t="s" s="37">
+      <c r="D56" s="36"/>
+      <c r="E56" t="s" s="35">
         <v>179</v>
       </c>
-      <c r="F56" t="s" s="37">
+      <c r="F56" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G56" t="s" s="37">
+      <c r="G56" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H56" s="39"/>
-      <c r="I56" t="str" s="24" cm="1">
+      <c r="H56" s="37"/>
+      <c r="I56" t="str" s="22" cm="1">
         <f t="array" ref="I56">B56:B56&amp;": "&amp;C56:C56</f>
         <v>Stack: Stack Basics</v>
       </c>
       <c r="J56" s="4"/>
     </row>
     <row r="57" ht="30" customHeight="1">
-      <c r="A57" s="30">
+      <c r="A57" s="28">
         <v>56</v>
       </c>
-      <c r="B57" t="s" s="31">
+      <c r="B57" t="s" s="29">
         <v>10</v>
       </c>
-      <c r="C57" t="s" s="31">
+      <c r="C57" t="s" s="29">
         <v>180</v>
       </c>
-      <c r="D57" s="30">
+      <c r="D57" s="28">
         <v>23</v>
       </c>
-      <c r="E57" t="s" s="31">
+      <c r="E57" t="s" s="29">
         <v>181</v>
       </c>
-      <c r="F57" t="s" s="31">
+      <c r="F57" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G57" t="s" s="31">
+      <c r="G57" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H57" s="35"/>
+      <c r="H57" s="33"/>
       <c r="I57" t="str" s="5" cm="1">
         <f t="array" ref="I57">B57:B57&amp;": "&amp;C57:C57</f>
         <v>Stack: Monotonic Stack</v>
@@ -5376,53 +5372,53 @@
       <c r="J57" s="5"/>
     </row>
     <row r="58" ht="30" customHeight="1">
-      <c r="A58" s="36">
+      <c r="A58" s="34">
         <v>57</v>
       </c>
-      <c r="B58" t="s" s="37">
+      <c r="B58" t="s" s="35">
         <v>10</v>
       </c>
-      <c r="C58" t="s" s="37">
+      <c r="C58" t="s" s="35">
         <v>183</v>
       </c>
-      <c r="D58" s="38"/>
-      <c r="E58" t="s" s="37">
+      <c r="D58" s="36"/>
+      <c r="E58" t="s" s="35">
         <v>184</v>
       </c>
-      <c r="F58" t="s" s="37">
+      <c r="F58" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G58" t="s" s="37">
+      <c r="G58" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H58" s="39"/>
-      <c r="I58" t="str" s="24" cm="1">
+      <c r="H58" s="37"/>
+      <c r="I58" t="str" s="22" cm="1">
         <f t="array" ref="I58">B58:B58&amp;": "&amp;C58:C58</f>
         <v>Stack: Next Greater Element</v>
       </c>
       <c r="J58" s="4"/>
     </row>
     <row r="59" ht="30" customHeight="1">
-      <c r="A59" s="30">
+      <c r="A59" s="28">
         <v>58</v>
       </c>
-      <c r="B59" t="s" s="31">
+      <c r="B59" t="s" s="29">
         <v>10</v>
       </c>
-      <c r="C59" t="s" s="31">
+      <c r="C59" t="s" s="29">
         <v>186</v>
       </c>
-      <c r="D59" s="50"/>
-      <c r="E59" t="s" s="31">
+      <c r="D59" s="48"/>
+      <c r="E59" t="s" s="29">
         <v>187</v>
       </c>
-      <c r="F59" t="s" s="31">
+      <c r="F59" t="s" s="29">
         <v>43</v>
       </c>
-      <c r="G59" t="s" s="31">
+      <c r="G59" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H59" s="35"/>
+      <c r="H59" s="33"/>
       <c r="I59" t="str" s="5" cm="1">
         <f t="array" ref="I59">B59:B59&amp;": "&amp;C59:C59</f>
         <v>Stack: Largest Rect in Hist</v>
@@ -5430,55 +5426,55 @@
       <c r="J59" s="5"/>
     </row>
     <row r="60" ht="30" customHeight="1">
-      <c r="A60" s="36">
+      <c r="A60" s="34">
         <v>59</v>
       </c>
-      <c r="B60" t="s" s="37">
+      <c r="B60" t="s" s="35">
         <v>189</v>
       </c>
-      <c r="C60" t="s" s="37">
+      <c r="C60" t="s" s="35">
         <v>190</v>
       </c>
-      <c r="D60" s="41">
+      <c r="D60" s="39">
         <v>24</v>
       </c>
-      <c r="E60" t="s" s="37">
+      <c r="E60" t="s" s="35">
         <v>191</v>
       </c>
-      <c r="F60" t="s" s="37">
+      <c r="F60" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G60" t="s" s="37">
+      <c r="G60" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H60" s="39"/>
-      <c r="I60" t="str" s="24" cm="1">
+      <c r="H60" s="37"/>
+      <c r="I60" t="str" s="22" cm="1">
         <f t="array" ref="I60">B60:B60&amp;": "&amp;C60:C60</f>
         <v>Queue: Queue + BFS Intro</v>
       </c>
       <c r="J60" s="4"/>
     </row>
     <row r="61" ht="30" customHeight="1">
-      <c r="A61" s="30">
+      <c r="A61" s="28">
         <v>60</v>
       </c>
-      <c r="B61" t="s" s="31">
+      <c r="B61" t="s" s="29">
         <v>189</v>
       </c>
-      <c r="C61" t="s" s="31">
+      <c r="C61" t="s" s="29">
         <v>193</v>
       </c>
-      <c r="D61" s="50"/>
-      <c r="E61" t="s" s="31">
+      <c r="D61" s="48"/>
+      <c r="E61" t="s" s="29">
         <v>194</v>
       </c>
-      <c r="F61" t="s" s="31">
+      <c r="F61" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G61" t="s" s="31">
+      <c r="G61" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H61" s="35"/>
+      <c r="H61" s="33"/>
       <c r="I61" t="str" s="5" cm="1">
         <f t="array" ref="I61">B61:B61&amp;": "&amp;C61:C61</f>
         <v>Queue: Implement Queue Using Stacks</v>
@@ -5486,55 +5482,55 @@
       <c r="J61" s="5"/>
     </row>
     <row r="62" ht="30" customHeight="1">
-      <c r="A62" s="36">
+      <c r="A62" s="34">
         <v>61</v>
       </c>
-      <c r="B62" t="s" s="37">
+      <c r="B62" t="s" s="35">
         <v>189</v>
       </c>
-      <c r="C62" t="s" s="37">
+      <c r="C62" t="s" s="35">
         <v>196</v>
       </c>
-      <c r="D62" s="41">
+      <c r="D62" s="39">
         <v>25</v>
       </c>
-      <c r="E62" t="s" s="37">
+      <c r="E62" t="s" s="35">
         <v>197</v>
       </c>
-      <c r="F62" t="s" s="37">
+      <c r="F62" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G62" t="s" s="37">
+      <c r="G62" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H62" s="39"/>
-      <c r="I62" t="str" s="24" cm="1">
+      <c r="H62" s="37"/>
+      <c r="I62" t="str" s="22" cm="1">
         <f t="array" ref="I62">B62:B62&amp;": "&amp;C62:C62</f>
         <v>Queue: Circular Queue</v>
       </c>
       <c r="J62" s="4"/>
     </row>
     <row r="63" ht="30" customHeight="1">
-      <c r="A63" s="30">
+      <c r="A63" s="28">
         <v>62</v>
       </c>
-      <c r="B63" t="s" s="31">
+      <c r="B63" t="s" s="29">
         <v>189</v>
       </c>
-      <c r="C63" t="s" s="31">
+      <c r="C63" t="s" s="29">
         <v>199</v>
       </c>
-      <c r="D63" s="50"/>
-      <c r="E63" t="s" s="31">
+      <c r="D63" s="48"/>
+      <c r="E63" t="s" s="29">
         <v>200</v>
       </c>
-      <c r="F63" t="s" s="31">
+      <c r="F63" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G63" t="s" s="31">
+      <c r="G63" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H63" s="35"/>
+      <c r="H63" s="33"/>
       <c r="I63" t="str" s="5" cm="1">
         <f t="array" ref="I63">B63:B63&amp;": "&amp;C63:C63</f>
         <v>Queue: Deque</v>
@@ -5542,55 +5538,55 @@
       <c r="J63" s="5"/>
     </row>
     <row r="64" ht="30" customHeight="1">
-      <c r="A64" s="36">
+      <c r="A64" s="34">
         <v>63</v>
       </c>
-      <c r="B64" t="s" s="37">
+      <c r="B64" t="s" s="35">
         <v>189</v>
       </c>
-      <c r="C64" t="s" s="37">
+      <c r="C64" t="s" s="35">
         <v>202</v>
       </c>
-      <c r="D64" s="41">
+      <c r="D64" s="39">
         <v>26</v>
       </c>
-      <c r="E64" t="s" s="37">
+      <c r="E64" t="s" s="35">
         <v>203</v>
       </c>
-      <c r="F64" t="s" s="37">
+      <c r="F64" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="G64" t="s" s="37">
+      <c r="G64" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H64" s="39"/>
-      <c r="I64" t="str" s="24" cm="1">
+      <c r="H64" s="37"/>
+      <c r="I64" t="str" s="22" cm="1">
         <f t="array" ref="I64">B64:B64&amp;": "&amp;C64:C64</f>
         <v>Queue: Monotonic Queue</v>
       </c>
       <c r="J64" s="4"/>
     </row>
     <row r="65" ht="30" customHeight="1">
-      <c r="A65" s="30">
+      <c r="A65" s="28">
         <v>64</v>
       </c>
-      <c r="B65" t="s" s="31">
+      <c r="B65" t="s" s="29">
         <v>189</v>
       </c>
-      <c r="C65" t="s" s="31">
+      <c r="C65" t="s" s="29">
         <v>202</v>
       </c>
-      <c r="D65" s="50"/>
-      <c r="E65" t="s" s="31">
+      <c r="D65" s="48"/>
+      <c r="E65" t="s" s="29">
         <v>205</v>
       </c>
-      <c r="F65" t="s" s="31">
+      <c r="F65" t="s" s="29">
         <v>43</v>
       </c>
-      <c r="G65" t="s" s="31">
+      <c r="G65" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H65" s="35"/>
+      <c r="H65" s="33"/>
       <c r="I65" t="str" s="5" cm="1">
         <f t="array" ref="I65">B65:B65&amp;": "&amp;C65:C65</f>
         <v>Queue: Monotonic Queue</v>
@@ -5598,55 +5594,55 @@
       <c r="J65" s="5"/>
     </row>
     <row r="66" ht="30" customHeight="1">
-      <c r="A66" s="36">
+      <c r="A66" s="34">
         <v>65</v>
       </c>
-      <c r="B66" t="s" s="37">
+      <c r="B66" t="s" s="35">
         <v>206</v>
       </c>
-      <c r="C66" t="s" s="37">
+      <c r="C66" t="s" s="35">
         <v>207</v>
       </c>
-      <c r="D66" s="41">
+      <c r="D66" s="39">
         <v>27</v>
       </c>
-      <c r="E66" t="s" s="37">
+      <c r="E66" t="s" s="35">
         <v>208</v>
       </c>
-      <c r="F66" t="s" s="37">
+      <c r="F66" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G66" t="s" s="37">
+      <c r="G66" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H66" s="39"/>
-      <c r="I66" t="str" s="24" cm="1">
+      <c r="H66" s="37"/>
+      <c r="I66" t="str" s="22" cm="1">
         <f t="array" ref="I66">B66:B66&amp;": "&amp;C66:C66</f>
         <v>Trees: Traversals</v>
       </c>
       <c r="J66" s="4"/>
     </row>
     <row r="67" ht="30" customHeight="1">
-      <c r="A67" s="30">
+      <c r="A67" s="28">
         <v>66</v>
       </c>
-      <c r="B67" t="s" s="31">
+      <c r="B67" t="s" s="29">
         <v>206</v>
       </c>
-      <c r="C67" t="s" s="31">
+      <c r="C67" t="s" s="29">
         <v>207</v>
       </c>
-      <c r="D67" s="50"/>
-      <c r="E67" t="s" s="31">
+      <c r="D67" s="48"/>
+      <c r="E67" t="s" s="29">
         <v>210</v>
       </c>
-      <c r="F67" t="s" s="31">
+      <c r="F67" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G67" t="s" s="31">
+      <c r="G67" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H67" s="35"/>
+      <c r="H67" s="33"/>
       <c r="I67" t="str" s="5" cm="1">
         <f t="array" ref="I67">B67:B67&amp;": "&amp;C67:C67</f>
         <v>Trees: Traversals</v>
@@ -5654,55 +5650,55 @@
       <c r="J67" s="5"/>
     </row>
     <row r="68" ht="30" customHeight="1">
-      <c r="A68" s="36">
+      <c r="A68" s="34">
         <v>67</v>
       </c>
-      <c r="B68" t="s" s="37">
+      <c r="B68" t="s" s="35">
         <v>206</v>
       </c>
-      <c r="C68" t="s" s="37">
+      <c r="C68" t="s" s="35">
         <v>211</v>
       </c>
-      <c r="D68" s="38"/>
-      <c r="E68" t="s" s="37">
+      <c r="D68" s="36"/>
+      <c r="E68" t="s" s="35">
         <v>212</v>
       </c>
-      <c r="F68" t="s" s="37">
+      <c r="F68" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G68" t="s" s="37">
+      <c r="G68" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H68" s="39"/>
-      <c r="I68" t="str" s="24" cm="1">
+      <c r="H68" s="37"/>
+      <c r="I68" t="str" s="22" cm="1">
         <f t="array" ref="I68">B68:B68&amp;": "&amp;C68:C68</f>
         <v>Trees: Views + Height</v>
       </c>
       <c r="J68" s="4"/>
     </row>
     <row r="69" ht="30" customHeight="1">
-      <c r="A69" s="30">
+      <c r="A69" s="28">
         <v>68</v>
       </c>
-      <c r="B69" t="s" s="31">
+      <c r="B69" t="s" s="29">
         <v>13</v>
       </c>
-      <c r="C69" t="s" s="31">
+      <c r="C69" t="s" s="29">
         <v>214</v>
       </c>
-      <c r="D69" s="30">
+      <c r="D69" s="28">
         <v>28</v>
       </c>
-      <c r="E69" t="s" s="31">
+      <c r="E69" t="s" s="29">
         <v>215</v>
       </c>
-      <c r="F69" t="s" s="31">
+      <c r="F69" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G69" t="s" s="31">
+      <c r="G69" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H69" s="35"/>
+      <c r="H69" s="33"/>
       <c r="I69" t="str" s="5" cm="1">
         <f t="array" ref="I69">B69:B69&amp;": "&amp;C69:C69</f>
         <v>BST: Search, Insert, Min</v>
@@ -5710,55 +5706,55 @@
       <c r="J69" s="5"/>
     </row>
     <row r="70" ht="30" customHeight="1">
-      <c r="A70" s="36">
+      <c r="A70" s="34">
         <v>69</v>
       </c>
-      <c r="B70" t="s" s="37">
+      <c r="B70" t="s" s="35">
         <v>13</v>
       </c>
-      <c r="C70" t="s" s="37">
+      <c r="C70" t="s" s="35">
         <v>217</v>
       </c>
-      <c r="D70" s="38"/>
-      <c r="E70" t="s" s="37">
+      <c r="D70" s="36"/>
+      <c r="E70" t="s" s="35">
         <v>218</v>
       </c>
-      <c r="F70" t="s" s="37">
+      <c r="F70" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G70" t="s" s="37">
+      <c r="G70" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H70" s="39"/>
-      <c r="I70" t="str" s="24" cm="1">
+      <c r="H70" s="37"/>
+      <c r="I70" t="str" s="22" cm="1">
         <f t="array" ref="I70">B70:B70&amp;": "&amp;C70:C70</f>
         <v>BST: Deletion</v>
       </c>
       <c r="J70" s="4"/>
     </row>
     <row r="71" ht="30" customHeight="1">
-      <c r="A71" s="30">
+      <c r="A71" s="28">
         <v>70</v>
       </c>
-      <c r="B71" t="s" s="31">
+      <c r="B71" t="s" s="29">
         <v>13</v>
       </c>
-      <c r="C71" t="s" s="31">
+      <c r="C71" t="s" s="29">
         <v>220</v>
       </c>
-      <c r="D71" s="30">
+      <c r="D71" s="28">
         <v>29</v>
       </c>
-      <c r="E71" t="s" s="31">
+      <c r="E71" t="s" s="29">
         <v>221</v>
       </c>
-      <c r="F71" t="s" s="31">
+      <c r="F71" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G71" t="s" s="31">
+      <c r="G71" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H71" s="35"/>
+      <c r="H71" s="33"/>
       <c r="I71" t="str" s="5" cm="1">
         <f t="array" ref="I71">B71:B71&amp;": "&amp;C71:C71</f>
         <v>BST: Validate BST</v>
@@ -5766,55 +5762,55 @@
       <c r="J71" s="5"/>
     </row>
     <row r="72" ht="30" customHeight="1">
-      <c r="A72" s="36">
+      <c r="A72" s="34">
         <v>71</v>
       </c>
-      <c r="B72" t="s" s="37">
+      <c r="B72" t="s" s="35">
         <v>13</v>
       </c>
-      <c r="C72" t="s" s="37">
+      <c r="C72" t="s" s="35">
         <v>223</v>
       </c>
-      <c r="D72" s="38"/>
-      <c r="E72" t="s" s="37">
+      <c r="D72" s="36"/>
+      <c r="E72" t="s" s="35">
         <v>224</v>
       </c>
-      <c r="F72" t="s" s="37">
+      <c r="F72" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G72" t="s" s="37">
+      <c r="G72" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H72" s="39"/>
-      <c r="I72" t="str" s="24" cm="1">
+      <c r="H72" s="37"/>
+      <c r="I72" t="str" s="22" cm="1">
         <f t="array" ref="I72">B72:B72&amp;": "&amp;C72:C72</f>
         <v>BST: Lowest Common Ancestor</v>
       </c>
       <c r="J72" s="4"/>
     </row>
     <row r="73" ht="30" customHeight="1">
-      <c r="A73" s="30">
+      <c r="A73" s="28">
         <v>72</v>
       </c>
-      <c r="B73" t="s" s="31">
+      <c r="B73" t="s" s="29">
         <v>226</v>
       </c>
-      <c r="C73" t="s" s="31">
+      <c r="C73" t="s" s="29">
         <v>227</v>
       </c>
-      <c r="D73" s="30">
+      <c r="D73" s="28">
         <v>30</v>
       </c>
-      <c r="E73" t="s" s="31">
+      <c r="E73" t="s" s="29">
         <v>228</v>
       </c>
       <c r="F73" t="s" s="53">
         <v>229</v>
       </c>
-      <c r="G73" t="s" s="45">
+      <c r="G73" t="s" s="43">
         <v>230</v>
       </c>
-      <c r="H73" s="46"/>
+      <c r="H73" s="44"/>
       <c r="I73" t="str" s="5" cm="1">
         <f t="array" ref="I73">B73:B73&amp;": "&amp;C73:C73</f>
         <v>Balanced Tree: AVL Tree</v>
@@ -5822,55 +5818,55 @@
       <c r="J73" s="5"/>
     </row>
     <row r="74" ht="30" customHeight="1">
-      <c r="A74" s="36">
+      <c r="A74" s="34">
         <v>73</v>
       </c>
-      <c r="B74" t="s" s="37">
+      <c r="B74" t="s" s="35">
         <v>226</v>
       </c>
-      <c r="C74" t="s" s="37">
+      <c r="C74" t="s" s="35">
         <v>232</v>
       </c>
-      <c r="D74" s="38"/>
-      <c r="E74" t="s" s="37">
+      <c r="D74" s="36"/>
+      <c r="E74" t="s" s="35">
         <v>228</v>
       </c>
-      <c r="F74" t="s" s="37">
+      <c r="F74" t="s" s="35">
         <v>229</v>
       </c>
-      <c r="G74" t="s" s="47">
+      <c r="G74" t="s" s="45">
         <v>233</v>
       </c>
-      <c r="H74" s="39"/>
-      <c r="I74" t="str" s="24" cm="1">
+      <c r="H74" s="37"/>
+      <c r="I74" t="str" s="22" cm="1">
         <f t="array" ref="I74">B74:B74&amp;": "&amp;C74:C74</f>
         <v>Balanced Tree: Red-Black Tree</v>
       </c>
       <c r="J74" s="4"/>
     </row>
     <row r="75" ht="30" customHeight="1">
-      <c r="A75" s="30">
+      <c r="A75" s="28">
         <v>74</v>
       </c>
-      <c r="B75" t="s" s="31">
+      <c r="B75" t="s" s="29">
         <v>235</v>
       </c>
-      <c r="C75" t="s" s="31">
+      <c r="C75" t="s" s="29">
         <v>236</v>
       </c>
-      <c r="D75" s="30">
+      <c r="D75" s="28">
         <v>31</v>
       </c>
-      <c r="E75" t="s" s="31">
+      <c r="E75" t="s" s="29">
         <v>237</v>
       </c>
-      <c r="F75" t="s" s="31">
+      <c r="F75" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G75" t="s" s="31">
+      <c r="G75" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H75" s="35"/>
+      <c r="H75" s="33"/>
       <c r="I75" t="str" s="5" cm="1">
         <f t="array" ref="I75">B75:B75&amp;": "&amp;C75:C75</f>
         <v>Heap: Min Heap Introduction</v>
@@ -5878,55 +5874,55 @@
       <c r="J75" s="5"/>
     </row>
     <row r="76" ht="30" customHeight="1">
-      <c r="A76" s="36">
+      <c r="A76" s="34">
         <v>75</v>
       </c>
-      <c r="B76" t="s" s="37">
+      <c r="B76" t="s" s="35">
         <v>235</v>
       </c>
-      <c r="C76" t="s" s="37">
+      <c r="C76" t="s" s="35">
         <v>239</v>
       </c>
-      <c r="D76" s="38"/>
-      <c r="E76" t="s" s="37">
+      <c r="D76" s="36"/>
+      <c r="E76" t="s" s="35">
         <v>240</v>
       </c>
-      <c r="F76" t="s" s="37">
+      <c r="F76" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G76" t="s" s="37">
+      <c r="G76" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H76" s="39"/>
-      <c r="I76" t="str" s="24" cm="1">
+      <c r="H76" s="37"/>
+      <c r="I76" t="str" s="22" cm="1">
         <f t="array" ref="I76">B76:B76&amp;": "&amp;C76:C76</f>
         <v>Heap: Priority Queue Usage</v>
       </c>
       <c r="J76" s="4"/>
     </row>
     <row r="77" ht="30" customHeight="1">
-      <c r="A77" s="30">
+      <c r="A77" s="28">
         <v>76</v>
       </c>
-      <c r="B77" t="s" s="31">
+      <c r="B77" t="s" s="29">
         <v>235</v>
       </c>
-      <c r="C77" t="s" s="31">
+      <c r="C77" t="s" s="29">
         <v>242</v>
       </c>
-      <c r="D77" s="30">
+      <c r="D77" s="28">
         <v>32</v>
       </c>
-      <c r="E77" t="s" s="31">
+      <c r="E77" t="s" s="29">
         <v>123</v>
       </c>
-      <c r="F77" t="s" s="31">
+      <c r="F77" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G77" t="s" s="31">
+      <c r="G77" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H77" s="35"/>
+      <c r="H77" s="33"/>
       <c r="I77" t="str" s="5" cm="1">
         <f t="array" ref="I77">B77:B77&amp;": "&amp;C77:C77</f>
         <v>Heap: Kth Largest Element</v>
@@ -5934,55 +5930,55 @@
       <c r="J77" s="5"/>
     </row>
     <row r="78" ht="30" customHeight="1">
-      <c r="A78" s="36">
+      <c r="A78" s="34">
         <v>77</v>
       </c>
-      <c r="B78" t="s" s="37">
+      <c r="B78" t="s" s="35">
         <v>235</v>
       </c>
-      <c r="C78" t="s" s="37">
+      <c r="C78" t="s" s="35">
         <v>244</v>
       </c>
-      <c r="D78" s="38"/>
-      <c r="E78" t="s" s="37">
+      <c r="D78" s="36"/>
+      <c r="E78" t="s" s="35">
         <v>245</v>
       </c>
-      <c r="F78" t="s" s="37">
+      <c r="F78" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G78" t="s" s="37">
+      <c r="G78" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H78" s="39"/>
-      <c r="I78" t="str" s="24" cm="1">
+      <c r="H78" s="37"/>
+      <c r="I78" t="str" s="22" cm="1">
         <f t="array" ref="I78">B78:B78&amp;": "&amp;C78:C78</f>
         <v>Heap: Kth Smallest Element</v>
       </c>
       <c r="J78" s="4"/>
     </row>
     <row r="79" ht="30" customHeight="1">
-      <c r="A79" s="30">
+      <c r="A79" s="28">
         <v>78</v>
       </c>
-      <c r="B79" t="s" s="31">
+      <c r="B79" t="s" s="29">
         <v>235</v>
       </c>
-      <c r="C79" t="s" s="31">
+      <c r="C79" t="s" s="29">
         <v>247</v>
       </c>
-      <c r="D79" s="30">
+      <c r="D79" s="28">
         <v>33</v>
       </c>
-      <c r="E79" t="s" s="31">
+      <c r="E79" t="s" s="29">
         <v>248</v>
       </c>
-      <c r="F79" t="s" s="31">
+      <c r="F79" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G79" t="s" s="31">
+      <c r="G79" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H79" s="35"/>
+      <c r="H79" s="33"/>
       <c r="I79" t="str" s="5" cm="1">
         <f t="array" ref="I79">B79:B79&amp;": "&amp;C79:C79</f>
         <v>Heap: Heap + Sorting Logic</v>
@@ -5990,55 +5986,55 @@
       <c r="J79" s="5"/>
     </row>
     <row r="80" ht="30" customHeight="1">
-      <c r="A80" s="36">
+      <c r="A80" s="34">
         <v>79</v>
       </c>
-      <c r="B80" t="s" s="37">
+      <c r="B80" t="s" s="35">
         <v>235</v>
       </c>
-      <c r="C80" t="s" s="37">
+      <c r="C80" t="s" s="35">
         <v>250</v>
       </c>
-      <c r="D80" s="38"/>
-      <c r="E80" t="s" s="37">
+      <c r="D80" s="36"/>
+      <c r="E80" t="s" s="35">
         <v>251</v>
       </c>
-      <c r="F80" t="s" s="37">
+      <c r="F80" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G80" t="s" s="37">
+      <c r="G80" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H80" s="39"/>
-      <c r="I80" t="str" s="24" cm="1">
+      <c r="H80" s="37"/>
+      <c r="I80" t="str" s="22" cm="1">
         <f t="array" ref="I80">B80:B80&amp;": "&amp;C80:C80</f>
         <v>Heap: Heap + Custom Comparator</v>
       </c>
       <c r="J80" s="4"/>
     </row>
     <row r="81" ht="30" customHeight="1">
-      <c r="A81" s="30">
+      <c r="A81" s="28">
         <v>80</v>
       </c>
-      <c r="B81" t="s" s="31">
+      <c r="B81" t="s" s="29">
         <v>253</v>
       </c>
-      <c r="C81" t="s" s="31">
+      <c r="C81" t="s" s="29">
         <v>254</v>
       </c>
-      <c r="D81" s="30">
+      <c r="D81" s="28">
         <v>34</v>
       </c>
-      <c r="E81" t="s" s="31">
+      <c r="E81" t="s" s="29">
         <v>255</v>
       </c>
-      <c r="F81" t="s" s="31">
+      <c r="F81" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G81" t="s" s="31">
+      <c r="G81" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H81" s="35"/>
+      <c r="H81" s="33"/>
       <c r="I81" t="str" s="5" cm="1">
         <f t="array" ref="I81">B81:B81&amp;": "&amp;C81:C81</f>
         <v>HashMap: Frequency Counting</v>
@@ -6046,53 +6042,53 @@
       <c r="J81" s="5"/>
     </row>
     <row r="82" ht="30" customHeight="1">
-      <c r="A82" s="36">
+      <c r="A82" s="34">
         <v>81</v>
       </c>
-      <c r="B82" t="s" s="37">
+      <c r="B82" t="s" s="35">
         <v>253</v>
       </c>
-      <c r="C82" t="s" s="37">
+      <c r="C82" t="s" s="35">
         <v>254</v>
       </c>
-      <c r="D82" s="38"/>
-      <c r="E82" t="s" s="37">
+      <c r="D82" s="36"/>
+      <c r="E82" t="s" s="35">
         <v>257</v>
       </c>
-      <c r="F82" t="s" s="37">
+      <c r="F82" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G82" t="s" s="37">
+      <c r="G82" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H82" s="39"/>
-      <c r="I82" t="str" s="24" cm="1">
+      <c r="H82" s="37"/>
+      <c r="I82" t="str" s="22" cm="1">
         <f t="array" ref="I82">B82:B82&amp;": "&amp;C82:C82</f>
         <v>HashMap: Frequency Counting</v>
       </c>
       <c r="J82" s="4"/>
     </row>
     <row r="83" ht="30" customHeight="1">
-      <c r="A83" s="30">
+      <c r="A83" s="28">
         <v>82</v>
       </c>
-      <c r="B83" t="s" s="31">
+      <c r="B83" t="s" s="29">
         <v>258</v>
       </c>
-      <c r="C83" t="s" s="31">
+      <c r="C83" t="s" s="29">
         <v>259</v>
       </c>
-      <c r="D83" s="50"/>
-      <c r="E83" t="s" s="31">
+      <c r="D83" s="48"/>
+      <c r="E83" t="s" s="29">
         <v>260</v>
       </c>
-      <c r="F83" t="s" s="31">
+      <c r="F83" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G83" t="s" s="31">
+      <c r="G83" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H83" s="35"/>
+      <c r="H83" s="33"/>
       <c r="I83" t="str" s="5" cm="1">
         <f t="array" ref="I83">B83:B83&amp;": "&amp;C83:C83</f>
         <v>HashSet: Uniqueness Check</v>
@@ -6100,55 +6096,55 @@
       <c r="J83" s="5"/>
     </row>
     <row r="84" ht="30" customHeight="1">
-      <c r="A84" s="36">
+      <c r="A84" s="34">
         <v>83</v>
       </c>
-      <c r="B84" t="s" s="37">
+      <c r="B84" t="s" s="35">
         <v>253</v>
       </c>
-      <c r="C84" t="s" s="37">
+      <c r="C84" t="s" s="35">
         <v>262</v>
       </c>
-      <c r="D84" s="41">
+      <c r="D84" s="39">
         <v>35</v>
       </c>
-      <c r="E84" t="s" s="37">
+      <c r="E84" t="s" s="35">
         <v>263</v>
       </c>
-      <c r="F84" t="s" s="37">
+      <c r="F84" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G84" t="s" s="37">
+      <c r="G84" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H84" s="39"/>
-      <c r="I84" t="str" s="24" cm="1">
+      <c r="H84" s="37"/>
+      <c r="I84" t="str" s="22" cm="1">
         <f t="array" ref="I84">B84:B84&amp;": "&amp;C84:C84</f>
         <v>HashMap: Prefix Sum Technique</v>
       </c>
       <c r="J84" s="4"/>
     </row>
     <row r="85" ht="30" customHeight="1">
-      <c r="A85" s="30">
+      <c r="A85" s="28">
         <v>84</v>
       </c>
-      <c r="B85" t="s" s="31">
+      <c r="B85" t="s" s="29">
         <v>253</v>
       </c>
-      <c r="C85" t="s" s="31">
+      <c r="C85" t="s" s="29">
         <v>265</v>
       </c>
-      <c r="D85" s="50"/>
-      <c r="E85" t="s" s="31">
+      <c r="D85" s="48"/>
+      <c r="E85" t="s" s="29">
         <v>266</v>
       </c>
-      <c r="F85" t="s" s="31">
+      <c r="F85" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G85" t="s" s="31">
+      <c r="G85" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H85" s="35"/>
+      <c r="H85" s="33"/>
       <c r="I85" t="str" s="5" cm="1">
         <f t="array" ref="I85">B85:B85&amp;": "&amp;C85:C85</f>
         <v>HashMap: Prefix Sum Variation</v>
@@ -6156,55 +6152,55 @@
       <c r="J85" s="5"/>
     </row>
     <row r="86" ht="30" customHeight="1">
-      <c r="A86" s="36">
+      <c r="A86" s="34">
         <v>85</v>
       </c>
-      <c r="B86" t="s" s="37">
+      <c r="B86" t="s" s="35">
         <v>253</v>
       </c>
-      <c r="C86" t="s" s="37">
+      <c r="C86" t="s" s="35">
         <v>268</v>
       </c>
-      <c r="D86" s="41">
+      <c r="D86" s="39">
         <v>36</v>
       </c>
-      <c r="E86" t="s" s="37">
+      <c r="E86" t="s" s="35">
         <v>269</v>
       </c>
-      <c r="F86" t="s" s="37">
+      <c r="F86" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G86" t="s" s="37">
+      <c r="G86" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H86" s="39"/>
-      <c r="I86" t="str" s="24" cm="1">
+      <c r="H86" s="37"/>
+      <c r="I86" t="str" s="22" cm="1">
         <f t="array" ref="I86">B86:B86&amp;": "&amp;C86:C86</f>
         <v>HashMap: Grouping Data</v>
       </c>
       <c r="J86" s="4"/>
     </row>
     <row r="87" ht="30" customHeight="1">
-      <c r="A87" s="30">
+      <c r="A87" s="28">
         <v>86</v>
       </c>
-      <c r="B87" t="s" s="31">
+      <c r="B87" t="s" s="29">
         <v>253</v>
       </c>
-      <c r="C87" t="s" s="31">
+      <c r="C87" t="s" s="29">
         <v>271</v>
       </c>
-      <c r="D87" s="50"/>
-      <c r="E87" t="s" s="31">
+      <c r="D87" s="48"/>
+      <c r="E87" t="s" s="29">
         <v>272</v>
       </c>
-      <c r="F87" t="s" s="31">
+      <c r="F87" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G87" t="s" s="31">
+      <c r="G87" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H87" s="35"/>
+      <c r="H87" s="33"/>
       <c r="I87" t="str" s="5" cm="1">
         <f t="array" ref="I87">B87:B87&amp;": "&amp;C87:C87</f>
         <v>HashMap: Longest Streak/Length</v>
@@ -6212,55 +6208,55 @@
       <c r="J87" s="5"/>
     </row>
     <row r="88" ht="30" customHeight="1">
-      <c r="A88" s="36">
+      <c r="A88" s="34">
         <v>87</v>
       </c>
-      <c r="B88" t="s" s="37">
+      <c r="B88" t="s" s="35">
         <v>274</v>
       </c>
-      <c r="C88" t="s" s="37">
+      <c r="C88" t="s" s="35">
         <v>275</v>
       </c>
-      <c r="D88" s="41">
+      <c r="D88" s="39">
         <v>37</v>
       </c>
-      <c r="E88" t="s" s="37">
+      <c r="E88" t="s" s="35">
         <v>276</v>
       </c>
-      <c r="F88" t="s" s="37">
+      <c r="F88" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G88" t="s" s="37">
+      <c r="G88" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H88" s="39"/>
-      <c r="I88" t="str" s="24" cm="1">
+      <c r="H88" s="37"/>
+      <c r="I88" t="str" s="22" cm="1">
         <f t="array" ref="I88">B88:B88&amp;": "&amp;C88:C88</f>
         <v>Graph: BFS Traversal</v>
       </c>
       <c r="J88" s="4"/>
     </row>
     <row r="89" ht="30" customHeight="1">
-      <c r="A89" s="30">
+      <c r="A89" s="28">
         <v>88</v>
       </c>
-      <c r="B89" t="s" s="31">
+      <c r="B89" t="s" s="29">
         <v>274</v>
       </c>
-      <c r="C89" t="s" s="31">
+      <c r="C89" t="s" s="29">
         <v>278</v>
       </c>
-      <c r="D89" s="50"/>
-      <c r="E89" t="s" s="31">
+      <c r="D89" s="48"/>
+      <c r="E89" t="s" s="29">
         <v>279</v>
       </c>
-      <c r="F89" t="s" s="31">
+      <c r="F89" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G89" t="s" s="31">
+      <c r="G89" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H89" s="35"/>
+      <c r="H89" s="33"/>
       <c r="I89" t="str" s="5" cm="1">
         <f t="array" ref="I89">B89:B89&amp;": "&amp;C89:C89</f>
         <v>Graph: DFS Traversal</v>
@@ -6268,55 +6264,55 @@
       <c r="J89" s="5"/>
     </row>
     <row r="90" ht="30" customHeight="1">
-      <c r="A90" s="36">
+      <c r="A90" s="34">
         <v>89</v>
       </c>
-      <c r="B90" t="s" s="37">
+      <c r="B90" t="s" s="35">
         <v>274</v>
       </c>
-      <c r="C90" t="s" s="37">
+      <c r="C90" t="s" s="35">
         <v>281</v>
       </c>
-      <c r="D90" s="38"/>
-      <c r="E90" t="s" s="37">
+      <c r="D90" s="36"/>
+      <c r="E90" t="s" s="35">
         <v>282</v>
       </c>
-      <c r="F90" t="s" s="37">
+      <c r="F90" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G90" t="s" s="37">
+      <c r="G90" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H90" s="39"/>
-      <c r="I90" t="str" s="24" cm="1">
+      <c r="H90" s="37"/>
+      <c r="I90" t="str" s="22" cm="1">
         <f t="array" ref="I90">B90:B90&amp;": "&amp;C90:C90</f>
         <v>Graph: BFS with Distance</v>
       </c>
       <c r="J90" s="4"/>
     </row>
     <row r="91" ht="30" customHeight="1">
-      <c r="A91" s="30">
+      <c r="A91" s="28">
         <v>90</v>
       </c>
-      <c r="B91" t="s" s="31">
+      <c r="B91" t="s" s="29">
         <v>274</v>
       </c>
-      <c r="C91" t="s" s="31">
+      <c r="C91" t="s" s="29">
         <v>284</v>
       </c>
-      <c r="D91" s="30">
+      <c r="D91" s="28">
         <v>38</v>
       </c>
-      <c r="E91" t="s" s="31">
+      <c r="E91" t="s" s="29">
         <v>285</v>
       </c>
-      <c r="F91" t="s" s="31">
+      <c r="F91" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G91" t="s" s="31">
+      <c r="G91" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H91" s="35"/>
+      <c r="H91" s="33"/>
       <c r="I91" t="str" s="5" cm="1">
         <f t="array" ref="I91">B91:B91&amp;": "&amp;C91:C91</f>
         <v>Graph: Dijkstra’s (Shortest Path)</v>
@@ -6324,53 +6320,53 @@
       <c r="J91" s="5"/>
     </row>
     <row r="92" ht="30" customHeight="1">
-      <c r="A92" s="36">
+      <c r="A92" s="34">
         <v>91</v>
       </c>
-      <c r="B92" t="s" s="37">
+      <c r="B92" t="s" s="35">
         <v>274</v>
       </c>
-      <c r="C92" t="s" s="37">
+      <c r="C92" t="s" s="35">
         <v>287</v>
       </c>
-      <c r="D92" s="38"/>
-      <c r="E92" t="s" s="37">
+      <c r="D92" s="36"/>
+      <c r="E92" t="s" s="35">
         <v>288</v>
       </c>
-      <c r="F92" t="s" s="37">
+      <c r="F92" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G92" t="s" s="37">
+      <c r="G92" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H92" s="39"/>
-      <c r="I92" t="str" s="24" cm="1">
+      <c r="H92" s="37"/>
+      <c r="I92" t="str" s="22" cm="1">
         <f t="array" ref="I92">B92:B92&amp;": "&amp;C92:C92</f>
         <v>Graph: Union Find</v>
       </c>
       <c r="J92" s="4"/>
     </row>
     <row r="93" ht="30" customHeight="1">
-      <c r="A93" s="30">
+      <c r="A93" s="28">
         <v>92</v>
       </c>
-      <c r="B93" t="s" s="31">
+      <c r="B93" t="s" s="29">
         <v>274</v>
       </c>
-      <c r="C93" t="s" s="31">
+      <c r="C93" t="s" s="29">
         <v>290</v>
       </c>
-      <c r="D93" s="50"/>
-      <c r="E93" t="s" s="31">
+      <c r="D93" s="48"/>
+      <c r="E93" t="s" s="29">
         <v>291</v>
       </c>
-      <c r="F93" t="s" s="31">
+      <c r="F93" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G93" t="s" s="31">
+      <c r="G93" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H93" s="35"/>
+      <c r="H93" s="33"/>
       <c r="I93" t="str" s="5" cm="1">
         <f t="array" ref="I93">B93:B93&amp;": "&amp;C93:C93</f>
         <v>Graph: Cycle Detection</v>
@@ -6378,55 +6374,55 @@
       <c r="J93" s="5"/>
     </row>
     <row r="94" ht="30" customHeight="1">
-      <c r="A94" s="36">
+      <c r="A94" s="34">
         <v>93</v>
       </c>
-      <c r="B94" t="s" s="37">
+      <c r="B94" t="s" s="35">
         <v>274</v>
       </c>
-      <c r="C94" t="s" s="37">
+      <c r="C94" t="s" s="35">
         <v>293</v>
       </c>
-      <c r="D94" s="41">
+      <c r="D94" s="39">
         <v>39</v>
       </c>
-      <c r="E94" t="s" s="37">
+      <c r="E94" t="s" s="35">
         <v>294</v>
       </c>
-      <c r="F94" t="s" s="37">
+      <c r="F94" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G94" t="s" s="37">
+      <c r="G94" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H94" s="39"/>
-      <c r="I94" t="str" s="24" cm="1">
+      <c r="H94" s="37"/>
+      <c r="I94" t="str" s="22" cm="1">
         <f t="array" ref="I94">B94:B94&amp;": "&amp;C94:C94</f>
         <v>Graph: Topological Sort</v>
       </c>
       <c r="J94" s="4"/>
     </row>
     <row r="95" ht="30" customHeight="1">
-      <c r="A95" s="30">
+      <c r="A95" s="28">
         <v>94</v>
       </c>
-      <c r="B95" t="s" s="31">
+      <c r="B95" t="s" s="29">
         <v>274</v>
       </c>
-      <c r="C95" t="s" s="31">
+      <c r="C95" t="s" s="29">
         <v>296</v>
       </c>
-      <c r="D95" s="50"/>
-      <c r="E95" t="s" s="31">
+      <c r="D95" s="48"/>
+      <c r="E95" t="s" s="29">
         <v>297</v>
       </c>
-      <c r="F95" t="s" s="31">
+      <c r="F95" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G95" t="s" s="31">
+      <c r="G95" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H95" s="35"/>
+      <c r="H95" s="33"/>
       <c r="I95" t="str" s="5" cm="1">
         <f t="array" ref="I95">B95:B95&amp;": "&amp;C95:C95</f>
         <v>Graph: Topo + Ordering</v>
@@ -6434,55 +6430,55 @@
       <c r="J95" s="5"/>
     </row>
     <row r="96" ht="30" customHeight="1">
-      <c r="A96" s="36">
+      <c r="A96" s="34">
         <v>95</v>
       </c>
-      <c r="B96" t="s" s="37">
+      <c r="B96" t="s" s="35">
         <v>274</v>
       </c>
-      <c r="C96" t="s" s="37">
+      <c r="C96" t="s" s="35">
         <v>299</v>
       </c>
-      <c r="D96" s="38"/>
-      <c r="E96" t="s" s="37">
+      <c r="D96" s="36"/>
+      <c r="E96" t="s" s="35">
         <v>300</v>
       </c>
-      <c r="F96" t="s" s="37">
+      <c r="F96" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G96" t="s" s="37">
+      <c r="G96" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H96" s="39"/>
-      <c r="I96" t="str" s="24" cm="1">
+      <c r="H96" s="37"/>
+      <c r="I96" t="str" s="22" cm="1">
         <f t="array" ref="I96">B96:B96&amp;": "&amp;C96:C96</f>
         <v>Graph: Kahn’s Algorithm</v>
       </c>
       <c r="J96" s="4"/>
     </row>
     <row r="97" ht="30" customHeight="1">
-      <c r="A97" s="30">
+      <c r="A97" s="28">
         <v>96</v>
       </c>
-      <c r="B97" t="s" s="31">
+      <c r="B97" t="s" s="29">
         <v>302</v>
       </c>
-      <c r="C97" t="s" s="31">
+      <c r="C97" t="s" s="29">
         <v>303</v>
       </c>
-      <c r="D97" s="30">
+      <c r="D97" s="28">
         <v>40</v>
       </c>
-      <c r="E97" t="s" s="31">
+      <c r="E97" t="s" s="29">
         <v>304</v>
       </c>
-      <c r="F97" t="s" s="31">
+      <c r="F97" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G97" t="s" s="31">
+      <c r="G97" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H97" s="35"/>
+      <c r="H97" s="33"/>
       <c r="I97" t="str" s="5" cm="1">
         <f t="array" ref="I97">B97:B97&amp;": "&amp;C97:C97</f>
         <v>DP: Fibonacci with Memo</v>
@@ -6490,53 +6486,53 @@
       <c r="J97" s="5"/>
     </row>
     <row r="98" ht="30" customHeight="1">
-      <c r="A98" s="36">
+      <c r="A98" s="34">
         <v>97</v>
       </c>
-      <c r="B98" t="s" s="37">
+      <c r="B98" t="s" s="35">
         <v>302</v>
       </c>
-      <c r="C98" t="s" s="37">
+      <c r="C98" t="s" s="35">
         <v>306</v>
       </c>
-      <c r="D98" s="38"/>
-      <c r="E98" t="s" s="37">
+      <c r="D98" s="36"/>
+      <c r="E98" t="s" s="35">
         <v>307</v>
       </c>
-      <c r="F98" t="s" s="37">
+      <c r="F98" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G98" t="s" s="37">
+      <c r="G98" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H98" s="39"/>
-      <c r="I98" t="str" s="24" cm="1">
+      <c r="H98" s="37"/>
+      <c r="I98" t="str" s="22" cm="1">
         <f t="array" ref="I98">B98:B98&amp;": "&amp;C98:C98</f>
         <v>DP: Climbing Stairs (1D)</v>
       </c>
       <c r="J98" s="4"/>
     </row>
     <row r="99" ht="30" customHeight="1">
-      <c r="A99" s="30">
+      <c r="A99" s="28">
         <v>98</v>
       </c>
-      <c r="B99" t="s" s="31">
+      <c r="B99" t="s" s="29">
         <v>302</v>
       </c>
-      <c r="C99" t="s" s="31">
+      <c r="C99" t="s" s="29">
         <v>309</v>
       </c>
-      <c r="D99" s="50"/>
-      <c r="E99" t="s" s="31">
+      <c r="D99" s="48"/>
+      <c r="E99" t="s" s="29">
         <v>310</v>
       </c>
-      <c r="F99" t="s" s="31">
+      <c r="F99" t="s" s="29">
         <v>32</v>
       </c>
-      <c r="G99" t="s" s="31">
+      <c r="G99" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H99" s="35"/>
+      <c r="H99" s="33"/>
       <c r="I99" t="str" s="5" cm="1">
         <f t="array" ref="I99">B99:B99&amp;": "&amp;C99:C99</f>
         <v>DP: Min Cost Climbing</v>
@@ -6544,55 +6540,55 @@
       <c r="J99" s="5"/>
     </row>
     <row r="100" ht="30" customHeight="1">
-      <c r="A100" s="36">
+      <c r="A100" s="34">
         <v>99</v>
       </c>
-      <c r="B100" t="s" s="37">
+      <c r="B100" t="s" s="35">
         <v>302</v>
       </c>
-      <c r="C100" t="s" s="37">
+      <c r="C100" t="s" s="35">
         <v>312</v>
       </c>
-      <c r="D100" s="41">
+      <c r="D100" s="39">
         <v>41</v>
       </c>
-      <c r="E100" t="s" s="37">
+      <c r="E100" t="s" s="35">
         <v>313</v>
       </c>
-      <c r="F100" t="s" s="37">
+      <c r="F100" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G100" t="s" s="37">
+      <c r="G100" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H100" s="39"/>
-      <c r="I100" t="str" s="24" cm="1">
+      <c r="H100" s="37"/>
+      <c r="I100" t="str" s="22" cm="1">
         <f t="array" ref="I100">B100:B100&amp;": "&amp;C100:C100</f>
         <v>DP: Longest Common Subseq</v>
       </c>
       <c r="J100" s="4"/>
     </row>
     <row r="101" ht="30" customHeight="1">
-      <c r="A101" s="30">
+      <c r="A101" s="28">
         <v>100</v>
       </c>
-      <c r="B101" t="s" s="31">
+      <c r="B101" t="s" s="29">
         <v>302</v>
       </c>
-      <c r="C101" t="s" s="31">
+      <c r="C101" t="s" s="29">
         <v>315</v>
       </c>
-      <c r="D101" s="50"/>
-      <c r="E101" t="s" s="31">
+      <c r="D101" s="48"/>
+      <c r="E101" t="s" s="29">
         <v>316</v>
       </c>
-      <c r="F101" t="s" s="31">
+      <c r="F101" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G101" t="s" s="31">
+      <c r="G101" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H101" s="35"/>
+      <c r="H101" s="33"/>
       <c r="I101" t="str" s="5" cm="1">
         <f t="array" ref="I101">B101:B101&amp;": "&amp;C101:C101</f>
         <v>DP: Longest Increasing Subseq</v>
@@ -6600,55 +6596,55 @@
       <c r="J101" s="5"/>
     </row>
     <row r="102" ht="30" customHeight="1">
-      <c r="A102" s="36">
+      <c r="A102" s="34">
         <v>101</v>
       </c>
-      <c r="B102" t="s" s="37">
+      <c r="B102" t="s" s="35">
         <v>302</v>
       </c>
-      <c r="C102" t="s" s="37">
+      <c r="C102" t="s" s="35">
         <v>318</v>
       </c>
-      <c r="D102" s="38"/>
-      <c r="E102" t="s" s="37">
+      <c r="D102" s="36"/>
+      <c r="E102" t="s" s="35">
         <v>319</v>
       </c>
-      <c r="F102" t="s" s="37">
+      <c r="F102" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G102" t="s" s="37">
+      <c r="G102" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H102" s="39"/>
-      <c r="I102" t="str" s="24" cm="1">
+      <c r="H102" s="37"/>
+      <c r="I102" t="str" s="22" cm="1">
         <f t="array" ref="I102">B102:B102&amp;": "&amp;C102:C102</f>
         <v>DP: Palindromic Substrings</v>
       </c>
       <c r="J102" s="4"/>
     </row>
     <row r="103" ht="30" customHeight="1">
-      <c r="A103" s="30">
+      <c r="A103" s="28">
         <v>102</v>
       </c>
-      <c r="B103" t="s" s="31">
+      <c r="B103" t="s" s="29">
         <v>302</v>
       </c>
-      <c r="C103" t="s" s="31">
+      <c r="C103" t="s" s="29">
         <v>321</v>
       </c>
-      <c r="D103" s="30">
+      <c r="D103" s="28">
         <v>42</v>
       </c>
-      <c r="E103" t="s" s="31">
+      <c r="E103" t="s" s="29">
         <v>322</v>
       </c>
-      <c r="F103" t="s" s="31">
+      <c r="F103" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G103" t="s" s="31">
+      <c r="G103" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H103" s="35"/>
+      <c r="H103" s="33"/>
       <c r="I103" t="str" s="5" cm="1">
         <f t="array" ref="I103">B103:B103&amp;": "&amp;C103:C103</f>
         <v>DP: Unique Paths (2D Grid)</v>
@@ -6656,53 +6652,53 @@
       <c r="J103" s="5"/>
     </row>
     <row r="104" ht="30" customHeight="1">
-      <c r="A104" s="36">
+      <c r="A104" s="34">
         <v>103</v>
       </c>
-      <c r="B104" t="s" s="37">
+      <c r="B104" t="s" s="35">
         <v>302</v>
       </c>
-      <c r="C104" t="s" s="37">
+      <c r="C104" t="s" s="35">
         <v>324</v>
       </c>
-      <c r="D104" s="38"/>
-      <c r="E104" t="s" s="37">
+      <c r="D104" s="36"/>
+      <c r="E104" t="s" s="35">
         <v>325</v>
       </c>
-      <c r="F104" t="s" s="37">
+      <c r="F104" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G104" t="s" s="37">
+      <c r="G104" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H104" s="39"/>
-      <c r="I104" t="str" s="24" cm="1">
+      <c r="H104" s="37"/>
+      <c r="I104" t="str" s="22" cm="1">
         <f t="array" ref="I104">B104:B104&amp;": "&amp;C104:C104</f>
         <v>DP: Partition Equal Sum</v>
       </c>
       <c r="J104" s="4"/>
     </row>
     <row r="105" ht="30" customHeight="1">
-      <c r="A105" s="30">
+      <c r="A105" s="28">
         <v>104</v>
       </c>
-      <c r="B105" t="s" s="31">
+      <c r="B105" t="s" s="29">
         <v>302</v>
       </c>
-      <c r="C105" t="s" s="31">
+      <c r="C105" t="s" s="29">
         <v>327</v>
       </c>
-      <c r="D105" s="50"/>
-      <c r="E105" t="s" s="31">
+      <c r="D105" s="48"/>
+      <c r="E105" t="s" s="29">
         <v>328</v>
       </c>
-      <c r="F105" t="s" s="31">
+      <c r="F105" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G105" t="s" s="31">
+      <c r="G105" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H105" s="35"/>
+      <c r="H105" s="33"/>
       <c r="I105" t="str" s="5" cm="1">
         <f t="array" ref="I105">B105:B105&amp;": "&amp;C105:C105</f>
         <v>DP: Target Sum (state model)</v>
@@ -6710,55 +6706,55 @@
       <c r="J105" s="5"/>
     </row>
     <row r="106" ht="30" customHeight="1">
-      <c r="A106" s="36">
+      <c r="A106" s="34">
         <v>105</v>
       </c>
-      <c r="B106" t="s" s="37">
+      <c r="B106" t="s" s="35">
         <v>21</v>
       </c>
-      <c r="C106" t="s" s="37">
+      <c r="C106" t="s" s="35">
         <v>330</v>
       </c>
-      <c r="D106" s="41">
+      <c r="D106" s="39">
         <v>43</v>
       </c>
-      <c r="E106" t="s" s="37">
+      <c r="E106" t="s" s="35">
         <v>134</v>
       </c>
-      <c r="F106" t="s" s="37">
+      <c r="F106" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G106" t="s" s="37">
+      <c r="G106" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H106" s="39"/>
-      <c r="I106" t="str" s="24" cm="1">
+      <c r="H106" s="37"/>
+      <c r="I106" t="str" s="22" cm="1">
         <f t="array" ref="I106">B106:B106&amp;": "&amp;C106:C106</f>
         <v>Greedy: Activity Selection (Intervals)</v>
       </c>
       <c r="J106" s="4"/>
     </row>
     <row r="107" ht="30" customHeight="1">
-      <c r="A107" s="30">
+      <c r="A107" s="28">
         <v>106</v>
       </c>
-      <c r="B107" t="s" s="31">
+      <c r="B107" t="s" s="29">
         <v>21</v>
       </c>
-      <c r="C107" t="s" s="31">
+      <c r="C107" t="s" s="29">
         <v>332</v>
       </c>
-      <c r="D107" s="50"/>
-      <c r="E107" t="s" s="31">
+      <c r="D107" s="48"/>
+      <c r="E107" t="s" s="29">
         <v>130</v>
       </c>
-      <c r="F107" t="s" s="31">
+      <c r="F107" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G107" t="s" s="31">
+      <c r="G107" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H107" s="35"/>
+      <c r="H107" s="33"/>
       <c r="I107" t="str" s="5" cm="1">
         <f t="array" ref="I107">B107:B107&amp;": "&amp;C107:C107</f>
         <v>Greedy: Interval Merging</v>
@@ -6766,55 +6762,55 @@
       <c r="J107" s="5"/>
     </row>
     <row r="108" ht="30" customHeight="1">
-      <c r="A108" s="36">
+      <c r="A108" s="34">
         <v>107</v>
       </c>
-      <c r="B108" t="s" s="37">
+      <c r="B108" t="s" s="35">
         <v>21</v>
       </c>
-      <c r="C108" t="s" s="37">
+      <c r="C108" t="s" s="35">
         <v>334</v>
       </c>
-      <c r="D108" s="38"/>
-      <c r="E108" t="s" s="37">
+      <c r="D108" s="36"/>
+      <c r="E108" t="s" s="35">
         <v>335</v>
       </c>
-      <c r="F108" t="s" s="37">
+      <c r="F108" t="s" s="35">
         <v>46</v>
       </c>
-      <c r="G108" t="s" s="37">
+      <c r="G108" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H108" s="39"/>
-      <c r="I108" t="str" s="24" cm="1">
+      <c r="H108" s="37"/>
+      <c r="I108" t="str" s="22" cm="1">
         <f t="array" ref="I108">B108:B108&amp;": "&amp;C108:C108</f>
         <v>Greedy: Gas Station Problem</v>
       </c>
       <c r="J108" s="4"/>
     </row>
     <row r="109" ht="30" customHeight="1">
-      <c r="A109" s="30">
+      <c r="A109" s="28">
         <v>108</v>
       </c>
-      <c r="B109" t="s" s="31">
+      <c r="B109" t="s" s="29">
         <v>21</v>
       </c>
-      <c r="C109" t="s" s="31">
+      <c r="C109" t="s" s="29">
         <v>337</v>
       </c>
-      <c r="D109" s="30">
+      <c r="D109" s="28">
         <v>44</v>
       </c>
-      <c r="E109" t="s" s="31">
+      <c r="E109" t="s" s="29">
         <v>338</v>
       </c>
-      <c r="F109" t="s" s="31">
+      <c r="F109" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G109" t="s" s="31">
+      <c r="G109" t="s" s="29">
         <v>33</v>
       </c>
-      <c r="H109" s="35"/>
+      <c r="H109" s="33"/>
       <c r="I109" t="str" s="5" cm="1">
         <f t="array" ref="I109">B109:B109&amp;": "&amp;C109:C109</f>
         <v>Greedy: Job Scheduling / Max Profit</v>
@@ -6822,53 +6818,53 @@
       <c r="J109" s="5"/>
     </row>
     <row r="110" ht="30" customHeight="1">
-      <c r="A110" s="36">
+      <c r="A110" s="34">
         <v>109</v>
       </c>
-      <c r="B110" t="s" s="37">
+      <c r="B110" t="s" s="35">
         <v>21</v>
       </c>
-      <c r="C110" t="s" s="37">
+      <c r="C110" t="s" s="35">
         <v>340</v>
       </c>
-      <c r="D110" s="38"/>
-      <c r="E110" t="s" s="37">
+      <c r="D110" s="36"/>
+      <c r="E110" t="s" s="35">
         <v>341</v>
       </c>
-      <c r="F110" t="s" s="37">
+      <c r="F110" t="s" s="35">
         <v>32</v>
       </c>
-      <c r="G110" t="s" s="37">
+      <c r="G110" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="H110" s="39"/>
-      <c r="I110" t="str" s="24" cm="1">
+      <c r="H110" s="37"/>
+      <c r="I110" t="str" s="22" cm="1">
         <f t="array" ref="I110">B110:B110&amp;": "&amp;C110:C110</f>
         <v>Greedy: Resource Assignment</v>
       </c>
       <c r="J110" s="4"/>
     </row>
     <row r="111" ht="30" customHeight="1">
-      <c r="A111" s="30">
+      <c r="A111" s="28">
         <v>110</v>
       </c>
-      <c r="B111" t="s" s="31">
+      <c r="B111" t="s" s="29">
         <v>21</v>
       </c>
-      <c r="C111" t="s" s="31">
+      <c r="C111" t="s" s="29">
         <v>343</v>
       </c>
-      <c r="D111" s="50"/>
-      <c r="E111" t="s" s="31">
+      <c r="D111" s="48"/>
+      <c r="E111" t="s" s="29">
         <v>344</v>
       </c>
-      <c r="F111" t="s" s="31">
+      <c r="F111" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="G111" t="s" s="31">
+      <c r="G111" t="s" s="29">
         <v>38</v>
       </c>
-      <c r="H111" s="35"/>
+      <c r="H111" s="33"/>
       <c r="I111" t="str" s="5" cm="1">
         <f t="array" ref="I111">B111:B111&amp;": "&amp;C111:C111</f>
         <v>Greedy: Jump Game</v>
@@ -6876,29 +6872,29 @@
       <c r="J111" s="5"/>
     </row>
     <row r="112" ht="30" customHeight="1">
-      <c r="A112" s="36">
+      <c r="A112" s="34">
         <v>111</v>
       </c>
-      <c r="B112" t="s" s="37">
+      <c r="B112" t="s" s="35">
         <v>346</v>
       </c>
-      <c r="C112" t="s" s="37">
+      <c r="C112" t="s" s="35">
         <v>347</v>
       </c>
-      <c r="D112" s="41">
+      <c r="D112" s="39">
         <v>45</v>
       </c>
-      <c r="E112" t="s" s="37">
+      <c r="E112" t="s" s="35">
         <v>348</v>
       </c>
-      <c r="F112" t="s" s="37">
+      <c r="F112" t="s" s="35">
         <v>349</v>
       </c>
-      <c r="G112" t="s" s="37">
+      <c r="G112" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="H112" s="39"/>
-      <c r="I112" t="str" s="24" cm="1">
+      <c r="H112" s="37"/>
+      <c r="I112" t="str" s="22" cm="1">
         <f t="array" ref="I112">B112:B112&amp;": "&amp;C112:C112</f>
         <v>Review: Strategy + Topic Recap</v>
       </c>
@@ -6929,14 +6925,14 @@
       <c r="J113" s="5"/>
     </row>
     <row r="114" ht="14.05" customHeight="1">
-      <c r="A114" s="18"/>
-      <c r="B114" s="18"/>
-      <c r="C114" s="18"/>
-      <c r="D114" s="18"/>
-      <c r="E114" s="18"/>
-      <c r="F114" s="18"/>
-      <c r="G114" s="18"/>
-      <c r="H114" s="18"/>
+      <c r="A114" s="17"/>
+      <c r="B114" s="17"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="17"/>
+      <c r="F114" s="17"/>
+      <c r="G114" s="17"/>
+      <c r="H114" s="17"/>
       <c r="I114" s="5"/>
       <c r="J114" s="5"/>
     </row>
@@ -6944,9 +6940,6 @@
   <conditionalFormatting sqref="G1:G22 G28:G114">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
       <formula>$G$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal" stopIfTrue="1">
-      <formula>$G$2</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>